<commit_message>
Updated load_package_data_tables.R to integrate Linakis' volatile chemical data and inhalation related physiologic information into Tables.RData. Do a batch search on the resulting chemicals present in chem.physical_and_invitro.data to check for matches between CAS and chemical name, as well as update the chemical parameters. Update physiologic information in pkdata.xlsx, using data sent from Matt Linakis.
</commit_message>
<xml_diff>
--- a/pkdata.xlsx
+++ b/pkdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\httkdatatables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msfeir\httkdatatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050BECAF-482B-4843-AA96-AAAFC2CD93E0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17683FB7-7FF9-4A74-9D66-037CEB6BE95A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="765" windowWidth="23595" windowHeight="15675" tabRatio="884" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="210" yWindow="0" windowWidth="20490" windowHeight="10335" tabRatio="884" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VolumeFlow" sheetId="14" r:id="rId1"/>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="350">
   <si>
     <t>Tissue</t>
   </si>
@@ -1739,6 +1739,15 @@
   <si>
     <t>EPA, Physiological Parameters Database for PBPK Modeling</t>
   </si>
+  <si>
+    <t>Pulmonary Ventilation Rate</t>
+  </si>
+  <si>
+    <t>l/h/kg^(3/4)</t>
+  </si>
+  <si>
+    <t>Alveolar Dead Space Fraction</t>
+  </si>
 </sst>
 </file>
 
@@ -1749,7 +1758,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1846,13 +1855,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1966,16 +1968,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3821,20 +3823,20 @@
       <c r="L61" s="2"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A62" s="28"/>
+      <c r="A62" s="26"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" s="29" t="s">
+      <c r="A63" s="27" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A64" s="27" t="s">
+      <c r="A64" s="25" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="27" t="s">
+      <c r="A65" s="25" t="s">
         <v>329</v>
       </c>
     </row>
@@ -3858,16 +3860,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -5227,20 +5229,20 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="29" t="s">
         <v>316</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25" t="s">
+      <c r="E1" s="29"/>
+      <c r="F1" s="29" t="s">
         <v>317</v>
       </c>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25" t="s">
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
@@ -6197,31 +6199,31 @@
       <c r="L27" s="2"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="26" t="s">
         <v>43</v>
       </c>
       <c r="L28" s="2"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="26" t="s">
         <v>42</v>
       </c>
       <c r="L29" s="2"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="28" t="s">
+      <c r="A30" s="26" t="s">
         <v>41</v>
       </c>
       <c r="L30" s="2"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="30" t="s">
+      <c r="A31" s="28" t="s">
         <v>345</v>
       </c>
       <c r="L31" s="2"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="26" t="s">
         <v>40</v>
       </c>
       <c r="L32" s="2"/>
@@ -6233,62 +6235,62 @@
       <c r="L33" s="2"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="27" t="s">
+      <c r="A34" s="25" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="25" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="27" t="s">
+      <c r="A36" s="25" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="27" t="s">
+      <c r="A37" s="25" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="27" t="s">
+      <c r="A38" s="25" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="27" t="s">
+      <c r="A39" s="25" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="27" t="s">
+      <c r="A40" s="25" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="27" t="s">
+      <c r="A41" s="25" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="27" t="s">
+      <c r="A42" s="25" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="27" t="s">
+      <c r="A43" s="25" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="27" t="s">
+      <c r="A44" s="25" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="27" t="s">
+      <c r="A45" s="25" t="s">
         <v>331</v>
       </c>
     </row>
@@ -6305,10 +6307,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6711,38 +6713,84 @@
         <v>5.7000000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>347</v>
+      </c>
+      <c r="B16" t="s">
+        <v>348</v>
+      </c>
+      <c r="C16">
+        <v>24.75</v>
+      </c>
+      <c r="D16">
+        <v>24.75</v>
+      </c>
+      <c r="E16">
+        <v>24.75</v>
+      </c>
+      <c r="F16">
+        <v>27.75</v>
+      </c>
+      <c r="G16">
+        <v>24.75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>349</v>
+      </c>
+      <c r="B17" t="s">
+        <v>312</v>
+      </c>
+      <c r="C17">
+        <v>0.33</v>
+      </c>
+      <c r="D17">
+        <v>0.33</v>
+      </c>
+      <c r="E17">
+        <v>0.33</v>
+      </c>
+      <c r="F17">
+        <v>0.33</v>
+      </c>
+      <c r="G17">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="25" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="27" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="25" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="27" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="25" t="s">
         <v>328</v>
       </c>
     </row>
@@ -6764,24 +6812,24 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26" t="s">
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -7759,17 +7807,17 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="25" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="25" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="25" t="s">
         <v>326</v>
       </c>
     </row>
@@ -7791,8 +7839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7802,20 +7850,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26" t="s">
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="2" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -8075,20 +8123,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26" t="s">
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="2" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -11079,26 +11127,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>

</xml_diff>

<commit_message>
Begin adding thyroid pk data sent from Katie Paul-Friedman (Pilari et al. 2017).
</commit_message>
<xml_diff>
--- a/pkdata.xlsx
+++ b/pkdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msfeir\httkdatatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17683FB7-7FF9-4A74-9D66-037CEB6BE95A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9E881D-6851-4952-A0F5-0ECEDDC87C7B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="0" windowWidth="20490" windowHeight="10335" tabRatio="884" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28605" yWindow="855" windowWidth="27525" windowHeight="13185" tabRatio="884" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VolumeFlow" sheetId="14" r:id="rId1"/>
@@ -26,10 +26,10 @@
     <sheet name="PlasmaLipid" sheetId="13" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="bbib18" localSheetId="1">TissueComp!$A$31</definedName>
+    <definedName name="bbib18" localSheetId="1">TissueComp!$A$32</definedName>
     <definedName name="bbib18" localSheetId="0">VolumeFlow!#REF!</definedName>
-    <definedName name="bbib8" localSheetId="1">TissueComp!$A$32</definedName>
-    <definedName name="bbib8" localSheetId="0">TissueComp!$A$36</definedName>
+    <definedName name="bbib8" localSheetId="1">TissueComp!$A$33</definedName>
+    <definedName name="bbib8" localSheetId="0">TissueComp!$A$37</definedName>
     <definedName name="btblfn10" localSheetId="1">TissueComp!#REF!</definedName>
     <definedName name="btblfn10" localSheetId="0">VolumeFlow!#REF!</definedName>
     <definedName name="btblfn11" localSheetId="1">TissueComp!#REF!</definedName>
@@ -40,11 +40,11 @@
     <definedName name="btblfn8" localSheetId="0">VolumeFlow!#REF!</definedName>
     <definedName name="btblfn9" localSheetId="1">TissueComp!#REF!</definedName>
     <definedName name="btblfn9" localSheetId="0">VolumeFlow!#REF!</definedName>
-    <definedName name="tblfn10" localSheetId="1">TissueComp!$A$30</definedName>
+    <definedName name="tblfn10" localSheetId="1">TissueComp!$A$31</definedName>
     <definedName name="tblfn10" localSheetId="0">VolumeFlow!#REF!</definedName>
-    <definedName name="tblfn8" localSheetId="1">TissueComp!$A$28</definedName>
+    <definedName name="tblfn8" localSheetId="1">TissueComp!$A$29</definedName>
     <definedName name="tblfn8" localSheetId="0">VolumeFlow!$A$62</definedName>
-    <definedName name="tblfn9" localSheetId="1">TissueComp!$A$29</definedName>
+    <definedName name="tblfn9" localSheetId="1">TissueComp!$A$30</definedName>
     <definedName name="tblfn9" localSheetId="0">VolumeFlow!$A$63</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="351">
   <si>
     <t>Tissue</t>
   </si>
@@ -1747,6 +1747,9 @@
   </si>
   <si>
     <t>Alveolar Dead Space Fraction</t>
+  </si>
+  <si>
+    <t>Pilari et al. 2017</t>
   </si>
 </sst>
 </file>
@@ -2319,7 +2322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A50" sqref="A50:XFD61"/>
     </sheetView>
   </sheetViews>
@@ -5210,10 +5213,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5701,7 +5704,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -5739,47 +5742,26 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>315</v>
+        <v>350</v>
       </c>
       <c r="D15">
-        <v>0.86</v>
+        <v>0.53500000000000003</v>
       </c>
       <c r="E15">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F15">
-        <v>2.88818990331598E-2</v>
-      </c>
-      <c r="G15">
-        <v>0.91918088619788096</v>
-      </c>
-      <c r="H15">
-        <v>5.1937214768959301E-2</v>
-      </c>
-      <c r="I15">
-        <v>0.99766081871345003</v>
-      </c>
-      <c r="J15">
-        <v>1.8713450292397701E-3</v>
-      </c>
-      <c r="K15">
-        <v>4.6783625730994197E-4</v>
-      </c>
-      <c r="L15">
-        <v>7.1</v>
+        <v>8.8999999999999996E-2</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
@@ -5788,36 +5770,36 @@
         <v>315</v>
       </c>
       <c r="D16">
-        <v>0.9</v>
+        <v>0.86</v>
       </c>
       <c r="E16">
-        <v>0.1</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F16">
-        <v>0.26</v>
+        <v>2.88818990331598E-2</v>
       </c>
       <c r="G16">
-        <v>0.02</v>
+        <v>0.91918088619788096</v>
       </c>
       <c r="H16">
-        <v>0.21</v>
+        <v>5.1937214768959301E-2</v>
       </c>
       <c r="I16">
-        <v>0.85</v>
+        <v>0.99766081871345003</v>
       </c>
       <c r="J16">
-        <v>0.11</v>
+        <v>1.8713450292397701E-3</v>
       </c>
       <c r="K16">
-        <v>0.04</v>
+        <v>4.6783625730994197E-4</v>
       </c>
       <c r="L16">
-        <v>7</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
@@ -5826,36 +5808,36 @@
         <v>315</v>
       </c>
       <c r="D17">
-        <v>0.83799999999999997</v>
+        <v>0.9</v>
       </c>
       <c r="E17">
-        <v>0.16200000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="F17">
-        <v>0.80292051232726702</v>
+        <v>0.26</v>
       </c>
       <c r="G17">
-        <v>0.115353333926677</v>
+        <v>0.02</v>
       </c>
       <c r="H17">
-        <v>8.1726153746056907E-2</v>
+        <v>0.21</v>
       </c>
       <c r="I17">
-        <v>0.95354523227383903</v>
+        <v>0.85</v>
       </c>
       <c r="J17">
-        <v>3.6674816625916901E-2</v>
+        <v>0.11</v>
       </c>
       <c r="K17">
-        <v>9.7799511002445005E-3</v>
+        <v>0.04</v>
       </c>
       <c r="L17">
-        <v>7.1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
@@ -5864,36 +5846,36 @@
         <v>315</v>
       </c>
       <c r="D18">
-        <v>0.9</v>
+        <v>0.83799999999999997</v>
       </c>
       <c r="E18">
-        <v>9.6000000000000002E-2</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="F18">
-        <v>0.78</v>
+        <v>0.80292051232726702</v>
       </c>
       <c r="G18">
-        <v>7.0000000000000007E-2</v>
+        <v>0.115353333926677</v>
       </c>
       <c r="H18">
-        <v>0.15</v>
+        <v>8.1726153746056907E-2</v>
       </c>
       <c r="I18">
-        <v>0.69</v>
+        <v>0.95354523227383903</v>
       </c>
       <c r="J18">
-        <v>0.26</v>
+        <v>3.6674816625916901E-2</v>
       </c>
       <c r="K18">
-        <v>0.05</v>
+        <v>9.7799511002445005E-3</v>
       </c>
       <c r="L18">
-        <v>7</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
@@ -5902,36 +5884,36 @@
         <v>315</v>
       </c>
       <c r="D19">
-        <v>0.86</v>
+        <v>0.9</v>
       </c>
       <c r="E19">
-        <v>0.14000000000000001</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="F19">
-        <v>0.76399672127125895</v>
+        <v>0.78</v>
       </c>
       <c r="G19">
-        <v>3.2882921622291603E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H19">
-        <v>0.20312035710644999</v>
+        <v>0.15</v>
       </c>
       <c r="I19">
-        <v>0.52141527001862198</v>
+        <v>0.69</v>
       </c>
       <c r="J19">
-        <v>0.39478584729981397</v>
+        <v>0.26</v>
       </c>
       <c r="K19">
-        <v>8.3798882681564199E-2</v>
+        <v>0.05</v>
       </c>
       <c r="L19">
-        <v>7.1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
         <v>17</v>
@@ -5940,36 +5922,36 @@
         <v>315</v>
       </c>
       <c r="D20">
-        <v>0.85399999999999998</v>
+        <v>0.86</v>
       </c>
       <c r="E20">
-        <v>0.14599999999999999</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F20">
-        <v>0.75362656390091898</v>
+        <v>0.76399672127125895</v>
       </c>
       <c r="G20">
-        <v>5.2658017463145301E-2</v>
+        <v>3.2882921622291603E-2</v>
       </c>
       <c r="H20">
-        <v>0.193715418635936</v>
+        <v>0.20312035710644999</v>
       </c>
       <c r="I20">
-        <v>0.29246892517669998</v>
+        <v>0.52141527001862198</v>
       </c>
       <c r="J20">
-        <v>0.58493785035339996</v>
+        <v>0.39478584729981397</v>
       </c>
       <c r="K20">
-        <v>0.12259322446989999</v>
+        <v>8.3798882681564199E-2</v>
       </c>
       <c r="L20">
-        <v>7.22</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="B21" t="s">
         <v>17</v>
@@ -5978,36 +5960,36 @@
         <v>315</v>
       </c>
       <c r="D21">
-        <v>0.873</v>
+        <v>0.85399999999999998</v>
       </c>
       <c r="E21">
-        <v>0.127</v>
+        <v>0.14599999999999999</v>
       </c>
       <c r="F21">
-        <v>0.68180834079295904</v>
+        <v>0.75362656390091898</v>
       </c>
       <c r="G21">
-        <v>6.2198013624446602E-2</v>
+        <v>5.2658017463145301E-2</v>
       </c>
       <c r="H21">
-        <v>0.25599364558259502</v>
+        <v>0.193715418635936</v>
       </c>
       <c r="I21">
-        <v>0.33050047214353201</v>
+        <v>0.29246892517669998</v>
       </c>
       <c r="J21">
-        <v>0.561850802644004</v>
+        <v>0.58493785035339996</v>
       </c>
       <c r="K21">
-        <v>0.107648725212465</v>
+        <v>0.12259322446989999</v>
       </c>
       <c r="L21">
-        <v>7.23</v>
+        <v>7.22</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
         <v>17</v>
@@ -6016,36 +5998,36 @@
         <v>315</v>
       </c>
       <c r="D22">
-        <v>0.67500000000000004</v>
+        <v>0.873</v>
       </c>
       <c r="E22">
-        <v>0.32500000000000001</v>
+        <v>0.127</v>
       </c>
       <c r="F22">
-        <v>0.75535011388568196</v>
+        <v>0.68180834079295904</v>
       </c>
       <c r="G22">
-        <v>8.3300793960692399E-2</v>
+        <v>6.2198013624446602E-2</v>
       </c>
       <c r="H22">
-        <v>0.161349092153626</v>
+        <v>0.25599364558259502</v>
       </c>
       <c r="I22">
-        <v>0.57576550641193402</v>
+        <v>0.33050047214353201</v>
       </c>
       <c r="J22">
-        <v>0.32190526040303602</v>
+        <v>0.561850802644004</v>
       </c>
       <c r="K22">
-        <v>0.10232923318503</v>
+        <v>0.107648725212465</v>
       </c>
       <c r="L22">
-        <v>6.6</v>
+        <v>7.23</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B23" t="s">
         <v>17</v>
@@ -6054,36 +6036,36 @@
         <v>315</v>
       </c>
       <c r="D23">
-        <v>0.876</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="E23">
-        <v>0.124</v>
+        <v>0.32500000000000001</v>
       </c>
       <c r="F23">
-        <v>0.77677543363722101</v>
+        <v>0.75535011388568196</v>
       </c>
       <c r="G23">
-        <v>2.3186412508439901E-2</v>
+        <v>8.3300793960692399E-2</v>
       </c>
       <c r="H23">
-        <v>0.20003815385434001</v>
+        <v>0.161349092153626</v>
       </c>
       <c r="I23">
-        <v>0.53390282968499703</v>
+        <v>0.57576550641193402</v>
       </c>
       <c r="J23">
-        <v>0.38441003737319801</v>
+        <v>0.32190526040303602</v>
       </c>
       <c r="K23">
-        <v>8.1687132941804602E-2</v>
+        <v>0.10232923318503</v>
       </c>
       <c r="L23">
-        <v>6.81</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B24" t="s">
         <v>17</v>
@@ -6092,36 +6074,36 @@
         <v>315</v>
       </c>
       <c r="D24">
-        <v>0.68100000000000005</v>
+        <v>0.876</v>
       </c>
       <c r="E24">
-        <v>0.31900000000000001</v>
+        <v>0.124</v>
       </c>
       <c r="F24">
-        <v>0.52200601546333902</v>
+        <v>0.77677543363722101</v>
       </c>
       <c r="G24">
-        <v>6.3830853345103702E-2</v>
+        <v>2.3186412508439901E-2</v>
       </c>
       <c r="H24">
-        <v>0.41416313119155701</v>
+        <v>0.20003815385434001</v>
       </c>
       <c r="I24">
-        <v>0.80753701211305495</v>
+        <v>0.53390282968499703</v>
       </c>
       <c r="J24">
-        <v>0.14804845222072699</v>
+        <v>0.38441003737319801</v>
       </c>
       <c r="K24">
-        <v>4.4414535666218002E-2</v>
+        <v>8.1687132941804602E-2</v>
       </c>
       <c r="L24">
-        <v>7</v>
+        <v>6.81</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B25" t="s">
         <v>17</v>
@@ -6130,28 +6112,28 @@
         <v>315</v>
       </c>
       <c r="D25">
-        <v>0.745</v>
+        <v>0.68100000000000005</v>
       </c>
       <c r="E25">
-        <v>0.255</v>
+        <v>0.31900000000000001</v>
       </c>
       <c r="F25">
-        <v>0.64498977178046801</v>
+        <v>0.52200601546333902</v>
       </c>
       <c r="G25">
-        <v>3.9570322823172903E-2</v>
+        <v>6.3830853345103702E-2</v>
       </c>
       <c r="H25">
-        <v>0.31543990539635902</v>
+        <v>0.41416313119155701</v>
       </c>
       <c r="I25">
-        <v>0.36563071297989003</v>
+        <v>0.80753701211305495</v>
       </c>
       <c r="J25">
-        <v>0.48903107861060302</v>
+        <v>0.14804845222072699</v>
       </c>
       <c r="K25">
-        <v>0.14533820840950601</v>
+        <v>4.4414535666218002E-2</v>
       </c>
       <c r="L25">
         <v>7</v>
@@ -6159,7 +6141,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="B26" t="s">
         <v>17</v>
@@ -6168,129 +6150,167 @@
         <v>315</v>
       </c>
       <c r="D26">
+        <v>0.745</v>
+      </c>
+      <c r="E26">
+        <v>0.255</v>
+      </c>
+      <c r="F26">
+        <v>0.64498977178046801</v>
+      </c>
+      <c r="G26">
+        <v>3.9570322823172903E-2</v>
+      </c>
+      <c r="H26">
+        <v>0.31543990539635902</v>
+      </c>
+      <c r="I26">
+        <v>0.36563071297989003</v>
+      </c>
+      <c r="J26">
+        <v>0.48903107861060302</v>
+      </c>
+      <c r="K26">
+        <v>0.14533820840950601</v>
+      </c>
+      <c r="L26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" t="s">
+        <v>315</v>
+      </c>
+      <c r="D27">
         <v>1</v>
       </c>
-      <c r="E26">
+      <c r="E27">
         <v>0</v>
       </c>
-      <c r="F26">
+      <c r="F27">
         <v>0.66399197592778303</v>
       </c>
-      <c r="G26">
+      <c r="G27">
         <v>5.0150451354062202E-3</v>
       </c>
-      <c r="H26">
+      <c r="H27">
         <v>0.33099297893681001</v>
       </c>
-      <c r="I26">
+      <c r="I27">
         <v>0.22727272727272699</v>
       </c>
-      <c r="J26">
+      <c r="J27">
         <v>0.65909090909090895</v>
       </c>
-      <c r="K26">
+      <c r="K27">
         <v>0.11363636363636399</v>
       </c>
-      <c r="L26">
+      <c r="L27">
         <v>7.2</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L27" s="2"/>
-    </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="26" t="s">
-        <v>43</v>
-      </c>
       <c r="L28" s="2"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L29" s="2"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="L30" s="2"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="28" t="s">
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="28" t="s">
         <v>345</v>
       </c>
-      <c r="L31" s="2"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="26" t="s">
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="L32" s="2"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="L33" s="2"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="25" t="s">
-        <v>343</v>
-      </c>
+      <c r="L34" s="2"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
-        <v>329</v>
+        <v>343</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="25" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="25" t="s">
         <v>331</v>
       </c>
     </row>
@@ -6309,8 +6329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8706,39 +8726,39 @@
         <v>Adipose</v>
       </c>
       <c r="B15" s="2">
-        <f>TissueComp!D15*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!D16*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
         <v>6.2434497816593805E-2</v>
       </c>
       <c r="C15" s="2">
-        <f>TissueComp!E15*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!E16*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
         <v>1.0163755458515271E-2</v>
       </c>
       <c r="D15" s="2">
-        <f>TissueComp!F15*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!F16*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
         <v>2.0967754210754631E-3</v>
       </c>
       <c r="E15" s="2">
-        <f>TissueComp!G15*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!G16*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
         <v>6.6730926781832969E-2</v>
       </c>
       <c r="F15" s="2">
-        <f>TissueComp!H15*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!H16*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
         <v>3.7705510722006431E-3</v>
       </c>
       <c r="G15" s="2">
-        <f>TissueComp!I15*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!I16*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
         <v>7.2428432799611725E-2</v>
       </c>
       <c r="H15" s="2">
-        <f>TissueComp!J15*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!J16*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
         <v>1.3585638039786523E-4</v>
       </c>
       <c r="I15" s="2">
-        <f>TissueComp!K15*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!K16*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
         <v>3.3964095099466268E-5</v>
       </c>
       <c r="J15" s="2">
-        <f>TissueComp!L15*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!L16*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
         <v>0.51544759825327446</v>
       </c>
       <c r="K15" t="s">
@@ -8751,39 +8771,39 @@
         <v>Bone</v>
       </c>
       <c r="B16" s="2">
-        <f>TissueComp!D16*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!D17*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
         <v>3.3245670301475308E-2</v>
       </c>
       <c r="C16" s="2">
-        <f>TissueComp!E16*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!E17*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
         <v>3.69396336683059E-3</v>
       </c>
       <c r="D16" s="2">
-        <f>TissueComp!F16*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!F17*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
         <v>9.6043047537595332E-3</v>
       </c>
       <c r="E16" s="2">
-        <f>TissueComp!G16*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!G17*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
         <v>7.3879267336611791E-4</v>
       </c>
       <c r="F16" s="2">
-        <f>TissueComp!H16*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!H17*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
         <v>7.7573230703442382E-3</v>
       </c>
       <c r="G16" s="2">
-        <f>TissueComp!I16*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!I17*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
         <v>3.1398688618060014E-2</v>
       </c>
       <c r="H16" s="2">
-        <f>TissueComp!J16*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!J17*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
         <v>4.0633597035136483E-3</v>
       </c>
       <c r="I16" s="2">
-        <f>TissueComp!K16*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!K17*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
         <v>1.4775853467322358E-3</v>
       </c>
       <c r="J16" s="2">
-        <f>TissueComp!L16*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!L17*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
         <v>0.25857743567814129</v>
       </c>
       <c r="K16" t="s">
@@ -8796,39 +8816,39 @@
         <v>Brain</v>
       </c>
       <c r="B17" s="2">
-        <f>TissueComp!D17*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!D18*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
         <v>4.6128440366972482E-3</v>
       </c>
       <c r="C17" s="2">
-        <f>TissueComp!E17*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!E18*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
         <v>8.9174311926605511E-4</v>
       </c>
       <c r="D17" s="2">
-        <f>TissueComp!F17*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!F18*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
         <v>4.4197459394161491E-3</v>
       </c>
       <c r="E17" s="2">
-        <f>TissueComp!G17*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!G18*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
         <v>6.3497248033033218E-4</v>
       </c>
       <c r="F17" s="2">
-        <f>TissueComp!H17*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!H18*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
         <v>4.4986873621682705E-4</v>
       </c>
       <c r="G17" s="2">
-        <f>TissueComp!I17*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!I18*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
         <v>5.2488728382046185E-3</v>
       </c>
       <c r="H17" s="2">
-        <f>TissueComp!J17*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!J18*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
         <v>2.0187972454633157E-4</v>
       </c>
       <c r="I17" s="2">
-        <f>TissueComp!K17*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!K18*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
         <v>5.3834593212355052E-5</v>
       </c>
       <c r="J17" s="2">
-        <f>TissueComp!L17*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!L18*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
         <v>3.908256880733945E-2</v>
       </c>
       <c r="K17" t="s">
@@ -8841,39 +8861,39 @@
         <v>Gut</v>
       </c>
       <c r="B18" s="2">
-        <f>TissueComp!D18*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!D19*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
         <v>2.3267100971039019E-2</v>
       </c>
       <c r="C18" s="2">
-        <f>TissueComp!E18*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!E19*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
         <v>2.4818241035774956E-3</v>
       </c>
       <c r="D18" s="2">
-        <f>TissueComp!F18*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!F19*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
         <v>2.0164820841567149E-2</v>
       </c>
       <c r="E18" s="2">
-        <f>TissueComp!G18*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!G19*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
         <v>1.8096634088585906E-3</v>
       </c>
       <c r="F18" s="2">
-        <f>TissueComp!H18*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!H19*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
         <v>3.8778501618398362E-3</v>
       </c>
       <c r="G18" s="2">
-        <f>TissueComp!I18*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!I19*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
         <v>1.7838110744463245E-2</v>
       </c>
       <c r="H18" s="2">
-        <f>TissueComp!J18*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!J19*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
         <v>6.72160694718905E-3</v>
       </c>
       <c r="I18" s="2">
-        <f>TissueComp!K18*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!K19*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
         <v>1.292616720613279E-3</v>
       </c>
       <c r="J18" s="2">
-        <f>TissueComp!L18*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!L19*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
         <v>0.18096634088585903</v>
       </c>
       <c r="K18" t="s">
@@ -8886,39 +8906,39 @@
         <v>Heart</v>
       </c>
       <c r="B19" s="2">
-        <f>TissueComp!D19*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!D20*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
         <v>2.7553398058252423E-3</v>
       </c>
       <c r="C19" s="2">
-        <f>TissueComp!E19*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!E20*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
         <v>4.4854368932038834E-4</v>
       </c>
       <c r="D19" s="2">
-        <f>TissueComp!F19*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!F20*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
         <v>2.4477564856263635E-3</v>
       </c>
       <c r="E19" s="2">
-        <f>TissueComp!G19*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!G20*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
         <v>1.0535304985782745E-4</v>
       </c>
       <c r="F19" s="2">
-        <f>TissueComp!H19*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!H20*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
         <v>6.5077395966144167E-4</v>
       </c>
       <c r="G19" s="2">
-        <f>TissueComp!I19*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!I20*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
         <v>1.6705537777295654E-3</v>
       </c>
       <c r="H19" s="2">
-        <f>TissueComp!J19*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!J20*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
         <v>1.2648478602809573E-3</v>
       </c>
       <c r="I19" s="2">
-        <f>TissueComp!K19*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!K20*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
         <v>2.684818571351086E-4</v>
       </c>
       <c r="J19" s="2">
-        <f>TissueComp!L19*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!L20*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
         <v>2.2747572815533978E-2</v>
       </c>
       <c r="K19" t="s">
@@ -8931,39 +8951,39 @@
         <v>Kidney</v>
       </c>
       <c r="B20" s="2">
-        <f>TissueComp!D20*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!D21*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
         <v>5.9373333333333327E-3</v>
       </c>
       <c r="C20" s="2">
-        <f>TissueComp!E20*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!E21*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
         <v>1.015047619047619E-3</v>
       </c>
       <c r="D20" s="2">
-        <f>TissueComp!F20*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!F21*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
         <v>5.2394989680730553E-3</v>
       </c>
       <c r="E20" s="2">
-        <f>TissueComp!G20*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!G21*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
         <v>3.6609859760091491E-4</v>
       </c>
       <c r="F20" s="2">
-        <f>TissueComp!H20*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!H21*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
         <v>1.3467833867069835E-3</v>
       </c>
       <c r="G20" s="2">
-        <f>TissueComp!I20*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!I21*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
         <v>2.0333553845618187E-3</v>
       </c>
       <c r="H20" s="2">
-        <f>TissueComp!J20*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!J21*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
         <v>4.0667107691236375E-3</v>
       </c>
       <c r="I20" s="2">
-        <f>TissueComp!K20*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!K21*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
         <v>8.5231479869549512E-4</v>
       </c>
       <c r="J20" s="2">
-        <f>TissueComp!L20*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!L21*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
         <v>5.0196190476190471E-2</v>
       </c>
       <c r="K20" t="s">
@@ -8976,39 +8996,39 @@
         <v>Liver</v>
       </c>
       <c r="B21" s="2">
-        <f>TissueComp!D21*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!D22*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
         <v>3.0430285714285715E-2</v>
       </c>
       <c r="C21" s="2">
-        <f>TissueComp!E21*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!E22*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
         <v>4.426857142857143E-3</v>
       </c>
       <c r="D21" s="2">
-        <f>TissueComp!F21*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!F22*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
         <v>2.3765890736211714E-2</v>
       </c>
       <c r="E21" s="2">
-        <f>TissueComp!G21*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!G22*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
         <v>2.1680450463378532E-3</v>
       </c>
       <c r="F21" s="2">
-        <f>TissueComp!H21*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!H22*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
         <v>8.9232070745933114E-3</v>
       </c>
       <c r="G21" s="2">
-        <f>TissueComp!I21*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!I22*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
         <v>1.1520302171860258E-2</v>
       </c>
       <c r="H21" s="2">
-        <f>TissueComp!J21*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!J22*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
         <v>1.9584513692162426E-2</v>
       </c>
       <c r="I21" s="2">
-        <f>TissueComp!K21*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!K22*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
         <v>3.7523269931202087E-3</v>
       </c>
       <c r="J21" s="2">
-        <f>TissueComp!L21*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!L22*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
         <v>0.25201714285714288</v>
       </c>
       <c r="K21" t="s">
@@ -9021,39 +9041,39 @@
         <v>Lung</v>
       </c>
       <c r="B22" s="2">
-        <f>TissueComp!D22*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!D23*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
         <v>3.2127558305568779E-3</v>
       </c>
       <c r="C22" s="2">
-        <f>TissueComp!E22*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!E23*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
         <v>1.5468824369347929E-3</v>
       </c>
       <c r="D22" s="2">
-        <f>TissueComp!F22*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!F23*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
         <v>3.5951933074044834E-3</v>
       </c>
       <c r="E22" s="2">
-        <f>TissueComp!G22*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!G23*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
         <v>3.9648164664775055E-4</v>
       </c>
       <c r="F22" s="2">
-        <f>TissueComp!H22*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!H23*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
         <v>7.6796331343943834E-4</v>
       </c>
       <c r="G22" s="2">
-        <f>TissueComp!I22*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!I23*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
         <v>2.7404355374199621E-3</v>
       </c>
       <c r="H22" s="2">
-        <f>TissueComp!J22*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!J23*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
         <v>1.5321525959211613E-3</v>
       </c>
       <c r="I22" s="2">
-        <f>TissueComp!K22*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!K23*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
         <v>4.8705013415054733E-4</v>
       </c>
       <c r="J22" s="2">
-        <f>TissueComp!L22*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!L23*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
         <v>3.1413612565445025E-2</v>
       </c>
       <c r="K22" t="s">
@@ -9066,39 +9086,39 @@
         <v>Muscle</v>
       </c>
       <c r="B23" s="2">
-        <f>TissueComp!D23*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!D24*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
         <v>0.34021786743515853</v>
       </c>
       <c r="C23" s="2">
-        <f>TissueComp!E23*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!E24*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
         <v>4.8158693563880882E-2</v>
       </c>
       <c r="D23" s="2">
-        <f>TissueComp!F23*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!F24*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
         <v>0.30168137158456143</v>
       </c>
       <c r="E23" s="2">
-        <f>TissueComp!G23*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!G24*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
         <v>9.0050591519329985E-3</v>
       </c>
       <c r="F23" s="2">
-        <f>TissueComp!H23*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!H24*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
         <v>7.7690130262545315E-2</v>
       </c>
       <c r="G23" s="2">
-        <f>TissueComp!I23*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!I24*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
         <v>0.20735534490071497</v>
       </c>
       <c r="H23" s="2">
-        <f>TissueComp!J23*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!J24*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
         <v>0.14929584832851484</v>
       </c>
       <c r="I23" s="2">
-        <f>TissueComp!K23*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!K24*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
         <v>3.1725367769809415E-2</v>
       </c>
       <c r="J23" s="2">
-        <f>TissueComp!L23*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!L24*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
         <v>2.644844380403458</v>
       </c>
       <c r="K23" t="s">
@@ -9111,39 +9131,39 @@
         <v>Skin</v>
       </c>
       <c r="B24" s="2">
-        <f>TissueComp!D24*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!D25*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
         <v>0.11598829325922648</v>
       </c>
       <c r="C24" s="2">
-        <f>TissueComp!E24*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!E25*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
         <v>5.4332254845364525E-2</v>
       </c>
       <c r="D24" s="2">
-        <f>TissueComp!F24*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!F25*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
         <v>8.8908350667609506E-2</v>
       </c>
       <c r="E24" s="2">
-        <f>TissueComp!G24*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!G25*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
         <v>1.0871705927721829E-2</v>
       </c>
       <c r="F24" s="2">
-        <f>TissueComp!H24*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!H25*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
         <v>7.0540491509259617E-2</v>
       </c>
       <c r="G24" s="2">
-        <f>TissueComp!I24*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!I25*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
         <v>0.13754014651783925</v>
       </c>
       <c r="H24" s="2">
-        <f>TissueComp!J24*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!J25*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
         <v>2.521569352827057E-2</v>
       </c>
       <c r="I24" s="2">
-        <f>TissueComp!K24*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!K25*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
         <v>7.5647080584811555E-3</v>
       </c>
       <c r="J24" s="2">
-        <f>TissueComp!L24*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!L25*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
         <v>1.1922438367321369</v>
       </c>
       <c r="K24" t="s">
@@ -9156,39 +9176,39 @@
         <v>Spleen</v>
       </c>
       <c r="B25" s="2">
-        <f>TissueComp!D25*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!D26*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
         <v>1.413662239089184E-3</v>
       </c>
       <c r="C25" s="2">
-        <f>TissueComp!E25*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!E26*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
         <v>4.8387096774193548E-4</v>
       </c>
       <c r="D25" s="2">
-        <f>TissueComp!F25*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!F26*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
         <v>1.2238895100198635E-3</v>
       </c>
       <c r="E25" s="2">
-        <f>TissueComp!G25*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!G26*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
         <v>7.5086001561997919E-5</v>
       </c>
       <c r="F25" s="2">
-        <f>TissueComp!H25*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!H26*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
         <v>5.9855769524925812E-4</v>
       </c>
       <c r="G25" s="2">
-        <f>TissueComp!I25*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!I26*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
         <v>6.9379641931667936E-4</v>
       </c>
       <c r="H25" s="2">
-        <f>TissueComp!J25*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!J26*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
         <v>9.2795271083605886E-4</v>
       </c>
       <c r="I25" s="2">
-        <f>TissueComp!K25*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!K26*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
         <v>2.7578407667837952E-4</v>
       </c>
       <c r="J25" s="2">
-        <f>TissueComp!L25*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!L26*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
         <v>1.3282732447817837E-2</v>
       </c>
       <c r="K25" t="s">
@@ -11118,7 +11138,7 @@
   <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Remove thyroid data that I had begun to add from pkdata.xlsx because the tissue components as listed for the human thyroid were imbalanced. Contact the author? Will wait until a better approach for the thyroid is clear. Update load_package_data_tables.R to use the .csv version of Linakis data, with references updated.
</commit_message>
<xml_diff>
--- a/pkdata.xlsx
+++ b/pkdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msfeir\httkdatatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9E881D-6851-4952-A0F5-0ECEDDC87C7B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FEF712-9D5E-4247-9F2F-16986FCF34D5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28605" yWindow="855" windowWidth="27525" windowHeight="13185" tabRatio="884" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28410" yWindow="435" windowWidth="27525" windowHeight="13185" tabRatio="884" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VolumeFlow" sheetId="14" r:id="rId1"/>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="350">
   <si>
     <t>Tissue</t>
   </si>
@@ -1747,9 +1747,6 @@
   </si>
   <si>
     <t>Alveolar Dead Space Fraction</t>
-  </si>
-  <si>
-    <t>Pilari et al. 2017</t>
   </si>
 </sst>
 </file>
@@ -5215,8 +5212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5742,26 +5739,47 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>350</v>
+        <v>315</v>
       </c>
       <c r="D15">
-        <v>0.53500000000000003</v>
+        <v>0.86</v>
       </c>
       <c r="E15">
-        <v>8.8999999999999996E-2</v>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F15">
+        <v>2.88818990331598E-2</v>
+      </c>
+      <c r="G15">
+        <v>0.91918088619788096</v>
+      </c>
+      <c r="H15">
+        <v>5.1937214768959301E-2</v>
+      </c>
+      <c r="I15">
+        <v>0.99766081871345003</v>
+      </c>
+      <c r="J15">
+        <v>1.8713450292397701E-3</v>
+      </c>
+      <c r="K15">
+        <v>4.6783625730994197E-4</v>
+      </c>
+      <c r="L15">
+        <v>7.1</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
@@ -5770,36 +5788,36 @@
         <v>315</v>
       </c>
       <c r="D16">
-        <v>0.86</v>
+        <v>0.9</v>
       </c>
       <c r="E16">
-        <v>0.14000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="F16">
-        <v>2.88818990331598E-2</v>
+        <v>0.26</v>
       </c>
       <c r="G16">
-        <v>0.91918088619788096</v>
+        <v>0.02</v>
       </c>
       <c r="H16">
-        <v>5.1937214768959301E-2</v>
+        <v>0.21</v>
       </c>
       <c r="I16">
-        <v>0.99766081871345003</v>
+        <v>0.85</v>
       </c>
       <c r="J16">
-        <v>1.8713450292397701E-3</v>
+        <v>0.11</v>
       </c>
       <c r="K16">
-        <v>4.6783625730994197E-4</v>
+        <v>0.04</v>
       </c>
       <c r="L16">
-        <v>7.1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
@@ -5808,36 +5826,36 @@
         <v>315</v>
       </c>
       <c r="D17">
-        <v>0.9</v>
+        <v>0.83799999999999997</v>
       </c>
       <c r="E17">
-        <v>0.1</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="F17">
-        <v>0.26</v>
+        <v>0.80292051232726702</v>
       </c>
       <c r="G17">
-        <v>0.02</v>
+        <v>0.115353333926677</v>
       </c>
       <c r="H17">
-        <v>0.21</v>
+        <v>8.1726153746056907E-2</v>
       </c>
       <c r="I17">
-        <v>0.85</v>
+        <v>0.95354523227383903</v>
       </c>
       <c r="J17">
-        <v>0.11</v>
+        <v>3.6674816625916901E-2</v>
       </c>
       <c r="K17">
-        <v>0.04</v>
+        <v>9.7799511002445005E-3</v>
       </c>
       <c r="L17">
-        <v>7</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
@@ -5846,36 +5864,36 @@
         <v>315</v>
       </c>
       <c r="D18">
-        <v>0.83799999999999997</v>
+        <v>0.9</v>
       </c>
       <c r="E18">
-        <v>0.16200000000000001</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="F18">
-        <v>0.80292051232726702</v>
+        <v>0.78</v>
       </c>
       <c r="G18">
-        <v>0.115353333926677</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H18">
-        <v>8.1726153746056907E-2</v>
+        <v>0.15</v>
       </c>
       <c r="I18">
-        <v>0.95354523227383903</v>
+        <v>0.69</v>
       </c>
       <c r="J18">
-        <v>3.6674816625916901E-2</v>
+        <v>0.26</v>
       </c>
       <c r="K18">
-        <v>9.7799511002445005E-3</v>
+        <v>0.05</v>
       </c>
       <c r="L18">
-        <v>7.1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
@@ -5884,36 +5902,36 @@
         <v>315</v>
       </c>
       <c r="D19">
-        <v>0.9</v>
+        <v>0.86</v>
       </c>
       <c r="E19">
-        <v>9.6000000000000002E-2</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F19">
-        <v>0.78</v>
+        <v>0.76399672127125895</v>
       </c>
       <c r="G19">
-        <v>7.0000000000000007E-2</v>
+        <v>3.2882921622291603E-2</v>
       </c>
       <c r="H19">
-        <v>0.15</v>
+        <v>0.20312035710644999</v>
       </c>
       <c r="I19">
-        <v>0.69</v>
+        <v>0.52141527001862198</v>
       </c>
       <c r="J19">
-        <v>0.26</v>
+        <v>0.39478584729981397</v>
       </c>
       <c r="K19">
-        <v>0.05</v>
+        <v>8.3798882681564199E-2</v>
       </c>
       <c r="L19">
-        <v>7</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
         <v>17</v>
@@ -5922,36 +5940,36 @@
         <v>315</v>
       </c>
       <c r="D20">
-        <v>0.86</v>
+        <v>0.85399999999999998</v>
       </c>
       <c r="E20">
-        <v>0.14000000000000001</v>
+        <v>0.14599999999999999</v>
       </c>
       <c r="F20">
-        <v>0.76399672127125895</v>
+        <v>0.75362656390091898</v>
       </c>
       <c r="G20">
-        <v>3.2882921622291603E-2</v>
+        <v>5.2658017463145301E-2</v>
       </c>
       <c r="H20">
-        <v>0.20312035710644999</v>
+        <v>0.193715418635936</v>
       </c>
       <c r="I20">
-        <v>0.52141527001862198</v>
+        <v>0.29246892517669998</v>
       </c>
       <c r="J20">
-        <v>0.39478584729981397</v>
+        <v>0.58493785035339996</v>
       </c>
       <c r="K20">
-        <v>8.3798882681564199E-2</v>
+        <v>0.12259322446989999</v>
       </c>
       <c r="L20">
-        <v>7.1</v>
+        <v>7.22</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
         <v>17</v>
@@ -5960,36 +5978,36 @@
         <v>315</v>
       </c>
       <c r="D21">
-        <v>0.85399999999999998</v>
+        <v>0.873</v>
       </c>
       <c r="E21">
-        <v>0.14599999999999999</v>
+        <v>0.127</v>
       </c>
       <c r="F21">
-        <v>0.75362656390091898</v>
+        <v>0.68180834079295904</v>
       </c>
       <c r="G21">
-        <v>5.2658017463145301E-2</v>
+        <v>6.2198013624446602E-2</v>
       </c>
       <c r="H21">
-        <v>0.193715418635936</v>
+        <v>0.25599364558259502</v>
       </c>
       <c r="I21">
-        <v>0.29246892517669998</v>
+        <v>0.33050047214353201</v>
       </c>
       <c r="J21">
-        <v>0.58493785035339996</v>
+        <v>0.561850802644004</v>
       </c>
       <c r="K21">
-        <v>0.12259322446989999</v>
+        <v>0.107648725212465</v>
       </c>
       <c r="L21">
-        <v>7.22</v>
+        <v>7.23</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="B22" t="s">
         <v>17</v>
@@ -5998,36 +6016,36 @@
         <v>315</v>
       </c>
       <c r="D22">
-        <v>0.873</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="E22">
-        <v>0.127</v>
+        <v>0.32500000000000001</v>
       </c>
       <c r="F22">
-        <v>0.68180834079295904</v>
+        <v>0.75535011388568196</v>
       </c>
       <c r="G22">
-        <v>6.2198013624446602E-2</v>
+        <v>8.3300793960692399E-2</v>
       </c>
       <c r="H22">
-        <v>0.25599364558259502</v>
+        <v>0.161349092153626</v>
       </c>
       <c r="I22">
-        <v>0.33050047214353201</v>
+        <v>0.57576550641193402</v>
       </c>
       <c r="J22">
-        <v>0.561850802644004</v>
+        <v>0.32190526040303602</v>
       </c>
       <c r="K22">
-        <v>0.107648725212465</v>
+        <v>0.10232923318503</v>
       </c>
       <c r="L22">
-        <v>7.23</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="B23" t="s">
         <v>17</v>
@@ -6036,36 +6054,36 @@
         <v>315</v>
       </c>
       <c r="D23">
-        <v>0.67500000000000004</v>
+        <v>0.876</v>
       </c>
       <c r="E23">
-        <v>0.32500000000000001</v>
+        <v>0.124</v>
       </c>
       <c r="F23">
-        <v>0.75535011388568196</v>
+        <v>0.77677543363722101</v>
       </c>
       <c r="G23">
-        <v>8.3300793960692399E-2</v>
+        <v>2.3186412508439901E-2</v>
       </c>
       <c r="H23">
-        <v>0.161349092153626</v>
+        <v>0.20003815385434001</v>
       </c>
       <c r="I23">
-        <v>0.57576550641193402</v>
+        <v>0.53390282968499703</v>
       </c>
       <c r="J23">
-        <v>0.32190526040303602</v>
+        <v>0.38441003737319801</v>
       </c>
       <c r="K23">
-        <v>0.10232923318503</v>
+        <v>8.1687132941804602E-2</v>
       </c>
       <c r="L23">
-        <v>6.6</v>
+        <v>6.81</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B24" t="s">
         <v>17</v>
@@ -6074,36 +6092,36 @@
         <v>315</v>
       </c>
       <c r="D24">
-        <v>0.876</v>
+        <v>0.68100000000000005</v>
       </c>
       <c r="E24">
-        <v>0.124</v>
+        <v>0.31900000000000001</v>
       </c>
       <c r="F24">
-        <v>0.77677543363722101</v>
+        <v>0.52200601546333902</v>
       </c>
       <c r="G24">
-        <v>2.3186412508439901E-2</v>
+        <v>6.3830853345103702E-2</v>
       </c>
       <c r="H24">
-        <v>0.20003815385434001</v>
+        <v>0.41416313119155701</v>
       </c>
       <c r="I24">
-        <v>0.53390282968499703</v>
+        <v>0.80753701211305495</v>
       </c>
       <c r="J24">
-        <v>0.38441003737319801</v>
+        <v>0.14804845222072699</v>
       </c>
       <c r="K24">
-        <v>8.1687132941804602E-2</v>
+        <v>4.4414535666218002E-2</v>
       </c>
       <c r="L24">
-        <v>6.81</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s">
         <v>17</v>
@@ -6112,28 +6130,28 @@
         <v>315</v>
       </c>
       <c r="D25">
-        <v>0.68100000000000005</v>
+        <v>0.745</v>
       </c>
       <c r="E25">
-        <v>0.31900000000000001</v>
+        <v>0.255</v>
       </c>
       <c r="F25">
-        <v>0.52200601546333902</v>
+        <v>0.64498977178046801</v>
       </c>
       <c r="G25">
-        <v>6.3830853345103702E-2</v>
+        <v>3.9570322823172903E-2</v>
       </c>
       <c r="H25">
-        <v>0.41416313119155701</v>
+        <v>0.31543990539635902</v>
       </c>
       <c r="I25">
-        <v>0.80753701211305495</v>
+        <v>0.36563071297989003</v>
       </c>
       <c r="J25">
-        <v>0.14804845222072699</v>
+        <v>0.48903107861060302</v>
       </c>
       <c r="K25">
-        <v>4.4414535666218002E-2</v>
+        <v>0.14533820840950601</v>
       </c>
       <c r="L25">
         <v>7</v>
@@ -6141,7 +6159,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="B26" t="s">
         <v>17</v>
@@ -6150,70 +6168,35 @@
         <v>315</v>
       </c>
       <c r="D26">
-        <v>0.745</v>
+        <v>1</v>
       </c>
       <c r="E26">
-        <v>0.255</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>0.64498977178046801</v>
+        <v>0.66399197592778303</v>
       </c>
       <c r="G26">
-        <v>3.9570322823172903E-2</v>
+        <v>5.0150451354062202E-3</v>
       </c>
       <c r="H26">
-        <v>0.31543990539635902</v>
+        <v>0.33099297893681001</v>
       </c>
       <c r="I26">
-        <v>0.36563071297989003</v>
+        <v>0.22727272727272699</v>
       </c>
       <c r="J26">
-        <v>0.48903107861060302</v>
+        <v>0.65909090909090895</v>
       </c>
       <c r="K26">
-        <v>0.14533820840950601</v>
+        <v>0.11363636363636399</v>
       </c>
       <c r="L26">
-        <v>7</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" t="s">
-        <v>315</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>0.66399197592778303</v>
-      </c>
-      <c r="G27">
-        <v>5.0150451354062202E-3</v>
-      </c>
-      <c r="H27">
-        <v>0.33099297893681001</v>
-      </c>
-      <c r="I27">
-        <v>0.22727272727272699</v>
-      </c>
-      <c r="J27">
-        <v>0.65909090909090895</v>
-      </c>
-      <c r="K27">
-        <v>0.11363636363636399</v>
-      </c>
-      <c r="L27">
-        <v>7.2</v>
-      </c>
+      <c r="L27" s="2"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L28" s="2"/>
@@ -6252,7 +6235,6 @@
       <c r="A34" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="L34" s="2"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
@@ -8726,39 +8708,39 @@
         <v>Adipose</v>
       </c>
       <c r="B15" s="2">
-        <f>TissueComp!D16*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!D15*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
         <v>6.2434497816593805E-2</v>
       </c>
       <c r="C15" s="2">
-        <f>TissueComp!E16*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!E15*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
         <v>1.0163755458515271E-2</v>
       </c>
       <c r="D15" s="2">
-        <f>TissueComp!F16*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!F15*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
         <v>2.0967754210754631E-3</v>
       </c>
       <c r="E15" s="2">
-        <f>TissueComp!G16*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!G15*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
         <v>6.6730926781832969E-2</v>
       </c>
       <c r="F15" s="2">
-        <f>TissueComp!H16*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!H15*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
         <v>3.7705510722006431E-3</v>
       </c>
       <c r="G15" s="2">
-        <f>TissueComp!I16*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!I15*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
         <v>7.2428432799611725E-2</v>
       </c>
       <c r="H15" s="2">
-        <f>TissueComp!J16*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!J15*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
         <v>1.3585638039786523E-4</v>
       </c>
       <c r="I15" s="2">
-        <f>TissueComp!K16*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!K15*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
         <v>3.3964095099466268E-5</v>
       </c>
       <c r="J15" s="2">
-        <f>TissueComp!L16*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!L15*INDEX(VolumeFlow!$A13:$D25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
         <v>0.51544759825327446</v>
       </c>
       <c r="K15" t="s">
@@ -8771,39 +8753,39 @@
         <v>Bone</v>
       </c>
       <c r="B16" s="2">
-        <f>TissueComp!D17*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!D16*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
         <v>3.3245670301475308E-2</v>
       </c>
       <c r="C16" s="2">
-        <f>TissueComp!E17*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!E16*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
         <v>3.69396336683059E-3</v>
       </c>
       <c r="D16" s="2">
-        <f>TissueComp!F17*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!F16*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
         <v>9.6043047537595332E-3</v>
       </c>
       <c r="E16" s="2">
-        <f>TissueComp!G17*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!G16*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
         <v>7.3879267336611791E-4</v>
       </c>
       <c r="F16" s="2">
-        <f>TissueComp!H17*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!H16*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
         <v>7.7573230703442382E-3</v>
       </c>
       <c r="G16" s="2">
-        <f>TissueComp!I17*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!I16*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
         <v>3.1398688618060014E-2</v>
       </c>
       <c r="H16" s="2">
-        <f>TissueComp!J17*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!J16*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
         <v>4.0633597035136483E-3</v>
       </c>
       <c r="I16" s="2">
-        <f>TissueComp!K17*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!K16*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
         <v>1.4775853467322358E-3</v>
       </c>
       <c r="J16" s="2">
-        <f>TissueComp!L17*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!L16*INDEX(VolumeFlow!$A14:$D26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
         <v>0.25857743567814129</v>
       </c>
       <c r="K16" t="s">
@@ -8816,39 +8798,39 @@
         <v>Brain</v>
       </c>
       <c r="B17" s="2">
-        <f>TissueComp!D18*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!D17*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
         <v>4.6128440366972482E-3</v>
       </c>
       <c r="C17" s="2">
-        <f>TissueComp!E18*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!E17*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
         <v>8.9174311926605511E-4</v>
       </c>
       <c r="D17" s="2">
-        <f>TissueComp!F18*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!F17*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
         <v>4.4197459394161491E-3</v>
       </c>
       <c r="E17" s="2">
-        <f>TissueComp!G18*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!G17*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
         <v>6.3497248033033218E-4</v>
       </c>
       <c r="F17" s="2">
-        <f>TissueComp!H18*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!H17*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
         <v>4.4986873621682705E-4</v>
       </c>
       <c r="G17" s="2">
-        <f>TissueComp!I18*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!I17*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
         <v>5.2488728382046185E-3</v>
       </c>
       <c r="H17" s="2">
-        <f>TissueComp!J18*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!J17*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
         <v>2.0187972454633157E-4</v>
       </c>
       <c r="I17" s="2">
-        <f>TissueComp!K18*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!K17*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
         <v>5.3834593212355052E-5</v>
       </c>
       <c r="J17" s="2">
-        <f>TissueComp!L18*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!L17*INDEX(VolumeFlow!$A15:$D27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
         <v>3.908256880733945E-2</v>
       </c>
       <c r="K17" t="s">
@@ -8861,39 +8843,39 @@
         <v>Gut</v>
       </c>
       <c r="B18" s="2">
-        <f>TissueComp!D19*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!D18*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
         <v>2.3267100971039019E-2</v>
       </c>
       <c r="C18" s="2">
-        <f>TissueComp!E19*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!E18*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
         <v>2.4818241035774956E-3</v>
       </c>
       <c r="D18" s="2">
-        <f>TissueComp!F19*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!F18*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
         <v>2.0164820841567149E-2</v>
       </c>
       <c r="E18" s="2">
-        <f>TissueComp!G19*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!G18*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
         <v>1.8096634088585906E-3</v>
       </c>
       <c r="F18" s="2">
-        <f>TissueComp!H19*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!H18*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
         <v>3.8778501618398362E-3</v>
       </c>
       <c r="G18" s="2">
-        <f>TissueComp!I19*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!I18*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
         <v>1.7838110744463245E-2</v>
       </c>
       <c r="H18" s="2">
-        <f>TissueComp!J19*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!J18*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
         <v>6.72160694718905E-3</v>
       </c>
       <c r="I18" s="2">
-        <f>TissueComp!K19*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!K18*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
         <v>1.292616720613279E-3</v>
       </c>
       <c r="J18" s="2">
-        <f>TissueComp!L19*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!L18*INDEX(VolumeFlow!$A16:$D28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
         <v>0.18096634088585903</v>
       </c>
       <c r="K18" t="s">
@@ -8906,39 +8888,39 @@
         <v>Heart</v>
       </c>
       <c r="B19" s="2">
-        <f>TissueComp!D20*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!D19*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
         <v>2.7553398058252423E-3</v>
       </c>
       <c r="C19" s="2">
-        <f>TissueComp!E20*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!E19*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
         <v>4.4854368932038834E-4</v>
       </c>
       <c r="D19" s="2">
-        <f>TissueComp!F20*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!F19*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
         <v>2.4477564856263635E-3</v>
       </c>
       <c r="E19" s="2">
-        <f>TissueComp!G20*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!G19*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
         <v>1.0535304985782745E-4</v>
       </c>
       <c r="F19" s="2">
-        <f>TissueComp!H20*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!H19*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
         <v>6.5077395966144167E-4</v>
       </c>
       <c r="G19" s="2">
-        <f>TissueComp!I20*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!I19*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
         <v>1.6705537777295654E-3</v>
       </c>
       <c r="H19" s="2">
-        <f>TissueComp!J20*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!J19*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
         <v>1.2648478602809573E-3</v>
       </c>
       <c r="I19" s="2">
-        <f>TissueComp!K20*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!K19*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
         <v>2.684818571351086E-4</v>
       </c>
       <c r="J19" s="2">
-        <f>TissueComp!L20*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!L19*INDEX(VolumeFlow!$A17:$D29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
         <v>2.2747572815533978E-2</v>
       </c>
       <c r="K19" t="s">
@@ -8951,39 +8933,39 @@
         <v>Kidney</v>
       </c>
       <c r="B20" s="2">
-        <f>TissueComp!D21*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!D20*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
         <v>5.9373333333333327E-3</v>
       </c>
       <c r="C20" s="2">
-        <f>TissueComp!E21*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!E20*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
         <v>1.015047619047619E-3</v>
       </c>
       <c r="D20" s="2">
-        <f>TissueComp!F21*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!F20*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
         <v>5.2394989680730553E-3</v>
       </c>
       <c r="E20" s="2">
-        <f>TissueComp!G21*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!G20*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
         <v>3.6609859760091491E-4</v>
       </c>
       <c r="F20" s="2">
-        <f>TissueComp!H21*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!H20*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
         <v>1.3467833867069835E-3</v>
       </c>
       <c r="G20" s="2">
-        <f>TissueComp!I21*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!I20*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
         <v>2.0333553845618187E-3</v>
       </c>
       <c r="H20" s="2">
-        <f>TissueComp!J21*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!J20*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
         <v>4.0667107691236375E-3</v>
       </c>
       <c r="I20" s="2">
-        <f>TissueComp!K21*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!K20*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
         <v>8.5231479869549512E-4</v>
       </c>
       <c r="J20" s="2">
-        <f>TissueComp!L21*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!L20*INDEX(VolumeFlow!$A18:$D30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
         <v>5.0196190476190471E-2</v>
       </c>
       <c r="K20" t="s">
@@ -8996,39 +8978,39 @@
         <v>Liver</v>
       </c>
       <c r="B21" s="2">
-        <f>TissueComp!D22*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!D21*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
         <v>3.0430285714285715E-2</v>
       </c>
       <c r="C21" s="2">
-        <f>TissueComp!E22*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!E21*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
         <v>4.426857142857143E-3</v>
       </c>
       <c r="D21" s="2">
-        <f>TissueComp!F22*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!F21*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
         <v>2.3765890736211714E-2</v>
       </c>
       <c r="E21" s="2">
-        <f>TissueComp!G22*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!G21*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
         <v>2.1680450463378532E-3</v>
       </c>
       <c r="F21" s="2">
-        <f>TissueComp!H22*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!H21*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
         <v>8.9232070745933114E-3</v>
       </c>
       <c r="G21" s="2">
-        <f>TissueComp!I22*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!I21*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
         <v>1.1520302171860258E-2</v>
       </c>
       <c r="H21" s="2">
-        <f>TissueComp!J22*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!J21*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
         <v>1.9584513692162426E-2</v>
       </c>
       <c r="I21" s="2">
-        <f>TissueComp!K22*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!K21*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
         <v>3.7523269931202087E-3</v>
       </c>
       <c r="J21" s="2">
-        <f>TissueComp!L22*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!L21*INDEX(VolumeFlow!$A19:$D31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
         <v>0.25201714285714288</v>
       </c>
       <c r="K21" t="s">
@@ -9041,39 +9023,39 @@
         <v>Lung</v>
       </c>
       <c r="B22" s="2">
-        <f>TissueComp!D23*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!D22*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
         <v>3.2127558305568779E-3</v>
       </c>
       <c r="C22" s="2">
-        <f>TissueComp!E23*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!E22*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
         <v>1.5468824369347929E-3</v>
       </c>
       <c r="D22" s="2">
-        <f>TissueComp!F23*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!F22*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
         <v>3.5951933074044834E-3</v>
       </c>
       <c r="E22" s="2">
-        <f>TissueComp!G23*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!G22*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
         <v>3.9648164664775055E-4</v>
       </c>
       <c r="F22" s="2">
-        <f>TissueComp!H23*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!H22*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
         <v>7.6796331343943834E-4</v>
       </c>
       <c r="G22" s="2">
-        <f>TissueComp!I23*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!I22*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
         <v>2.7404355374199621E-3</v>
       </c>
       <c r="H22" s="2">
-        <f>TissueComp!J23*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!J22*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
         <v>1.5321525959211613E-3</v>
       </c>
       <c r="I22" s="2">
-        <f>TissueComp!K23*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!K22*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
         <v>4.8705013415054733E-4</v>
       </c>
       <c r="J22" s="2">
-        <f>TissueComp!L23*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!L22*INDEX(VolumeFlow!$A20:$D32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
         <v>3.1413612565445025E-2</v>
       </c>
       <c r="K22" t="s">
@@ -9086,39 +9068,39 @@
         <v>Muscle</v>
       </c>
       <c r="B23" s="2">
-        <f>TissueComp!D24*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!D23*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
         <v>0.34021786743515853</v>
       </c>
       <c r="C23" s="2">
-        <f>TissueComp!E24*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!E23*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
         <v>4.8158693563880882E-2</v>
       </c>
       <c r="D23" s="2">
-        <f>TissueComp!F24*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!F23*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
         <v>0.30168137158456143</v>
       </c>
       <c r="E23" s="2">
-        <f>TissueComp!G24*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!G23*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
         <v>9.0050591519329985E-3</v>
       </c>
       <c r="F23" s="2">
-        <f>TissueComp!H24*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!H23*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
         <v>7.7690130262545315E-2</v>
       </c>
       <c r="G23" s="2">
-        <f>TissueComp!I24*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!I23*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
         <v>0.20735534490071497</v>
       </c>
       <c r="H23" s="2">
-        <f>TissueComp!J24*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!J23*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
         <v>0.14929584832851484</v>
       </c>
       <c r="I23" s="2">
-        <f>TissueComp!K24*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!K23*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
         <v>3.1725367769809415E-2</v>
       </c>
       <c r="J23" s="2">
-        <f>TissueComp!L24*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!L23*INDEX(VolumeFlow!$A21:$D33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
         <v>2.644844380403458</v>
       </c>
       <c r="K23" t="s">
@@ -9131,39 +9113,39 @@
         <v>Skin</v>
       </c>
       <c r="B24" s="2">
-        <f>TissueComp!D25*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!D24*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
         <v>0.11598829325922648</v>
       </c>
       <c r="C24" s="2">
-        <f>TissueComp!E25*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!E24*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
         <v>5.4332254845364525E-2</v>
       </c>
       <c r="D24" s="2">
-        <f>TissueComp!F25*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!F24*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
         <v>8.8908350667609506E-2</v>
       </c>
       <c r="E24" s="2">
-        <f>TissueComp!G25*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!G24*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
         <v>1.0871705927721829E-2</v>
       </c>
       <c r="F24" s="2">
-        <f>TissueComp!H25*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!H24*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
         <v>7.0540491509259617E-2</v>
       </c>
       <c r="G24" s="2">
-        <f>TissueComp!I25*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!I24*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
         <v>0.13754014651783925</v>
       </c>
       <c r="H24" s="2">
-        <f>TissueComp!J25*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!J24*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
         <v>2.521569352827057E-2</v>
       </c>
       <c r="I24" s="2">
-        <f>TissueComp!K25*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!K24*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
         <v>7.5647080584811555E-3</v>
       </c>
       <c r="J24" s="2">
-        <f>TissueComp!L25*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!L24*INDEX(VolumeFlow!$A22:$D34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
         <v>1.1922438367321369</v>
       </c>
       <c r="K24" t="s">
@@ -9176,39 +9158,39 @@
         <v>Spleen</v>
       </c>
       <c r="B25" s="2">
-        <f>TissueComp!D26*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!D25*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
         <v>1.413662239089184E-3</v>
       </c>
       <c r="C25" s="2">
-        <f>TissueComp!E26*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!E25*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
         <v>4.8387096774193548E-4</v>
       </c>
       <c r="D25" s="2">
-        <f>TissueComp!F26*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!F25*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
         <v>1.2238895100198635E-3</v>
       </c>
       <c r="E25" s="2">
-        <f>TissueComp!G26*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!G25*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
         <v>7.5086001561997919E-5</v>
       </c>
       <c r="F25" s="2">
-        <f>TissueComp!H26*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!H25*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
         <v>5.9855769524925812E-4</v>
       </c>
       <c r="G25" s="2">
-        <f>TissueComp!I26*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!I25*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
         <v>6.9379641931667936E-4</v>
       </c>
       <c r="H25" s="2">
-        <f>TissueComp!J26*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!J25*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
         <v>9.2795271083605886E-4</v>
       </c>
       <c r="I25" s="2">
-        <f>TissueComp!K26*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!K25*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
         <v>2.7578407667837952E-4</v>
       </c>
       <c r="J25" s="2">
-        <f>TissueComp!L26*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!L25*INDEX(VolumeFlow!$A23:$D35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
         <v>1.3282732447817837E-2</v>
       </c>
       <c r="K25" t="s">

</xml_diff>

<commit_message>
Converted Wetmore 2015 tables to txt files
</commit_message>
<xml_diff>
--- a/pkdata.xlsx
+++ b/pkdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\httkdatatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050BECAF-482B-4843-AA96-AAAFC2CD93E0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F22DD421-57BD-4F16-AA13-92F616884941}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="765" windowWidth="23595" windowHeight="15675" tabRatio="884" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1230" yWindow="0" windowWidth="19620" windowHeight="11520" tabRatio="884" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VolumeFlow" sheetId="14" r:id="rId1"/>
@@ -43,9 +43,9 @@
     <definedName name="tblfn10" localSheetId="1">TissueComp!$A$30</definedName>
     <definedName name="tblfn10" localSheetId="0">VolumeFlow!#REF!</definedName>
     <definedName name="tblfn8" localSheetId="1">TissueComp!$A$28</definedName>
-    <definedName name="tblfn8" localSheetId="0">VolumeFlow!$A$62</definedName>
+    <definedName name="tblfn8" localSheetId="0">VolumeFlow!$A$75</definedName>
     <definedName name="tblfn9" localSheetId="1">TissueComp!$A$29</definedName>
-    <definedName name="tblfn9" localSheetId="0">VolumeFlow!$A$63</definedName>
+    <definedName name="tblfn9" localSheetId="0">VolumeFlow!$A$76</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="348">
   <si>
     <t>Tissue</t>
   </si>
@@ -1278,9 +1278,6 @@
     <t>Plasma Effective Neutral Lipid Volume Fraction</t>
   </si>
   <si>
-    <t>Pearce 2017</t>
-  </si>
-  <si>
     <r>
       <t>Davies, Brian, and Tim Morris. "Physiological parameters in laboratory animals and humans." </t>
     </r>
@@ -1426,30 +1423,6 @@
   </si>
   <si>
     <r>
-      <t>Pearce, Robert G., et al. "Httk: R package for high-throughput toxicokinetics." </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF222222"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Journal of statistical software</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF222222"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> 79.4 (2017): 1.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Gomez, N. N., M. S. Ojeda, and M. S. Gimenez. "Lung lipid composition in zinc-deficient rats." </t>
     </r>
     <r>
@@ -1689,9 +1662,6 @@
     </r>
   </si>
   <si>
-    <t>Refeences</t>
-  </si>
-  <si>
     <t>References:</t>
   </si>
   <si>
@@ -1739,6 +1709,18 @@
   <si>
     <t>EPA, Physiological Parameters Database for PBPK Modeling</t>
   </si>
+  <si>
+    <t>Monkey</t>
+  </si>
+  <si>
+    <t>Gauvin, David V. "Electrocardiogram, hemodynamics, and core body temperatures of the normal freely moving cynomolgus monkey by remote radiotelemetry", Journal of Pharmacological and Toxicological Methods</t>
+  </si>
+  <si>
+    <t>RabbitRaw</t>
+  </si>
+  <si>
+    <t>Davies and Morris 1993</t>
+  </si>
 </sst>
 </file>
 
@@ -1749,7 +1731,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1848,13 +1830,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
@@ -1916,7 +1891,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1966,16 +1941,19 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2315,10 +2293,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L83"/>
+  <dimension ref="A1:L96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:XFD61"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2352,14 +2330,14 @@
         <v>35</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D2" s="21">
         <f>INDEX('Percent BW'!P$4:P$22,MATCH($A26,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>0.20862445414847144</v>
       </c>
       <c r="E2" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A2,Flows!$A$3:$A$21,0),MATCH($B2,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A2,Flows!$A$3:$A$21,0),MATCH($B2,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A2,Flows!$A$3:$A$21,0),MATCH($B2,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A2,Flows!$A$3:$A$21,0),MATCH($B2,Flows!$B$2:$E$2,0)))</f>
         <v>10.743599688785142</v>
       </c>
       <c r="F2" s="7"/>
@@ -2378,14 +2356,14 @@
         <v>35</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D3" s="21">
         <f>INDEX('Percent BW'!P$4:P$22,MATCH($A27,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>7.2310597961656342E-2</v>
       </c>
       <c r="E3" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A3,Flows!$A$3:$A$21,0),MATCH($B3,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A3,Flows!$A$3:$A$21,0),MATCH($B3,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A3,Flows!$A$3:$A$21,0),MATCH($B3,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A3,Flows!$A$3:$A$21,0),MATCH($B3,Flows!$B$2:$E$2,0)))</f>
         <v>9.7188255646240975</v>
       </c>
       <c r="F3" s="7"/>
@@ -2404,14 +2382,14 @@
         <v>35</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D4" s="21">
         <f>INDEX('Percent BW'!P$4:P$22,MATCH($A28,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>1.9314340898116854E-2</v>
       </c>
       <c r="E4" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A4,Flows!$A$3:$A$21,0),MATCH($B4,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A4,Flows!$A$3:$A$21,0),MATCH($B4,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A4,Flows!$A$3:$A$21,0),MATCH($B4,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A4,Flows!$A$3:$A$21,0),MATCH($B4,Flows!$B$2:$E$2,0)))</f>
         <v>28.925076085190767</v>
       </c>
       <c r="F4" s="7"/>
@@ -2430,14 +2408,14 @@
         <v>35</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D5" s="21">
         <f>SUM('Percent BW'!P8:P10)</f>
         <v>1.5802847456629968E-2</v>
       </c>
       <c r="E5" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A5,Flows!$A$3:$A$21,0),MATCH($B5,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A5,Flows!$A$3:$A$21,0),MATCH($B5,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A5,Flows!$A$3:$A$21,0),MATCH($B5,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A5,Flows!$A$3:$A$21,0),MATCH($B5,Flows!$B$2:$E$2,0)))</f>
         <v>47.519767854241969</v>
       </c>
       <c r="F5" s="7"/>
@@ -2456,14 +2434,14 @@
         <v>35</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D6" s="21">
         <f>INDEX('Percent BW'!P$4:P$22,MATCH($A30,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>4.5631067961165043E-3</v>
       </c>
       <c r="E6" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A6,Flows!$A$3:$A$21,0),MATCH($B6,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A6,Flows!$A$3:$A$21,0),MATCH($B6,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A6,Flows!$A$3:$A$21,0),MATCH($B6,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A6,Flows!$A$3:$A$21,0),MATCH($B6,Flows!$B$2:$E$2,0)))</f>
         <v>9.9171689434939783</v>
       </c>
       <c r="F6" s="7"/>
@@ -2482,14 +2460,14 @@
         <v>35</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D7" s="21">
         <f>INDEX('Percent BW'!P$4:P$22,MATCH($A31,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>4.1904761904761906E-3</v>
       </c>
       <c r="E7" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A7,Flows!$A$3:$A$21,0),MATCH($B7,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A7,Flows!$A$3:$A$21,0),MATCH($B7,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A7,Flows!$A$3:$A$21,0),MATCH($B7,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A7,Flows!$A$3:$A$21,0),MATCH($B7,Flows!$B$2:$E$2,0)))</f>
         <v>51.238706208052214</v>
       </c>
       <c r="F7" s="7"/>
@@ -2508,14 +2486,14 @@
         <v>35</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D8" s="21">
         <f>INDEX('Percent BW'!P$4:P$22,MATCH($A32,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>2.4476190476190471E-2</v>
       </c>
       <c r="E8" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A8,Flows!$A$3:$A$21,0),MATCH($B8,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A8,Flows!$A$3:$A$21,0),MATCH($B8,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A8,Flows!$A$3:$A$21,0),MATCH($B8,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A8,Flows!$A$3:$A$21,0),MATCH($B8,Flows!$B$2:$E$2,0)))</f>
         <v>59.91622903360944</v>
       </c>
       <c r="F8" s="7"/>
@@ -2534,14 +2512,14 @@
         <v>35</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D9" s="21">
         <f>INDEX('Percent BW'!P$4:P$22,MATCH($A33,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>7.234650166587339E-3</v>
       </c>
       <c r="E9" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A9,Flows!$A$3:$A$21,0),MATCH($B9,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A9,Flows!$A$3:$A$21,0),MATCH($B9,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A9,Flows!$A$3:$A$21,0),MATCH($B9,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A9,Flows!$A$3:$A$21,0),MATCH($B9,Flows!$B$2:$E$2,0)))</f>
         <v>5.7850152170381541</v>
       </c>
       <c r="F9" s="7"/>
@@ -2560,14 +2538,14 @@
         <v>35</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D10" s="21">
         <f>INDEX('Percent BW'!P$4:P$22,MATCH($A34,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>0.38424591738712782</v>
       </c>
       <c r="E10" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A10,Flows!$A$3:$A$21,0),MATCH($B10,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A10,Flows!$A$3:$A$21,0),MATCH($B10,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A10,Flows!$A$3:$A$21,0),MATCH($B10,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A10,Flows!$A$3:$A$21,0),MATCH($B10,Flows!$B$2:$E$2,0)))</f>
         <v>30.991152948418677</v>
       </c>
       <c r="F10" s="7"/>
@@ -2586,14 +2564,14 @@
         <v>35</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D11" s="21">
         <f>INDEX('Percent BW'!P$4:P$22,MATCH($A35,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>3.3204899288913951E-2</v>
       </c>
       <c r="E11" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A11,Flows!$A$3:$A$21,0),MATCH($B11,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A11,Flows!$A$3:$A$21,0),MATCH($B11,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A11,Flows!$A$3:$A$21,0),MATCH($B11,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A11,Flows!$A$3:$A$21,0),MATCH($B11,Flows!$B$2:$E$2,0)))</f>
         <v>12.396461179367471</v>
       </c>
       <c r="F11" s="7"/>
@@ -2612,14 +2590,14 @@
         <v>35</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D12" s="21">
         <f>INDEX('Percent BW'!P$4:P$22,MATCH($A36,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>2.4667931688804553E-3</v>
       </c>
       <c r="E12" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A12,Flows!$A$3:$A$21,0),MATCH($B12,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A12,Flows!$A$3:$A$21,0),MATCH($B12,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A12,Flows!$A$3:$A$21,0),MATCH($B12,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A12,Flows!$A$3:$A$21,0),MATCH($B12,Flows!$B$2:$E$2,0)))</f>
         <v>3.1817583693709843</v>
       </c>
       <c r="F12" s="7"/>
@@ -2638,14 +2616,14 @@
         <v>35</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D13" s="21">
         <f>'Percent BW'!P23-'Percent BW'!P22-'Percent BW'!P20-SUM(VolumeFlow!D2:D12)</f>
         <v>5.1820372533547543E-2</v>
       </c>
       <c r="E13" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A13,Flows!$A$3:$A$21,0),MATCH($B13,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A13,Flows!$A$3:$A$21,0),MATCH($B13,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A13,Flows!$A$3:$A$21,0),MATCH($B13,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A13,Flows!$A$3:$A$21,0),MATCH($B13,Flows!$B$2:$E$2,0)))</f>
         <v>4.1900038786262614</v>
       </c>
       <c r="F13" s="7"/>
@@ -2664,14 +2642,14 @@
         <v>17</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D14" s="21">
         <f>INDEX('Percent BW'!L$4:L$22,MATCH($A26,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>7.2598253275109076E-2</v>
       </c>
       <c r="E14" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A14,Flows!$A$3:$A$21,0),MATCH($B14,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A14,Flows!$A$3:$A$21,0),MATCH($B14,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A14,Flows!$A$3:$A$21,0),MATCH($B14,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A14,Flows!$A$3:$A$21,0),MATCH($B14,Flows!$B$2:$E$2,0)))</f>
         <v>1.131370849898476</v>
       </c>
       <c r="F14" s="7"/>
@@ -2690,14 +2668,14 @@
         <v>17</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D15" s="21">
         <f>INDEX('Percent BW'!L$4:L$22,MATCH($A27,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>3.6939633668305896E-2</v>
       </c>
       <c r="E15" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A15,Flows!$A$3:$A$21,0),MATCH($B15,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A15,Flows!$A$3:$A$21,0),MATCH($B15,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A15,Flows!$A$3:$A$21,0),MATCH($B15,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A15,Flows!$A$3:$A$21,0),MATCH($B15,Flows!$B$2:$E$2,0)))</f>
         <v>25.535040082208603</v>
       </c>
       <c r="F15" s="7"/>
@@ -2716,14 +2694,14 @@
         <v>17</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D16" s="21">
         <f>INDEX('Percent BW'!L$4:L$22,MATCH($A28,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>5.5045871559633031E-3</v>
       </c>
       <c r="E16" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A16,Flows!$A$3:$A$21,0),MATCH($B16,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A16,Flows!$A$3:$A$21,0),MATCH($B16,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A16,Flows!$A$3:$A$21,0),MATCH($B16,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A16,Flows!$A$3:$A$21,0),MATCH($B16,Flows!$B$2:$E$2,0)))</f>
         <v>3.676955262170047</v>
       </c>
       <c r="F16" s="7"/>
@@ -2742,14 +2720,14 @@
         <v>17</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D17" s="21">
         <f>SUM('Percent BW'!L8:L10)</f>
         <v>2.5852334412265577E-2</v>
       </c>
       <c r="E17" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A17,Flows!$A$3:$A$21,0),MATCH($B17,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A17,Flows!$A$3:$A$21,0),MATCH($B17,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A17,Flows!$A$3:$A$21,0),MATCH($B17,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A17,Flows!$A$3:$A$21,0),MATCH($B17,Flows!$B$2:$E$2,0)))</f>
         <v>27.718585822512662</v>
       </c>
       <c r="F17" s="7"/>
@@ -2768,14 +2746,14 @@
         <v>17</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D18" s="21">
         <f>INDEX('Percent BW'!L$4:L$22,MATCH($A30,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>3.2038834951456309E-3</v>
       </c>
       <c r="E18" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A18,Flows!$A$3:$A$21,0),MATCH($B18,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A18,Flows!$A$3:$A$21,0),MATCH($B18,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A18,Flows!$A$3:$A$21,0),MATCH($B18,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A18,Flows!$A$3:$A$21,0),MATCH($B18,Flows!$B$2:$E$2,0)))</f>
         <v>11.030865786510139</v>
       </c>
       <c r="F18" s="7"/>
@@ -2794,14 +2772,14 @@
         <v>17</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D19" s="21">
         <f>INDEX('Percent BW'!L$4:L$22,MATCH($A31,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>6.9523809523809521E-3</v>
       </c>
       <c r="E19" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A19,Flows!$A$3:$A$21,0),MATCH($B19,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A19,Flows!$A$3:$A$21,0),MATCH($B19,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A19,Flows!$A$3:$A$21,0),MATCH($B19,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A19,Flows!$A$3:$A$21,0),MATCH($B19,Flows!$B$2:$E$2,0)))</f>
         <v>26.021529547664947</v>
       </c>
       <c r="F19" s="7"/>
@@ -2820,14 +2798,14 @@
         <v>17</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D20" s="21">
         <f>INDEX('Percent BW'!L$4:L$22,MATCH($A32,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>3.4857142857142857E-2</v>
       </c>
       <c r="E20" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A20,Flows!$A$3:$A$21,0),MATCH($B20,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A20,Flows!$A$3:$A$21,0),MATCH($B20,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A20,Flows!$A$3:$A$21,0),MATCH($B20,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A20,Flows!$A$3:$A$21,0),MATCH($B20,Flows!$B$2:$E$2,0)))</f>
         <v>33.375440072005041</v>
       </c>
       <c r="F20" s="7"/>
@@ -2846,14 +2824,14 @@
         <v>17</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D21" s="21">
         <f>INDEX('Percent BW'!L$4:L$22,MATCH($A33,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>4.7596382674916704E-3</v>
       </c>
       <c r="E21" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A21,Flows!$A$3:$A$21,0),MATCH($B21,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A21,Flows!$A$3:$A$21,0),MATCH($B21,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A21,Flows!$A$3:$A$21,0),MATCH($B21,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A21,Flows!$A$3:$A$21,0),MATCH($B21,Flows!$B$2:$E$2,0)))</f>
         <v>4.3953757518555792</v>
       </c>
       <c r="F21" s="7"/>
@@ -2872,14 +2850,14 @@
         <v>17</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D22" s="21">
         <f>INDEX('Percent BW'!L$4:L$22,MATCH($A34,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>0.38837656099903939</v>
       </c>
       <c r="E22" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A22,Flows!$A$3:$A$21,0),MATCH($B22,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A22,Flows!$A$3:$A$21,0),MATCH($B22,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A22,Flows!$A$3:$A$21,0),MATCH($B22,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A22,Flows!$A$3:$A$21,0),MATCH($B22,Flows!$B$2:$E$2,0)))</f>
         <v>21.213203435596427</v>
       </c>
       <c r="F22" s="7"/>
@@ -2898,14 +2876,14 @@
         <v>17</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D23" s="21">
         <f>INDEX('Percent BW'!L$4:L$22,MATCH($A35,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>0.17032054810459099</v>
       </c>
       <c r="E23" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A23,Flows!$A$3:$A$21,0),MATCH($B23,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A23,Flows!$A$3:$A$21,0),MATCH($B23,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A23,Flows!$A$3:$A$21,0),MATCH($B23,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A23,Flows!$A$3:$A$21,0),MATCH($B23,Flows!$B$2:$E$2,0)))</f>
         <v>16.404877323527902</v>
       </c>
       <c r="F23" s="7"/>
@@ -2924,14 +2902,14 @@
         <v>17</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D24" s="21">
         <f>INDEX('Percent BW'!L$4:L$22,MATCH($A36,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>1.8975332068311196E-3</v>
       </c>
       <c r="E24" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A24,Flows!$A$3:$A$21,0),MATCH($B24,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A24,Flows!$A$3:$A$21,0),MATCH($B24,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A24,Flows!$A$3:$A$21,0),MATCH($B24,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A24,Flows!$A$3:$A$21,0),MATCH($B24,Flows!$B$2:$E$2,0)))</f>
         <v>2.8779245994292482</v>
       </c>
       <c r="F24" s="7"/>
@@ -2950,14 +2928,14 @@
         <v>17</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D25" s="21">
         <f>'Percent BW'!L23-'Percent BW'!L22-'Percent BW'!L20-SUM(VolumeFlow!D14:D24)</f>
         <v>5.2399992921151606E-2</v>
       </c>
       <c r="E25" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A25,Flows!$A$3:$A$21,0),MATCH($B25,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A25,Flows!$A$3:$A$21,0),MATCH($B25,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A25,Flows!$A$3:$A$21,0),MATCH($B25,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A25,Flows!$A$3:$A$21,0),MATCH($B25,Flows!$B$2:$E$2,0)))</f>
         <v>59.664255982958501</v>
       </c>
       <c r="F25" s="7"/>
@@ -2976,14 +2954,14 @@
         <v>34</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D26" s="21">
         <f>INDEX('Percent BW'!J$4:J$22,MATCH($A26,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>7.3169652284369002E-2</v>
       </c>
       <c r="E26" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A26,Flows!$A$3:$A$21,0),MATCH($B26,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A26,Flows!$A$3:$A$21,0),MATCH($B26,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A26,Flows!$A$3:$A$21,0),MATCH($B26,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A26,Flows!$A$3:$A$21,0),MATCH($B26,Flows!$B$2:$E$2,0)))</f>
         <v>4.0614836065401096</v>
       </c>
     </row>
@@ -2995,14 +2973,14 @@
         <v>34</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D27" s="21">
         <f>INDEX('Percent BW'!J$4:J$22,MATCH($A27,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>5.429620126861949E-2</v>
       </c>
       <c r="E27" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A27,Flows!$A$3:$A$21,0),MATCH($B27,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A27,Flows!$A$3:$A$21,0),MATCH($B27,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A27,Flows!$A$3:$A$21,0),MATCH($B27,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A27,Flows!$A$3:$A$21,0),MATCH($B27,Flows!$B$2:$E$2,0)))</f>
         <v>8.766383654772504</v>
       </c>
     </row>
@@ -3014,14 +2992,14 @@
         <v>34</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D28" s="21">
         <f>INDEX('Percent BW'!J$4:J$22,MATCH($A28,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>1.5934331240946405E-2</v>
       </c>
       <c r="E28" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A28,Flows!$A$3:$A$21,0),MATCH($B28,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A28,Flows!$A$3:$A$21,0),MATCH($B28,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A28,Flows!$A$3:$A$21,0),MATCH($B28,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A28,Flows!$A$3:$A$21,0),MATCH($B28,Flows!$B$2:$E$2,0)))</f>
         <v>4.963996082874039</v>
       </c>
     </row>
@@ -3033,14 +3011,14 @@
         <v>34</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D29" s="21">
         <f>SUM('Percent BW'!J8:J10)</f>
         <v>4.0408654780552319E-2</v>
       </c>
       <c r="E29" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A29,Flows!$A$3:$A$21,0),MATCH($B29,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A29,Flows!$A$3:$A$21,0),MATCH($B29,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A29,Flows!$A$3:$A$21,0),MATCH($B29,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A29,Flows!$A$3:$A$21,0),MATCH($B29,Flows!$B$2:$E$2,0)))</f>
         <v>27.264372424876349</v>
       </c>
     </row>
@@ -3052,14 +3030,14 @@
         <v>34</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D30" s="21">
         <f>INDEX('Percent BW'!J$4:J$22,MATCH($A30,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>4.8543689320388345E-3</v>
       </c>
       <c r="E30" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A30,Flows!$A$3:$A$21,0),MATCH($B30,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A30,Flows!$A$3:$A$21,0),MATCH($B30,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A30,Flows!$A$3:$A$21,0),MATCH($B30,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A30,Flows!$A$3:$A$21,0),MATCH($B30,Flows!$B$2:$E$2,0)))</f>
         <v>5.2648443303209511</v>
       </c>
     </row>
@@ -3071,14 +3049,14 @@
         <v>34</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D31" s="21">
         <f>INDEX('Percent BW'!J$4:J$22,MATCH($A31,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>1.5904761904761904E-2</v>
       </c>
       <c r="E31" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A31,Flows!$A$3:$A$21,0),MATCH($B31,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A31,Flows!$A$3:$A$21,0),MATCH($B31,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A31,Flows!$A$3:$A$21,0),MATCH($B31,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A31,Flows!$A$3:$A$21,0),MATCH($B31,Flows!$B$2:$E$2,0)))</f>
         <v>24.443920105061554</v>
       </c>
     </row>
@@ -3090,14 +3068,14 @@
         <v>34</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D32" s="21">
         <f>INDEX('Percent BW'!J$4:J$22,MATCH($A32,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>5.228571428571429E-2</v>
       </c>
       <c r="E32" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A32,Flows!$A$3:$A$21,0),MATCH($B32,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A32,Flows!$A$3:$A$21,0),MATCH($B32,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A32,Flows!$A$3:$A$21,0),MATCH($B32,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A32,Flows!$A$3:$A$21,0),MATCH($B32,Flows!$B$2:$E$2,0)))</f>
         <v>33.845427837777535</v>
       </c>
     </row>
@@ -3109,14 +3087,14 @@
         <v>34</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D33" s="21">
         <f>INDEX('Percent BW'!J$4:J$22,MATCH($A33,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>6.9490718705378391E-3</v>
       </c>
       <c r="E33" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A33,Flows!$A$3:$A$21,0),MATCH($B33,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A33,Flows!$A$3:$A$21,0),MATCH($B33,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A33,Flows!$A$3:$A$21,0),MATCH($B33,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A33,Flows!$A$3:$A$21,0),MATCH($B33,Flows!$B$2:$E$2,0)))</f>
         <v>0.75212061861727864</v>
       </c>
     </row>
@@ -3128,14 +3106,14 @@
         <v>34</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D34" s="21">
         <f>INDEX('Percent BW'!J$4:J$22,MATCH($A34,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>0.36887608069164268</v>
       </c>
       <c r="E34" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A34,Flows!$A$3:$A$21,0),MATCH($B34,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A34,Flows!$A$3:$A$21,0),MATCH($B34,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A34,Flows!$A$3:$A$21,0),MATCH($B34,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A34,Flows!$A$3:$A$21,0),MATCH($B34,Flows!$B$2:$E$2,0)))</f>
         <v>17.110744073543088</v>
       </c>
     </row>
@@ -3147,14 +3125,14 @@
         <v>34</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D35" s="21">
         <f>INDEX('Percent BW'!J$4:J$22,MATCH($A35,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>0.14794527904198049</v>
       </c>
       <c r="E35" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A35,Flows!$A$3:$A$21,0),MATCH($B35,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A35,Flows!$A$3:$A$21,0),MATCH($B35,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A35,Flows!$A$3:$A$21,0),MATCH($B35,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A35,Flows!$A$3:$A$21,0),MATCH($B35,Flows!$B$2:$E$2,0)))</f>
         <v>7.709236340827105</v>
       </c>
     </row>
@@ -3166,14 +3144,14 @@
         <v>34</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D36" s="21">
         <f>INDEX('Percent BW'!J$4:J$22,MATCH($A36,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>1.0473620615192194E-3</v>
       </c>
       <c r="E36" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A36,Flows!$A$3:$A$21,0),MATCH($B36,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A36,Flows!$A$3:$A$21,0),MATCH($B36,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A36,Flows!$A$3:$A$21,0),MATCH($B36,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A36,Flows!$A$3:$A$21,0),MATCH($B36,Flows!$B$2:$E$2,0)))</f>
         <v>2.0683317011975162</v>
       </c>
     </row>
@@ -3185,14 +3163,14 @@
         <v>34</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D37" s="21">
         <f>'Percent BW'!J23-'Percent BW'!J22-'Percent BW'!J20-SUM(VolumeFlow!D26:D36)</f>
         <v>2.5418908119054118E-2</v>
       </c>
       <c r="E37" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A37,Flows!$A$3:$A$21,0),MATCH($B37,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A37,Flows!$A$3:$A$21,0),MATCH($B37,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A37,Flows!$A$3:$A$21,0),MATCH($B37,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A37,Flows!$A$3:$A$21,0),MATCH($B37,Flows!$B$2:$E$2,0)))</f>
         <v>38.629718395752846</v>
       </c>
     </row>
@@ -3204,14 +3182,14 @@
         <v>18</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D38" s="21">
         <f>INDEX('Percent BW'!N$4:N$22,MATCH($A26,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>4.7303493449781797E-2</v>
       </c>
       <c r="E38" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A38,Flows!$A$3:$A$21,0),MATCH($B38,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A38,Flows!$A$3:$A$21,0),MATCH($B38,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A38,Flows!$A$3:$A$21,0),MATCH($B38,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A38,Flows!$A$3:$A$21,0),MATCH($B38,Flows!$B$2:$E$2,0)))</f>
         <v>6.2239779351362285</v>
       </c>
       <c r="F38" s="7"/>
@@ -3230,14 +3208,14 @@
         <v>18</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D39" s="21">
         <f>INDEX('Percent BW'!N$4:N$22,MATCH($A27,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>4.098781270044901E-2</v>
       </c>
       <c r="E39" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A39,Flows!$A$3:$A$21,0),MATCH($B39,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A39,Flows!$A$3:$A$21,0),MATCH($B39,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A39,Flows!$A$3:$A$21,0),MATCH($B39,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A39,Flows!$A$3:$A$21,0),MATCH($B39,Flows!$B$2:$E$2,0)))</f>
         <v>2.3117632330505993</v>
       </c>
       <c r="F39" s="7"/>
@@ -3256,14 +3234,14 @@
         <v>18</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D40" s="21">
         <f>INDEX('Percent BW'!N$4:N$22,MATCH($A28,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>7.532592950265574E-3</v>
       </c>
       <c r="E40" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A40,Flows!$A$3:$A$21,0),MATCH($B40,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A40,Flows!$A$3:$A$21,0),MATCH($B40,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A40,Flows!$A$3:$A$21,0),MATCH($B40,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A40,Flows!$A$3:$A$21,0),MATCH($B40,Flows!$B$2:$E$2,0)))</f>
         <v>8.0022573451751509</v>
       </c>
       <c r="F40" s="7"/>
@@ -3282,14 +3260,14 @@
         <v>18</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D41" s="21">
         <f>SUM('Percent BW'!N8:N10)</f>
         <v>3.5218119758327587E-2</v>
       </c>
       <c r="E41" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A41,Flows!$A$3:$A$21,0),MATCH($B41,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A41,Flows!$A$3:$A$21,0),MATCH($B41,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A41,Flows!$A$3:$A$21,0),MATCH($B41,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A41,Flows!$A$3:$A$21,0),MATCH($B41,Flows!$B$2:$E$2,0)))</f>
         <v>40.900426430895223</v>
       </c>
       <c r="F41" s="7"/>
@@ -3308,14 +3286,14 @@
         <v>18</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D42" s="21">
         <f>INDEX('Percent BW'!N$4:N$22,MATCH($A30,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>7.5728155339805829E-3</v>
       </c>
       <c r="E42" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A42,Flows!$A$3:$A$21,0),MATCH($B42,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A42,Flows!$A$3:$A$21,0),MATCH($B42,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A42,Flows!$A$3:$A$21,0),MATCH($B42,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A42,Flows!$A$3:$A$21,0),MATCH($B42,Flows!$B$2:$E$2,0)))</f>
         <v>9.6027088142101817</v>
       </c>
       <c r="F42" s="7"/>
@@ -3334,14 +3312,14 @@
         <v>18</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D43" s="21">
         <f>INDEX('Percent BW'!N$4:N$22,MATCH($A31,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>5.2380952380952387E-3</v>
       </c>
       <c r="E43" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A43,Flows!$A$3:$A$21,0),MATCH($B43,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A43,Flows!$A$3:$A$21,0),MATCH($B43,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A43,Flows!$A$3:$A$21,0),MATCH($B43,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A43,Flows!$A$3:$A$21,0),MATCH($B43,Flows!$B$2:$E$2,0)))</f>
         <v>38.410835256840727</v>
       </c>
       <c r="F43" s="7"/>
@@ -3360,14 +3338,14 @@
         <v>18</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D44" s="21">
         <f>INDEX('Percent BW'!N$4:N$22,MATCH($A32,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>3.1333333333333331E-2</v>
       </c>
       <c r="E44" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A44,Flows!$A$3:$A$21,0),MATCH($B44,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A44,Flows!$A$3:$A$21,0),MATCH($B44,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A44,Flows!$A$3:$A$21,0),MATCH($B44,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A44,Flows!$A$3:$A$21,0),MATCH($B44,Flows!$B$2:$E$2,0)))</f>
         <v>54.948833770202704</v>
       </c>
       <c r="F44" s="7"/>
@@ -3386,14 +3364,14 @@
         <v>18</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D45" s="21">
         <f>INDEX('Percent BW'!N$4:N$22,MATCH($A33,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>7.8058067586863388E-3</v>
       </c>
       <c r="E45" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A45,Flows!$A$3:$A$21,0),MATCH($B45,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A45,Flows!$A$3:$A$21,0),MATCH($B45,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A45,Flows!$A$3:$A$21,0),MATCH($B45,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A45,Flows!$A$3:$A$21,0),MATCH($B45,Flows!$B$2:$E$2,0)))</f>
         <v>18.778630570011025</v>
       </c>
       <c r="F45" s="7"/>
@@ -3412,14 +3390,14 @@
         <v>18</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D46" s="21">
         <f>INDEX('Percent BW'!N$4:N$22,MATCH($A34,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>0.43852065321805955</v>
       </c>
       <c r="E46" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A46,Flows!$A$3:$A$21,0),MATCH($B46,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A46,Flows!$A$3:$A$21,0),MATCH($B46,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A46,Flows!$A$3:$A$21,0),MATCH($B46,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A46,Flows!$A$3:$A$21,0),MATCH($B46,Flows!$B$2:$E$2,0)))</f>
         <v>44.456985250973062</v>
       </c>
       <c r="F46" s="7"/>
@@ -3438,14 +3416,14 @@
         <v>18</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D47" s="21">
         <f>INDEX('Percent BW'!N$4:N$22,MATCH($A35,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>0.17005204487583964</v>
       </c>
       <c r="E47" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A47,Flows!$A$3:$A$21,0),MATCH($B47,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A47,Flows!$A$3:$A$21,0),MATCH($B47,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A47,Flows!$A$3:$A$21,0),MATCH($B47,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A47,Flows!$A$3:$A$21,0),MATCH($B47,Flows!$B$2:$E$2,0)))</f>
         <v>17.782794100389225</v>
       </c>
       <c r="F47" s="7"/>
@@ -3464,14 +3442,14 @@
         <v>18</v>
       </c>
       <c r="C48" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D48" s="21">
         <f>INDEX('Percent BW'!N$4:N$22,MATCH($A36,'Percent BW'!$A$4:$A$22,0),1)</f>
         <v>2.5616698292220113E-3</v>
       </c>
       <c r="E48" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A48,Flows!$A$3:$A$21,0),MATCH($B48,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A48,Flows!$A$3:$A$21,0),MATCH($B48,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A48,Flows!$A$3:$A$21,0),MATCH($B48,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A48,Flows!$A$3:$A$21,0),MATCH($B48,Flows!$B$2:$E$2,0)))</f>
         <v>2.934161026564222</v>
       </c>
       <c r="F48" s="7"/>
@@ -3490,14 +3468,14 @@
         <v>18</v>
       </c>
       <c r="C49" s="20" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="D49" s="21">
         <f>'Percent BW'!N23-'Percent BW'!N22-'Percent BW'!N20-SUM(VolumeFlow!D38:D48)</f>
         <v>2.3649226512727495E-3</v>
       </c>
       <c r="E49" s="22">
-        <f>IF(INDEX(Flows!$F$3:$I$21,MATCH($A49,Flows!$A$3:$A$21,0),MATCH($B49,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$F$3:$I$21,MATCH($A49,Flows!$A$3:$A$21,0),MATCH($B49,Flows!$B$2:$E$2,0)))</f>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A49,Flows!$A$3:$A$21,0),MATCH($B49,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A49,Flows!$A$3:$A$21,0),MATCH($B49,Flows!$B$2:$E$2,0)))</f>
         <v>6.0994983764335551</v>
       </c>
       <c r="F49" s="7"/>
@@ -3516,17 +3494,17 @@
         <v>104</v>
       </c>
       <c r="C50" s="20" t="s">
-        <v>323</v>
+        <v>347</v>
       </c>
       <c r="D50" s="21">
         <f>0.048</f>
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="E50" s="20">
-        <f>12.8*2.5^(1/4)</f>
-        <v>16.095147899941576</v>
-      </c>
-      <c r="F50" s="7"/>
+      <c r="E50" s="22">
+        <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A50,Flows!$A$3:$A$21,0),MATCH($B50,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A50,Flows!$A$3:$A$21,0),MATCH($B50,Flows!$B$2:$G$2,0)))</f>
+        <v>1.3222891924658635</v>
+      </c>
+      <c r="F50" s="20"/>
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
       <c r="I50" s="2"/>
@@ -3542,17 +3520,17 @@
         <v>104</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>323</v>
+        <v>347</v>
       </c>
       <c r="D51" s="21">
         <f>0.03694</f>
         <v>3.6940000000000001E-2</v>
       </c>
-      <c r="E51" s="20">
-        <f>36.112*2.5^(1/4)</f>
-        <v>45.408436012710169</v>
-      </c>
-      <c r="F51" s="7"/>
+      <c r="E51" s="22">
+        <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A51,Flows!$A$3:$A$21,0),MATCH($B51,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A51,Flows!$A$3:$A$21,0),MATCH($B51,Flows!$B$2:$G$2,0)))</f>
+        <v>1.2763075040542471</v>
+      </c>
+      <c r="F51" s="20"/>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
       <c r="I51" s="2"/>
@@ -3568,17 +3546,17 @@
         <v>104</v>
       </c>
       <c r="C52" s="20" t="s">
-        <v>323</v>
+        <v>347</v>
       </c>
       <c r="D52" s="21">
         <f>0.0055</f>
         <v>5.4999999999999997E-3</v>
       </c>
-      <c r="E52" s="20">
-        <f>5.2*2.5^(1/4)</f>
-        <v>6.5386538343512646</v>
-      </c>
-      <c r="F52" s="7"/>
+      <c r="E52" s="22">
+        <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A52,Flows!$A$3:$A$21,0),MATCH($B52,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A52,Flows!$A$3:$A$21,0),MATCH($B52,Flows!$B$2:$G$2,0)))</f>
+        <v>1.166567024887343</v>
+      </c>
+      <c r="F52" s="20"/>
       <c r="G52" s="7"/>
       <c r="H52" s="7"/>
       <c r="I52" s="2"/>
@@ -3594,17 +3572,17 @@
         <v>104</v>
       </c>
       <c r="C53" s="20" t="s">
-        <v>323</v>
+        <v>347</v>
       </c>
       <c r="D53" s="21">
         <f>0.048</f>
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="E53" s="20">
-        <f>44.4*2.5^(1/4)</f>
-        <v>55.830044277922333</v>
-      </c>
-      <c r="F53" s="7"/>
+      <c r="E53" s="22">
+        <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A53,Flows!$A$3:$A$21,0),MATCH($B53,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A53,Flows!$A$3:$A$21,0),MATCH($B53,Flows!$B$2:$G$2,0)))</f>
+        <v>4.5866906363659643</v>
+      </c>
+      <c r="F53" s="20"/>
       <c r="G53" s="7"/>
       <c r="H53" s="7"/>
       <c r="I53" s="2"/>
@@ -3620,17 +3598,17 @@
         <v>104</v>
       </c>
       <c r="C54" s="20" t="s">
-        <v>323</v>
+        <v>347</v>
       </c>
       <c r="D54" s="21">
         <f>0.0024</f>
         <v>2.3999999999999998E-3</v>
       </c>
-      <c r="E54" s="20">
-        <f>6.4*2.5^(1/4)</f>
-        <v>8.0475739499707881</v>
-      </c>
-      <c r="F54" s="7"/>
+      <c r="E54" s="22">
+        <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A54,Flows!$A$3:$A$21,0),MATCH($B54,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A54,Flows!$A$3:$A$21,0),MATCH($B54,Flows!$B$2:$G$2,0)))</f>
+        <v>0.66114459623293176</v>
+      </c>
+      <c r="F54" s="20"/>
       <c r="G54" s="7"/>
       <c r="H54" s="7"/>
       <c r="I54" s="2"/>
@@ -3646,17 +3624,17 @@
         <v>104</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>323</v>
+        <v>347</v>
       </c>
       <c r="D55" s="21">
         <f>0.006</f>
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="E55" s="20">
-        <f>32*2.5^(1/4)</f>
-        <v>40.237869749853935</v>
-      </c>
-      <c r="F55" s="7"/>
+      <c r="E55" s="22">
+        <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A55,Flows!$A$3:$A$21,0),MATCH($B55,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A55,Flows!$A$3:$A$21,0),MATCH($B55,Flows!$B$2:$G$2,0)))</f>
+        <v>3.3057229811646591</v>
+      </c>
+      <c r="F55" s="20"/>
       <c r="G55" s="7"/>
       <c r="H55" s="7"/>
       <c r="I55" s="2"/>
@@ -3672,17 +3650,17 @@
         <v>104</v>
       </c>
       <c r="C56" s="20" t="s">
-        <v>323</v>
+        <v>347</v>
       </c>
       <c r="D56" s="21">
         <f>0.04</f>
         <v>0.04</v>
       </c>
-      <c r="E56" s="20">
-        <f>70.8*2.5^(1/4)</f>
-        <v>89.026286821551835</v>
-      </c>
-      <c r="F56" s="7"/>
+      <c r="E56" s="22">
+        <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A56,Flows!$A$3:$A$21,0),MATCH($B56,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A56,Flows!$A$3:$A$21,0),MATCH($B56,Flows!$B$2:$G$2,0)))</f>
+        <v>7.313912095826808</v>
+      </c>
+      <c r="F56" s="20"/>
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
       <c r="I56" s="2"/>
@@ -3698,17 +3676,17 @@
         <v>104</v>
       </c>
       <c r="C57" s="20" t="s">
-        <v>323</v>
+        <v>347</v>
       </c>
       <c r="D57" s="21">
         <f>0.0068</f>
         <v>6.7999999999999996E-3</v>
       </c>
-      <c r="E57" s="20">
-        <f>6.216*2.5^(1/4)</f>
-        <v>7.8162061989091276</v>
-      </c>
-      <c r="F57" s="7"/>
+      <c r="E57" s="22">
+        <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A57,Flows!$A$3:$A$21,0),MATCH($B57,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A57,Flows!$A$3:$A$21,0),MATCH($B57,Flows!$B$2:$G$2,0)))</f>
+        <v>0.76103941257000129</v>
+      </c>
+      <c r="F57" s="20"/>
       <c r="G57" s="7"/>
       <c r="H57" s="7"/>
       <c r="I57" s="2"/>
@@ -3724,17 +3702,17 @@
         <v>104</v>
       </c>
       <c r="C58" s="20" t="s">
-        <v>323</v>
+        <v>347</v>
       </c>
       <c r="D58" s="21">
         <f>0.54</f>
         <v>0.54</v>
       </c>
-      <c r="E58" s="20">
-        <f>62*2.5^(1/4)</f>
-        <v>77.960872640342004</v>
-      </c>
-      <c r="F58" s="7"/>
+      <c r="E58" s="22">
+        <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A58,Flows!$A$3:$A$21,0),MATCH($B58,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A58,Flows!$A$3:$A$21,0),MATCH($B58,Flows!$B$2:$G$2,0)))</f>
+        <v>6.4048382760065268</v>
+      </c>
+      <c r="F58" s="20"/>
       <c r="G58" s="7"/>
       <c r="H58" s="7"/>
       <c r="I58" s="2"/>
@@ -3750,17 +3728,17 @@
         <v>104</v>
       </c>
       <c r="C59" s="20" t="s">
-        <v>323</v>
+        <v>347</v>
       </c>
       <c r="D59" s="21">
         <f>0.044</f>
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="E59" s="20">
-        <f>23.2*2.5^(1/4)</f>
-        <v>29.172455568644104</v>
-      </c>
-      <c r="F59" s="7"/>
+      <c r="E59" s="22">
+        <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A59,Flows!$A$3:$A$21,0),MATCH($B59,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A59,Flows!$A$3:$A$21,0),MATCH($B59,Flows!$B$2:$G$2,0)))</f>
+        <v>1.4592965792195598</v>
+      </c>
+      <c r="F59" s="20"/>
       <c r="G59" s="7"/>
       <c r="H59" s="7"/>
       <c r="I59" s="2"/>
@@ -3776,17 +3754,17 @@
         <v>104</v>
       </c>
       <c r="C60" s="20" t="s">
-        <v>323</v>
+        <v>347</v>
       </c>
       <c r="D60" s="21">
         <f>0.0004</f>
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="E60" s="20">
-        <f>3.6*2.5^(1/4)</f>
-        <v>4.526760346858568</v>
-      </c>
-      <c r="F60" s="7"/>
+      <c r="E60" s="22">
+        <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A60,Flows!$A$3:$A$21,0),MATCH($B60,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A60,Flows!$A$3:$A$21,0),MATCH($B60,Flows!$B$2:$G$2,0)))</f>
+        <v>0.37189383538102411</v>
+      </c>
+      <c r="F60" s="20"/>
       <c r="G60" s="7"/>
       <c r="H60" s="7"/>
       <c r="I60" s="2"/>
@@ -3802,17 +3780,16 @@
         <v>104</v>
       </c>
       <c r="C61" s="20" t="s">
-        <v>323</v>
+        <v>347</v>
       </c>
       <c r="D61" s="21">
         <f>0.02541891</f>
         <v>2.5418909999999999E-2</v>
       </c>
-      <c r="E61" s="20">
-        <f>90.002*2.5^(1/4)</f>
-        <v>113.17152353832356</v>
-      </c>
-      <c r="F61" s="7"/>
+      <c r="E61" s="22">
+        <v>0</v>
+      </c>
+      <c r="F61" s="20"/>
       <c r="G61" s="7"/>
       <c r="H61" s="7"/>
       <c r="I61" s="2"/>
@@ -3821,25 +3798,313 @@
       <c r="L61" s="2"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A62" s="28"/>
+      <c r="A62" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B62" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="C62" s="20" t="s">
+        <v>347</v>
+      </c>
+      <c r="D62" s="21"/>
+      <c r="E62" s="22">
+        <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A62,Flows!$A$3:$A$21,0),MATCH($B62,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A62,Flows!$A$3:$A$21,0),MATCH($B62,Flows!$B$2:$G$2,0)))</f>
+        <v>3.5565588200778446</v>
+      </c>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="7"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" s="29" t="s">
+      <c r="A63" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="C63" s="20" t="s">
+        <v>347</v>
+      </c>
+      <c r="D63" s="21"/>
+      <c r="E63" s="22">
+        <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A63,Flows!$A$3:$A$21,0),MATCH($B63,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A63,Flows!$A$3:$A$21,0),MATCH($B63,Flows!$B$2:$G$2,0)))</f>
+        <v>0.20726834457009219</v>
+      </c>
+      <c r="F63" s="7"/>
+      <c r="G63" s="7"/>
+      <c r="H63" s="7"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B64" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="C64" s="20" t="s">
+        <v>347</v>
+      </c>
+      <c r="D64" s="21"/>
+      <c r="E64" s="22">
+        <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A64,Flows!$A$3:$A$21,0),MATCH($B64,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A64,Flows!$A$3:$A$21,0),MATCH($B64,Flows!$B$2:$G$2,0)))</f>
+        <v>12.803611752280242</v>
+      </c>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+      <c r="K64" s="2"/>
+      <c r="L64" s="2"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B65" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="C65" s="20" t="s">
+        <v>347</v>
+      </c>
+      <c r="D65" s="21"/>
+      <c r="E65" s="22">
+        <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A65,Flows!$A$3:$A$21,0),MATCH($B65,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A65,Flows!$A$3:$A$21,0),MATCH($B65,Flows!$B$2:$G$2,0)))</f>
+        <v>22.228492625486531</v>
+      </c>
+      <c r="F65" s="7"/>
+      <c r="G65" s="7"/>
+      <c r="H65" s="7"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
+      <c r="L65" s="2"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B66" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="C66" s="20" t="s">
+        <v>347</v>
+      </c>
+      <c r="D66" s="21"/>
+      <c r="E66" s="22">
+        <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A66,Flows!$A$3:$A$21,0),MATCH($B66,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A66,Flows!$A$3:$A$21,0),MATCH($B66,Flows!$B$2:$G$2,0)))</f>
+        <v>10.669676460233534</v>
+      </c>
+      <c r="F66" s="7"/>
+      <c r="G66" s="7"/>
+      <c r="H66" s="7"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="2"/>
+      <c r="K66" s="2"/>
+      <c r="L66" s="2"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B67" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="C67" s="20" t="s">
+        <v>347</v>
+      </c>
+      <c r="D67" s="21"/>
+      <c r="E67" s="22">
+        <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A67,Flows!$A$3:$A$21,0),MATCH($B67,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A67,Flows!$A$3:$A$21,0),MATCH($B67,Flows!$B$2:$G$2,0)))</f>
+        <v>24.54025585853713</v>
+      </c>
+      <c r="F67" s="7"/>
+      <c r="G67" s="7"/>
+      <c r="H67" s="7"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="2"/>
+      <c r="K67" s="2"/>
+      <c r="L67" s="2"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B68" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="C68" s="20" t="s">
+        <v>347</v>
+      </c>
+      <c r="D68" s="21"/>
+      <c r="E68" s="22">
+        <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A68,Flows!$A$3:$A$21,0),MATCH($B68,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A68,Flows!$A$3:$A$21,0),MATCH($B68,Flows!$B$2:$G$2,0)))</f>
+        <v>38.766491138848508</v>
+      </c>
+      <c r="F68" s="7"/>
+      <c r="G68" s="7"/>
+      <c r="H68" s="7"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
+      <c r="L68" s="2"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B69" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="C69" s="20" t="s">
+        <v>347</v>
+      </c>
+      <c r="D69" s="21"/>
+      <c r="E69" s="22">
+        <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A69,Flows!$A$3:$A$21,0),MATCH($B69,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A69,Flows!$A$3:$A$21,0),MATCH($B69,Flows!$B$2:$G$2,0)))</f>
+        <v>6.7109597515753876</v>
+      </c>
+      <c r="F69" s="7"/>
+      <c r="G69" s="7"/>
+      <c r="H69" s="7"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
+      <c r="L69" s="2"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B70" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="C70" s="20" t="s">
+        <v>347</v>
+      </c>
+      <c r="D70" s="21"/>
+      <c r="E70" s="22">
+        <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A70,Flows!$A$3:$A$21,0),MATCH($B70,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A70,Flows!$A$3:$A$21,0),MATCH($B70,Flows!$B$2:$G$2,0)))</f>
+        <v>16.004514690350302</v>
+      </c>
+      <c r="F70" s="7"/>
+      <c r="G70" s="7"/>
+      <c r="H70" s="7"/>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2"/>
+      <c r="K70" s="2"/>
+      <c r="L70" s="2"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B71" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="C71" s="20" t="s">
+        <v>347</v>
+      </c>
+      <c r="D71" s="21"/>
+      <c r="E71" s="22">
+        <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A71,Flows!$A$3:$A$21,0),MATCH($B71,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A71,Flows!$A$3:$A$21,0),MATCH($B71,Flows!$B$2:$G$2,0)))</f>
+        <v>9.6027088142101817</v>
+      </c>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
+      <c r="H71" s="7"/>
+      <c r="I71" s="2"/>
+      <c r="J71" s="2"/>
+      <c r="K71" s="2"/>
+      <c r="L71" s="2"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B72" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="C72" s="20" t="s">
+        <v>347</v>
+      </c>
+      <c r="D72" s="21"/>
+      <c r="E72" s="22">
+        <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A72,Flows!$A$3:$A$21,0),MATCH($B72,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A72,Flows!$A$3:$A$21,0),MATCH($B72,Flows!$B$2:$G$2,0)))</f>
+        <v>3.7343867610817369</v>
+      </c>
+      <c r="F72" s="7"/>
+      <c r="G72" s="7"/>
+      <c r="H72" s="7"/>
+      <c r="I72" s="2"/>
+      <c r="J72" s="2"/>
+      <c r="K72" s="2"/>
+      <c r="L72" s="2"/>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B73" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="C73" s="20" t="s">
+        <v>347</v>
+      </c>
+      <c r="D73" s="21"/>
+      <c r="E73" s="22">
+        <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A73,Flows!$A$3:$A$21,0),MATCH($B73,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A73,Flows!$A$3:$A$21,0),MATCH($B73,Flows!$B$2:$G$2,0)))</f>
+        <v>59.341154275008662</v>
+      </c>
+      <c r="F73" s="7"/>
+      <c r="G73" s="7"/>
+      <c r="H73" s="7"/>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2"/>
+      <c r="K73" s="2"/>
+      <c r="L73" s="2"/>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" s="20"/>
+      <c r="B74" s="20"/>
+      <c r="C74" s="20"/>
+      <c r="D74" s="21"/>
+      <c r="E74" s="20"/>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
+      <c r="H74" s="7"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="2"/>
+      <c r="K74" s="2"/>
+      <c r="L74" s="2"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" s="27"/>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" s="28" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A64" s="27" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="27" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="83" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J83" s="7"/>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" s="26" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78" s="26"/>
+    </row>
+    <row r="96" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J96" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3858,16 +4123,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -5227,20 +5492,20 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25" t="s">
+      <c r="E1" s="30"/>
+      <c r="F1" s="30" t="s">
         <v>317</v>
       </c>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25" t="s">
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
@@ -6197,99 +6462,99 @@
       <c r="L27" s="2"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="27" t="s">
         <v>43</v>
       </c>
       <c r="L28" s="2"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="27" t="s">
         <v>42</v>
       </c>
       <c r="L29" s="2"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="28" t="s">
+      <c r="A30" s="27" t="s">
         <v>41</v>
       </c>
       <c r="L30" s="2"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="30" t="s">
-        <v>345</v>
+      <c r="A31" s="29" t="s">
+        <v>342</v>
       </c>
       <c r="L31" s="2"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="27" t="s">
         <v>40</v>
       </c>
       <c r="L32" s="2"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="L33" s="2"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="27" t="s">
-        <v>343</v>
+      <c r="A34" s="26" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="26" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="26" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="26" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="26" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="26" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="26" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="26" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="26" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="26" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="26" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="26" t="s">
         <v>329</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="27" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="27" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="27" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="27" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="27" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="27" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="27" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="27" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="27" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="27" t="s">
-        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -6305,10 +6570,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6317,7 +6582,7 @@
     <col min="3" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>76</v>
       </c>
@@ -6339,8 +6604,11 @@
       <c r="G1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>78</v>
       </c>
@@ -6367,8 +6635,12 @@
         <f>716*G6</f>
         <v>40.812000000000005</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <f>3465/5</f>
+        <v>693</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>79</v>
       </c>
@@ -6395,8 +6667,12 @@
         <f>44*G5</f>
         <v>110</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <f>224/5</f>
+        <v>44.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -6404,27 +6680,31 @@
         <v>109</v>
       </c>
       <c r="C4" s="24">
-        <f>Flows!F3</f>
+        <f>Flows!H3</f>
         <v>150.42412372345572</v>
       </c>
       <c r="D4" s="24">
-        <f>Flows!G3</f>
+        <f>Flows!I3</f>
         <v>209.30360723121805</v>
       </c>
       <c r="E4" s="24">
-        <f>Flows!H3</f>
+        <f>Flows!J3</f>
         <v>213.3935292046707</v>
       </c>
       <c r="F4" s="24">
-        <f>Flows!I3</f>
+        <f>Flows!K3</f>
         <v>231.40060868152614</v>
       </c>
       <c r="G4" s="24">
         <f>212*G5^(1/4)</f>
         <v>266.5758870927823</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <f>375/24/60/5</f>
+        <v>5.2083333333333336E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>80</v>
       </c>
@@ -6446,8 +6726,11 @@
       <c r="G5" s="24">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>82</v>
       </c>
@@ -6473,8 +6756,12 @@
       <c r="G6" s="24">
         <v>5.7000000000000002E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <f>8.8/100</f>
+        <v>8.8000000000000009E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -6500,8 +6787,12 @@
       <c r="G7" s="24">
         <v>3.8699999999999998E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <f>4.93/100</f>
+        <v>4.9299999999999997E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>85</v>
       </c>
@@ -6527,8 +6818,12 @@
       <c r="G8" s="24">
         <v>1.2999999999999999E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <f>0.24/100</f>
+        <v>2.3999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>86</v>
       </c>
@@ -6550,8 +6845,11 @@
       <c r="G9" s="24">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="24">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>71</v>
       </c>
@@ -6559,26 +6857,30 @@
         <v>109</v>
       </c>
       <c r="C10" s="24">
-        <f>Flows!F19</f>
+        <f>Flows!H19</f>
         <v>1.3057649628772197E-2</v>
       </c>
       <c r="D10" s="24">
-        <f>Flows!G19</f>
+        <f>Flows!I19</f>
         <v>9.8209275164798271E-2</v>
       </c>
       <c r="E10" s="24">
-        <f>Flows!H19</f>
+        <f>Flows!J19</f>
         <v>3.704748770914422E-2</v>
       </c>
       <c r="F10" s="24">
-        <f>Flows!I19</f>
+        <f>Flows!K19</f>
         <v>4.0173716784987171E-2</v>
       </c>
       <c r="G10" s="24">
         <v>4.1700000000000001E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <f>1086/24/60/5</f>
+        <v>0.15083333333333332</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -6586,26 +6888,30 @@
         <v>109</v>
       </c>
       <c r="C11" s="24">
-        <f>Flows!F20</f>
+        <f>Flows!H20</f>
         <v>2.6115299257544394E-2</v>
       </c>
       <c r="D11" s="24">
-        <f>Flows!G20</f>
+        <f>Flows!I20</f>
         <v>4.4194173824159216E-2</v>
       </c>
       <c r="E11" s="24">
-        <f>Flows!H20</f>
+        <f>Flows!J20</f>
         <v>1.4818995083657686E-2</v>
       </c>
       <c r="F11" s="24">
-        <f>Flows!I20</f>
+        <f>Flows!K20</f>
         <v>1.0043429196246793E-2</v>
       </c>
       <c r="G11" s="24">
         <v>8.3299999999999999E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <f>125/24/260/5</f>
+        <v>4.0064102564102561E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>73</v>
       </c>
@@ -6613,26 +6919,30 @@
         <v>109</v>
       </c>
       <c r="C12" s="24">
-        <f>Flows!F21</f>
+        <f>Flows!H21</f>
         <v>5.2648443303209502</v>
       </c>
       <c r="D12" s="24">
-        <f>Flows!G21</f>
+        <f>Flows!I21</f>
         <v>3.705239533417509</v>
       </c>
       <c r="E12" s="24">
-        <f>Flows!H21</f>
+        <f>Flows!J21</f>
         <v>10.900852783538594</v>
       </c>
       <c r="F12" s="24">
-        <f>Flows!I21</f>
+        <f>Flows!K21</f>
         <v>5.1651921580697797</v>
       </c>
       <c r="G12" s="24">
         <v>3.12</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <f>10.4/5</f>
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>110</v>
       </c>
@@ -6655,8 +6965,11 @@
         <f>(40.1+38.6)/2</f>
         <v>39.35</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="24">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>322</v>
       </c>
@@ -6682,8 +6995,11 @@
         <f xml:space="preserve"> (0.001+0.3*0.0008)/(0.001 + 0.0008+0.00009) * 0.003/(0.003+0.06+0.94)</f>
         <v>1.9623668676510149E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="24">
+        <v>7.3000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>115</v>
       </c>
@@ -6710,25 +7026,29 @@
         <f>G6</f>
         <v>5.7000000000000002E-2</v>
       </c>
+      <c r="H15" s="24">
+        <f xml:space="preserve"> 0.07 / (0.928+0.07+0.009)</f>
+        <v>6.95134061569017E-2</v>
+      </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="26" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="26" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="26" t="s">
         <v>325</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
@@ -6737,13 +7057,18 @@
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="26" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="26" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="27" t="s">
-        <v>328</v>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -6755,35 +7080,39 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:T40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:A26"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="26" t="s">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B1" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26" t="s">
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>34</v>
       </c>
@@ -6797,31 +7126,52 @@
         <v>35</v>
       </c>
       <c r="F2" t="s">
+        <v>344</v>
+      </c>
+      <c r="G2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H2" t="s">
         <v>34</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>35</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
+        <v>344</v>
+      </c>
+      <c r="M2" t="s">
+        <v>104</v>
+      </c>
+      <c r="N2" t="s">
         <v>34</v>
       </c>
-      <c r="K2" t="s">
+      <c r="O2" t="s">
         <v>17</v>
       </c>
-      <c r="L2" t="s">
+      <c r="P2" t="s">
         <v>18</v>
       </c>
-      <c r="M2" t="s">
+      <c r="Q2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="R2" t="s">
+        <v>344</v>
+      </c>
+      <c r="S2" t="s">
+        <v>346</v>
+      </c>
+      <c r="T2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -6837,45 +7187,67 @@
       <c r="E3" s="3">
         <v>5600</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="3">
+        <v>1086</v>
+      </c>
+      <c r="G3" s="3">
+        <v>530</v>
+      </c>
+      <c r="H3" s="2">
         <f>B3/(0.02)^(3/4)</f>
         <v>150.42412372345572</v>
       </c>
-      <c r="G3" s="2">
+      <c r="I3" s="2">
         <f>C3/0.25^(3/4)</f>
         <v>209.30360723121805</v>
       </c>
-      <c r="H3" s="2">
+      <c r="J3" s="2">
         <f>D3/(10^(3/4))</f>
         <v>213.3935292046707</v>
       </c>
-      <c r="I3" s="2">
+      <c r="K3" s="2">
         <f>E3/(70^(3/4))</f>
         <v>231.40060868152614</v>
       </c>
-      <c r="J3" s="4">
-        <f t="shared" ref="J3:J15" si="0">IF(ISBLANK(B3),"",B3/B$3)</f>
+      <c r="L3" s="2">
+        <f t="shared" ref="L3:L21" si="0">F3/(10^(3/4))</f>
+        <v>193.12114393022696</v>
+      </c>
+      <c r="M3" s="2">
+        <f t="shared" ref="M3:M21" si="1">G3/(70^(3/4))</f>
+        <v>21.900414750215866</v>
+      </c>
+      <c r="N3" s="4">
+        <f t="shared" ref="N3:N15" si="2">IF(ISBLANK(B3),"",B3/B$3)</f>
         <v>1</v>
       </c>
-      <c r="K3" s="4">
-        <f t="shared" ref="K3:K15" si="1">IF(ISBLANK(C3),"",C3/C$3)</f>
+      <c r="O3" s="4">
+        <f t="shared" ref="O3:O15" si="3">IF(ISBLANK(C3),"",C3/C$3)</f>
         <v>1</v>
       </c>
-      <c r="L3" s="4">
-        <f t="shared" ref="L3:L15" si="2">IF(ISBLANK(D3),"",D3/D$3)</f>
+      <c r="P3" s="4">
+        <f t="shared" ref="P3:P15" si="4">IF(ISBLANK(D3),"",D3/D$3)</f>
         <v>1</v>
       </c>
-      <c r="M3" s="4">
-        <f t="shared" ref="M3:M16" si="3">IF(ISBLANK(E3),"",E3/E$3)</f>
+      <c r="Q3" s="4">
+        <f t="shared" ref="Q3:Q16" si="5">IF(ISBLANK(E3),"",E3/E$3)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="R3" s="4">
+        <f t="shared" ref="R3:S18" si="6">IF(ISBLANK(F3),"",F3/F$3)</f>
+        <v>1</v>
+      </c>
+      <c r="S3" s="4">
+        <f t="shared" ref="S3:S18" si="7">IF(ISBLANK(G3),"",G3/G$3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="5">
-        <f>F4*0.02</f>
+        <f>H4*0.02</f>
         <v>8.1229672130802191E-2</v>
       </c>
       <c r="C4" s="3">
@@ -6887,45 +7259,71 @@
       <c r="E4" s="3">
         <v>260</v>
       </c>
-      <c r="F4" s="9">
-        <f>$F$3*J4</f>
+      <c r="F4" s="3">
+        <v>20</v>
+      </c>
+      <c r="G4" s="3">
+        <v>32</v>
+      </c>
+      <c r="H4" s="9">
+        <f>$H$3*N4</f>
         <v>4.0614836065401096</v>
       </c>
-      <c r="G4" s="9">
-        <f t="shared" ref="G4:I4" si="4">G$3*K4</f>
+      <c r="I4" s="9">
+        <f>I$3*O4</f>
         <v>1.131370849898476</v>
       </c>
-      <c r="H4" s="9">
+      <c r="J4" s="9">
+        <f>J$3*P4</f>
+        <v>6.2239779351362285</v>
+      </c>
+      <c r="K4" s="9">
+        <f>K$3*Q4</f>
+        <v>10.743599688785142</v>
+      </c>
+      <c r="L4" s="2">
+        <f t="shared" si="0"/>
+        <v>3.5565588200778446</v>
+      </c>
+      <c r="M4" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3222891924658635</v>
+      </c>
+      <c r="N4" s="4">
+        <f>AVERAGE(O4:Q4)</f>
+        <v>2.7000214500214503E-2</v>
+      </c>
+      <c r="O4" s="4">
+        <f t="shared" si="3"/>
+        <v>5.4054054054054057E-3</v>
+      </c>
+      <c r="P4" s="4">
         <f t="shared" si="4"/>
-        <v>6.2239779351362285</v>
-      </c>
-      <c r="I4" s="9">
-        <f t="shared" si="4"/>
-        <v>10.743599688785142</v>
-      </c>
-      <c r="J4" s="4">
-        <f>AVERAGE(K4:M4)</f>
-        <v>2.7000214500214503E-2</v>
-      </c>
-      <c r="K4" s="4">
-        <f t="shared" si="1"/>
-        <v>5.4054054054054057E-3</v>
-      </c>
-      <c r="L4" s="4">
-        <f t="shared" si="2"/>
         <v>2.9166666666666667E-2</v>
       </c>
-      <c r="M4" s="4">
-        <f t="shared" si="3"/>
+      <c r="Q4" s="4">
+        <f t="shared" si="5"/>
         <v>4.642857142857143E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="R4" s="4">
+        <f t="shared" si="6"/>
+        <v>1.841620626151013E-2</v>
+      </c>
+      <c r="S4" s="4">
+        <f t="shared" si="7"/>
+        <v>6.0377358490566038E-2</v>
+      </c>
+      <c r="T4" s="4">
+        <f>S4/(SUM(S$4:S$17)-S$12)</f>
+        <v>5.6864106313847307E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5">
-        <f>F5*0.02</f>
+        <f>H5*0.02</f>
         <v>8.0226199319176385E-3</v>
       </c>
       <c r="C5" s="3">
@@ -6940,45 +7338,73 @@
         <f>0.3/100*E3</f>
         <v>16.8</v>
       </c>
-      <c r="F5" s="9">
-        <f t="shared" ref="F5:F18" si="5">$F$3*J5</f>
+      <c r="F5" s="3">
+        <f>R5*F$3</f>
+        <v>2.8960000000000004</v>
+      </c>
+      <c r="G5" s="3">
+        <f>S5*G$3</f>
+        <v>1.4133333333333336</v>
+      </c>
+      <c r="H5" s="9">
+        <f t="shared" ref="H5:H18" si="8">$H$3*N5</f>
         <v>0.40113099659588192</v>
       </c>
-      <c r="G5" s="9">
-        <f t="shared" ref="G5:G18" si="6">G$3*K5</f>
+      <c r="I5" s="9">
+        <f t="shared" ref="I5:I18" si="9">I$3*O5</f>
         <v>0.6279108216936542</v>
       </c>
-      <c r="H5" s="9">
-        <f t="shared" ref="H5:H18" si="7">H$3*L5</f>
+      <c r="J5" s="9">
+        <f t="shared" ref="J5:J18" si="10">J$3*P5</f>
         <v>0.42678705840934139</v>
       </c>
-      <c r="I5" s="9">
-        <f t="shared" ref="I5:I18" si="8">I$3*M5</f>
+      <c r="K5" s="9">
+        <f t="shared" ref="K5:K18" si="11">K$3*Q5</f>
         <v>0.69420182604457847</v>
       </c>
-      <c r="J5" s="4">
-        <f>AVERAGE(K5:M5)</f>
+      <c r="L5" s="2">
+        <f t="shared" si="0"/>
+        <v>0.51498971714727204</v>
+      </c>
+      <c r="M5" s="2">
+        <f t="shared" si="1"/>
+        <v>5.8401106000575652E-2</v>
+      </c>
+      <c r="N5" s="4">
+        <f>AVERAGE(O5:Q5)</f>
         <v>2.6666666666666666E-3</v>
       </c>
-      <c r="K5" s="4">
-        <f t="shared" si="1"/>
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="L5" s="4">
-        <f t="shared" si="2"/>
-        <v>2E-3</v>
-      </c>
-      <c r="M5" s="4">
+      <c r="O5" s="4">
         <f t="shared" si="3"/>
         <v>3.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P5" s="4">
+        <f t="shared" si="4"/>
+        <v>2E-3</v>
+      </c>
+      <c r="Q5" s="4">
+        <f t="shared" si="5"/>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="R5" s="4">
+        <f>AVERAGE($N5:$Q5)</f>
+        <v>2.666666666666667E-3</v>
+      </c>
+      <c r="S5" s="4">
+        <f>AVERAGE($N5:$Q5)</f>
+        <v>2.666666666666667E-3</v>
+      </c>
+      <c r="T5" s="4">
+        <f t="shared" ref="T5:T17" si="12">S5/(SUM(S$4:S$17)-S$12)</f>
+        <v>2.5114980288615898E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="5">
-        <f>F6*0.02</f>
+        <f>H6*0.02</f>
         <v>0.17532767309545008</v>
       </c>
       <c r="C6" s="3">
@@ -6992,40 +7418,68 @@
         <f>4.2/100*E3</f>
         <v>235.20000000000002</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="3">
+        <f>R6*F4</f>
+        <v>1.1655555555555557</v>
+      </c>
+      <c r="G6" s="3">
+        <f>S6*G$3</f>
+        <v>30.887222222222228</v>
+      </c>
+      <c r="H6" s="9">
+        <f t="shared" si="8"/>
+        <v>8.766383654772504</v>
+      </c>
+      <c r="I6" s="9">
+        <f t="shared" si="9"/>
+        <v>25.535040082208603</v>
+      </c>
+      <c r="J6" s="9">
+        <f t="shared" si="10"/>
+        <v>2.3117632330505993</v>
+      </c>
+      <c r="K6" s="9">
+        <f t="shared" si="11"/>
+        <v>9.7188255646240975</v>
+      </c>
+      <c r="L6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.20726834457009219</v>
+      </c>
+      <c r="M6" s="2">
+        <f t="shared" si="1"/>
+        <v>1.2763075040542471</v>
+      </c>
+      <c r="N6" s="4">
+        <f>AVERAGE(O6:Q6)</f>
+        <v>5.8277777777777789E-2</v>
+      </c>
+      <c r="O6" s="4">
+        <f t="shared" si="3"/>
+        <v>0.12200000000000001</v>
+      </c>
+      <c r="P6" s="4">
+        <f t="shared" si="4"/>
+        <v>1.0833333333333334E-2</v>
+      </c>
+      <c r="Q6" s="4">
         <f t="shared" si="5"/>
-        <v>8.766383654772504</v>
-      </c>
-      <c r="G6" s="9">
-        <f t="shared" si="6"/>
-        <v>25.535040082208603</v>
-      </c>
-      <c r="H6" s="9">
-        <f t="shared" si="7"/>
-        <v>2.3117632330505993</v>
-      </c>
-      <c r="I6" s="9">
-        <f t="shared" si="8"/>
-        <v>9.7188255646240975</v>
-      </c>
-      <c r="J6" s="4">
-        <f>AVERAGE(K6:M6)</f>
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="R6" s="4">
+        <f>AVERAGE($N6:$Q6)</f>
         <v>5.8277777777777789E-2</v>
       </c>
-      <c r="K6" s="4">
-        <f t="shared" si="1"/>
-        <v>0.12200000000000001</v>
-      </c>
-      <c r="L6" s="4">
-        <f t="shared" si="2"/>
-        <v>1.0833333333333334E-2</v>
-      </c>
-      <c r="M6" s="4">
-        <f t="shared" si="3"/>
-        <v>4.2000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S6" s="4">
+        <f>AVERAGE($N6:$Q6)</f>
+        <v>5.8277777777777789E-2</v>
+      </c>
+      <c r="T6" s="4">
+        <f t="shared" si="12"/>
+        <v>5.4886696505745992E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -7042,40 +7496,67 @@
       <c r="E7" s="3">
         <v>700</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="3">
+        <v>72</v>
+      </c>
+      <c r="G7" s="3">
+        <f>S7*G$3</f>
+        <v>28.2314527027027</v>
+      </c>
+      <c r="H7" s="9">
+        <f t="shared" si="8"/>
+        <v>4.963996082874039</v>
+      </c>
+      <c r="I7" s="9">
+        <f t="shared" si="9"/>
+        <v>3.676955262170047</v>
+      </c>
+      <c r="J7" s="9">
+        <f t="shared" si="10"/>
+        <v>8.0022573451751509</v>
+      </c>
+      <c r="K7" s="9">
+        <f t="shared" si="11"/>
+        <v>28.925076085190767</v>
+      </c>
+      <c r="L7" s="2">
+        <f t="shared" si="0"/>
+        <v>12.803611752280242</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="1"/>
+        <v>1.166567024887343</v>
+      </c>
+      <c r="N7" s="4">
+        <f t="shared" si="2"/>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="O7" s="4">
+        <f t="shared" si="3"/>
+        <v>1.7567567567567569E-2</v>
+      </c>
+      <c r="P7" s="4">
+        <f t="shared" si="4"/>
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="Q7" s="4">
         <f t="shared" si="5"/>
-        <v>4.963996082874039</v>
-      </c>
-      <c r="G7" s="9">
+        <v>0.125</v>
+      </c>
+      <c r="R7" s="4">
         <f t="shared" si="6"/>
-        <v>3.676955262170047</v>
-      </c>
-      <c r="H7" s="9">
-        <f t="shared" si="7"/>
-        <v>8.0022573451751509</v>
-      </c>
-      <c r="I7" s="9">
-        <f t="shared" si="8"/>
-        <v>28.925076085190767</v>
-      </c>
-      <c r="J7" s="4">
-        <f t="shared" si="0"/>
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="K7" s="4">
-        <f t="shared" si="1"/>
-        <v>1.7567567567567569E-2</v>
-      </c>
-      <c r="L7" s="4">
-        <f t="shared" si="2"/>
-        <v>3.7499999999999999E-2</v>
-      </c>
-      <c r="M7" s="4">
-        <f t="shared" si="3"/>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <v>6.6298342541436461E-2</v>
+      </c>
+      <c r="S7" s="4">
+        <f>AVERAGE($N7:$Q7)</f>
+        <v>5.326689189189189E-2</v>
+      </c>
+      <c r="T7" s="4">
+        <f t="shared" si="12"/>
+        <v>5.0167385246276196E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -7091,40 +7572,66 @@
       <c r="E8" s="3">
         <v>240</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="3">
+        <v>60</v>
+      </c>
+      <c r="G8" s="3">
+        <v>16</v>
+      </c>
+      <c r="H8" s="9">
+        <f t="shared" si="8"/>
+        <v>5.2648443303209511</v>
+      </c>
+      <c r="I8" s="9">
+        <f t="shared" si="9"/>
+        <v>11.030865786510139</v>
+      </c>
+      <c r="J8" s="9">
+        <f t="shared" si="10"/>
+        <v>9.6027088142101817</v>
+      </c>
+      <c r="K8" s="9">
+        <f t="shared" si="11"/>
+        <v>9.9171689434939783</v>
+      </c>
+      <c r="L8" s="2">
+        <f t="shared" si="0"/>
+        <v>10.669676460233534</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.66114459623293176</v>
+      </c>
+      <c r="N8" s="4">
+        <f t="shared" si="2"/>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="O8" s="4">
+        <f t="shared" si="3"/>
+        <v>5.2702702702702699E-2</v>
+      </c>
+      <c r="P8" s="4">
+        <f t="shared" si="4"/>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="Q8" s="4">
         <f t="shared" si="5"/>
-        <v>5.2648443303209511</v>
-      </c>
-      <c r="G8" s="9">
+        <v>4.2857142857142858E-2</v>
+      </c>
+      <c r="R8" s="4">
         <f t="shared" si="6"/>
-        <v>11.030865786510139</v>
-      </c>
-      <c r="H8" s="9">
+        <v>5.5248618784530384E-2</v>
+      </c>
+      <c r="S8" s="4">
         <f t="shared" si="7"/>
-        <v>9.6027088142101817</v>
-      </c>
-      <c r="I8" s="9">
-        <f t="shared" si="8"/>
-        <v>9.9171689434939783</v>
-      </c>
-      <c r="J8" s="4">
-        <f t="shared" si="0"/>
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="K8" s="4">
-        <f t="shared" si="1"/>
-        <v>5.2702702702702699E-2</v>
-      </c>
-      <c r="L8" s="4">
-        <f t="shared" si="2"/>
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="M8" s="4">
-        <f t="shared" si="3"/>
-        <v>4.2857142857142858E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>3.0188679245283019E-2</v>
+      </c>
+      <c r="T8" s="4">
+        <f t="shared" si="12"/>
+        <v>2.8432053156923653E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -7140,40 +7647,66 @@
       <c r="E9" s="3">
         <v>1240</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="3">
+        <v>138</v>
+      </c>
+      <c r="G9" s="3">
+        <v>80</v>
+      </c>
+      <c r="H9" s="9">
+        <f t="shared" si="8"/>
+        <v>24.443920105061554</v>
+      </c>
+      <c r="I9" s="9">
+        <f t="shared" si="9"/>
+        <v>26.021529547664947</v>
+      </c>
+      <c r="J9" s="9">
+        <f t="shared" si="10"/>
+        <v>38.410835256840727</v>
+      </c>
+      <c r="K9" s="9">
+        <f t="shared" si="11"/>
+        <v>51.238706208052214</v>
+      </c>
+      <c r="L9" s="2">
+        <f t="shared" si="0"/>
+        <v>24.54025585853713</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="1"/>
+        <v>3.3057229811646591</v>
+      </c>
+      <c r="N9" s="4">
+        <f t="shared" si="2"/>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="O9" s="4">
+        <f t="shared" si="3"/>
+        <v>0.12432432432432432</v>
+      </c>
+      <c r="P9" s="4">
+        <f t="shared" si="4"/>
+        <v>0.18</v>
+      </c>
+      <c r="Q9" s="4">
         <f t="shared" si="5"/>
-        <v>24.443920105061554</v>
-      </c>
-      <c r="G9" s="9">
+        <v>0.22142857142857142</v>
+      </c>
+      <c r="R9" s="4">
         <f t="shared" si="6"/>
-        <v>26.021529547664947</v>
-      </c>
-      <c r="H9" s="9">
+        <v>0.1270718232044199</v>
+      </c>
+      <c r="S9" s="4">
         <f t="shared" si="7"/>
-        <v>38.410835256840727</v>
-      </c>
-      <c r="I9" s="9">
-        <f t="shared" si="8"/>
-        <v>51.238706208052214</v>
-      </c>
-      <c r="J9" s="4">
-        <f t="shared" si="0"/>
-        <v>0.16250000000000001</v>
-      </c>
-      <c r="K9" s="4">
-        <f t="shared" si="1"/>
-        <v>0.12432432432432432</v>
-      </c>
-      <c r="L9" s="4">
-        <f t="shared" si="2"/>
-        <v>0.18</v>
-      </c>
-      <c r="M9" s="4">
-        <f t="shared" si="3"/>
-        <v>0.22142857142857142</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.15094339622641509</v>
+      </c>
+      <c r="T9" s="4">
+        <f t="shared" si="12"/>
+        <v>0.14216026578461827</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -7189,40 +7722,66 @@
       <c r="E10" s="3">
         <v>300</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="3">
+        <v>51</v>
+      </c>
+      <c r="G10" s="3">
+        <v>37</v>
+      </c>
+      <c r="H10" s="9">
+        <f t="shared" si="8"/>
+        <v>6.5810554129011871</v>
+      </c>
+      <c r="I10" s="9">
+        <f t="shared" si="9"/>
+        <v>5.6568542494923797</v>
+      </c>
+      <c r="J10" s="9">
+        <f t="shared" si="10"/>
+        <v>14.048407339307486</v>
+      </c>
+      <c r="K10" s="9">
+        <f t="shared" si="11"/>
+        <v>12.396461179367471</v>
+      </c>
+      <c r="L10" s="2">
+        <f t="shared" si="0"/>
+        <v>9.0692249911985048</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="1"/>
+        <v>1.5288968787886548</v>
+      </c>
+      <c r="N10" s="4">
+        <f t="shared" si="2"/>
+        <v>4.3749999999999997E-2</v>
+      </c>
+      <c r="O10" s="4">
+        <f t="shared" si="3"/>
+        <v>2.7027027027027029E-2</v>
+      </c>
+      <c r="P10" s="4">
+        <f t="shared" si="4"/>
+        <v>6.5833333333333327E-2</v>
+      </c>
+      <c r="Q10" s="4">
         <f t="shared" si="5"/>
-        <v>6.5810554129011871</v>
-      </c>
-      <c r="G10" s="9">
+        <v>5.3571428571428568E-2</v>
+      </c>
+      <c r="R10" s="4">
         <f t="shared" si="6"/>
-        <v>5.6568542494923797</v>
-      </c>
-      <c r="H10" s="9">
+        <v>4.6961325966850827E-2</v>
+      </c>
+      <c r="S10" s="4">
         <f t="shared" si="7"/>
-        <v>14.048407339307486</v>
-      </c>
-      <c r="I10" s="9">
-        <f t="shared" si="8"/>
-        <v>12.396461179367471</v>
-      </c>
-      <c r="J10" s="4">
-        <f t="shared" si="0"/>
-        <v>4.3749999999999997E-2</v>
-      </c>
-      <c r="K10" s="4">
-        <f t="shared" si="1"/>
-        <v>2.7027027027027029E-2</v>
-      </c>
-      <c r="L10" s="4">
-        <f t="shared" si="2"/>
-        <v>6.5833333333333327E-2</v>
-      </c>
-      <c r="M10" s="4">
-        <f t="shared" si="3"/>
-        <v>5.3571428571428568E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <v>6.981132075471698E-2</v>
+      </c>
+      <c r="T10" s="4">
+        <f t="shared" si="12"/>
+        <v>6.5749122925385942E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -7238,40 +7797,66 @@
       <c r="E11" s="3">
         <v>1150</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="3">
+        <v>125</v>
+      </c>
+      <c r="G11" s="3">
+        <v>111</v>
+      </c>
+      <c r="H11" s="9">
+        <f t="shared" si="8"/>
+        <v>27.264372424876349</v>
+      </c>
+      <c r="I11" s="9">
+        <f t="shared" si="9"/>
+        <v>27.718585822512662</v>
+      </c>
+      <c r="J11" s="9">
+        <f t="shared" si="10"/>
+        <v>40.900426430895223</v>
+      </c>
+      <c r="K11" s="9">
+        <f t="shared" si="11"/>
+        <v>47.519767854241969</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" si="0"/>
+        <v>22.228492625486531</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="1"/>
+        <v>4.5866906363659643</v>
+      </c>
+      <c r="N11" s="4">
+        <f t="shared" si="2"/>
+        <v>0.18124999999999999</v>
+      </c>
+      <c r="O11" s="4">
+        <f t="shared" si="3"/>
+        <v>0.13243243243243244</v>
+      </c>
+      <c r="P11" s="4">
+        <f t="shared" si="4"/>
+        <v>0.19166666666666668</v>
+      </c>
+      <c r="Q11" s="4">
         <f t="shared" si="5"/>
-        <v>27.264372424876349</v>
-      </c>
-      <c r="G11" s="9">
+        <v>0.20535714285714285</v>
+      </c>
+      <c r="R11" s="4">
         <f t="shared" si="6"/>
-        <v>27.718585822512662</v>
-      </c>
-      <c r="H11" s="9">
+        <v>0.1151012891344383</v>
+      </c>
+      <c r="S11" s="4">
         <f t="shared" si="7"/>
-        <v>40.900426430895223</v>
-      </c>
-      <c r="I11" s="9">
-        <f t="shared" si="8"/>
-        <v>47.519767854241969</v>
-      </c>
-      <c r="J11" s="4">
-        <f t="shared" si="0"/>
-        <v>0.18124999999999999</v>
-      </c>
-      <c r="K11" s="4">
-        <f t="shared" si="1"/>
-        <v>0.13243243243243244</v>
-      </c>
-      <c r="L11" s="4">
-        <f t="shared" si="2"/>
-        <v>0.19166666666666668</v>
-      </c>
-      <c r="M11" s="4">
-        <f t="shared" si="3"/>
-        <v>0.20535714285714285</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.20943396226415095</v>
+      </c>
+      <c r="T11" s="4">
+        <f t="shared" si="12"/>
+        <v>0.19724736877615787</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -7280,51 +7865,77 @@
         <v>1.7999999999999998</v>
       </c>
       <c r="C12" s="3">
-        <f t="shared" ref="C12:M12" si="9">SUM(C10:C11)</f>
+        <f t="shared" ref="C12:Q12" si="13">SUM(C10:C11)</f>
         <v>11.8</v>
       </c>
       <c r="D12" s="3">
+        <f t="shared" si="13"/>
+        <v>309</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="13"/>
+        <v>1450</v>
+      </c>
+      <c r="F12" s="3">
+        <v>218</v>
+      </c>
+      <c r="G12" s="3">
+        <v>177</v>
+      </c>
+      <c r="H12" s="9">
+        <f t="shared" si="8"/>
+        <v>33.845427837777535</v>
+      </c>
+      <c r="I12" s="9">
         <f t="shared" si="9"/>
-        <v>309</v>
-      </c>
-      <c r="E12" s="3">
-        <f t="shared" si="9"/>
-        <v>1450</v>
-      </c>
-      <c r="F12" s="9">
-        <f t="shared" si="5"/>
-        <v>33.845427837777535</v>
-      </c>
-      <c r="G12" s="9">
+        <v>33.375440072005041</v>
+      </c>
+      <c r="J12" s="9">
+        <f t="shared" si="10"/>
+        <v>54.948833770202704</v>
+      </c>
+      <c r="K12" s="9">
+        <f t="shared" si="11"/>
+        <v>59.91622903360944</v>
+      </c>
+      <c r="L12" s="2">
+        <f t="shared" si="0"/>
+        <v>38.766491138848508</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" si="1"/>
+        <v>7.313912095826808</v>
+      </c>
+      <c r="N12" s="4">
+        <f t="shared" si="13"/>
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="O12" s="4">
+        <f t="shared" si="13"/>
+        <v>0.15945945945945947</v>
+      </c>
+      <c r="P12" s="4">
+        <f t="shared" si="13"/>
+        <v>0.25750000000000001</v>
+      </c>
+      <c r="Q12" s="4">
+        <f t="shared" si="13"/>
+        <v>0.2589285714285714</v>
+      </c>
+      <c r="R12" s="4">
         <f t="shared" si="6"/>
-        <v>33.375440072005041</v>
-      </c>
-      <c r="H12" s="9">
+        <v>0.20073664825046039</v>
+      </c>
+      <c r="S12" s="4">
         <f t="shared" si="7"/>
-        <v>54.948833770202704</v>
-      </c>
-      <c r="I12" s="9">
-        <f t="shared" si="8"/>
-        <v>59.91622903360944</v>
-      </c>
-      <c r="J12" s="4">
-        <f t="shared" si="9"/>
-        <v>0.22499999999999998</v>
-      </c>
-      <c r="K12" s="4">
-        <f t="shared" si="9"/>
-        <v>0.15945945945945947</v>
-      </c>
-      <c r="L12" s="4">
-        <f t="shared" si="9"/>
-        <v>0.25750000000000001</v>
-      </c>
-      <c r="M12" s="4">
-        <f t="shared" si="9"/>
-        <v>0.2589285714285714</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.33396226415094338</v>
+      </c>
+      <c r="T12" s="4">
+        <f t="shared" si="12"/>
+        <v>0.31452958804846792</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -7344,40 +7955,68 @@
         <f>2.5/100*E3</f>
         <v>140</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="3">
+        <f>R13*F$3</f>
+        <v>37.738500000000002</v>
+      </c>
+      <c r="G13" s="3">
+        <f>S13*G$3</f>
+        <v>18.4175</v>
+      </c>
+      <c r="H13" s="9">
+        <f t="shared" si="8"/>
+        <v>0.75212061861727864</v>
+      </c>
+      <c r="I13" s="9">
+        <f t="shared" si="9"/>
+        <v>4.3953757518555792</v>
+      </c>
+      <c r="J13" s="9">
+        <f t="shared" si="10"/>
+        <v>18.778630570011025</v>
+      </c>
+      <c r="K13" s="9">
+        <f t="shared" si="11"/>
+        <v>5.7850152170381541</v>
+      </c>
+      <c r="L13" s="2">
+        <f t="shared" si="0"/>
+        <v>6.7109597515753876</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="1"/>
+        <v>0.76103941257000129</v>
+      </c>
+      <c r="N13" s="4">
+        <f t="shared" si="2"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="O13" s="4">
+        <f t="shared" si="3"/>
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="P13" s="4">
+        <f t="shared" si="4"/>
+        <v>8.8000000000000009E-2</v>
+      </c>
+      <c r="Q13" s="4">
         <f t="shared" si="5"/>
-        <v>0.75212061861727864</v>
-      </c>
-      <c r="G13" s="9">
-        <f t="shared" si="6"/>
-        <v>4.3953757518555792</v>
-      </c>
-      <c r="H13" s="9">
-        <f t="shared" si="7"/>
-        <v>18.778630570011025</v>
-      </c>
-      <c r="I13" s="9">
-        <f t="shared" si="8"/>
-        <v>5.7850152170381541</v>
-      </c>
-      <c r="J13" s="4">
-        <f t="shared" si="0"/>
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="K13" s="4">
-        <f t="shared" si="1"/>
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="L13" s="4">
-        <f t="shared" si="2"/>
-        <v>8.8000000000000009E-2</v>
-      </c>
-      <c r="M13" s="4">
-        <f t="shared" si="3"/>
         <v>2.5000000000000001E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="R13" s="4">
+        <f>AVERAGE($N13:$Q13)</f>
+        <v>3.4750000000000003E-2</v>
+      </c>
+      <c r="S13" s="4">
+        <f>AVERAGE($N13:$Q13)</f>
+        <v>3.4750000000000003E-2</v>
+      </c>
+      <c r="T13" s="4">
+        <f t="shared" si="12"/>
+        <v>3.2727958688602593E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -7393,40 +8032,66 @@
       <c r="E14" s="3">
         <v>750</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="3">
+        <v>90</v>
+      </c>
+      <c r="G14" s="3">
+        <v>155</v>
+      </c>
+      <c r="H14" s="9">
+        <f t="shared" si="8"/>
+        <v>17.110744073543088</v>
+      </c>
+      <c r="I14" s="9">
+        <f t="shared" si="9"/>
+        <v>21.213203435596427</v>
+      </c>
+      <c r="J14" s="9">
+        <f t="shared" si="10"/>
+        <v>44.456985250973062</v>
+      </c>
+      <c r="K14" s="9">
+        <f t="shared" si="11"/>
+        <v>30.991152948418677</v>
+      </c>
+      <c r="L14" s="2">
+        <f t="shared" si="0"/>
+        <v>16.004514690350302</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="1"/>
+        <v>6.4048382760065268</v>
+      </c>
+      <c r="N14" s="4">
+        <f t="shared" si="2"/>
+        <v>0.11375</v>
+      </c>
+      <c r="O14" s="4">
+        <f t="shared" si="3"/>
+        <v>0.10135135135135136</v>
+      </c>
+      <c r="P14" s="4">
+        <f t="shared" si="4"/>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="Q14" s="4">
         <f t="shared" si="5"/>
-        <v>17.110744073543088</v>
-      </c>
-      <c r="G14" s="9">
+        <v>0.13392857142857142</v>
+      </c>
+      <c r="R14" s="4">
         <f t="shared" si="6"/>
-        <v>21.213203435596427</v>
-      </c>
-      <c r="H14" s="9">
+        <v>8.2872928176795577E-2</v>
+      </c>
+      <c r="S14" s="4">
         <f t="shared" si="7"/>
-        <v>44.456985250973062</v>
-      </c>
-      <c r="I14" s="9">
-        <f t="shared" si="8"/>
-        <v>30.991152948418677</v>
-      </c>
-      <c r="J14" s="4">
-        <f t="shared" si="0"/>
-        <v>0.11375</v>
-      </c>
-      <c r="K14" s="4">
-        <f t="shared" si="1"/>
-        <v>0.10135135135135136</v>
-      </c>
-      <c r="L14" s="4">
-        <f t="shared" si="2"/>
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="M14" s="4">
-        <f t="shared" si="3"/>
-        <v>0.13392857142857142</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.29245283018867924</v>
+      </c>
+      <c r="T14" s="4">
+        <f t="shared" si="12"/>
+        <v>0.27543551495769786</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -7442,199 +8107,308 @@
       <c r="E15" s="3">
         <v>300</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="3">
+        <v>54</v>
+      </c>
+      <c r="G15" s="3">
+        <f>S15*G$3</f>
+        <v>35.315641087516084</v>
+      </c>
+      <c r="H15" s="9">
+        <f t="shared" si="8"/>
+        <v>7.709236340827105</v>
+      </c>
+      <c r="I15" s="9">
+        <f t="shared" si="9"/>
+        <v>16.404877323527902</v>
+      </c>
+      <c r="J15" s="9">
+        <f t="shared" si="10"/>
+        <v>17.782794100389225</v>
+      </c>
+      <c r="K15" s="9">
+        <f t="shared" si="11"/>
+        <v>12.396461179367471</v>
+      </c>
+      <c r="L15" s="2">
+        <f t="shared" si="0"/>
+        <v>9.6027088142101817</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="1"/>
+        <v>1.4592965792195598</v>
+      </c>
+      <c r="N15" s="4">
+        <f t="shared" si="2"/>
+        <v>5.1249999999999997E-2</v>
+      </c>
+      <c r="O15" s="4">
+        <f t="shared" si="3"/>
+        <v>7.8378378378378383E-2</v>
+      </c>
+      <c r="P15" s="4">
+        <f t="shared" si="4"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="Q15" s="4">
         <f t="shared" si="5"/>
-        <v>7.709236340827105</v>
-      </c>
-      <c r="G15" s="9">
+        <v>5.3571428571428568E-2</v>
+      </c>
+      <c r="R15" s="4">
         <f t="shared" si="6"/>
-        <v>16.404877323527902</v>
-      </c>
-      <c r="H15" s="9">
-        <f t="shared" si="7"/>
-        <v>17.782794100389225</v>
-      </c>
-      <c r="I15" s="9">
-        <f t="shared" si="8"/>
-        <v>12.396461179367471</v>
-      </c>
-      <c r="J15" s="4">
-        <f t="shared" si="0"/>
-        <v>5.1249999999999997E-2</v>
-      </c>
-      <c r="K15" s="4">
-        <f t="shared" si="1"/>
-        <v>7.8378378378378383E-2</v>
-      </c>
-      <c r="L15" s="4">
-        <f t="shared" si="2"/>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="M15" s="4">
-        <f t="shared" si="3"/>
-        <v>5.3571428571428568E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+        <v>4.9723756906077346E-2</v>
+      </c>
+      <c r="S15" s="4">
+        <f>AVERAGE($N15:$Q15)</f>
+        <v>6.6633285070785059E-2</v>
+      </c>
+      <c r="T15" s="4">
+        <f t="shared" si="12"/>
+        <v>6.2756011541943393E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="5">
-        <f>F16*0.02</f>
+        <f>H16*0.02</f>
         <v>4.8135719591505838E-2</v>
       </c>
       <c r="C16" s="5">
-        <f>H16*0.25</f>
+        <f>J16*0.25</f>
         <v>0.85357411681868278</v>
       </c>
       <c r="D16" s="5">
-        <f>H16*10</f>
+        <f>J16*10</f>
         <v>34.142964672747311</v>
       </c>
       <c r="E16" s="3">
         <f>1.6/100*E3</f>
         <v>89.600000000000009</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="3">
+        <f>R16*F$3</f>
+        <v>17.376000000000001</v>
+      </c>
+      <c r="G16" s="3">
+        <f>S16*G$3</f>
+        <v>8.48</v>
+      </c>
+      <c r="H16" s="9">
+        <f t="shared" si="8"/>
+        <v>2.4067859795752917</v>
+      </c>
+      <c r="I16" s="9">
+        <f t="shared" si="9"/>
+        <v>3.3488577156994888</v>
+      </c>
+      <c r="J16" s="9">
+        <f t="shared" si="10"/>
+        <v>3.4142964672747311</v>
+      </c>
+      <c r="K16" s="9">
+        <f t="shared" si="11"/>
+        <v>3.7024097389044184</v>
+      </c>
+      <c r="L16" s="2">
+        <f t="shared" si="0"/>
+        <v>3.0899383028836316</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" si="1"/>
+        <v>0.35040663600345384</v>
+      </c>
+      <c r="N16" s="6">
+        <f>Q16</f>
+        <v>1.6E-2</v>
+      </c>
+      <c r="O16" s="6">
+        <f>Q16</f>
+        <v>1.6E-2</v>
+      </c>
+      <c r="P16" s="6">
+        <f>Q16</f>
+        <v>1.6E-2</v>
+      </c>
+      <c r="Q16" s="4">
         <f t="shared" si="5"/>
-        <v>2.4067859795752917</v>
-      </c>
-      <c r="G16" s="9">
-        <f t="shared" si="6"/>
-        <v>3.3488577156994888</v>
-      </c>
-      <c r="H16" s="9">
-        <f t="shared" si="7"/>
-        <v>3.4142964672747311</v>
-      </c>
-      <c r="I16" s="9">
-        <f t="shared" si="8"/>
-        <v>3.7024097389044184</v>
-      </c>
-      <c r="J16" s="6">
-        <f>M16</f>
         <v>1.6E-2</v>
       </c>
-      <c r="K16" s="6">
-        <f>M16</f>
+      <c r="R16" s="4">
+        <f>AVERAGE($N16:$Q16)</f>
         <v>1.6E-2</v>
       </c>
-      <c r="L16" s="6">
-        <f>M16</f>
+      <c r="S16" s="4">
+        <f>AVERAGE($N16:$Q16)</f>
         <v>1.6E-2</v>
       </c>
-      <c r="M16" s="4">
-        <f t="shared" si="3"/>
-        <v>1.6E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="T16" s="4">
+        <f t="shared" si="12"/>
+        <v>1.5068988173169536E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="5">
-        <f>F17*0.02</f>
+        <f>H17*0.02</f>
         <v>4.1366634023950327E-2</v>
       </c>
       <c r="C17" s="5">
-        <f>H17*0.25</f>
+        <f>J17*0.25</f>
         <v>0.73354025664105549</v>
       </c>
       <c r="D17" s="5">
-        <f>H17*10</f>
+        <f>J17*10</f>
         <v>29.34161026564222</v>
       </c>
       <c r="E17" s="3">
         <f>1.1*70</f>
         <v>77</v>
       </c>
-      <c r="F17" s="9">
-        <f t="shared" si="5"/>
+      <c r="F17" s="3">
+        <v>21</v>
+      </c>
+      <c r="G17" s="3">
+        <v>9</v>
+      </c>
+      <c r="H17" s="9">
+        <f t="shared" si="8"/>
         <v>2.0683317011975162</v>
       </c>
-      <c r="G17" s="9">
-        <f t="shared" si="6"/>
+      <c r="I17" s="9">
+        <f t="shared" si="9"/>
         <v>2.8779245994292482</v>
       </c>
-      <c r="H17" s="9">
-        <f t="shared" si="7"/>
+      <c r="J17" s="9">
+        <f t="shared" si="10"/>
         <v>2.934161026564222</v>
       </c>
-      <c r="I17" s="9">
-        <f t="shared" si="8"/>
+      <c r="K17" s="9">
+        <f t="shared" si="11"/>
         <v>3.1817583693709843</v>
       </c>
-      <c r="J17" s="6">
-        <f>M17</f>
+      <c r="L17" s="2">
+        <f t="shared" si="0"/>
+        <v>3.7343867610817369</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" si="1"/>
+        <v>0.37189383538102411</v>
+      </c>
+      <c r="N17" s="6">
+        <f>Q17</f>
         <v>1.375E-2</v>
       </c>
-      <c r="K17" s="6">
-        <f>M17</f>
+      <c r="O17" s="6">
+        <f>Q17</f>
         <v>1.375E-2</v>
       </c>
-      <c r="L17" s="6">
-        <f>M17</f>
+      <c r="P17" s="6">
+        <f>Q17</f>
         <v>1.375E-2</v>
       </c>
-      <c r="M17" s="4">
+      <c r="Q17" s="4">
         <f>IF(ISBLANK(E17),"",E17/E$3)</f>
         <v>1.375E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="R17" s="4">
+        <f t="shared" si="6"/>
+        <v>1.9337016574585635E-2</v>
+      </c>
+      <c r="S17" s="4">
+        <f t="shared" si="7"/>
+        <v>1.6981132075471698E-2</v>
+      </c>
+      <c r="T17" s="4">
+        <f t="shared" si="12"/>
+        <v>1.5993029900769555E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>30</v>
       </c>
       <c r="B18" s="5">
-        <f>B3*J18</f>
+        <f>B3*N18</f>
         <v>2.0544427284427274</v>
       </c>
       <c r="C18" s="5">
-        <f>C3*K18</f>
+        <f>C3*O18</f>
         <v>21.0945</v>
       </c>
       <c r="D18" s="5">
-        <f>D3*L18</f>
+        <f>D3*P18</f>
         <v>34.300000000000288</v>
       </c>
       <c r="E18" s="5">
-        <f>E3*M18</f>
+        <f>E3*Q18</f>
         <v>101.40000000000136</v>
       </c>
-      <c r="F18" s="9">
-        <f t="shared" si="5"/>
+      <c r="F18" s="3">
+        <f>R18*F$3</f>
+        <v>333.69983333333329</v>
+      </c>
+      <c r="G18" s="3">
+        <f>T18*G$3</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="9">
+        <f t="shared" si="8"/>
         <v>38.629718395752846</v>
       </c>
-      <c r="G18" s="9">
-        <f t="shared" si="6"/>
+      <c r="I18" s="9">
+        <f t="shared" si="9"/>
         <v>59.664255982958501</v>
       </c>
-      <c r="H18" s="9">
-        <f t="shared" si="7"/>
+      <c r="J18" s="9">
+        <f t="shared" si="10"/>
         <v>6.0994983764335551</v>
       </c>
-      <c r="I18" s="9">
-        <f t="shared" si="8"/>
+      <c r="K18" s="9">
+        <f t="shared" si="11"/>
         <v>4.1900038786262614</v>
       </c>
-      <c r="J18" s="6">
-        <f>1-SUM(J4:J17)+J12</f>
+      <c r="L18" s="2">
+        <f t="shared" si="0"/>
+        <v>59.341154275008662</v>
+      </c>
+      <c r="M18" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="6">
+        <f>1-SUM(N4:N17)+N12</f>
         <v>0.25680534105534092</v>
       </c>
-      <c r="K18" s="6">
-        <f>1-SUM(K4:K17)+K12</f>
+      <c r="O18" s="6">
+        <f>1-SUM(O4:O17)+O12</f>
         <v>0.28506081081081081</v>
       </c>
-      <c r="L18" s="6">
-        <f>1-SUM(L4:L17)+L12</f>
+      <c r="P18" s="6">
+        <f>1-SUM(P4:P17)+P12</f>
         <v>2.8583333333333572E-2</v>
       </c>
-      <c r="M18" s="6">
-        <f>1-SUM(M4:M17)+M12</f>
+      <c r="Q18" s="6">
+        <f>1-SUM(Q4:Q17)+Q12</f>
         <v>1.8107142857143099E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="R18" s="6">
+        <f>1-SUM(R4:R17)+R12</f>
+        <v>0.30727424800491093</v>
+      </c>
+      <c r="S18" s="6">
+        <f>1-SUM(S4:S17)+S12</f>
+        <v>-6.1783300652404727E-2</v>
+      </c>
+      <c r="T18" s="6">
+        <f>1-SUM(T4:T17)+T12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>71</v>
       </c>
@@ -7654,28 +8428,43 @@
         <f>1400/60/24</f>
         <v>0.97222222222222221</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="3">
+        <f>375/24/60</f>
+        <v>0.26041666666666669</v>
+      </c>
+      <c r="G19" s="3">
+        <v>150</v>
+      </c>
+      <c r="H19" s="2">
         <f>B19/(0.02)^(3/4)</f>
         <v>1.3057649628772197E-2</v>
       </c>
-      <c r="G19" s="2">
+      <c r="I19" s="2">
         <f>C19/0.25^(3/4)</f>
         <v>9.8209275164798271E-2</v>
       </c>
-      <c r="H19" s="2">
+      <c r="J19" s="2">
         <f>D19/(10^(3/4))</f>
         <v>3.704748770914422E-2</v>
       </c>
-      <c r="I19" s="2">
+      <c r="K19" s="2">
         <f>E19/(70^(3/4))</f>
         <v>4.0173716784987171E-2</v>
       </c>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L19" s="2">
+        <f t="shared" si="0"/>
+        <v>4.6309359636430271E-2</v>
+      </c>
+      <c r="M19" s="2">
+        <f t="shared" si="1"/>
+        <v>6.1982305896837353</v>
+      </c>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -7695,28 +8484,43 @@
         <f>350/60/24</f>
         <v>0.24305555555555555</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="3">
+        <f>125/24/60</f>
+        <v>8.6805555555555552E-2</v>
+      </c>
+      <c r="G20" s="3">
+        <v>300</v>
+      </c>
+      <c r="H20" s="2">
         <f>B20/(0.02)^(3/4)</f>
         <v>2.6115299257544394E-2</v>
       </c>
-      <c r="G20" s="2">
+      <c r="I20" s="2">
         <f>C20/0.25^(3/4)</f>
         <v>4.4194173824159216E-2</v>
       </c>
-      <c r="H20" s="2">
+      <c r="J20" s="2">
         <f>D20/(10^(3/4))</f>
         <v>1.4818995083657686E-2</v>
       </c>
-      <c r="I20" s="2">
+      <c r="K20" s="2">
         <f>E20/(70^(3/4))</f>
         <v>1.0043429196246793E-2</v>
       </c>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L20" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5436453212143424E-2</v>
+      </c>
+      <c r="M20" s="2">
+        <f t="shared" si="1"/>
+        <v>12.396461179367471</v>
+      </c>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>73</v>
       </c>
@@ -7732,55 +8536,70 @@
       <c r="E21" s="3">
         <v>125</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="3">
+        <f>10.4</f>
+        <v>10.4</v>
+      </c>
+      <c r="G21" s="3">
+        <v>7.8</v>
+      </c>
+      <c r="H21" s="2">
         <f>B21/(0.02)^(3/4)</f>
         <v>5.2648443303209502</v>
       </c>
-      <c r="G21" s="2">
+      <c r="I21" s="2">
         <f>C21/0.25^(3/4)</f>
         <v>3.705239533417509</v>
       </c>
-      <c r="H21" s="2">
+      <c r="J21" s="2">
         <f>D21/(10^(3/4))</f>
         <v>10.900852783538594</v>
       </c>
-      <c r="I21" s="2">
+      <c r="K21" s="2">
         <f>E21/(70^(3/4))</f>
         <v>5.1651921580697797</v>
       </c>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L21" s="2">
+        <f t="shared" si="0"/>
+        <v>1.8494105864404793</v>
+      </c>
+      <c r="M21" s="2">
+        <f t="shared" si="1"/>
+        <v>0.32230799066355426</v>
+      </c>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="27" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="40" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H40" s="7"/>
+    <row r="40" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J40" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="H1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7791,7 +8610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -7802,20 +8621,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26" t="s">
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -8075,20 +8894,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26" t="s">
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
     </row>
     <row r="2" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -10302,39 +11121,39 @@
         <v>Bone</v>
       </c>
       <c r="B52" s="2">
-        <f>TissueComp!D$4*INDEX(VolumeFlow!$A50:$D62,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A50:$A62,0),4)</f>
+        <f>TissueComp!D$4*INDEX(VolumeFlow!$A50:$D75,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A50:$A75,0),4)</f>
         <v>3.3246000000000005E-2</v>
       </c>
       <c r="C52" s="2">
-        <f>TissueComp!E$4*INDEX(VolumeFlow!$A50:$D62,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A50:$A62,0),4)</f>
+        <f>TissueComp!E$4*INDEX(VolumeFlow!$A50:$D75,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A50:$A75,0),4)</f>
         <v>3.6940000000000002E-3</v>
       </c>
       <c r="D52" s="2">
-        <f>TissueComp!F$4*INDEX(VolumeFlow!$A50:$D62,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A50:$A62,0),4)</f>
+        <f>TissueComp!F$4*INDEX(VolumeFlow!$A50:$D75,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A50:$A75,0),4)</f>
         <v>9.6044000000000008E-3</v>
       </c>
       <c r="E52" s="2">
-        <f>TissueComp!G$4*INDEX(VolumeFlow!$A50:$D62,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A50:$A62,0),4)</f>
+        <f>TissueComp!G$4*INDEX(VolumeFlow!$A50:$D75,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A50:$A75,0),4)</f>
         <v>7.3880000000000007E-4</v>
       </c>
       <c r="F52" s="2">
-        <f>TissueComp!H$4*INDEX(VolumeFlow!$A50:$D62,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A50:$A62,0),4)</f>
+        <f>TissueComp!H$4*INDEX(VolumeFlow!$A50:$D75,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A50:$A75,0),4)</f>
         <v>7.7574000000000002E-3</v>
       </c>
       <c r="G52" s="2">
-        <f>TissueComp!I$4*INDEX(VolumeFlow!$A50:$D62,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A50:$A62,0),4)</f>
+        <f>TissueComp!I$4*INDEX(VolumeFlow!$A50:$D75,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A50:$A75,0),4)</f>
         <v>3.1398999999999996E-2</v>
       </c>
       <c r="H52" s="2">
-        <f>TissueComp!J$4*INDEX(VolumeFlow!$A50:$D62,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A50:$A62,0),4)</f>
+        <f>TissueComp!J$4*INDEX(VolumeFlow!$A50:$D75,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A50:$A75,0),4)</f>
         <v>4.0634E-3</v>
       </c>
       <c r="I52" s="2">
-        <f>TissueComp!K$4*INDEX(VolumeFlow!$A50:$D62,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A50:$A62,0),4)</f>
+        <f>TissueComp!K$4*INDEX(VolumeFlow!$A50:$D75,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A50:$A75,0),4)</f>
         <v>1.4776000000000001E-3</v>
       </c>
       <c r="J52" s="2">
-        <f>TissueComp!L$4*INDEX(VolumeFlow!$A50:$D62,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A50:$A62,0),4)</f>
+        <f>TissueComp!L$4*INDEX(VolumeFlow!$A50:$D75,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A50:$A75,0),4)</f>
         <v>0.25858000000000003</v>
       </c>
       <c r="K52" t="s">
@@ -10347,39 +11166,39 @@
         <v>Brain</v>
       </c>
       <c r="B53" s="2">
-        <f>TissueComp!D$5*INDEX(VolumeFlow!$A51:$D63,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A51:$A63,0),4)</f>
+        <f>TissueComp!D$5*INDEX(VolumeFlow!$A51:$D76,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A51:$A76,0),4)</f>
         <v>5.4724999999999999E-3</v>
       </c>
       <c r="C53" s="2">
-        <f>TissueComp!E$5*INDEX(VolumeFlow!$A51:$D63,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A51:$A63,0),4)</f>
+        <f>TissueComp!E$5*INDEX(VolumeFlow!$A51:$D76,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A51:$A76,0),4)</f>
         <v>2.7499999999999998E-5</v>
       </c>
       <c r="D53" s="2">
-        <f>TissueComp!F$5*INDEX(VolumeFlow!$A51:$D63,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A51:$A63,0),4)</f>
+        <f>TissueComp!F$5*INDEX(VolumeFlow!$A51:$D76,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A51:$A76,0),4)</f>
         <v>4.4235833610764344E-3</v>
       </c>
       <c r="E53" s="2">
-        <f>TissueComp!G$5*INDEX(VolumeFlow!$A51:$D63,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A51:$A63,0),4)</f>
+        <f>TissueComp!G$5*INDEX(VolumeFlow!$A51:$D76,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A51:$A76,0),4)</f>
         <v>6.1764545366767092E-4</v>
       </c>
       <c r="F53" s="2">
-        <f>TissueComp!H$5*INDEX(VolumeFlow!$A51:$D63,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A51:$A63,0),4)</f>
+        <f>TissueComp!H$5*INDEX(VolumeFlow!$A51:$D76,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A51:$A76,0),4)</f>
         <v>4.5877118525589278E-4</v>
       </c>
       <c r="G53" s="2">
-        <f>TissueComp!I$5*INDEX(VolumeFlow!$A51:$D63,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A51:$A63,0),4)</f>
+        <f>TissueComp!I$5*INDEX(VolumeFlow!$A51:$D76,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A51:$A76,0),4)</f>
         <v>2.053601062064387E-3</v>
       </c>
       <c r="H53" s="2">
-        <f>TissueComp!J$5*INDEX(VolumeFlow!$A51:$D63,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A51:$A63,0),4)</f>
+        <f>TissueComp!J$5*INDEX(VolumeFlow!$A51:$D76,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A51:$A76,0),4)</f>
         <v>2.5236475273813482E-3</v>
       </c>
       <c r="I53" s="2">
-        <f>TissueComp!K$5*INDEX(VolumeFlow!$A51:$D63,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A51:$A63,0),4)</f>
+        <f>TissueComp!K$5*INDEX(VolumeFlow!$A51:$D76,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A51:$A76,0),4)</f>
         <v>9.227514105542645E-4</v>
       </c>
       <c r="J53" s="2">
-        <f>TissueComp!L$5*INDEX(VolumeFlow!$A51:$D63,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A51:$A63,0),4)</f>
+        <f>TissueComp!L$5*INDEX(VolumeFlow!$A51:$D76,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A51:$A76,0),4)</f>
         <v>3.9049999999999994E-2</v>
       </c>
       <c r="K53" t="s">
@@ -10392,39 +11211,39 @@
         <v>Gut</v>
       </c>
       <c r="B54" s="2">
-        <f>TissueComp!D$6*INDEX(VolumeFlow!$A52:$D64,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A52:$A64,0),4)</f>
+        <f>TissueComp!D$6*INDEX(VolumeFlow!$A52:$D77,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A52:$A77,0),4)</f>
         <v>4.3200000000000002E-2</v>
       </c>
       <c r="C54" s="2">
-        <f>TissueComp!E$6*INDEX(VolumeFlow!$A52:$D64,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A52:$A64,0),4)</f>
+        <f>TissueComp!E$6*INDEX(VolumeFlow!$A52:$D77,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A52:$A77,0),4)</f>
         <v>4.6080000000000001E-3</v>
       </c>
       <c r="D54" s="2">
-        <f>TissueComp!F$6*INDEX(VolumeFlow!$A52:$D64,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A52:$A64,0),4)</f>
+        <f>TissueComp!F$6*INDEX(VolumeFlow!$A52:$D77,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A52:$A77,0),4)</f>
         <v>3.7440000000000001E-2</v>
       </c>
       <c r="E54" s="2">
-        <f>TissueComp!G$6*INDEX(VolumeFlow!$A52:$D64,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A52:$A64,0),4)</f>
+        <f>TissueComp!G$6*INDEX(VolumeFlow!$A52:$D77,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A52:$A77,0),4)</f>
         <v>3.3600000000000006E-3</v>
       </c>
       <c r="F54" s="2">
-        <f>TissueComp!H$6*INDEX(VolumeFlow!$A52:$D64,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A52:$A64,0),4)</f>
+        <f>TissueComp!H$6*INDEX(VolumeFlow!$A52:$D77,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A52:$A77,0),4)</f>
         <v>7.1999999999999998E-3</v>
       </c>
       <c r="G54" s="2">
-        <f>TissueComp!I$6*INDEX(VolumeFlow!$A52:$D64,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A52:$A64,0),4)</f>
+        <f>TissueComp!I$6*INDEX(VolumeFlow!$A52:$D77,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A52:$A77,0),4)</f>
         <v>3.3119999999999997E-2</v>
       </c>
       <c r="H54" s="2">
-        <f>TissueComp!J$6*INDEX(VolumeFlow!$A52:$D64,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A52:$A64,0),4)</f>
+        <f>TissueComp!J$6*INDEX(VolumeFlow!$A52:$D77,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A52:$A77,0),4)</f>
         <v>1.2480000000000002E-2</v>
       </c>
       <c r="I54" s="2">
-        <f>TissueComp!K$6*INDEX(VolumeFlow!$A52:$D64,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A52:$A64,0),4)</f>
+        <f>TissueComp!K$6*INDEX(VolumeFlow!$A52:$D77,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A52:$A77,0),4)</f>
         <v>2.4000000000000002E-3</v>
       </c>
       <c r="J54" s="2">
-        <f>TissueComp!L$6*INDEX(VolumeFlow!$A52:$D64,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A52:$A64,0),4)</f>
+        <f>TissueComp!L$6*INDEX(VolumeFlow!$A52:$D77,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A52:$A77,0),4)</f>
         <v>0.33600000000000002</v>
       </c>
       <c r="K54" t="s">
@@ -10437,39 +11256,39 @@
         <v>Heart</v>
       </c>
       <c r="B55" s="2">
-        <f>TissueComp!D$7*INDEX(VolumeFlow!$A53:$D65,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A53:$A65,0),4)</f>
+        <f>TissueComp!D$7*INDEX(VolumeFlow!$A53:$D78,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A53:$A78,0),4)</f>
         <v>1.8E-3</v>
       </c>
       <c r="C55" s="2">
-        <f>TissueComp!E$7*INDEX(VolumeFlow!$A53:$D65,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A53:$A65,0),4)</f>
+        <f>TissueComp!E$7*INDEX(VolumeFlow!$A53:$D78,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A53:$A78,0),4)</f>
         <v>5.9999999999999995E-4</v>
       </c>
       <c r="D55" s="2">
-        <f>TissueComp!F$7*INDEX(VolumeFlow!$A53:$D65,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A53:$A65,0),4)</f>
+        <f>TissueComp!F$7*INDEX(VolumeFlow!$A53:$D78,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A53:$A78,0),4)</f>
         <v>1.669673441146632E-3</v>
       </c>
       <c r="E55" s="2">
-        <f>TissueComp!G$7*INDEX(VolumeFlow!$A53:$D65,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A53:$A65,0),4)</f>
+        <f>TissueComp!G$7*INDEX(VolumeFlow!$A53:$D78,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A53:$A78,0),4)</f>
         <v>3.3006704486848796E-4</v>
       </c>
       <c r="F55" s="2">
-        <f>TissueComp!H$7*INDEX(VolumeFlow!$A53:$D65,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A53:$A65,0),4)</f>
+        <f>TissueComp!H$7*INDEX(VolumeFlow!$A53:$D78,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A53:$A78,0),4)</f>
         <v>4.0025951398487997E-4</v>
       </c>
       <c r="G55" s="2">
-        <f>TissueComp!I$7*INDEX(VolumeFlow!$A53:$D65,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A53:$A65,0),4)</f>
+        <f>TissueComp!I$7*INDEX(VolumeFlow!$A53:$D78,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A53:$A78,0),4)</f>
         <v>2.1362136213621359E-3</v>
       </c>
       <c r="H55" s="2">
-        <f>TissueComp!J$7*INDEX(VolumeFlow!$A53:$D65,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A53:$A65,0),4)</f>
+        <f>TissueComp!J$7*INDEX(VolumeFlow!$A53:$D78,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A53:$A78,0),4)</f>
         <v>1.8961896189618956E-4</v>
       </c>
       <c r="I55" s="2">
-        <f>TissueComp!K$7*INDEX(VolumeFlow!$A53:$D65,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A53:$A65,0),4)</f>
+        <f>TissueComp!K$7*INDEX(VolumeFlow!$A53:$D78,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A53:$A78,0),4)</f>
         <v>7.4167416741674152E-5</v>
       </c>
       <c r="J55" s="2">
-        <f>TissueComp!L$7*INDEX(VolumeFlow!$A53:$D65,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A53:$A65,0),4)</f>
+        <f>TissueComp!L$7*INDEX(VolumeFlow!$A53:$D78,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A53:$A78,0),4)</f>
         <v>1.7039999999999996E-2</v>
       </c>
       <c r="K55" t="s">
@@ -10482,39 +11301,39 @@
         <v>Kidney</v>
       </c>
       <c r="B56" s="2">
-        <f>TissueComp!D$8*INDEX(VolumeFlow!$A54:$D66,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A54:$A66,0),4)</f>
+        <f>TissueComp!D$8*INDEX(VolumeFlow!$A54:$D79,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A54:$A79,0),4)</f>
         <v>5.0099999999999997E-3</v>
       </c>
       <c r="C56" s="2">
-        <f>TissueComp!E$8*INDEX(VolumeFlow!$A54:$D66,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A54:$A66,0),4)</f>
+        <f>TissueComp!E$8*INDEX(VolumeFlow!$A54:$D79,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A54:$A79,0),4)</f>
         <v>9.8999999999999999E-4</v>
       </c>
       <c r="D56" s="2">
-        <f>TissueComp!F$8*INDEX(VolumeFlow!$A54:$D66,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A54:$A66,0),4)</f>
+        <f>TissueComp!F$8*INDEX(VolumeFlow!$A54:$D79,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A54:$A79,0),4)</f>
         <v>4.5966214967421001E-3</v>
       </c>
       <c r="E56" s="2">
-        <f>TissueComp!G$8*INDEX(VolumeFlow!$A54:$D66,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A54:$A66,0),4)</f>
+        <f>TissueComp!G$8*INDEX(VolumeFlow!$A54:$D79,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A54:$A79,0),4)</f>
         <v>3.8443612800121265E-4</v>
       </c>
       <c r="F56" s="2">
-        <f>TissueComp!H$8*INDEX(VolumeFlow!$A54:$D66,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A54:$A66,0),4)</f>
+        <f>TissueComp!H$8*INDEX(VolumeFlow!$A54:$D79,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A54:$A79,0),4)</f>
         <v>1.018942375256688E-3</v>
       </c>
       <c r="G56" s="2">
-        <f>TissueComp!I$8*INDEX(VolumeFlow!$A54:$D66,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A54:$A66,0),4)</f>
+        <f>TissueComp!I$8*INDEX(VolumeFlow!$A54:$D79,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A54:$A79,0),4)</f>
         <v>3.825039844165044E-3</v>
       </c>
       <c r="H56" s="2">
-        <f>TissueComp!J$8*INDEX(VolumeFlow!$A54:$D66,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A54:$A66,0),4)</f>
+        <f>TissueComp!J$8*INDEX(VolumeFlow!$A54:$D79,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A54:$A79,0),4)</f>
         <v>1.7637683725872119E-3</v>
       </c>
       <c r="I56" s="2">
-        <f>TissueComp!K$8*INDEX(VolumeFlow!$A54:$D66,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A54:$A66,0),4)</f>
+        <f>TissueComp!K$8*INDEX(VolumeFlow!$A54:$D79,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A54:$A79,0),4)</f>
         <v>4.1119178324774215E-4</v>
       </c>
       <c r="J56" s="2">
-        <f>TissueComp!L$8*INDEX(VolumeFlow!$A54:$D66,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A54:$A66,0),4)</f>
+        <f>TissueComp!L$8*INDEX(VolumeFlow!$A54:$D79,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A54:$A79,0),4)</f>
         <v>4.3319999999999997E-2</v>
       </c>
       <c r="K56" t="s">
@@ -10527,39 +11346,39 @@
         <v>Liver</v>
       </c>
       <c r="B57" s="2">
-        <f>TissueComp!D$9*INDEX(VolumeFlow!$A55:$D67,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A55:$A67,0),4)</f>
+        <f>TissueComp!D$9*INDEX(VolumeFlow!$A55:$D80,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A55:$A80,0),4)</f>
         <v>3.0800000000000001E-2</v>
       </c>
       <c r="C57" s="2">
-        <f>TissueComp!E$9*INDEX(VolumeFlow!$A55:$D67,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A55:$A67,0),4)</f>
+        <f>TissueComp!E$9*INDEX(VolumeFlow!$A55:$D80,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A55:$A80,0),4)</f>
         <v>9.1999999999999998E-3</v>
       </c>
       <c r="D57" s="2">
-        <f>TissueComp!F$9*INDEX(VolumeFlow!$A55:$D67,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A55:$A67,0),4)</f>
+        <f>TissueComp!F$9*INDEX(VolumeFlow!$A55:$D80,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A55:$A80,0),4)</f>
         <v>2.8976389480787401E-2</v>
       </c>
       <c r="E57" s="2">
-        <f>TissueComp!G$9*INDEX(VolumeFlow!$A55:$D67,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A55:$A67,0),4)</f>
+        <f>TissueComp!G$9*INDEX(VolumeFlow!$A55:$D80,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A55:$A80,0),4)</f>
         <v>3.69246709157594E-3</v>
       </c>
       <c r="F57" s="2">
-        <f>TissueComp!H$9*INDEX(VolumeFlow!$A55:$D67,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A55:$A67,0),4)</f>
+        <f>TissueComp!H$9*INDEX(VolumeFlow!$A55:$D80,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A55:$A80,0),4)</f>
         <v>7.3311434276366405E-3</v>
       </c>
       <c r="G57" s="2">
-        <f>TissueComp!I$9*INDEX(VolumeFlow!$A55:$D67,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A55:$A67,0),4)</f>
+        <f>TissueComp!I$9*INDEX(VolumeFlow!$A55:$D80,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A55:$A80,0),4)</f>
         <v>2.897415818324196E-2</v>
       </c>
       <c r="H57" s="2">
-        <f>TissueComp!J$9*INDEX(VolumeFlow!$A55:$D67,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A55:$A67,0),4)</f>
+        <f>TissueComp!J$9*INDEX(VolumeFlow!$A55:$D80,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A55:$A80,0),4)</f>
         <v>9.0054815974941211E-3</v>
       </c>
       <c r="I57" s="2">
-        <f>TissueComp!K$9*INDEX(VolumeFlow!$A55:$D67,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A55:$A67,0),4)</f>
+        <f>TissueComp!K$9*INDEX(VolumeFlow!$A55:$D80,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A55:$A80,0),4)</f>
         <v>2.0203602192639001E-3</v>
       </c>
       <c r="J57" s="2">
-        <f>TissueComp!L$9*INDEX(VolumeFlow!$A55:$D67,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A55:$A67,0),4)</f>
+        <f>TissueComp!L$9*INDEX(VolumeFlow!$A55:$D80,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A55:$A80,0),4)</f>
         <v>0.28920000000000001</v>
       </c>
       <c r="K57" t="s">
@@ -10572,39 +11391,39 @@
         <v>Lung</v>
       </c>
       <c r="B58" s="2">
-        <f>TissueComp!D$10*INDEX(VolumeFlow!$A56:$D68,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A56:$A68,0),4)</f>
+        <f>TissueComp!D$10*INDEX(VolumeFlow!$A56:$D81,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A56:$A81,0),4)</f>
         <v>5.4400000000000004E-3</v>
       </c>
       <c r="C58" s="2">
-        <f>TissueComp!E$10*INDEX(VolumeFlow!$A56:$D68,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A56:$A68,0),4)</f>
+        <f>TissueComp!E$10*INDEX(VolumeFlow!$A56:$D81,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A56:$A81,0),4)</f>
         <v>1.3600000000000001E-3</v>
       </c>
       <c r="D58" s="2">
-        <f>TissueComp!F$10*INDEX(VolumeFlow!$A56:$D68,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A56:$A68,0),4)</f>
+        <f>TissueComp!F$10*INDEX(VolumeFlow!$A56:$D81,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A56:$A81,0),4)</f>
         <v>5.4658291956305857E-3</v>
       </c>
       <c r="E58" s="2">
-        <f>TissueComp!G$10*INDEX(VolumeFlow!$A56:$D68,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A56:$A68,0),4)</f>
+        <f>TissueComp!G$10*INDEX(VolumeFlow!$A56:$D81,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A56:$A81,0),4)</f>
         <v>8.9473684210526264E-5</v>
       </c>
       <c r="F58" s="2">
-        <f>TissueComp!H$10*INDEX(VolumeFlow!$A56:$D68,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A56:$A68,0),4)</f>
+        <f>TissueComp!H$10*INDEX(VolumeFlow!$A56:$D81,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A56:$A81,0),4)</f>
         <v>1.2446971201588884E-3</v>
       </c>
       <c r="G58" s="2">
-        <f>TissueComp!I$10*INDEX(VolumeFlow!$A56:$D68,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A56:$A68,0),4)</f>
+        <f>TissueComp!I$10*INDEX(VolumeFlow!$A56:$D81,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A56:$A81,0),4)</f>
         <v>2.0399999999999997E-3</v>
       </c>
       <c r="H58" s="2">
-        <f>TissueComp!J$10*INDEX(VolumeFlow!$A56:$D68,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A56:$A68,0),4)</f>
+        <f>TissueComp!J$10*INDEX(VolumeFlow!$A56:$D81,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A56:$A81,0),4)</f>
         <v>3.8080000000000002E-3</v>
       </c>
       <c r="I58" s="2">
-        <f>TissueComp!K$10*INDEX(VolumeFlow!$A56:$D68,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A56:$A68,0),4)</f>
+        <f>TissueComp!K$10*INDEX(VolumeFlow!$A56:$D81,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A56:$A81,0),4)</f>
         <v>9.5200000000000005E-4</v>
       </c>
       <c r="J58" s="2">
-        <f>TissueComp!L$10*INDEX(VolumeFlow!$A56:$D68,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A56:$A68,0),4)</f>
+        <f>TissueComp!L$10*INDEX(VolumeFlow!$A56:$D81,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A56:$A81,0),4)</f>
         <v>4.4879999999999996E-2</v>
       </c>
       <c r="K58" t="s">
@@ -10617,39 +11436,39 @@
         <v>Muscle</v>
       </c>
       <c r="B59" s="2">
-        <f>TissueComp!D$11*INDEX(VolumeFlow!$A57:$D69,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A57:$A69,0),4)</f>
+        <f>TissueComp!D$11*INDEX(VolumeFlow!$A57:$D82,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A57:$A82,0),4)</f>
         <v>0.45900000000000002</v>
       </c>
       <c r="C59" s="2">
-        <f>TissueComp!E$11*INDEX(VolumeFlow!$A57:$D69,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A57:$A69,0),4)</f>
+        <f>TissueComp!E$11*INDEX(VolumeFlow!$A57:$D82,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A57:$A82,0),4)</f>
         <v>8.1000000000000003E-2</v>
       </c>
       <c r="D59" s="2">
-        <f>TissueComp!F$11*INDEX(VolumeFlow!$A57:$D69,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A57:$A69,0),4)</f>
+        <f>TissueComp!F$11*INDEX(VolumeFlow!$A57:$D82,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A57:$A82,0),4)</f>
         <v>0.4315373589608773</v>
       </c>
       <c r="E59" s="2">
-        <f>TissueComp!G$11*INDEX(VolumeFlow!$A57:$D69,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A57:$A69,0),4)</f>
+        <f>TissueComp!G$11*INDEX(VolumeFlow!$A57:$D82,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A57:$A82,0),4)</f>
         <v>1.2889042429571947E-2</v>
       </c>
       <c r="F59" s="2">
-        <f>TissueComp!H$11*INDEX(VolumeFlow!$A57:$D69,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A57:$A69,0),4)</f>
+        <f>TissueComp!H$11*INDEX(VolumeFlow!$A57:$D82,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A57:$A82,0),4)</f>
         <v>9.5573598609551225E-2</v>
       </c>
       <c r="G59" s="2">
-        <f>TissueComp!I$11*INDEX(VolumeFlow!$A57:$D69,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A57:$A69,0),4)</f>
+        <f>TissueComp!I$11*INDEX(VolumeFlow!$A57:$D82,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A57:$A82,0),4)</f>
         <v>0.29128630705394165</v>
       </c>
       <c r="H59" s="2">
-        <f>TissueComp!J$11*INDEX(VolumeFlow!$A57:$D69,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A57:$A69,0),4)</f>
+        <f>TissueComp!J$11*INDEX(VolumeFlow!$A57:$D82,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A57:$A82,0),4)</f>
         <v>0.20614107883817448</v>
       </c>
       <c r="I59" s="2">
-        <f>TissueComp!K$11*INDEX(VolumeFlow!$A57:$D69,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A57:$A69,0),4)</f>
+        <f>TissueComp!K$11*INDEX(VolumeFlow!$A57:$D82,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A57:$A82,0),4)</f>
         <v>4.2572614107883815E-2</v>
       </c>
       <c r="J59" s="2">
-        <f>TissueComp!L$11*INDEX(VolumeFlow!$A57:$D69,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A57:$A69,0),4)</f>
+        <f>TissueComp!L$11*INDEX(VolumeFlow!$A57:$D82,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A57:$A82,0),4)</f>
         <v>3.6774</v>
       </c>
       <c r="K59" t="s">
@@ -10662,39 +11481,39 @@
         <v>Skin</v>
       </c>
       <c r="B60" s="2">
-        <f>TissueComp!D$12*INDEX(VolumeFlow!$A58:$D70,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A58:$A70,0),4)</f>
+        <f>TissueComp!D$12*INDEX(VolumeFlow!$A58:$D83,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A58:$A83,0),4)</f>
         <v>1.7600000000000001E-2</v>
       </c>
       <c r="C60" s="2">
-        <f>TissueComp!E$12*INDEX(VolumeFlow!$A58:$D70,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A58:$A70,0),4)</f>
+        <f>TissueComp!E$12*INDEX(VolumeFlow!$A58:$D83,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A58:$A83,0),4)</f>
         <v>2.6399999999999996E-2</v>
       </c>
       <c r="D60" s="2">
-        <f>TissueComp!F$12*INDEX(VolumeFlow!$A58:$D70,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A58:$A70,0),4)</f>
+        <f>TissueComp!F$12*INDEX(VolumeFlow!$A58:$D83,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A58:$A83,0),4)</f>
         <v>1.8789250107683394E-2</v>
       </c>
       <c r="E60" s="2">
-        <f>TissueComp!G$12*INDEX(VolumeFlow!$A58:$D70,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A58:$A70,0),4)</f>
+        <f>TissueComp!G$12*INDEX(VolumeFlow!$A58:$D83,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A58:$A83,0),4)</f>
         <v>1.2457531143827879E-2</v>
       </c>
       <c r="F60" s="2">
-        <f>TissueComp!H$12*INDEX(VolumeFlow!$A58:$D70,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A58:$A70,0),4)</f>
+        <f>TissueComp!H$12*INDEX(VolumeFlow!$A58:$D83,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A58:$A83,0),4)</f>
         <v>1.2753218748488768E-2</v>
       </c>
       <c r="G60" s="2">
-        <f>TissueComp!I$12*INDEX(VolumeFlow!$A58:$D70,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A58:$A70,0),4)</f>
+        <f>TissueComp!I$12*INDEX(VolumeFlow!$A58:$D83,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A58:$A83,0),4)</f>
         <v>1.5836832633473324E-2</v>
       </c>
       <c r="H60" s="2">
-        <f>TissueComp!J$12*INDEX(VolumeFlow!$A58:$D70,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A58:$A70,0),4)</f>
+        <f>TissueComp!J$12*INDEX(VolumeFlow!$A58:$D83,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A58:$A83,0),4)</f>
         <v>2.2083583283343339E-2</v>
       </c>
       <c r="I60" s="2">
-        <f>TissueComp!K$12*INDEX(VolumeFlow!$A58:$D70,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A58:$A70,0),4)</f>
+        <f>TissueComp!K$12*INDEX(VolumeFlow!$A58:$D83,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A58:$A83,0),4)</f>
         <v>6.0795840831833793E-3</v>
       </c>
       <c r="J60" s="2">
-        <f>TissueComp!L$12*INDEX(VolumeFlow!$A58:$D70,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A58:$A70,0),4)</f>
+        <f>TissueComp!L$12*INDEX(VolumeFlow!$A58:$D83,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A58:$A83,0),4)</f>
         <v>0.308</v>
       </c>
       <c r="K60" t="s">
@@ -10707,39 +11526,39 @@
         <v>Spleen</v>
       </c>
       <c r="B61" s="2">
-        <f>TissueComp!D$13*INDEX(VolumeFlow!$A59:$D71,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A59:$A71,0),4)</f>
+        <f>TissueComp!D$13*INDEX(VolumeFlow!$A59:$D84,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A59:$A84,0),4)</f>
         <v>2.9800000000000003E-4</v>
       </c>
       <c r="C61" s="2">
-        <f>TissueComp!E$13*INDEX(VolumeFlow!$A59:$D71,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A59:$A71,0),4)</f>
+        <f>TissueComp!E$13*INDEX(VolumeFlow!$A59:$D84,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A59:$A84,0),4)</f>
         <v>1.0200000000000001E-4</v>
       </c>
       <c r="D61" s="2">
-        <f>TissueComp!F$13*INDEX(VolumeFlow!$A59:$D71,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A59:$A71,0),4)</f>
+        <f>TissueComp!F$13*INDEX(VolumeFlow!$A59:$D84,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A59:$A84,0),4)</f>
         <v>3.0795311900358121E-4</v>
       </c>
       <c r="E61" s="2">
-        <f>TissueComp!G$13*INDEX(VolumeFlow!$A59:$D71,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A59:$A71,0),4)</f>
+        <f>TissueComp!G$13*INDEX(VolumeFlow!$A59:$D84,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A59:$A84,0),4)</f>
         <v>1.5782433517379522E-5</v>
       </c>
       <c r="F61" s="2">
-        <f>TissueComp!H$13*INDEX(VolumeFlow!$A59:$D71,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A59:$A71,0),4)</f>
+        <f>TissueComp!H$13*INDEX(VolumeFlow!$A59:$D84,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A59:$A84,0),4)</f>
         <v>7.6264447479039202E-5</v>
       </c>
       <c r="G61" s="2">
-        <f>TissueComp!I$13*INDEX(VolumeFlow!$A59:$D71,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A59:$A71,0),4)</f>
+        <f>TissueComp!I$13*INDEX(VolumeFlow!$A59:$D84,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A59:$A84,0),4)</f>
         <v>2.1365890881343004E-4</v>
       </c>
       <c r="H61" s="2">
-        <f>TissueComp!J$13*INDEX(VolumeFlow!$A59:$D71,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A59:$A71,0),4)</f>
+        <f>TissueComp!J$13*INDEX(VolumeFlow!$A59:$D84,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A59:$A84,0),4)</f>
         <v>1.571919114841664E-4</v>
       </c>
       <c r="I61" s="2">
-        <f>TissueComp!K$13*INDEX(VolumeFlow!$A59:$D71,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A59:$A71,0),4)</f>
+        <f>TissueComp!K$13*INDEX(VolumeFlow!$A59:$D84,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A59:$A84,0),4)</f>
         <v>2.9149179702403686E-5</v>
       </c>
       <c r="J61" s="2">
-        <f>TissueComp!L$13*INDEX(VolumeFlow!$A59:$D71,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A59:$A71,0),4)</f>
+        <f>TissueComp!L$13*INDEX(VolumeFlow!$A59:$D84,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A59:$A84,0),4)</f>
         <v>2.8E-3</v>
       </c>
       <c r="K61" t="s">
@@ -10800,7 +11619,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11057,7 +11876,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -11070,7 +11889,7 @@
   <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11079,26 +11898,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -11112,7 +11931,7 @@
         <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="J2" t="s">
         <v>16</v>
@@ -11124,7 +11943,7 @@
         <v>18</v>
       </c>
       <c r="P2" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Manually add alveolar deadspace fraction and pulmonary ventilation rate values for different species (not including monkey) to the basic pk sheet in pkdata.xlsx. I had received and incorporated the values from Matt Linakis previously, and likely lost them amid different merges/pulls from origin. This posed a problem for parameterizing the gas_pbtk model.
</commit_message>
<xml_diff>
--- a/pkdata.xlsx
+++ b/pkdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\httkdatatables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msfeir\httkdatatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C322C2-4616-46E4-9060-CE62631E3121}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48D5116-BA60-43B1-A565-5C3DBBE2A1BC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13440" yWindow="825" windowWidth="15090" windowHeight="13710" tabRatio="884" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25455" yWindow="1560" windowWidth="18555" windowHeight="10875" tabRatio="884" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic PK" sheetId="7" r:id="rId1"/>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="359">
   <si>
     <t>Tissue</t>
   </si>
@@ -1744,6 +1744,15 @@
   </si>
   <si>
     <t>Pearce 2017</t>
+  </si>
+  <si>
+    <t>Pulmonary Ventilation Rate</t>
+  </si>
+  <si>
+    <t>l/h/kg^(3/4)</t>
+  </si>
+  <si>
+    <t>Alveolar Dead Space Fraction</t>
   </si>
 </sst>
 </file>
@@ -1981,14 +1990,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2329,10 +2338,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2790,43 +2799,89 @@
         <v>6.95134061569017E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>356</v>
+      </c>
+      <c r="B16" t="s">
+        <v>357</v>
+      </c>
+      <c r="C16">
+        <v>24.75</v>
+      </c>
+      <c r="D16">
+        <v>24.75</v>
+      </c>
+      <c r="E16">
+        <v>24.75</v>
+      </c>
+      <c r="F16">
+        <v>27.75</v>
+      </c>
+      <c r="G16">
+        <v>24.75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>358</v>
+      </c>
+      <c r="B17" t="s">
+        <v>311</v>
+      </c>
+      <c r="C17">
+        <v>0.33</v>
+      </c>
+      <c r="D17">
+        <v>0.33</v>
+      </c>
+      <c r="E17">
+        <v>0.33</v>
+      </c>
+      <c r="F17">
+        <v>0.33</v>
+      </c>
+      <c r="G17">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="26" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="26" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="26" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="s">
         <v>344</v>
       </c>
     </row>
@@ -2852,20 +2907,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32" t="s">
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
     </row>
     <row r="2" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -3125,20 +3180,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32" t="s">
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
     </row>
     <row r="2" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -5849,7 +5904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
@@ -5972,7 +6027,7 @@
       <c r="B5" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C5" s="31">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Stomach",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B5,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Large Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B5,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Small Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B5,'Percent BW'!$N$2:$X$2,0))</f>
         <v>1.5802847456629968E-2</v>
       </c>
@@ -6196,7 +6251,7 @@
       <c r="B13" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="33">
+      <c r="C13" s="31">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Total",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B13,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("GI Contents",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B13,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("Blood",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B13,'Percent BW'!$N$2:$X$2,0))-SUM(C2:C12)</f>
         <v>5.1820372533547543E-2</v>
       </c>
@@ -6308,7 +6363,7 @@
       <c r="B17" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="33">
+      <c r="C17" s="31">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Stomach",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B17,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Large Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B17,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Small Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B17,'Percent BW'!$N$2:$X$2,0))</f>
         <v>2.5852334412265577E-2</v>
       </c>
@@ -6532,7 +6587,7 @@
       <c r="B25" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="33">
+      <c r="C25" s="31">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Total",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B25,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("GI Contents",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B25,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("Blood",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B25,'Percent BW'!$N$2:$X$2,0))-SUM(C14:C24)</f>
         <v>5.2399992921151606E-2</v>
       </c>
@@ -6626,7 +6681,7 @@
       <c r="B29" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="33">
+      <c r="C29" s="31">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Stomach",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B29,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Large Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B29,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Small Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B29,'Percent BW'!$N$2:$X$2,0))</f>
         <v>4.0408654780552319E-2</v>
       </c>
@@ -6802,7 +6857,7 @@
       <c r="B37" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="33">
+      <c r="C37" s="31">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Total",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B37,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("GI Contents",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B37,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("Blood",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B37,'Percent BW'!$N$2:$X$2,0))-SUM(C26:C36)</f>
         <v>2.5418908119054118E-2</v>
       </c>
@@ -6908,7 +6963,7 @@
       <c r="B41" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="33">
+      <c r="C41" s="31">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Stomach",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B41,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Large Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B41,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Small Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B41,'Percent BW'!$N$2:$X$2,0))</f>
         <v>3.521811975832758E-2</v>
       </c>
@@ -7132,7 +7187,7 @@
       <c r="B49" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C49" s="33">
+      <c r="C49" s="31">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Total",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B49,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("GI Contents",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B49,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("Blood",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B49,'Percent BW'!$N$2:$X$2,0))-SUM(C38:C48)</f>
         <v>2.3649226512727495E-3</v>
       </c>
@@ -7244,7 +7299,7 @@
       <c r="B53" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="C53" s="33">
+      <c r="C53" s="31">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Stomach",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B53,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Large Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B53,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Small Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B53,'Percent BW'!$N$2:$X$2,0))</f>
         <v>4.8000000000000001E-2</v>
       </c>
@@ -7468,7 +7523,7 @@
       <c r="B61" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="C61" s="33">
+      <c r="C61" s="31">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Total",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B61,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("GI Contents",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B61,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("Blood",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B61,'Percent BW'!$N$2:$X$2,0))-SUM(C50:C60)</f>
         <v>2.5662489315418147E-2</v>
       </c>
@@ -7575,7 +7630,7 @@
       <c r="B65" s="20" t="s">
         <v>343</v>
       </c>
-      <c r="C65" s="33">
+      <c r="C65" s="31">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Stomach",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B65,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Large Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B65,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Small Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B65,'Percent BW'!$N$2:$X$2,0))</f>
         <v>4.5999999999999999E-2</v>
       </c>
@@ -7799,7 +7854,7 @@
       <c r="B73" s="20" t="s">
         <v>343</v>
       </c>
-      <c r="C73" s="33">
+      <c r="C73" s="31">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Total",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B73,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("GI Contents",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B73,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("Blood",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B73,'Percent BW'!$N$2:$X$2,0))-SUM(C62:C72)</f>
         <v>1.7528264277473893E-2</v>
       </c>
@@ -7885,20 +7940,20 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="32" t="s">
         <v>315</v>
       </c>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31" t="s">
+      <c r="E1" s="32"/>
+      <c r="F1" s="32" t="s">
         <v>316</v>
       </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31" t="s">
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
@@ -8972,28 +9027,28 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
       <c r="F1" s="25"/>
       <c r="G1" s="25"/>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
       <c r="L1" s="25"/>
       <c r="M1" s="25"/>
-      <c r="N1" s="32" t="s">
+      <c r="N1" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -10774,30 +10829,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
       <c r="J1" s="30"/>
       <c r="K1" s="30"/>
       <c r="L1" s="30"/>
       <c r="M1" s="30"/>
-      <c r="N1" s="32" t="s">
+      <c r="N1" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -12438,16 +12493,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>

</xml_diff>

<commit_message>
Add in monkey physiology values for pulmonary ventilation rate and alveolar dead space fraction as the same as corresponding human values, in absence of measured values. Add note to file to document.
</commit_message>
<xml_diff>
--- a/pkdata.xlsx
+++ b/pkdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msfeir\httkdatatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48D5116-BA60-43B1-A565-5C3DBBE2A1BC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5AD2B2-E59C-4983-ACEA-484D1CF0AB3A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25455" yWindow="1560" windowWidth="18555" windowHeight="10875" tabRatio="884" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="361">
   <si>
     <t>Tissue</t>
   </si>
@@ -1754,6 +1754,25 @@
   <si>
     <t>Alveolar Dead Space Fraction</t>
   </si>
+  <si>
+    <r>
+      <t>Monkey</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a</t>
+    </r>
+  </si>
+  <si>
+    <t>a  : Monkey values for pulmonary ventilation rate and alveolar dead space are set equal to corresponding human values, in the absence of known measurement</t>
+  </si>
 </sst>
 </file>
 
@@ -1764,7 +1783,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1874,6 +1893,14 @@
       <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -2338,10 +2365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2350,7 +2377,7 @@
     <col min="3" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>76</v>
       </c>
@@ -2373,7 +2400,7 @@
         <v>104</v>
       </c>
       <c r="H1" t="s">
-        <v>343</v>
+        <v>359</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2821,8 +2848,11 @@
       <c r="G16">
         <v>24.75</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>27.75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>358</v>
       </c>
@@ -2844,44 +2874,52 @@
       <c r="G17">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="H17" s="24">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="26" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="26" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="26" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="26" t="s">
         <v>344</v>
       </c>
     </row>
@@ -5904,7 +5942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A76" workbookViewId="0">
       <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
@@ -7923,7 +7961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
@@ -9020,7 +9058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Run load_package_data_tables.R again to revert 'Monkey' column name in pkdata.xlsx back to 'Monkey'. Previously, I had attempted to add a superscript indicating a note, 'a', to the 'Monkey' name, with this was interpreted as part of the 'Monkey' string, which I fear may be prompting the current 'data not found for requested species' error that get_chem_info returns, in at least our test cases.
</commit_message>
<xml_diff>
--- a/pkdata.xlsx
+++ b/pkdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msfeir\httkdatatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5AD2B2-E59C-4983-ACEA-484D1CF0AB3A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32004A68-4F33-4F85-BADD-6AA4CDCBB62C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25455" yWindow="1560" windowWidth="18555" windowHeight="10875" tabRatio="884" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="360">
   <si>
     <t>Tissue</t>
   </si>
@@ -1755,23 +1755,7 @@
     <t>Alveolar Dead Space Fraction</t>
   </si>
   <si>
-    <r>
-      <t>Monkey</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>a</t>
-    </r>
-  </si>
-  <si>
-    <t>a  : Monkey values for pulmonary ventilation rate and alveolar dead space are set equal to corresponding human values, in the absence of known measurement</t>
+    <t>Note:  Monkey values for pulmonary ventilation rate and alveolar dead space are set equal to corresponding human values, in the absence of known measurements</t>
   </si>
 </sst>
 </file>
@@ -1783,7 +1767,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1893,14 +1877,6 @@
       <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -2400,7 +2376,7 @@
         <v>104</v>
       </c>
       <c r="H1" t="s">
-        <v>359</v>
+        <v>343</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2880,7 +2856,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -7961,7 +7937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update notes in pkdata.xlsx on the sources of physiological data, and which species' values are being used as substitutes.
</commit_message>
<xml_diff>
--- a/pkdata.xlsx
+++ b/pkdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msfeir\httkdatatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32004A68-4F33-4F85-BADD-6AA4CDCBB62C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF19C265-D277-4F4E-B39A-93BB84B4DD9D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25455" yWindow="1560" windowWidth="18555" windowHeight="10875" tabRatio="884" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="884" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic PK" sheetId="7" r:id="rId1"/>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="361">
   <si>
     <t>Tissue</t>
   </si>
@@ -1755,7 +1755,10 @@
     <t>Alveolar Dead Space Fraction</t>
   </si>
   <si>
-    <t>Note:  Monkey values for pulmonary ventilation rate and alveolar dead space are set equal to corresponding human values, in the absence of known measurements</t>
+    <t>Notes:  Monkey values for pulmonary ventilation rate and alveolar dead space are set equal to corresponding human values, in the absence of known measurements.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rat pulmonary ventilation and alveolar dead space fraction values have been assigned to the species other than human and monkey. </t>
   </si>
 </sst>
 </file>
@@ -2341,10 +2344,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2859,43 +2862,48 @@
         <v>359</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>338</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="26" t="s">
         <v>344</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add thyroid values to TissueComp page from Pilari et al. 2017, as well as from Chow et al. 1982 and Virreira et al. 2017. I noted the computations I did to derive certain numbers in the thyroid row from Pilari et al. 2017 data in my OneNote.
I also transferred placental tissue values that had previously been hard-coded in httk's fetal materials to the table. The reference(s) for these data are
still unknown.
</commit_message>
<xml_diff>
--- a/pkdata.xlsx
+++ b/pkdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msfeir\httkdatatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF19C265-D277-4F4E-B39A-93BB84B4DD9D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2404DF4C-B45D-4D59-8D1D-C4CACBDC0F7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="884" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="750" yWindow="480" windowWidth="19560" windowHeight="10440" tabRatio="884" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic PK" sheetId="7" r:id="rId1"/>
@@ -26,10 +26,10 @@
     <sheet name="Average Properties Calc" sheetId="8" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="bbib18" localSheetId="2">TissueComp!$A$31</definedName>
+    <definedName name="bbib18" localSheetId="2">TissueComp!$A$34</definedName>
     <definedName name="bbib18" localSheetId="1">VolumeFlow!#REF!</definedName>
-    <definedName name="bbib8" localSheetId="2">TissueComp!$A$32</definedName>
-    <definedName name="bbib8" localSheetId="1">TissueComp!$A$36</definedName>
+    <definedName name="bbib8" localSheetId="2">TissueComp!$A$35</definedName>
+    <definedName name="bbib8" localSheetId="1">TissueComp!$A$47</definedName>
     <definedName name="btblfn10" localSheetId="2">TissueComp!#REF!</definedName>
     <definedName name="btblfn10" localSheetId="1">VolumeFlow!#REF!</definedName>
     <definedName name="btblfn11" localSheetId="2">TissueComp!#REF!</definedName>
@@ -40,11 +40,11 @@
     <definedName name="btblfn8" localSheetId="1">VolumeFlow!#REF!</definedName>
     <definedName name="btblfn9" localSheetId="2">TissueComp!#REF!</definedName>
     <definedName name="btblfn9" localSheetId="1">VolumeFlow!#REF!</definedName>
-    <definedName name="tblfn10" localSheetId="2">TissueComp!$A$30</definedName>
+    <definedName name="tblfn10" localSheetId="2">TissueComp!$A$33</definedName>
     <definedName name="tblfn10" localSheetId="1">VolumeFlow!#REF!</definedName>
-    <definedName name="tblfn8" localSheetId="2">TissueComp!$A$28</definedName>
+    <definedName name="tblfn8" localSheetId="2">TissueComp!$A$31</definedName>
     <definedName name="tblfn8" localSheetId="1">VolumeFlow!$A$75</definedName>
-    <definedName name="tblfn9" localSheetId="2">TissueComp!$A$29</definedName>
+    <definedName name="tblfn9" localSheetId="2">TissueComp!$A$32</definedName>
     <definedName name="tblfn9" localSheetId="1">VolumeFlow!$A$76</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -52,7 +52,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -112,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="373">
   <si>
     <t>Tissue</t>
   </si>
@@ -1177,38 +1179,6 @@
   </si>
   <si>
     <r>
-      <t>Fraction of total volume</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>a</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Fraction of cell volume</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>b</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Neutral Lipid</t>
     </r>
     <r>
@@ -1253,22 +1223,6 @@
         <family val="2"/>
       </rPr>
       <t>c</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pH</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>d</t>
     </r>
   </si>
   <si>
@@ -1689,76 +1643,162 @@
     <t>References</t>
   </si>
   <si>
+    <t>EPA, Physiological Parameters Database for PBPK Modeling</t>
+  </si>
+  <si>
+    <t>Monkey</t>
+  </si>
+  <si>
+    <t>Gauvin, David V. "Electrocardiogram, hemodynamics, and core body temperatures of the normal freely moving cynomolgus monkey by remote radiotelemetry", Journal of Pharmacological and Toxicological Methods</t>
+  </si>
+  <si>
+    <t>RabbitRaw</t>
+  </si>
+  <si>
+    <t>Davies and Morris 1993</t>
+  </si>
+  <si>
+    <t>Physiological Parameter Values for PBPK Models, ILSI-RSI, 1994</t>
+  </si>
+  <si>
+    <t>ILSI-RSI 1994</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>Davies and Morris, 1993</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Pearce et al., 2017</t>
+  </si>
+  <si>
+    <t>b,c</t>
+  </si>
+  <si>
+    <t>Davies 1993</t>
+  </si>
+  <si>
+    <t>Pearce 2017</t>
+  </si>
+  <si>
+    <t>Pulmonary Ventilation Rate</t>
+  </si>
+  <si>
+    <t>l/h/kg^(3/4)</t>
+  </si>
+  <si>
+    <t>Alveolar Dead Space Fraction</t>
+  </si>
+  <si>
+    <t>Notes:  Monkey values for pulmonary ventilation rate and alveolar dead space are set equal to corresponding human values, in the absence of known measurements.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rat pulmonary ventilation and alveolar dead space fraction values have been assigned to the species other than human and monkey. </t>
+  </si>
+  <si>
+    <t>Placenta</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>f Placenta values transferred from hard-coded sequence in predict_partitioning_schmitt, where fractions of total lipid comprised by neutral lipid, neutral phospholipid, and acidic phospholipid are tentatively calculated as the average of the corresponding values for all other listed tissues in the human.</t>
+  </si>
+  <si>
+    <t>d Values taken from ([Waddell and Bates, 1969], [Malan et al., 1985], [Wood and Schaefer, 1978], [Schanker and Less, 1977], [Harrison and Walker, 1979] and [Civelek et al., 1996]). Mean values were calculated when more than one value was found for the same tissue.</t>
+  </si>
+  <si>
     <r>
-      <t>d</t>
+      <t>Fraction of total volume</t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>a,g</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Fraction of cell volume</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>b,h</t>
+    </r>
+  </si>
+  <si>
+    <t>g Thyroid values taken from Pilari et al. 2017's "Development of Physiologically…" with tissue total volume fractions normalized to exclude vascular and luminal space. That is, the same total thyroid volume is assumed to be made up of cellular and interstitial components only, in proportion to one another as presented in the Pilari et al. 2017 data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h Thyroid fractional cellular volume components are computed using the Pilari et al. 2017 data, with the help of a key assumption. After the total thyroid volume is assumed to be made up of only cells and interstitum, the interstitium is assumed to be made up of 100% volume. That leaves the protein and lipid content in the tissue to be assumed to be only in the cellular component. With these assumptions, the Pilari data gives numbers from which each of the cellular volume fractions of water, lipid, and protein can be directly calculated. For instance, the cellular volume that is made up of water is ( the tissue volume fraction of cellular water ) divided by ( the tissue volume fraction of cells ).  </t>
+  </si>
+  <si>
+    <r>
+      <t>Fraction of total lipid</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t> Values taken from ([Waddell and Bates, 1969], [Malan et al., 1985], [Wood and Schaefer, 1978], [Schanker and Less, 1977], [Harrison and Walker, 1979] and [Civelek et al., 1996]). Mean values were calculated when more than one value was found for the same tissue.</t>
+      <t>i</t>
     </r>
   </si>
   <si>
-    <t>EPA, Physiological Parameters Database for PBPK Modeling</t>
-  </si>
-  <si>
-    <t>Monkey</t>
-  </si>
-  <si>
-    <t>Gauvin, David V. "Electrocardiogram, hemodynamics, and core body temperatures of the normal freely moving cynomolgus monkey by remote radiotelemetry", Journal of Pharmacological and Toxicological Methods</t>
-  </si>
-  <si>
-    <t>RabbitRaw</t>
-  </si>
-  <si>
-    <t>Davies and Morris 1993</t>
-  </si>
-  <si>
-    <t>Physiological Parameter Values for PBPK Models, ILSI-RSI, 1994</t>
-  </si>
-  <si>
-    <t>ILSI-RSI 1994</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>Davies and Morris, 1993</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>Pearce et al., 2017</t>
-  </si>
-  <si>
-    <t>b,c</t>
-  </si>
-  <si>
-    <t>Davies 1993</t>
-  </si>
-  <si>
-    <t>Pearce 2017</t>
-  </si>
-  <si>
-    <t>Pulmonary Ventilation Rate</t>
-  </si>
-  <si>
-    <t>l/h/kg^(3/4)</t>
-  </si>
-  <si>
-    <t>Alveolar Dead Space Fraction</t>
-  </si>
-  <si>
-    <t>Notes:  Monkey values for pulmonary ventilation rate and alveolar dead space are set equal to corresponding human values, in the absence of known measurements.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rat pulmonary ventilation and alveolar dead space fraction values have been assigned to the species other than human and monkey. </t>
+    <t xml:space="preserve">Pilari et al. "Development of Physiologically Based Organ Models to Evaluate the Pharmacokinetics of Drugs in the Testes and the Thyroid Gland." CPT Pharmacometrics Syst. Pharmacol. (2017) 6, 532–542. PMID 28571120. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">i For the fractional volumes of total lipid content, the neutral lipid fraction is determined by subtracting Pilari et al.'s number for total phospholipid from total lipid, as they indicate that they meant to do in table 2, though they presented a number inconsistent with this method. The neutral phospholipid fraction of the total lipid content was computed simply as the neutral phospholipid tissue volume fraction divided by the total lipid tissue volume fraction. The acidic phospholipid fraction of the total lipid content was computed similarly, though the acidic phospholipid tissue volume fraction was calculated by converting from units of ( mg acidic phospholipid per g tissue ) to ( g acidic phospholipid per g tissue), with an assumption that the weight fraction is equivalent to the volume fraction. </t>
+  </si>
+  <si>
+    <t>Pilari et al. 2017; Chow et al. 1982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chow et al. "Effects of Thyrotropin, Acetazolamide…" Journal of Pharmacology and Experimental Therapeutics 225.1 (1982): 17-23. </t>
+  </si>
+  <si>
+    <r>
+      <t>pH</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>d,j</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Virreira et al. "Expression, Localization, and Regulation of the Sodium Bicarbonate Cotransporter NBCe1 in the Thyroid." Thyroid 29.2 (2019). </t>
+  </si>
+  <si>
+    <t>j Thyroid tissue pH is estimated at 7.3, in accordance with the measurements of turtle thyroid follicular cell pH made by Chow et al. 1982. According to a study of humans and rats by Virreira et al. in 2019, thyroid intrafollicular space pH thyrotropin was measured at 7.6 after stimulation with thyrotropin, which is approximately the same as the 7.7 pH in the turtle follicular cells measured by Chow et al. 1982 after thyrotropin stimulation.</t>
   </si>
 </sst>
 </file>
@@ -1770,7 +1810,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1880,6 +1920,15 @@
       <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -2346,7 +2395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
@@ -2379,7 +2428,7 @@
         <v>104</v>
       </c>
       <c r="H1" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2745,7 +2794,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B14" t="s">
         <v>311</v>
@@ -2807,10 +2856,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B16" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C16">
         <v>24.75</v>
@@ -2833,7 +2882,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B17" t="s">
         <v>311</v>
@@ -2859,32 +2908,32 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2894,17 +2943,17 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -3785,39 +3834,39 @@
         <v>Adipose</v>
       </c>
       <c r="B15" s="2" t="e">
-        <f>TissueComp!D15*INDEX(VolumeFlow!$A13:$B25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!D17*INDEX(VolumeFlow!$A13:$B25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C15" s="2" t="e">
-        <f>TissueComp!E15*INDEX(VolumeFlow!$A13:$B25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!E17*INDEX(VolumeFlow!$A13:$B25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D15" s="2" t="e">
-        <f>TissueComp!F15*INDEX(VolumeFlow!$A13:$B25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!F17*INDEX(VolumeFlow!$A13:$B25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E15" s="2" t="e">
-        <f>TissueComp!G15*INDEX(VolumeFlow!$A13:$B25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!G17*INDEX(VolumeFlow!$A13:$B25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F15" s="2" t="e">
-        <f>TissueComp!H15*INDEX(VolumeFlow!$A13:$B25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!H17*INDEX(VolumeFlow!$A13:$B25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G15" s="2" t="e">
-        <f>TissueComp!I15*INDEX(VolumeFlow!$A13:$B25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!I17*INDEX(VolumeFlow!$A13:$B25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H15" s="2" t="e">
-        <f>TissueComp!J15*INDEX(VolumeFlow!$A13:$B25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!J17*INDEX(VolumeFlow!$A13:$B25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I15" s="2" t="e">
-        <f>TissueComp!K15*INDEX(VolumeFlow!$A13:$B25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!K17*INDEX(VolumeFlow!$A13:$B25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J15" s="2" t="e">
-        <f>TissueComp!L15*INDEX(VolumeFlow!$A13:$B25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!L17*INDEX(VolumeFlow!$A13:$B25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K15" t="s">
@@ -3830,39 +3879,39 @@
         <v>Bone</v>
       </c>
       <c r="B16" s="2" t="e">
-        <f>TissueComp!D16*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!D18*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C16" s="2" t="e">
-        <f>TissueComp!E16*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!E18*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D16" s="2" t="e">
-        <f>TissueComp!F16*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!F18*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E16" s="2" t="e">
-        <f>TissueComp!G16*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!G18*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F16" s="2" t="e">
-        <f>TissueComp!H16*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!H18*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G16" s="2" t="e">
-        <f>TissueComp!I16*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!I18*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H16" s="2" t="e">
-        <f>TissueComp!J16*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!J18*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I16" s="2" t="e">
-        <f>TissueComp!K16*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!K18*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J16" s="2" t="e">
-        <f>TissueComp!L16*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!L18*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K16" t="s">
@@ -3875,39 +3924,39 @@
         <v>Brain</v>
       </c>
       <c r="B17" s="2" t="e">
-        <f>TissueComp!D17*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!D19*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C17" s="2" t="e">
-        <f>TissueComp!E17*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!E19*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D17" s="2" t="e">
-        <f>TissueComp!F17*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!F19*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E17" s="2" t="e">
-        <f>TissueComp!G17*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!G19*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F17" s="2" t="e">
-        <f>TissueComp!H17*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!H19*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G17" s="2" t="e">
-        <f>TissueComp!I17*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!I19*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H17" s="2" t="e">
-        <f>TissueComp!J17*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!J19*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I17" s="2" t="e">
-        <f>TissueComp!K17*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!K19*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J17" s="2" t="e">
-        <f>TissueComp!L17*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!L19*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K17" t="s">
@@ -3920,39 +3969,39 @@
         <v>Gut</v>
       </c>
       <c r="B18" s="2" t="e">
-        <f>TissueComp!D18*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!D20*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C18" s="2" t="e">
-        <f>TissueComp!E18*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!E20*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D18" s="2" t="e">
-        <f>TissueComp!F18*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!F20*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E18" s="2" t="e">
-        <f>TissueComp!G18*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!G20*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F18" s="2" t="e">
-        <f>TissueComp!H18*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!H20*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G18" s="2" t="e">
-        <f>TissueComp!I18*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!I20*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H18" s="2" t="e">
-        <f>TissueComp!J18*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!J20*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I18" s="2" t="e">
-        <f>TissueComp!K18*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!K20*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J18" s="2" t="e">
-        <f>TissueComp!L18*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!L20*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K18" t="s">
@@ -3965,39 +4014,39 @@
         <v>Heart</v>
       </c>
       <c r="B19" s="2" t="e">
-        <f>TissueComp!D19*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!D21*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C19" s="2" t="e">
-        <f>TissueComp!E19*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!E21*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D19" s="2" t="e">
-        <f>TissueComp!F19*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!F21*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E19" s="2" t="e">
-        <f>TissueComp!G19*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!G21*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F19" s="2" t="e">
-        <f>TissueComp!H19*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!H21*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G19" s="2" t="e">
-        <f>TissueComp!I19*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!I21*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H19" s="2" t="e">
-        <f>TissueComp!J19*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!J21*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I19" s="2" t="e">
-        <f>TissueComp!K19*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!K21*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J19" s="2" t="e">
-        <f>TissueComp!L19*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!L21*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K19" t="s">
@@ -4010,39 +4059,39 @@
         <v>Kidney</v>
       </c>
       <c r="B20" s="2" t="e">
-        <f>TissueComp!D20*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!D22*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C20" s="2" t="e">
-        <f>TissueComp!E20*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!E22*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D20" s="2" t="e">
-        <f>TissueComp!F20*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!F22*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E20" s="2" t="e">
-        <f>TissueComp!G20*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!G22*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F20" s="2" t="e">
-        <f>TissueComp!H20*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!H22*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G20" s="2" t="e">
-        <f>TissueComp!I20*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!I22*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H20" s="2" t="e">
-        <f>TissueComp!J20*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!J22*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I20" s="2" t="e">
-        <f>TissueComp!K20*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!K22*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J20" s="2" t="e">
-        <f>TissueComp!L20*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!L22*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K20" t="s">
@@ -4055,39 +4104,39 @@
         <v>Liver</v>
       </c>
       <c r="B21" s="2" t="e">
-        <f>TissueComp!D21*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!D23*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C21" s="2" t="e">
-        <f>TissueComp!E21*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!E23*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D21" s="2" t="e">
-        <f>TissueComp!F21*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!F23*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E21" s="2" t="e">
-        <f>TissueComp!G21*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!G23*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F21" s="2" t="e">
-        <f>TissueComp!H21*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!H23*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G21" s="2" t="e">
-        <f>TissueComp!I21*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!I23*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H21" s="2" t="e">
-        <f>TissueComp!J21*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!J23*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I21" s="2" t="e">
-        <f>TissueComp!K21*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!K23*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J21" s="2" t="e">
-        <f>TissueComp!L21*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!L23*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K21" t="s">
@@ -4100,39 +4149,39 @@
         <v>Lung</v>
       </c>
       <c r="B22" s="2" t="e">
-        <f>TissueComp!D22*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!D24*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C22" s="2" t="e">
-        <f>TissueComp!E22*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!E24*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D22" s="2" t="e">
-        <f>TissueComp!F22*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!F24*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E22" s="2" t="e">
-        <f>TissueComp!G22*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!G24*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F22" s="2" t="e">
-        <f>TissueComp!H22*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!H24*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G22" s="2" t="e">
-        <f>TissueComp!I22*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!I24*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H22" s="2" t="e">
-        <f>TissueComp!J22*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!J24*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I22" s="2" t="e">
-        <f>TissueComp!K22*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!K24*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J22" s="2" t="e">
-        <f>TissueComp!L22*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!L24*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K22" t="s">
@@ -4145,39 +4194,39 @@
         <v>Muscle</v>
       </c>
       <c r="B23" s="2" t="e">
-        <f>TissueComp!D23*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!D25*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C23" s="2" t="e">
-        <f>TissueComp!E23*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!E25*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D23" s="2" t="e">
-        <f>TissueComp!F23*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!F25*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E23" s="2" t="e">
-        <f>TissueComp!G23*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!G25*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F23" s="2" t="e">
-        <f>TissueComp!H23*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!H25*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G23" s="2" t="e">
-        <f>TissueComp!I23*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!I25*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H23" s="2" t="e">
-        <f>TissueComp!J23*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!J25*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I23" s="2" t="e">
-        <f>TissueComp!K23*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!K25*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J23" s="2" t="e">
-        <f>TissueComp!L23*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!L25*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K23" t="s">
@@ -4190,39 +4239,39 @@
         <v>Skin</v>
       </c>
       <c r="B24" s="2" t="e">
-        <f>TissueComp!D24*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!D26*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C24" s="2" t="e">
-        <f>TissueComp!E24*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!E26*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D24" s="2" t="e">
-        <f>TissueComp!F24*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!F26*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E24" s="2" t="e">
-        <f>TissueComp!G24*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!G26*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F24" s="2" t="e">
-        <f>TissueComp!H24*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!H26*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G24" s="2" t="e">
-        <f>TissueComp!I24*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!I26*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H24" s="2" t="e">
-        <f>TissueComp!J24*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!J26*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I24" s="2" t="e">
-        <f>TissueComp!K24*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!K26*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J24" s="2" t="e">
-        <f>TissueComp!L24*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!L26*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K24" t="s">
@@ -4235,39 +4284,39 @@
         <v>Spleen</v>
       </c>
       <c r="B25" s="2" t="e">
-        <f>TissueComp!D25*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!D27*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C25" s="2" t="e">
-        <f>TissueComp!E25*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!E27*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D25" s="2" t="e">
-        <f>TissueComp!F25*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!F27*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E25" s="2" t="e">
-        <f>TissueComp!G25*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!G27*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F25" s="2" t="e">
-        <f>TissueComp!H25*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!H27*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G25" s="2" t="e">
-        <f>TissueComp!I25*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!I27*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H25" s="2" t="e">
-        <f>TissueComp!J25*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!J27*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I25" s="2" t="e">
-        <f>TissueComp!K25*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!K27*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J25" s="2" t="e">
-        <f>TissueComp!L25*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!L27*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K25" t="s">
@@ -5926,7 +5975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
@@ -5970,14 +6019,14 @@
         <v>0.20862445414847144</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E2" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A2,Flows!$A$3:$A$21,0),MATCH($B2,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A2,Flows!$A$3:$A$21,0),MATCH($B2,Flows!$B$2:$E$2,0)))</f>
         <v>10.743599688785142</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -5998,14 +6047,14 @@
         <v>7.2310597961656342E-2</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E3" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A3,Flows!$A$3:$A$21,0),MATCH($B3,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A3,Flows!$A$3:$A$21,0),MATCH($B3,Flows!$B$2:$E$2,0)))</f>
         <v>9.7188255646240975</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -6026,14 +6075,14 @@
         <v>1.9314340898116854E-2</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E4" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A4,Flows!$A$3:$A$21,0),MATCH($B4,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A4,Flows!$A$3:$A$21,0),MATCH($B4,Flows!$B$2:$E$2,0)))</f>
         <v>28.925076085190767</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -6054,14 +6103,14 @@
         <v>1.5802847456629968E-2</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E5" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A5,Flows!$A$3:$A$21,0),MATCH($B5,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A5,Flows!$A$3:$A$21,0),MATCH($B5,Flows!$B$2:$E$2,0)))</f>
         <v>47.519767854241969</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -6082,14 +6131,14 @@
         <v>4.5631067961165043E-3</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E6" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A6,Flows!$A$3:$A$21,0),MATCH($B6,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A6,Flows!$A$3:$A$21,0),MATCH($B6,Flows!$B$2:$E$2,0)))</f>
         <v>9.9171689434939783</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
@@ -6110,14 +6159,14 @@
         <v>4.1904761904761906E-3</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E7" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A7,Flows!$A$3:$A$21,0),MATCH($B7,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A7,Flows!$A$3:$A$21,0),MATCH($B7,Flows!$B$2:$E$2,0)))</f>
         <v>51.238706208052214</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -6138,14 +6187,14 @@
         <v>2.4476190476190471E-2</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E8" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A8,Flows!$A$3:$A$21,0),MATCH($B8,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A8,Flows!$A$3:$A$21,0),MATCH($B8,Flows!$B$2:$E$2,0)))</f>
         <v>59.91622903360944</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
@@ -6166,14 +6215,14 @@
         <v>7.234650166587339E-3</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E9" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A9,Flows!$A$3:$A$21,0),MATCH($B9,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A9,Flows!$A$3:$A$21,0),MATCH($B9,Flows!$B$2:$E$2,0)))</f>
         <v>5.7850152170381541</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
@@ -6194,14 +6243,14 @@
         <v>0.38424591738712782</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E10" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A10,Flows!$A$3:$A$21,0),MATCH($B10,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A10,Flows!$A$3:$A$21,0),MATCH($B10,Flows!$B$2:$E$2,0)))</f>
         <v>30.991152948418677</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
@@ -6222,14 +6271,14 @@
         <v>3.3204899288913951E-2</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E11" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A11,Flows!$A$3:$A$21,0),MATCH($B11,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A11,Flows!$A$3:$A$21,0),MATCH($B11,Flows!$B$2:$E$2,0)))</f>
         <v>12.396461179367471</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
@@ -6250,14 +6299,14 @@
         <v>2.4667931688804553E-3</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E12" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A12,Flows!$A$3:$A$21,0),MATCH($B12,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A12,Flows!$A$3:$A$21,0),MATCH($B12,Flows!$B$2:$E$2,0)))</f>
         <v>3.1817583693709843</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
@@ -6278,14 +6327,14 @@
         <v>5.1820372533547543E-2</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E13" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A13,Flows!$A$3:$A$21,0),MATCH($B13,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A13,Flows!$A$3:$A$21,0),MATCH($B13,Flows!$B$2:$E$2,0)))</f>
         <v>4.1900038786262614</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
@@ -6306,14 +6355,14 @@
         <v>7.2598253275109076E-2</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E14" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A14,Flows!$A$3:$A$21,0),MATCH($B14,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A14,Flows!$A$3:$A$21,0),MATCH($B14,Flows!$B$2:$E$2,0)))</f>
         <v>1.131370849898476</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
@@ -6334,14 +6383,14 @@
         <v>3.6939633668305896E-2</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E15" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A15,Flows!$A$3:$A$21,0),MATCH($B15,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A15,Flows!$A$3:$A$21,0),MATCH($B15,Flows!$B$2:$E$2,0)))</f>
         <v>25.535040082208603</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
@@ -6362,14 +6411,14 @@
         <v>5.5045871559633031E-3</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E16" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A16,Flows!$A$3:$A$21,0),MATCH($B16,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A16,Flows!$A$3:$A$21,0),MATCH($B16,Flows!$B$2:$E$2,0)))</f>
         <v>3.676955262170047</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
@@ -6390,14 +6439,14 @@
         <v>2.5852334412265577E-2</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E17" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A17,Flows!$A$3:$A$21,0),MATCH($B17,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A17,Flows!$A$3:$A$21,0),MATCH($B17,Flows!$B$2:$E$2,0)))</f>
         <v>27.718585822512662</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
@@ -6418,14 +6467,14 @@
         <v>3.2038834951456309E-3</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E18" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A18,Flows!$A$3:$A$21,0),MATCH($B18,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A18,Flows!$A$3:$A$21,0),MATCH($B18,Flows!$B$2:$E$2,0)))</f>
         <v>11.030865786510139</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
@@ -6446,14 +6495,14 @@
         <v>6.9523809523809521E-3</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E19" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A19,Flows!$A$3:$A$21,0),MATCH($B19,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A19,Flows!$A$3:$A$21,0),MATCH($B19,Flows!$B$2:$E$2,0)))</f>
         <v>26.021529547664947</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
@@ -6474,14 +6523,14 @@
         <v>3.4857142857142857E-2</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E20" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A20,Flows!$A$3:$A$21,0),MATCH($B20,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A20,Flows!$A$3:$A$21,0),MATCH($B20,Flows!$B$2:$E$2,0)))</f>
         <v>33.375440072005041</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
@@ -6502,14 +6551,14 @@
         <v>4.7596382674916704E-3</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E21" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A21,Flows!$A$3:$A$21,0),MATCH($B21,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A21,Flows!$A$3:$A$21,0),MATCH($B21,Flows!$B$2:$E$2,0)))</f>
         <v>4.3953757518555792</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
@@ -6530,14 +6579,14 @@
         <v>0.38837656099903939</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E22" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A22,Flows!$A$3:$A$21,0),MATCH($B22,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A22,Flows!$A$3:$A$21,0),MATCH($B22,Flows!$B$2:$E$2,0)))</f>
         <v>21.213203435596427</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
@@ -6558,14 +6607,14 @@
         <v>0.17032054810459099</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E23" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A23,Flows!$A$3:$A$21,0),MATCH($B23,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A23,Flows!$A$3:$A$21,0),MATCH($B23,Flows!$B$2:$E$2,0)))</f>
         <v>16.404877323527902</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
@@ -6586,14 +6635,14 @@
         <v>1.8975332068311196E-3</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E24" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A24,Flows!$A$3:$A$21,0),MATCH($B24,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A24,Flows!$A$3:$A$21,0),MATCH($B24,Flows!$B$2:$E$2,0)))</f>
         <v>2.8779245994292482</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
@@ -6614,14 +6663,14 @@
         <v>5.2399992921151606E-2</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E25" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A25,Flows!$A$3:$A$21,0),MATCH($B25,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A25,Flows!$A$3:$A$21,0),MATCH($B25,Flows!$B$2:$E$2,0)))</f>
         <v>59.664255982958501</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
@@ -6642,14 +6691,14 @@
         <v>7.3169652284369002E-2</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E26" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A26,Flows!$A$3:$A$21,0),MATCH($B26,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A26,Flows!$A$3:$A$21,0),MATCH($B26,Flows!$B$2:$E$2,0)))</f>
         <v>4.0614836065401096</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -6664,14 +6713,14 @@
         <v>5.429620126861949E-2</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E27" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A27,Flows!$A$3:$A$21,0),MATCH($B27,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A27,Flows!$A$3:$A$21,0),MATCH($B27,Flows!$B$2:$E$2,0)))</f>
         <v>8.766383654772504</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -6686,14 +6735,14 @@
         <v>1.5934331240946405E-2</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E28" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A28,Flows!$A$3:$A$21,0),MATCH($B28,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A28,Flows!$A$3:$A$21,0),MATCH($B28,Flows!$B$2:$E$2,0)))</f>
         <v>4.963996082874039</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -6708,14 +6757,14 @@
         <v>4.0408654780552319E-2</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E29" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A29,Flows!$A$3:$A$21,0),MATCH($B29,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A29,Flows!$A$3:$A$21,0),MATCH($B29,Flows!$B$2:$E$2,0)))</f>
         <v>27.264372424876349</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -6730,14 +6779,14 @@
         <v>4.8543689320388345E-3</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E30" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A30,Flows!$A$3:$A$21,0),MATCH($B30,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A30,Flows!$A$3:$A$21,0),MATCH($B30,Flows!$B$2:$E$2,0)))</f>
         <v>5.2648443303209511</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -6752,14 +6801,14 @@
         <v>1.5904761904761904E-2</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E31" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A31,Flows!$A$3:$A$21,0),MATCH($B31,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A31,Flows!$A$3:$A$21,0),MATCH($B31,Flows!$B$2:$E$2,0)))</f>
         <v>24.443920105061554</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -6774,14 +6823,14 @@
         <v>5.228571428571429E-2</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E32" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A32,Flows!$A$3:$A$21,0),MATCH($B32,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A32,Flows!$A$3:$A$21,0),MATCH($B32,Flows!$B$2:$E$2,0)))</f>
         <v>33.845427837777535</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -6796,14 +6845,14 @@
         <v>6.9490718705378391E-3</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E33" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A33,Flows!$A$3:$A$21,0),MATCH($B33,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A33,Flows!$A$3:$A$21,0),MATCH($B33,Flows!$B$2:$E$2,0)))</f>
         <v>0.75212061861727864</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -6818,14 +6867,14 @@
         <v>0.36887608069164268</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E34" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A34,Flows!$A$3:$A$21,0),MATCH($B34,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A34,Flows!$A$3:$A$21,0),MATCH($B34,Flows!$B$2:$E$2,0)))</f>
         <v>17.110744073543088</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -6840,14 +6889,14 @@
         <v>0.14794527904198049</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E35" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A35,Flows!$A$3:$A$21,0),MATCH($B35,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A35,Flows!$A$3:$A$21,0),MATCH($B35,Flows!$B$2:$E$2,0)))</f>
         <v>7.709236340827105</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -6862,14 +6911,14 @@
         <v>1.0473620615192194E-3</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E36" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A36,Flows!$A$3:$A$21,0),MATCH($B36,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A36,Flows!$A$3:$A$21,0),MATCH($B36,Flows!$B$2:$E$2,0)))</f>
         <v>2.0683317011975162</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -6884,14 +6933,14 @@
         <v>2.5418908119054118E-2</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E37" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A37,Flows!$A$3:$A$21,0),MATCH($B37,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A37,Flows!$A$3:$A$21,0),MATCH($B37,Flows!$B$2:$E$2,0)))</f>
         <v>38.629718395752846</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -6906,14 +6955,14 @@
         <v>4.7303493449781797E-2</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E38" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A38,Flows!$A$3:$A$21,0),MATCH($B38,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A38,Flows!$A$3:$A$21,0),MATCH($B38,Flows!$B$2:$E$2,0)))</f>
         <v>6.2239779351362285</v>
       </c>
       <c r="F38" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
@@ -6934,14 +6983,14 @@
         <v>4.098781270044901E-2</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E39" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A39,Flows!$A$3:$A$21,0),MATCH($B39,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A39,Flows!$A$3:$A$21,0),MATCH($B39,Flows!$B$2:$E$2,0)))</f>
         <v>2.3117632330505993</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
@@ -6962,14 +7011,14 @@
         <v>7.532592950265574E-3</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E40" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A40,Flows!$A$3:$A$21,0),MATCH($B40,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A40,Flows!$A$3:$A$21,0),MATCH($B40,Flows!$B$2:$E$2,0)))</f>
         <v>8.0022573451751509</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
@@ -6990,14 +7039,14 @@
         <v>3.521811975832758E-2</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E41" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A41,Flows!$A$3:$A$21,0),MATCH($B41,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A41,Flows!$A$3:$A$21,0),MATCH($B41,Flows!$B$2:$E$2,0)))</f>
         <v>40.900426430895223</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
@@ -7018,14 +7067,14 @@
         <v>7.5728155339805829E-3</v>
       </c>
       <c r="D42" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E42" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A42,Flows!$A$3:$A$21,0),MATCH($B42,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A42,Flows!$A$3:$A$21,0),MATCH($B42,Flows!$B$2:$E$2,0)))</f>
         <v>9.6027088142101817</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G42" s="7"/>
       <c r="H42" s="7"/>
@@ -7046,14 +7095,14 @@
         <v>5.2380952380952387E-3</v>
       </c>
       <c r="D43" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E43" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A43,Flows!$A$3:$A$21,0),MATCH($B43,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A43,Flows!$A$3:$A$21,0),MATCH($B43,Flows!$B$2:$E$2,0)))</f>
         <v>38.410835256840727</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
@@ -7074,14 +7123,14 @@
         <v>3.1333333333333331E-2</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E44" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A44,Flows!$A$3:$A$21,0),MATCH($B44,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A44,Flows!$A$3:$A$21,0),MATCH($B44,Flows!$B$2:$E$2,0)))</f>
         <v>54.948833770202704</v>
       </c>
       <c r="F44" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G44" s="7"/>
       <c r="H44" s="7"/>
@@ -7102,14 +7151,14 @@
         <v>7.8058067586863388E-3</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E45" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A45,Flows!$A$3:$A$21,0),MATCH($B45,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A45,Flows!$A$3:$A$21,0),MATCH($B45,Flows!$B$2:$E$2,0)))</f>
         <v>18.778630570011025</v>
       </c>
       <c r="F45" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G45" s="7"/>
       <c r="H45" s="7"/>
@@ -7130,14 +7179,14 @@
         <v>0.43852065321805955</v>
       </c>
       <c r="D46" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E46" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A46,Flows!$A$3:$A$21,0),MATCH($B46,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A46,Flows!$A$3:$A$21,0),MATCH($B46,Flows!$B$2:$E$2,0)))</f>
         <v>44.456985250973062</v>
       </c>
       <c r="F46" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
@@ -7158,14 +7207,14 @@
         <v>0.17005204487583964</v>
       </c>
       <c r="D47" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E47" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A47,Flows!$A$3:$A$21,0),MATCH($B47,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A47,Flows!$A$3:$A$21,0),MATCH($B47,Flows!$B$2:$E$2,0)))</f>
         <v>17.782794100389225</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
@@ -7186,14 +7235,14 @@
         <v>2.5616698292220113E-3</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E48" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A48,Flows!$A$3:$A$21,0),MATCH($B48,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A48,Flows!$A$3:$A$21,0),MATCH($B48,Flows!$B$2:$E$2,0)))</f>
         <v>2.934161026564222</v>
       </c>
       <c r="F48" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
@@ -7214,14 +7263,14 @@
         <v>2.3649226512727495E-3</v>
       </c>
       <c r="D49" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E49" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A49,Flows!$A$3:$A$21,0),MATCH($B49,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A49,Flows!$A$3:$A$21,0),MATCH($B49,Flows!$B$2:$E$2,0)))</f>
         <v>6.0994983764335551</v>
       </c>
       <c r="F49" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G49" s="7"/>
       <c r="H49" s="7"/>
@@ -7242,14 +7291,14 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="D50" s="21" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E50" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A50,Flows!$A$3:$A$21,0),MATCH($B50,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A50,Flows!$A$3:$A$21,0),MATCH($B50,Flows!$B$2:$G$2,0)))</f>
         <v>16.095147899941573</v>
       </c>
       <c r="F50" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
@@ -7270,14 +7319,14 @@
         <v>3.6900000000000002E-2</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="E51" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A51,Flows!$A$3:$A$21,0),MATCH($B51,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A51,Flows!$A$3:$A$21,0),MATCH($B51,Flows!$B$2:$G$2,0)))</f>
         <v>15.535450308907148</v>
       </c>
       <c r="F51" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
@@ -7298,14 +7347,14 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="D52" s="21" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E52" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A52,Flows!$A$3:$A$21,0),MATCH($B52,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A52,Flows!$A$3:$A$21,0),MATCH($B52,Flows!$B$2:$G$2,0)))</f>
         <v>14.199668958756412</v>
       </c>
       <c r="F52" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G52" s="7"/>
       <c r="H52" s="7"/>
@@ -7326,14 +7375,14 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="D53" s="21" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E53" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A53,Flows!$A$3:$A$21,0),MATCH($B53,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A53,Flows!$A$3:$A$21,0),MATCH($B53,Flows!$B$2:$G$2,0)))</f>
         <v>55.830044277922326</v>
       </c>
       <c r="F53" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G53" s="7"/>
       <c r="H53" s="7"/>
@@ -7354,14 +7403,14 @@
         <v>2.3999999999999998E-3</v>
       </c>
       <c r="D54" s="21" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E54" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A54,Flows!$A$3:$A$21,0),MATCH($B54,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A54,Flows!$A$3:$A$21,0),MATCH($B54,Flows!$B$2:$G$2,0)))</f>
         <v>8.0475739499707863</v>
       </c>
       <c r="F54" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G54" s="7"/>
       <c r="H54" s="7"/>
@@ -7382,14 +7431,14 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="D55" s="21" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E55" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A55,Flows!$A$3:$A$21,0),MATCH($B55,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A55,Flows!$A$3:$A$21,0),MATCH($B55,Flows!$B$2:$G$2,0)))</f>
         <v>40.237869749853928</v>
       </c>
       <c r="F55" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G55" s="7"/>
       <c r="H55" s="7"/>
@@ -7410,14 +7459,14 @@
         <v>0.04</v>
       </c>
       <c r="D56" s="21" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E56" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A56,Flows!$A$3:$A$21,0),MATCH($B56,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A56,Flows!$A$3:$A$21,0),MATCH($B56,Flows!$B$2:$G$2,0)))</f>
         <v>89.026286821551821</v>
       </c>
       <c r="F56" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
@@ -7438,14 +7487,14 @@
         <v>6.7999999999999996E-3</v>
       </c>
       <c r="D57" s="21" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E57" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A57,Flows!$A$3:$A$21,0),MATCH($B57,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A57,Flows!$A$3:$A$21,0),MATCH($B57,Flows!$B$2:$G$2,0)))</f>
         <v>9.2635120764741856</v>
       </c>
       <c r="F57" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G57" s="7"/>
       <c r="H57" s="7"/>
@@ -7466,14 +7515,14 @@
         <v>0.54</v>
       </c>
       <c r="D58" s="21" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E58" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A58,Flows!$A$3:$A$21,0),MATCH($B58,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A58,Flows!$A$3:$A$21,0),MATCH($B58,Flows!$B$2:$G$2,0)))</f>
         <v>77.960872640341989</v>
       </c>
       <c r="F58" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G58" s="7"/>
       <c r="H58" s="7"/>
@@ -7494,14 +7543,14 @@
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="D59" s="21" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E59" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A59,Flows!$A$3:$A$21,0),MATCH($B59,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A59,Flows!$A$3:$A$21,0),MATCH($B59,Flows!$B$2:$G$2,0)))</f>
         <v>17.762827077650776</v>
       </c>
       <c r="F59" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G59" s="7"/>
       <c r="H59" s="7"/>
@@ -7522,14 +7571,14 @@
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="D60" s="21" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E60" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A60,Flows!$A$3:$A$21,0),MATCH($B60,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A60,Flows!$A$3:$A$21,0),MATCH($B60,Flows!$B$2:$G$2,0)))</f>
         <v>4.5267603468585671</v>
       </c>
       <c r="F60" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G60" s="7"/>
       <c r="H60" s="7"/>
@@ -7550,13 +7599,13 @@
         <v>2.5662489315418147E-2</v>
       </c>
       <c r="D61" s="21" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E61" s="22">
         <v>0</v>
       </c>
       <c r="F61" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G61" s="7"/>
       <c r="H61" s="7"/>
@@ -7570,21 +7619,21 @@
         <v>3</v>
       </c>
       <c r="B62" s="20" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C62" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A62,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B62,'Percent BW'!$N$2:$X$2,0))</f>
         <v>2.7000000000000003E-2</v>
       </c>
       <c r="D62" s="21" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E62" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A62,Flows!$A$3:$A$21,0),MATCH($B62,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A62,Flows!$A$3:$A$21,0),MATCH($B62,Flows!$B$2:$G$2,0)))</f>
         <v>5.9813951248848829</v>
       </c>
       <c r="F62" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G62" s="7"/>
       <c r="H62" s="7"/>
@@ -7598,7 +7647,7 @@
         <v>5</v>
       </c>
       <c r="B63" s="20" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C63" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A63,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B63,'Percent BW'!$N$2:$X$2,0))</f>
@@ -7610,7 +7659,7 @@
         <v>0.34858241588912464</v>
       </c>
       <c r="F63" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G63" s="7"/>
       <c r="H63" s="7"/>
@@ -7624,7 +7673,7 @@
         <v>6</v>
       </c>
       <c r="B64" s="20" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C64" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A64,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B64,'Percent BW'!$N$2:$X$2,0))</f>
@@ -7636,7 +7685,7 @@
         <v>21.53302244958558</v>
       </c>
       <c r="F64" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G64" s="7"/>
       <c r="H64" s="7"/>
@@ -7650,21 +7699,21 @@
         <v>45</v>
       </c>
       <c r="B65" s="20" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C65" s="31">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Stomach",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B65,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Large Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B65,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Small Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B65,'Percent BW'!$N$2:$X$2,0))</f>
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="D65" s="21" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E65" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A65,Flows!$A$3:$A$21,0),MATCH($B65,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A65,Flows!$A$3:$A$21,0),MATCH($B65,Flows!$B$2:$G$2,0)))</f>
         <v>37.38371953053052</v>
       </c>
       <c r="F65" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G65" s="7"/>
       <c r="H65" s="7"/>
@@ -7678,21 +7727,21 @@
         <v>8</v>
       </c>
       <c r="B66" s="20" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C66" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A66,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B66,'Percent BW'!$N$2:$X$2,0))</f>
         <v>3.4000000000000002E-3</v>
       </c>
       <c r="D66" s="21" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E66" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A66,Flows!$A$3:$A$21,0),MATCH($B66,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A66,Flows!$A$3:$A$21,0),MATCH($B66,Flows!$B$2:$G$2,0)))</f>
         <v>17.944185374654648</v>
       </c>
       <c r="F66" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G66" s="7"/>
       <c r="H66" s="7"/>
@@ -7706,21 +7755,21 @@
         <v>38</v>
       </c>
       <c r="B67" s="20" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C67" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A67,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B67,'Percent BW'!$N$2:$X$2,0))</f>
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="D67" s="21" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E67" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A67,Flows!$A$3:$A$21,0),MATCH($B67,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A67,Flows!$A$3:$A$21,0),MATCH($B67,Flows!$B$2:$G$2,0)))</f>
         <v>41.271626361705692</v>
       </c>
       <c r="F67" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G67" s="7"/>
       <c r="H67" s="7"/>
@@ -7734,21 +7783,21 @@
         <v>10</v>
       </c>
       <c r="B68" s="20" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C68" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A68,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B68,'Percent BW'!$N$2:$X$2,0))</f>
         <v>2.7000000000000003E-2</v>
       </c>
       <c r="D68" s="21" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E68" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A68,Flows!$A$3:$A$21,0),MATCH($B68,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A68,Flows!$A$3:$A$21,0),MATCH($B68,Flows!$B$2:$G$2,0)))</f>
         <v>65.19720686124522</v>
       </c>
       <c r="F68" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G68" s="7"/>
       <c r="H68" s="7"/>
@@ -7762,21 +7811,21 @@
         <v>37</v>
       </c>
       <c r="B69" s="20" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C69" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A69,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B69,'Percent BW'!$N$2:$X$2,0))</f>
         <v>7.234650166587339E-3</v>
       </c>
       <c r="D69" s="21" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E69" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A69,Flows!$A$3:$A$21,0),MATCH($B69,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A69,Flows!$A$3:$A$21,0),MATCH($B69,Flows!$B$2:$G$2,0)))</f>
         <v>11.286443996023408</v>
       </c>
       <c r="F69" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G69" s="7"/>
       <c r="H69" s="7"/>
@@ -7790,21 +7839,21 @@
         <v>11</v>
       </c>
       <c r="B70" s="20" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C70" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A70,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B70,'Percent BW'!$N$2:$X$2,0))</f>
         <v>0.5</v>
       </c>
       <c r="D70" s="21" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E70" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A70,Flows!$A$3:$A$21,0),MATCH($B70,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A70,Flows!$A$3:$A$21,0),MATCH($B70,Flows!$B$2:$G$2,0)))</f>
         <v>26.916278061981973</v>
       </c>
       <c r="F70" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G70" s="7"/>
       <c r="H70" s="7"/>
@@ -7818,21 +7867,21 @@
         <v>13</v>
       </c>
       <c r="B71" s="20" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C71" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A71,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B71,'Percent BW'!$N$2:$X$2,0))</f>
         <v>0.1</v>
       </c>
       <c r="D71" s="21" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E71" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A71,Flows!$A$3:$A$21,0),MATCH($B71,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A71,Flows!$A$3:$A$21,0),MATCH($B71,Flows!$B$2:$G$2,0)))</f>
         <v>16.149766837189183</v>
       </c>
       <c r="F71" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G71" s="7"/>
       <c r="H71" s="7"/>
@@ -7846,21 +7895,21 @@
         <v>14</v>
       </c>
       <c r="B72" s="20" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C72" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A72,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B72,'Percent BW'!$N$2:$X$2,0))</f>
         <v>2.4667931688804553E-3</v>
       </c>
       <c r="D72" s="21" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E72" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A72,Flows!$A$3:$A$21,0),MATCH($B72,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A72,Flows!$A$3:$A$21,0),MATCH($B72,Flows!$B$2:$G$2,0)))</f>
         <v>6.2804648811291273</v>
       </c>
       <c r="F72" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G72" s="7"/>
       <c r="H72" s="7"/>
@@ -7874,7 +7923,7 @@
         <v>30</v>
       </c>
       <c r="B73" s="20" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C73" s="31">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Total",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B73,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("GI Contents",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B73,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("Blood",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B73,'Percent BW'!$N$2:$X$2,0))-SUM(C62:C72)</f>
@@ -7886,7 +7935,7 @@
         <v>99.799527813744888</v>
       </c>
       <c r="F73" s="20" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G73" s="7"/>
       <c r="H73" s="7"/>
@@ -7914,22 +7963,22 @@
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="28" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="26" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="95" spans="10:10" x14ac:dyDescent="0.25">
@@ -7943,10 +7992,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7963,16 +8012,16 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="32" t="s">
-        <v>315</v>
+        <v>361</v>
       </c>
       <c r="E1" s="32"/>
       <c r="F1" s="32" t="s">
-        <v>316</v>
+        <v>362</v>
       </c>
       <c r="G1" s="32"/>
       <c r="H1" s="32"/>
       <c r="I1" s="32" t="s">
-        <v>55</v>
+        <v>365</v>
       </c>
       <c r="J1" s="32"/>
       <c r="K1" s="32"/>
@@ -8004,16 +8053,16 @@
         <v>50</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>319</v>
-      </c>
       <c r="L2" s="1" t="s">
-        <v>320</v>
+        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -8474,13 +8523,13 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>314</v>
+        <v>368</v>
       </c>
       <c r="D15">
         <v>0.86</v>
@@ -8489,68 +8538,71 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="F15">
-        <v>2.88818990331598E-2</v>
+        <v>0.69</v>
       </c>
       <c r="G15">
-        <v>0.91918088619788096</v>
+        <v>0.05</v>
       </c>
       <c r="H15">
-        <v>5.1937214768959301E-2</v>
+        <v>0.16</v>
       </c>
       <c r="I15">
-        <v>0.99766081871345003</v>
+        <v>0.92</v>
       </c>
       <c r="J15">
-        <v>1.8713450292397701E-3</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="K15">
-        <v>4.6783625730994197E-4</v>
+        <v>1.4E-2</v>
       </c>
       <c r="L15">
-        <v>7.1</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>357</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>358</v>
       </c>
       <c r="C16" t="s">
-        <v>314</v>
+        <v>358</v>
       </c>
       <c r="D16">
-        <v>0.9</v>
+        <v>0.72399999999999998</v>
       </c>
       <c r="E16">
-        <v>0.1</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="F16">
-        <v>0.26</v>
+        <v>0.79300000000000004</v>
       </c>
       <c r="G16">
-        <v>0.02</v>
+        <v>8.3000000000000001E-3</v>
       </c>
       <c r="H16">
-        <v>0.21</v>
+        <v>0.1535</v>
       </c>
       <c r="I16">
-        <v>0.85</v>
+        <f>AVERAGE(I3:I15)</f>
+        <v>0.62729972078921881</v>
       </c>
       <c r="J16">
-        <v>0.11</v>
+        <f>AVERAGE(J3:J15)</f>
+        <v>0.29874183536494969</v>
       </c>
       <c r="K16">
-        <v>0.04</v>
+        <f>AVERAGE(K3:K15)</f>
+        <v>7.3804597691985455E-2</v>
       </c>
       <c r="L16">
-        <v>7</v>
+        <v>7.24</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
@@ -8559,28 +8611,28 @@
         <v>314</v>
       </c>
       <c r="D17">
-        <v>0.83799999999999997</v>
+        <v>0.86</v>
       </c>
       <c r="E17">
-        <v>0.16200000000000001</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F17">
-        <v>0.80292051232726702</v>
+        <v>2.88818990331598E-2</v>
       </c>
       <c r="G17">
-        <v>0.115353333926677</v>
+        <v>0.91918088619788096</v>
       </c>
       <c r="H17">
-        <v>8.1726153746056907E-2</v>
+        <v>5.1937214768959301E-2</v>
       </c>
       <c r="I17">
-        <v>0.95354523227383903</v>
+        <v>0.99766081871345003</v>
       </c>
       <c r="J17">
-        <v>3.6674816625916901E-2</v>
+        <v>1.8713450292397701E-3</v>
       </c>
       <c r="K17">
-        <v>9.7799511002445005E-3</v>
+        <v>4.6783625730994197E-4</v>
       </c>
       <c r="L17">
         <v>7.1</v>
@@ -8588,7 +8640,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
@@ -8600,25 +8652,25 @@
         <v>0.9</v>
       </c>
       <c r="E18">
-        <v>9.6000000000000002E-2</v>
+        <v>0.1</v>
       </c>
       <c r="F18">
-        <v>0.78</v>
+        <v>0.26</v>
       </c>
       <c r="G18">
-        <v>7.0000000000000007E-2</v>
+        <v>0.02</v>
       </c>
       <c r="H18">
-        <v>0.15</v>
+        <v>0.21</v>
       </c>
       <c r="I18">
-        <v>0.69</v>
+        <v>0.85</v>
       </c>
       <c r="J18">
-        <v>0.26</v>
+        <v>0.11</v>
       </c>
       <c r="K18">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="L18">
         <v>7</v>
@@ -8626,7 +8678,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
@@ -8635,28 +8687,28 @@
         <v>314</v>
       </c>
       <c r="D19">
-        <v>0.86</v>
+        <v>0.83799999999999997</v>
       </c>
       <c r="E19">
-        <v>0.14000000000000001</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="F19">
-        <v>0.76399672127125895</v>
+        <v>0.80292051232726702</v>
       </c>
       <c r="G19">
-        <v>3.2882921622291603E-2</v>
+        <v>0.115353333926677</v>
       </c>
       <c r="H19">
-        <v>0.20312035710644999</v>
+        <v>8.1726153746056907E-2</v>
       </c>
       <c r="I19">
-        <v>0.52141527001862198</v>
+        <v>0.95354523227383903</v>
       </c>
       <c r="J19">
-        <v>0.39478584729981397</v>
+        <v>3.6674816625916901E-2</v>
       </c>
       <c r="K19">
-        <v>8.3798882681564199E-2</v>
+        <v>9.7799511002445005E-3</v>
       </c>
       <c r="L19">
         <v>7.1</v>
@@ -8664,7 +8716,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
         <v>17</v>
@@ -8673,36 +8725,36 @@
         <v>314</v>
       </c>
       <c r="D20">
-        <v>0.85399999999999998</v>
+        <v>0.9</v>
       </c>
       <c r="E20">
-        <v>0.14599999999999999</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="F20">
-        <v>0.75362656390091898</v>
+        <v>0.78</v>
       </c>
       <c r="G20">
-        <v>5.2658017463145301E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H20">
-        <v>0.193715418635936</v>
+        <v>0.15</v>
       </c>
       <c r="I20">
-        <v>0.29246892517669998</v>
+        <v>0.69</v>
       </c>
       <c r="J20">
-        <v>0.58493785035339996</v>
+        <v>0.26</v>
       </c>
       <c r="K20">
-        <v>0.12259322446989999</v>
+        <v>0.05</v>
       </c>
       <c r="L20">
-        <v>7.22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
         <v>17</v>
@@ -8711,36 +8763,36 @@
         <v>314</v>
       </c>
       <c r="D21">
-        <v>0.873</v>
+        <v>0.86</v>
       </c>
       <c r="E21">
-        <v>0.127</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F21">
-        <v>0.68180834079295904</v>
+        <v>0.76399672127125895</v>
       </c>
       <c r="G21">
-        <v>6.2198013624446602E-2</v>
+        <v>3.2882921622291603E-2</v>
       </c>
       <c r="H21">
-        <v>0.25599364558259502</v>
+        <v>0.20312035710644999</v>
       </c>
       <c r="I21">
-        <v>0.33050047214353201</v>
+        <v>0.52141527001862198</v>
       </c>
       <c r="J21">
-        <v>0.561850802644004</v>
+        <v>0.39478584729981397</v>
       </c>
       <c r="K21">
-        <v>0.107648725212465</v>
+        <v>8.3798882681564199E-2</v>
       </c>
       <c r="L21">
-        <v>7.23</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
         <v>17</v>
@@ -8749,36 +8801,36 @@
         <v>314</v>
       </c>
       <c r="D22">
-        <v>0.67500000000000004</v>
+        <v>0.85399999999999998</v>
       </c>
       <c r="E22">
-        <v>0.32500000000000001</v>
+        <v>0.14599999999999999</v>
       </c>
       <c r="F22">
-        <v>0.75535011388568196</v>
+        <v>0.75362656390091898</v>
       </c>
       <c r="G22">
-        <v>8.3300793960692399E-2</v>
+        <v>5.2658017463145301E-2</v>
       </c>
       <c r="H22">
-        <v>0.161349092153626</v>
+        <v>0.193715418635936</v>
       </c>
       <c r="I22">
-        <v>0.57576550641193402</v>
+        <v>0.29246892517669998</v>
       </c>
       <c r="J22">
-        <v>0.32190526040303602</v>
+        <v>0.58493785035339996</v>
       </c>
       <c r="K22">
-        <v>0.10232923318503</v>
+        <v>0.12259322446989999</v>
       </c>
       <c r="L22">
-        <v>6.6</v>
+        <v>7.22</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B23" t="s">
         <v>17</v>
@@ -8787,36 +8839,36 @@
         <v>314</v>
       </c>
       <c r="D23">
-        <v>0.876</v>
+        <v>0.873</v>
       </c>
       <c r="E23">
-        <v>0.124</v>
+        <v>0.127</v>
       </c>
       <c r="F23">
-        <v>0.77677543363722101</v>
+        <v>0.68180834079295904</v>
       </c>
       <c r="G23">
-        <v>2.3186412508439901E-2</v>
+        <v>6.2198013624446602E-2</v>
       </c>
       <c r="H23">
-        <v>0.20003815385434001</v>
+        <v>0.25599364558259502</v>
       </c>
       <c r="I23">
-        <v>0.53390282968499703</v>
+        <v>0.33050047214353201</v>
       </c>
       <c r="J23">
-        <v>0.38441003737319801</v>
+        <v>0.561850802644004</v>
       </c>
       <c r="K23">
-        <v>8.1687132941804602E-2</v>
+        <v>0.107648725212465</v>
       </c>
       <c r="L23">
-        <v>6.81</v>
+        <v>7.23</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="B24" t="s">
         <v>17</v>
@@ -8825,36 +8877,36 @@
         <v>314</v>
       </c>
       <c r="D24">
-        <v>0.68100000000000005</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="E24">
-        <v>0.31900000000000001</v>
+        <v>0.32500000000000001</v>
       </c>
       <c r="F24">
-        <v>0.52200601546333902</v>
+        <v>0.75535011388568196</v>
       </c>
       <c r="G24">
-        <v>6.3830853345103702E-2</v>
+        <v>8.3300793960692399E-2</v>
       </c>
       <c r="H24">
-        <v>0.41416313119155701</v>
+        <v>0.161349092153626</v>
       </c>
       <c r="I24">
-        <v>0.80753701211305495</v>
+        <v>0.57576550641193402</v>
       </c>
       <c r="J24">
-        <v>0.14804845222072699</v>
+        <v>0.32190526040303602</v>
       </c>
       <c r="K24">
-        <v>4.4414535666218002E-2</v>
+        <v>0.10232923318503</v>
       </c>
       <c r="L24">
-        <v>7</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B25" t="s">
         <v>17</v>
@@ -8863,36 +8915,36 @@
         <v>314</v>
       </c>
       <c r="D25">
-        <v>0.745</v>
+        <v>0.876</v>
       </c>
       <c r="E25">
-        <v>0.255</v>
+        <v>0.124</v>
       </c>
       <c r="F25">
-        <v>0.64498977178046801</v>
+        <v>0.77677543363722101</v>
       </c>
       <c r="G25">
-        <v>3.9570322823172903E-2</v>
+        <v>2.3186412508439901E-2</v>
       </c>
       <c r="H25">
-        <v>0.31543990539635902</v>
+        <v>0.20003815385434001</v>
       </c>
       <c r="I25">
-        <v>0.36563071297989003</v>
+        <v>0.53390282968499703</v>
       </c>
       <c r="J25">
-        <v>0.48903107861060302</v>
+        <v>0.38441003737319801</v>
       </c>
       <c r="K25">
-        <v>0.14533820840950601</v>
+        <v>8.1687132941804602E-2</v>
       </c>
       <c r="L25">
-        <v>7</v>
+        <v>6.81</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="B26" t="s">
         <v>17</v>
@@ -8901,130 +8953,256 @@
         <v>314</v>
       </c>
       <c r="D26">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="E26">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="F26">
+        <v>0.52200601546333902</v>
+      </c>
+      <c r="G26">
+        <v>6.3830853345103702E-2</v>
+      </c>
+      <c r="H26">
+        <v>0.41416313119155701</v>
+      </c>
+      <c r="I26">
+        <v>0.80753701211305495</v>
+      </c>
+      <c r="J26">
+        <v>0.14804845222072699</v>
+      </c>
+      <c r="K26">
+        <v>4.4414535666218002E-2</v>
+      </c>
+      <c r="L26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" t="s">
+        <v>314</v>
+      </c>
+      <c r="D27">
+        <v>0.745</v>
+      </c>
+      <c r="E27">
+        <v>0.255</v>
+      </c>
+      <c r="F27">
+        <v>0.64498977178046801</v>
+      </c>
+      <c r="G27">
+        <v>3.9570322823172903E-2</v>
+      </c>
+      <c r="H27">
+        <v>0.31543990539635902</v>
+      </c>
+      <c r="I27">
+        <v>0.36563071297989003</v>
+      </c>
+      <c r="J27">
+        <v>0.48903107861060302</v>
+      </c>
+      <c r="K27">
+        <v>0.14533820840950601</v>
+      </c>
+      <c r="L27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" t="s">
+        <v>314</v>
+      </c>
+      <c r="D28">
         <v>1</v>
       </c>
-      <c r="E26">
+      <c r="E28">
         <v>0</v>
       </c>
-      <c r="F26">
+      <c r="F28">
         <v>0.66399197592778303</v>
       </c>
-      <c r="G26">
+      <c r="G28">
         <v>5.0150451354062202E-3</v>
       </c>
-      <c r="H26">
+      <c r="H28">
         <v>0.33099297893681001</v>
       </c>
-      <c r="I26">
+      <c r="I28">
         <v>0.22727272727272699</v>
       </c>
-      <c r="J26">
+      <c r="J28">
         <v>0.65909090909090895</v>
       </c>
-      <c r="K26">
+      <c r="K28">
         <v>0.11363636363636399</v>
       </c>
-      <c r="L26">
+      <c r="L28">
         <v>7.2</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L27" s="2"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="27" t="s">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="27" t="s">
         <v>43</v>
-      </c>
-      <c r="L28" s="2"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="L29" s="2"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="L30" s="2"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="29" t="s">
-        <v>341</v>
       </c>
       <c r="L31" s="2"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="29" t="s">
+        <v>360</v>
+      </c>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="L32" s="2"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="L33" s="2"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="26" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="26" t="s">
-        <v>327</v>
-      </c>
+      <c r="L35" s="2"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="s">
+      <c r="A36" s="27" t="s">
+        <v>359</v>
+      </c>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="27" t="s">
+        <v>363</v>
+      </c>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="27" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="27" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="27" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="27"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="27"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="27"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>337</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="26" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="26" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="26" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="26" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="26" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="26" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="26" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="26" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="26" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="26" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="26" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="26" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="26" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="26" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="26" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="26" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="26" t="s">
         <v>328</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="26" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="26" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="26" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="26" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="26" t="s">
+        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -9042,8 +9220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9086,7 +9264,7 @@
         <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="G2" t="s">
         <v>104</v>
@@ -9104,7 +9282,7 @@
         <v>35</v>
       </c>
       <c r="L2" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="M2" t="s">
         <v>104</v>
@@ -9122,10 +9300,10 @@
         <v>35</v>
       </c>
       <c r="R2" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="S2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="T2" t="s">
         <v>104</v>
@@ -10534,22 +10712,22 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="40" spans="10:10" x14ac:dyDescent="0.25">
@@ -10828,7 +11006,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -10894,7 +11072,7 @@
         <v>104</v>
       </c>
       <c r="L2" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="N2" t="s">
         <v>34</v>
@@ -10912,7 +11090,7 @@
         <v>104</v>
       </c>
       <c r="X2" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -12256,10 +12434,10 @@
         <v>105</v>
       </c>
       <c r="V24" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="X24" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
@@ -12267,23 +12445,23 @@
         <v>105</v>
       </c>
       <c r="B26" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="B27" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B28" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve documentation for thyroid follicular pH estimate based on measurements in turtles and mice.
</commit_message>
<xml_diff>
--- a/pkdata.xlsx
+++ b/pkdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msfeir\httkdatatables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msfeir\httkdatatablesGitHub\httkdatatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2404DF4C-B45D-4D59-8D1D-C4CACBDC0F7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84F83D4-FD38-4764-81F1-4FF4B1400550}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="480" windowWidth="19560" windowHeight="10440" tabRatio="884" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="405" yWindow="255" windowWidth="19560" windowHeight="10440" tabRatio="884" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic PK" sheetId="7" r:id="rId1"/>
@@ -1795,10 +1795,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Virreira et al. "Expression, Localization, and Regulation of the Sodium Bicarbonate Cotransporter NBCe1 in the Thyroid." Thyroid 29.2 (2019). </t>
-  </si>
-  <si>
-    <t>j Thyroid tissue pH is estimated at 7.3, in accordance with the measurements of turtle thyroid follicular cell pH made by Chow et al. 1982. According to a study of humans and rats by Virreira et al. in 2019, thyroid intrafollicular space pH thyrotropin was measured at 7.6 after stimulation with thyrotropin, which is approximately the same as the 7.7 pH in the turtle follicular cells measured by Chow et al. 1982 after thyrotropin stimulation.</t>
+    <t>Wangemann et al. "Developmental delays consistent with cochlear hypothyroidism contribute to failure to develop hearing in mice lacking Slc26a4/pendrin expression." American Journal of Physiology: Renal Physiology. 2009;297(5):F1435-F1447.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">j Human thyroid tissue pH is estimated at 7.3, based on the measurements of turtle thyroid follicular cell pH made by Chow et al. 1982. Also, according to a study of mice by Wangemann et al. in 2009, thyroid follicular pH was measured at 7.6. </t>
   </si>
 </sst>
 </file>
@@ -7994,7 +7994,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add "Human" to species column for the placenta tissue composition data. This has not yet been confirmed based on our references (the references argument is still unknown), but I will assume it for now for the sake of running the parameterization code (which requires a known species argument). This is a good time to note that I have also erroneously set the "species" entry for the thyroid tissue comp data to "Human," when really our estimates are based on mice and turtles. I will consult John to see what the best documentation practice is here, and whether I should either change the species value and otherwise accommodate.
</commit_message>
<xml_diff>
--- a/pkdata.xlsx
+++ b/pkdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msfeir\httkdatatablesGitHub\httkdatatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84F83D4-FD38-4764-81F1-4FF4B1400550}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D9FC5C-DAAE-4499-85A0-3114CA27B8FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="405" yWindow="255" windowWidth="19560" windowHeight="10440" tabRatio="884" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7995,7 +7995,7 @@
   <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8564,7 +8564,7 @@
         <v>357</v>
       </c>
       <c r="B16" t="s">
-        <v>358</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
         <v>358</v>

</xml_diff>

<commit_message>
Change load_package_data_tables prompt for updating the chemical data for which no CAS match is made (it had previously instructed to use unavailable CAS data instead of the known chemical names in EPA batch search). Add note to pkdata.xlsx's tissue composition sheet to indicate that the placental parameters used for the Schmitt method are based on general estimates for rapidly perfused tissue that httk collaborators like Annie Lumen have made in the past.
</commit_message>
<xml_diff>
--- a/pkdata.xlsx
+++ b/pkdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msfeir\httkdatatablesGitHub\httkdatatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D9FC5C-DAAE-4499-85A0-3114CA27B8FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766665F4-423C-4501-BDB1-6DC5D66F2DA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="405" yWindow="255" windowWidth="19560" windowHeight="10440" tabRatio="884" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="375">
   <si>
     <t>Tissue</t>
   </si>
@@ -1703,9 +1703,6 @@
     <t>Placenta</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
     <t>f Placenta values transferred from hard-coded sequence in predict_partitioning_schmitt, where fractions of total lipid comprised by neutral lipid, neutral phospholipid, and acidic phospholipid are tentatively calculated as the average of the corresponding values for all other listed tissues in the human.</t>
   </si>
   <si>
@@ -1799,6 +1796,29 @@
   </si>
   <si>
     <t xml:space="preserve">j Human thyroid tissue pH is estimated at 7.3, based on the measurements of turtle thyroid follicular cell pH made by Chow et al. 1982. Also, according to a study of mice by Wangemann et al. in 2009, thyroid follicular pH was measured at 7.6. </t>
+  </si>
+  <si>
+    <t>Httk estimate</t>
+  </si>
+  <si>
+    <r>
+      <t>Reference</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>k</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">k Httk collaborators have generally used estimates for placental parameters based on rapidly perfused tissue generally, and that is how the placental parameters were set here. More information on this estimate process is needed. </t>
   </si>
 </sst>
 </file>
@@ -7994,7 +8014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -8012,16 +8032,16 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="32" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E1" s="32"/>
       <c r="F1" s="32" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G1" s="32"/>
       <c r="H1" s="32"/>
       <c r="I1" s="32" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="J1" s="32"/>
       <c r="K1" s="32"/>
@@ -8035,7 +8055,7 @@
         <v>118</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>312</v>
+        <v>373</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>54</v>
@@ -8062,7 +8082,7 @@
         <v>317</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -8529,7 +8549,7 @@
         <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D15">
         <v>0.86</v>
@@ -8567,7 +8587,7 @@
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>358</v>
+        <v>372</v>
       </c>
       <c r="D16">
         <v>0.72399999999999998</v>
@@ -9079,7 +9099,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="L34" s="2"/>
     </row>
@@ -9091,33 +9111,35 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="L36" s="2"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="27" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="L37" s="2"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="27" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="27" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="27"/>
+      <c r="A41" s="27" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="27"/>
@@ -9192,17 +9214,17 @@
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="26" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="26" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="26" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add thyroid relative body weight measurement to pkdata.xlsx file. Should be used in parameterization in httk.
</commit_message>
<xml_diff>
--- a/pkdata.xlsx
+++ b/pkdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msfeir\httkdatatablesGitHub\httkdatatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766665F4-423C-4501-BDB1-6DC5D66F2DA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32751531-4CE9-4B0E-9830-88215DE748DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="405" yWindow="255" windowWidth="19560" windowHeight="10440" tabRatio="884" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="630" yWindow="405" windowWidth="19560" windowHeight="10440" tabRatio="884" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic PK" sheetId="7" r:id="rId1"/>
@@ -43,9 +43,9 @@
     <definedName name="tblfn10" localSheetId="2">TissueComp!$A$33</definedName>
     <definedName name="tblfn10" localSheetId="1">VolumeFlow!#REF!</definedName>
     <definedName name="tblfn8" localSheetId="2">TissueComp!$A$31</definedName>
-    <definedName name="tblfn8" localSheetId="1">VolumeFlow!$A$75</definedName>
+    <definedName name="tblfn8" localSheetId="1">VolumeFlow!$A$76</definedName>
     <definedName name="tblfn9" localSheetId="2">TissueComp!$A$32</definedName>
-    <definedName name="tblfn9" localSheetId="1">VolumeFlow!$A$76</definedName>
+    <definedName name="tblfn9" localSheetId="1">VolumeFlow!$A$77</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="375">
   <si>
     <t>Tissue</t>
   </si>
@@ -3321,39 +3321,39 @@
         <v>Adipose</v>
       </c>
       <c r="B3" s="2" t="e">
-        <f>TissueComp!D3*INDEX(VolumeFlow!$A1:$B13,MATCH('Average Properties Calc'!$A3,VolumeFlow!$A1:$A13,0),4)</f>
+        <f>TissueComp!D3*INDEX(VolumeFlow!$A1:$B14,MATCH('Average Properties Calc'!$A3,VolumeFlow!$A1:$A14,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C3" s="2" t="e">
-        <f>TissueComp!E3*INDEX(VolumeFlow!$A1:$B13,MATCH('Average Properties Calc'!$A3,VolumeFlow!$A1:$A13,0),4)</f>
+        <f>TissueComp!E3*INDEX(VolumeFlow!$A1:$B14,MATCH('Average Properties Calc'!$A3,VolumeFlow!$A1:$A14,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D3" s="2" t="e">
-        <f>TissueComp!F3*INDEX(VolumeFlow!$A1:$B13,MATCH('Average Properties Calc'!$A3,VolumeFlow!$A1:$A13,0),4)</f>
+        <f>TissueComp!F3*INDEX(VolumeFlow!$A1:$B14,MATCH('Average Properties Calc'!$A3,VolumeFlow!$A1:$A14,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E3" s="2" t="e">
-        <f>TissueComp!G3*INDEX(VolumeFlow!$A1:$B13,MATCH('Average Properties Calc'!$A3,VolumeFlow!$A1:$A13,0),4)</f>
+        <f>TissueComp!G3*INDEX(VolumeFlow!$A1:$B14,MATCH('Average Properties Calc'!$A3,VolumeFlow!$A1:$A14,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F3" s="2" t="e">
-        <f>TissueComp!H3*INDEX(VolumeFlow!$A1:$B13,MATCH('Average Properties Calc'!$A3,VolumeFlow!$A1:$A13,0),4)</f>
+        <f>TissueComp!H3*INDEX(VolumeFlow!$A1:$B14,MATCH('Average Properties Calc'!$A3,VolumeFlow!$A1:$A14,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G3" s="2" t="e">
-        <f>TissueComp!I3*INDEX(VolumeFlow!$A1:$B13,MATCH('Average Properties Calc'!$A3,VolumeFlow!$A1:$A13,0),4)</f>
+        <f>TissueComp!I3*INDEX(VolumeFlow!$A1:$B14,MATCH('Average Properties Calc'!$A3,VolumeFlow!$A1:$A14,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H3" s="2" t="e">
-        <f>TissueComp!J3*INDEX(VolumeFlow!$A1:$B13,MATCH('Average Properties Calc'!$A3,VolumeFlow!$A1:$A13,0),4)</f>
+        <f>TissueComp!J3*INDEX(VolumeFlow!$A1:$B14,MATCH('Average Properties Calc'!$A3,VolumeFlow!$A1:$A14,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I3" s="2" t="e">
-        <f>TissueComp!K3*INDEX(VolumeFlow!$A1:$B13,MATCH('Average Properties Calc'!$A3,VolumeFlow!$A1:$A13,0),4)</f>
+        <f>TissueComp!K3*INDEX(VolumeFlow!$A1:$B14,MATCH('Average Properties Calc'!$A3,VolumeFlow!$A1:$A14,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J3" s="2" t="e">
-        <f>TissueComp!L3*INDEX(VolumeFlow!$A1:$B13,MATCH('Average Properties Calc'!$A3,VolumeFlow!$A1:$A13,0),4)</f>
+        <f>TissueComp!L3*INDEX(VolumeFlow!$A1:$B14,MATCH('Average Properties Calc'!$A3,VolumeFlow!$A1:$A14,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K3" t="s">
@@ -3366,39 +3366,39 @@
         <v>Bone</v>
       </c>
       <c r="B4" s="2" t="e">
-        <f>TissueComp!D4*INDEX(VolumeFlow!$A2:$B14,MATCH('Average Properties Calc'!$A4,VolumeFlow!$A2:$A14,0),4)</f>
+        <f>TissueComp!D4*INDEX(VolumeFlow!$A2:$B15,MATCH('Average Properties Calc'!$A4,VolumeFlow!$A2:$A15,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C4" s="2" t="e">
-        <f>TissueComp!E4*INDEX(VolumeFlow!$A2:$B14,MATCH('Average Properties Calc'!$A4,VolumeFlow!$A2:$A14,0),4)</f>
+        <f>TissueComp!E4*INDEX(VolumeFlow!$A2:$B15,MATCH('Average Properties Calc'!$A4,VolumeFlow!$A2:$A15,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D4" s="2" t="e">
-        <f>TissueComp!F4*INDEX(VolumeFlow!$A2:$B14,MATCH('Average Properties Calc'!$A4,VolumeFlow!$A2:$A14,0),4)</f>
+        <f>TissueComp!F4*INDEX(VolumeFlow!$A2:$B15,MATCH('Average Properties Calc'!$A4,VolumeFlow!$A2:$A15,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E4" s="2" t="e">
-        <f>TissueComp!G4*INDEX(VolumeFlow!$A2:$B14,MATCH('Average Properties Calc'!$A4,VolumeFlow!$A2:$A14,0),4)</f>
+        <f>TissueComp!G4*INDEX(VolumeFlow!$A2:$B15,MATCH('Average Properties Calc'!$A4,VolumeFlow!$A2:$A15,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F4" s="2" t="e">
-        <f>TissueComp!H4*INDEX(VolumeFlow!$A2:$B14,MATCH('Average Properties Calc'!$A4,VolumeFlow!$A2:$A14,0),4)</f>
+        <f>TissueComp!H4*INDEX(VolumeFlow!$A2:$B15,MATCH('Average Properties Calc'!$A4,VolumeFlow!$A2:$A15,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G4" s="2" t="e">
-        <f>TissueComp!I4*INDEX(VolumeFlow!$A2:$B14,MATCH('Average Properties Calc'!$A4,VolumeFlow!$A2:$A14,0),4)</f>
+        <f>TissueComp!I4*INDEX(VolumeFlow!$A2:$B15,MATCH('Average Properties Calc'!$A4,VolumeFlow!$A2:$A15,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H4" s="2" t="e">
-        <f>TissueComp!J4*INDEX(VolumeFlow!$A2:$B14,MATCH('Average Properties Calc'!$A4,VolumeFlow!$A2:$A14,0),4)</f>
+        <f>TissueComp!J4*INDEX(VolumeFlow!$A2:$B15,MATCH('Average Properties Calc'!$A4,VolumeFlow!$A2:$A15,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I4" s="2" t="e">
-        <f>TissueComp!K4*INDEX(VolumeFlow!$A2:$B14,MATCH('Average Properties Calc'!$A4,VolumeFlow!$A2:$A14,0),4)</f>
+        <f>TissueComp!K4*INDEX(VolumeFlow!$A2:$B15,MATCH('Average Properties Calc'!$A4,VolumeFlow!$A2:$A15,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J4" s="2" t="e">
-        <f>TissueComp!L4*INDEX(VolumeFlow!$A2:$B14,MATCH('Average Properties Calc'!$A4,VolumeFlow!$A2:$A14,0),4)</f>
+        <f>TissueComp!L4*INDEX(VolumeFlow!$A2:$B15,MATCH('Average Properties Calc'!$A4,VolumeFlow!$A2:$A15,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K4" t="s">
@@ -3411,39 +3411,39 @@
         <v>Brain</v>
       </c>
       <c r="B5" s="2" t="e">
-        <f>TissueComp!D5*INDEX(VolumeFlow!$A3:$B15,MATCH('Average Properties Calc'!$A5,VolumeFlow!$A3:$A15,0),4)</f>
+        <f>TissueComp!D5*INDEX(VolumeFlow!$A3:$B16,MATCH('Average Properties Calc'!$A5,VolumeFlow!$A3:$A16,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C5" s="2" t="e">
-        <f>TissueComp!E5*INDEX(VolumeFlow!$A3:$B15,MATCH('Average Properties Calc'!$A5,VolumeFlow!$A3:$A15,0),4)</f>
+        <f>TissueComp!E5*INDEX(VolumeFlow!$A3:$B16,MATCH('Average Properties Calc'!$A5,VolumeFlow!$A3:$A16,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D5" s="2" t="e">
-        <f>TissueComp!F5*INDEX(VolumeFlow!$A3:$B15,MATCH('Average Properties Calc'!$A5,VolumeFlow!$A3:$A15,0),4)</f>
+        <f>TissueComp!F5*INDEX(VolumeFlow!$A3:$B16,MATCH('Average Properties Calc'!$A5,VolumeFlow!$A3:$A16,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E5" s="2" t="e">
-        <f>TissueComp!G5*INDEX(VolumeFlow!$A3:$B15,MATCH('Average Properties Calc'!$A5,VolumeFlow!$A3:$A15,0),4)</f>
+        <f>TissueComp!G5*INDEX(VolumeFlow!$A3:$B16,MATCH('Average Properties Calc'!$A5,VolumeFlow!$A3:$A16,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F5" s="2" t="e">
-        <f>TissueComp!H5*INDEX(VolumeFlow!$A3:$B15,MATCH('Average Properties Calc'!$A5,VolumeFlow!$A3:$A15,0),4)</f>
+        <f>TissueComp!H5*INDEX(VolumeFlow!$A3:$B16,MATCH('Average Properties Calc'!$A5,VolumeFlow!$A3:$A16,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G5" s="2" t="e">
-        <f>TissueComp!I5*INDEX(VolumeFlow!$A3:$B15,MATCH('Average Properties Calc'!$A5,VolumeFlow!$A3:$A15,0),4)</f>
+        <f>TissueComp!I5*INDEX(VolumeFlow!$A3:$B16,MATCH('Average Properties Calc'!$A5,VolumeFlow!$A3:$A16,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H5" s="2" t="e">
-        <f>TissueComp!J5*INDEX(VolumeFlow!$A3:$B15,MATCH('Average Properties Calc'!$A5,VolumeFlow!$A3:$A15,0),4)</f>
+        <f>TissueComp!J5*INDEX(VolumeFlow!$A3:$B16,MATCH('Average Properties Calc'!$A5,VolumeFlow!$A3:$A16,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I5" s="2" t="e">
-        <f>TissueComp!K5*INDEX(VolumeFlow!$A3:$B15,MATCH('Average Properties Calc'!$A5,VolumeFlow!$A3:$A15,0),4)</f>
+        <f>TissueComp!K5*INDEX(VolumeFlow!$A3:$B16,MATCH('Average Properties Calc'!$A5,VolumeFlow!$A3:$A16,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J5" s="2" t="e">
-        <f>TissueComp!L5*INDEX(VolumeFlow!$A3:$B15,MATCH('Average Properties Calc'!$A5,VolumeFlow!$A3:$A15,0),4)</f>
+        <f>TissueComp!L5*INDEX(VolumeFlow!$A3:$B16,MATCH('Average Properties Calc'!$A5,VolumeFlow!$A3:$A16,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K5" t="s">
@@ -3456,39 +3456,39 @@
         <v>Gut</v>
       </c>
       <c r="B6" s="2" t="e">
-        <f>TissueComp!D6*INDEX(VolumeFlow!$A4:$B16,MATCH('Average Properties Calc'!$A6,VolumeFlow!$A4:$A16,0),4)</f>
+        <f>TissueComp!D6*INDEX(VolumeFlow!$A4:$B17,MATCH('Average Properties Calc'!$A6,VolumeFlow!$A4:$A17,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C6" s="2" t="e">
-        <f>TissueComp!E6*INDEX(VolumeFlow!$A4:$B16,MATCH('Average Properties Calc'!$A6,VolumeFlow!$A4:$A16,0),4)</f>
+        <f>TissueComp!E6*INDEX(VolumeFlow!$A4:$B17,MATCH('Average Properties Calc'!$A6,VolumeFlow!$A4:$A17,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D6" s="2" t="e">
-        <f>TissueComp!F6*INDEX(VolumeFlow!$A4:$B16,MATCH('Average Properties Calc'!$A6,VolumeFlow!$A4:$A16,0),4)</f>
+        <f>TissueComp!F6*INDEX(VolumeFlow!$A4:$B17,MATCH('Average Properties Calc'!$A6,VolumeFlow!$A4:$A17,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E6" s="2" t="e">
-        <f>TissueComp!G6*INDEX(VolumeFlow!$A4:$B16,MATCH('Average Properties Calc'!$A6,VolumeFlow!$A4:$A16,0),4)</f>
+        <f>TissueComp!G6*INDEX(VolumeFlow!$A4:$B17,MATCH('Average Properties Calc'!$A6,VolumeFlow!$A4:$A17,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F6" s="2" t="e">
-        <f>TissueComp!H6*INDEX(VolumeFlow!$A4:$B16,MATCH('Average Properties Calc'!$A6,VolumeFlow!$A4:$A16,0),4)</f>
+        <f>TissueComp!H6*INDEX(VolumeFlow!$A4:$B17,MATCH('Average Properties Calc'!$A6,VolumeFlow!$A4:$A17,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G6" s="2" t="e">
-        <f>TissueComp!I6*INDEX(VolumeFlow!$A4:$B16,MATCH('Average Properties Calc'!$A6,VolumeFlow!$A4:$A16,0),4)</f>
+        <f>TissueComp!I6*INDEX(VolumeFlow!$A4:$B17,MATCH('Average Properties Calc'!$A6,VolumeFlow!$A4:$A17,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H6" s="2" t="e">
-        <f>TissueComp!J6*INDEX(VolumeFlow!$A4:$B16,MATCH('Average Properties Calc'!$A6,VolumeFlow!$A4:$A16,0),4)</f>
+        <f>TissueComp!J6*INDEX(VolumeFlow!$A4:$B17,MATCH('Average Properties Calc'!$A6,VolumeFlow!$A4:$A17,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I6" s="2" t="e">
-        <f>TissueComp!K6*INDEX(VolumeFlow!$A4:$B16,MATCH('Average Properties Calc'!$A6,VolumeFlow!$A4:$A16,0),4)</f>
+        <f>TissueComp!K6*INDEX(VolumeFlow!$A4:$B17,MATCH('Average Properties Calc'!$A6,VolumeFlow!$A4:$A17,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J6" s="2" t="e">
-        <f>TissueComp!L6*INDEX(VolumeFlow!$A4:$B16,MATCH('Average Properties Calc'!$A6,VolumeFlow!$A4:$A16,0),4)</f>
+        <f>TissueComp!L6*INDEX(VolumeFlow!$A4:$B17,MATCH('Average Properties Calc'!$A6,VolumeFlow!$A4:$A17,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K6" t="s">
@@ -3501,39 +3501,39 @@
         <v>Heart</v>
       </c>
       <c r="B7" s="2" t="e">
-        <f>TissueComp!D7*INDEX(VolumeFlow!$A5:$B17,MATCH('Average Properties Calc'!$A7,VolumeFlow!$A5:$A17,0),4)</f>
+        <f>TissueComp!D7*INDEX(VolumeFlow!$A5:$B18,MATCH('Average Properties Calc'!$A7,VolumeFlow!$A5:$A18,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C7" s="2" t="e">
-        <f>TissueComp!E7*INDEX(VolumeFlow!$A5:$B17,MATCH('Average Properties Calc'!$A7,VolumeFlow!$A5:$A17,0),4)</f>
+        <f>TissueComp!E7*INDEX(VolumeFlow!$A5:$B18,MATCH('Average Properties Calc'!$A7,VolumeFlow!$A5:$A18,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D7" s="2" t="e">
-        <f>TissueComp!F7*INDEX(VolumeFlow!$A5:$B17,MATCH('Average Properties Calc'!$A7,VolumeFlow!$A5:$A17,0),4)</f>
+        <f>TissueComp!F7*INDEX(VolumeFlow!$A5:$B18,MATCH('Average Properties Calc'!$A7,VolumeFlow!$A5:$A18,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E7" s="2" t="e">
-        <f>TissueComp!G7*INDEX(VolumeFlow!$A5:$B17,MATCH('Average Properties Calc'!$A7,VolumeFlow!$A5:$A17,0),4)</f>
+        <f>TissueComp!G7*INDEX(VolumeFlow!$A5:$B18,MATCH('Average Properties Calc'!$A7,VolumeFlow!$A5:$A18,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F7" s="2" t="e">
-        <f>TissueComp!H7*INDEX(VolumeFlow!$A5:$B17,MATCH('Average Properties Calc'!$A7,VolumeFlow!$A5:$A17,0),4)</f>
+        <f>TissueComp!H7*INDEX(VolumeFlow!$A5:$B18,MATCH('Average Properties Calc'!$A7,VolumeFlow!$A5:$A18,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G7" s="2" t="e">
-        <f>TissueComp!I7*INDEX(VolumeFlow!$A5:$B17,MATCH('Average Properties Calc'!$A7,VolumeFlow!$A5:$A17,0),4)</f>
+        <f>TissueComp!I7*INDEX(VolumeFlow!$A5:$B18,MATCH('Average Properties Calc'!$A7,VolumeFlow!$A5:$A18,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H7" s="2" t="e">
-        <f>TissueComp!J7*INDEX(VolumeFlow!$A5:$B17,MATCH('Average Properties Calc'!$A7,VolumeFlow!$A5:$A17,0),4)</f>
+        <f>TissueComp!J7*INDEX(VolumeFlow!$A5:$B18,MATCH('Average Properties Calc'!$A7,VolumeFlow!$A5:$A18,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I7" s="2" t="e">
-        <f>TissueComp!K7*INDEX(VolumeFlow!$A5:$B17,MATCH('Average Properties Calc'!$A7,VolumeFlow!$A5:$A17,0),4)</f>
+        <f>TissueComp!K7*INDEX(VolumeFlow!$A5:$B18,MATCH('Average Properties Calc'!$A7,VolumeFlow!$A5:$A18,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J7" s="2" t="e">
-        <f>TissueComp!L7*INDEX(VolumeFlow!$A5:$B17,MATCH('Average Properties Calc'!$A7,VolumeFlow!$A5:$A17,0),4)</f>
+        <f>TissueComp!L7*INDEX(VolumeFlow!$A5:$B18,MATCH('Average Properties Calc'!$A7,VolumeFlow!$A5:$A18,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K7" t="s">
@@ -3546,39 +3546,39 @@
         <v>Kidney</v>
       </c>
       <c r="B8" s="2" t="e">
-        <f>TissueComp!D8*INDEX(VolumeFlow!$A6:$B18,MATCH('Average Properties Calc'!$A8,VolumeFlow!$A6:$A18,0),4)</f>
+        <f>TissueComp!D8*INDEX(VolumeFlow!$A6:$B19,MATCH('Average Properties Calc'!$A8,VolumeFlow!$A6:$A19,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C8" s="2" t="e">
-        <f>TissueComp!E8*INDEX(VolumeFlow!$A6:$B18,MATCH('Average Properties Calc'!$A8,VolumeFlow!$A6:$A18,0),4)</f>
+        <f>TissueComp!E8*INDEX(VolumeFlow!$A6:$B19,MATCH('Average Properties Calc'!$A8,VolumeFlow!$A6:$A19,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D8" s="2" t="e">
-        <f>TissueComp!F8*INDEX(VolumeFlow!$A6:$B18,MATCH('Average Properties Calc'!$A8,VolumeFlow!$A6:$A18,0),4)</f>
+        <f>TissueComp!F8*INDEX(VolumeFlow!$A6:$B19,MATCH('Average Properties Calc'!$A8,VolumeFlow!$A6:$A19,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E8" s="2" t="e">
-        <f>TissueComp!G8*INDEX(VolumeFlow!$A6:$B18,MATCH('Average Properties Calc'!$A8,VolumeFlow!$A6:$A18,0),4)</f>
+        <f>TissueComp!G8*INDEX(VolumeFlow!$A6:$B19,MATCH('Average Properties Calc'!$A8,VolumeFlow!$A6:$A19,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F8" s="2" t="e">
-        <f>TissueComp!H8*INDEX(VolumeFlow!$A6:$B18,MATCH('Average Properties Calc'!$A8,VolumeFlow!$A6:$A18,0),4)</f>
+        <f>TissueComp!H8*INDEX(VolumeFlow!$A6:$B19,MATCH('Average Properties Calc'!$A8,VolumeFlow!$A6:$A19,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G8" s="2" t="e">
-        <f>TissueComp!I8*INDEX(VolumeFlow!$A6:$B18,MATCH('Average Properties Calc'!$A8,VolumeFlow!$A6:$A18,0),4)</f>
+        <f>TissueComp!I8*INDEX(VolumeFlow!$A6:$B19,MATCH('Average Properties Calc'!$A8,VolumeFlow!$A6:$A19,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H8" s="2" t="e">
-        <f>TissueComp!J8*INDEX(VolumeFlow!$A6:$B18,MATCH('Average Properties Calc'!$A8,VolumeFlow!$A6:$A18,0),4)</f>
+        <f>TissueComp!J8*INDEX(VolumeFlow!$A6:$B19,MATCH('Average Properties Calc'!$A8,VolumeFlow!$A6:$A19,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I8" s="2" t="e">
-        <f>TissueComp!K8*INDEX(VolumeFlow!$A6:$B18,MATCH('Average Properties Calc'!$A8,VolumeFlow!$A6:$A18,0),4)</f>
+        <f>TissueComp!K8*INDEX(VolumeFlow!$A6:$B19,MATCH('Average Properties Calc'!$A8,VolumeFlow!$A6:$A19,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J8" s="2" t="e">
-        <f>TissueComp!L8*INDEX(VolumeFlow!$A6:$B18,MATCH('Average Properties Calc'!$A8,VolumeFlow!$A6:$A18,0),4)</f>
+        <f>TissueComp!L8*INDEX(VolumeFlow!$A6:$B19,MATCH('Average Properties Calc'!$A8,VolumeFlow!$A6:$A19,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K8" t="s">
@@ -3591,39 +3591,39 @@
         <v>Liver</v>
       </c>
       <c r="B9" s="2" t="e">
-        <f>TissueComp!D9*INDEX(VolumeFlow!$A7:$B19,MATCH('Average Properties Calc'!$A9,VolumeFlow!$A7:$A19,0),4)</f>
+        <f>TissueComp!D9*INDEX(VolumeFlow!$A7:$B20,MATCH('Average Properties Calc'!$A9,VolumeFlow!$A7:$A20,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C9" s="2" t="e">
-        <f>TissueComp!E9*INDEX(VolumeFlow!$A7:$B19,MATCH('Average Properties Calc'!$A9,VolumeFlow!$A7:$A19,0),4)</f>
+        <f>TissueComp!E9*INDEX(VolumeFlow!$A7:$B20,MATCH('Average Properties Calc'!$A9,VolumeFlow!$A7:$A20,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D9" s="2" t="e">
-        <f>TissueComp!F9*INDEX(VolumeFlow!$A7:$B19,MATCH('Average Properties Calc'!$A9,VolumeFlow!$A7:$A19,0),4)</f>
+        <f>TissueComp!F9*INDEX(VolumeFlow!$A7:$B20,MATCH('Average Properties Calc'!$A9,VolumeFlow!$A7:$A20,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E9" s="2" t="e">
-        <f>TissueComp!G9*INDEX(VolumeFlow!$A7:$B19,MATCH('Average Properties Calc'!$A9,VolumeFlow!$A7:$A19,0),4)</f>
+        <f>TissueComp!G9*INDEX(VolumeFlow!$A7:$B20,MATCH('Average Properties Calc'!$A9,VolumeFlow!$A7:$A20,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F9" s="2" t="e">
-        <f>TissueComp!H9*INDEX(VolumeFlow!$A7:$B19,MATCH('Average Properties Calc'!$A9,VolumeFlow!$A7:$A19,0),4)</f>
+        <f>TissueComp!H9*INDEX(VolumeFlow!$A7:$B20,MATCH('Average Properties Calc'!$A9,VolumeFlow!$A7:$A20,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G9" s="2" t="e">
-        <f>TissueComp!I9*INDEX(VolumeFlow!$A7:$B19,MATCH('Average Properties Calc'!$A9,VolumeFlow!$A7:$A19,0),4)</f>
+        <f>TissueComp!I9*INDEX(VolumeFlow!$A7:$B20,MATCH('Average Properties Calc'!$A9,VolumeFlow!$A7:$A20,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H9" s="2" t="e">
-        <f>TissueComp!J9*INDEX(VolumeFlow!$A7:$B19,MATCH('Average Properties Calc'!$A9,VolumeFlow!$A7:$A19,0),4)</f>
+        <f>TissueComp!J9*INDEX(VolumeFlow!$A7:$B20,MATCH('Average Properties Calc'!$A9,VolumeFlow!$A7:$A20,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I9" s="2" t="e">
-        <f>TissueComp!K9*INDEX(VolumeFlow!$A7:$B19,MATCH('Average Properties Calc'!$A9,VolumeFlow!$A7:$A19,0),4)</f>
+        <f>TissueComp!K9*INDEX(VolumeFlow!$A7:$B20,MATCH('Average Properties Calc'!$A9,VolumeFlow!$A7:$A20,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J9" s="2" t="e">
-        <f>TissueComp!L9*INDEX(VolumeFlow!$A7:$B19,MATCH('Average Properties Calc'!$A9,VolumeFlow!$A7:$A19,0),4)</f>
+        <f>TissueComp!L9*INDEX(VolumeFlow!$A7:$B20,MATCH('Average Properties Calc'!$A9,VolumeFlow!$A7:$A20,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K9" t="s">
@@ -3636,39 +3636,39 @@
         <v>Lung</v>
       </c>
       <c r="B10" s="2" t="e">
-        <f>TissueComp!D10*INDEX(VolumeFlow!$A8:$B20,MATCH('Average Properties Calc'!$A10,VolumeFlow!$A8:$A20,0),4)</f>
+        <f>TissueComp!D10*INDEX(VolumeFlow!$A8:$B21,MATCH('Average Properties Calc'!$A10,VolumeFlow!$A8:$A21,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C10" s="2" t="e">
-        <f>TissueComp!E10*INDEX(VolumeFlow!$A8:$B20,MATCH('Average Properties Calc'!$A10,VolumeFlow!$A8:$A20,0),4)</f>
+        <f>TissueComp!E10*INDEX(VolumeFlow!$A8:$B21,MATCH('Average Properties Calc'!$A10,VolumeFlow!$A8:$A21,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D10" s="2" t="e">
-        <f>TissueComp!F10*INDEX(VolumeFlow!$A8:$B20,MATCH('Average Properties Calc'!$A10,VolumeFlow!$A8:$A20,0),4)</f>
+        <f>TissueComp!F10*INDEX(VolumeFlow!$A8:$B21,MATCH('Average Properties Calc'!$A10,VolumeFlow!$A8:$A21,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E10" s="2" t="e">
-        <f>TissueComp!G10*INDEX(VolumeFlow!$A8:$B20,MATCH('Average Properties Calc'!$A10,VolumeFlow!$A8:$A20,0),4)</f>
+        <f>TissueComp!G10*INDEX(VolumeFlow!$A8:$B21,MATCH('Average Properties Calc'!$A10,VolumeFlow!$A8:$A21,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F10" s="2" t="e">
-        <f>TissueComp!H10*INDEX(VolumeFlow!$A8:$B20,MATCH('Average Properties Calc'!$A10,VolumeFlow!$A8:$A20,0),4)</f>
+        <f>TissueComp!H10*INDEX(VolumeFlow!$A8:$B21,MATCH('Average Properties Calc'!$A10,VolumeFlow!$A8:$A21,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G10" s="2" t="e">
-        <f>TissueComp!I10*INDEX(VolumeFlow!$A8:$B20,MATCH('Average Properties Calc'!$A10,VolumeFlow!$A8:$A20,0),4)</f>
+        <f>TissueComp!I10*INDEX(VolumeFlow!$A8:$B21,MATCH('Average Properties Calc'!$A10,VolumeFlow!$A8:$A21,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H10" s="2" t="e">
-        <f>TissueComp!J10*INDEX(VolumeFlow!$A8:$B20,MATCH('Average Properties Calc'!$A10,VolumeFlow!$A8:$A20,0),4)</f>
+        <f>TissueComp!J10*INDEX(VolumeFlow!$A8:$B21,MATCH('Average Properties Calc'!$A10,VolumeFlow!$A8:$A21,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I10" s="2" t="e">
-        <f>TissueComp!K10*INDEX(VolumeFlow!$A8:$B20,MATCH('Average Properties Calc'!$A10,VolumeFlow!$A8:$A20,0),4)</f>
+        <f>TissueComp!K10*INDEX(VolumeFlow!$A8:$B21,MATCH('Average Properties Calc'!$A10,VolumeFlow!$A8:$A21,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J10" s="2" t="e">
-        <f>TissueComp!L10*INDEX(VolumeFlow!$A8:$B20,MATCH('Average Properties Calc'!$A10,VolumeFlow!$A8:$A20,0),4)</f>
+        <f>TissueComp!L10*INDEX(VolumeFlow!$A8:$B21,MATCH('Average Properties Calc'!$A10,VolumeFlow!$A8:$A21,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K10" t="s">
@@ -3681,39 +3681,39 @@
         <v>Muscle</v>
       </c>
       <c r="B11" s="2" t="e">
-        <f>TissueComp!D11*INDEX(VolumeFlow!$A9:$B21,MATCH('Average Properties Calc'!$A11,VolumeFlow!$A9:$A21,0),4)</f>
+        <f>TissueComp!D11*INDEX(VolumeFlow!$A9:$B22,MATCH('Average Properties Calc'!$A11,VolumeFlow!$A9:$A22,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C11" s="2" t="e">
-        <f>TissueComp!E11*INDEX(VolumeFlow!$A9:$B21,MATCH('Average Properties Calc'!$A11,VolumeFlow!$A9:$A21,0),4)</f>
+        <f>TissueComp!E11*INDEX(VolumeFlow!$A9:$B22,MATCH('Average Properties Calc'!$A11,VolumeFlow!$A9:$A22,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D11" s="2" t="e">
-        <f>TissueComp!F11*INDEX(VolumeFlow!$A9:$B21,MATCH('Average Properties Calc'!$A11,VolumeFlow!$A9:$A21,0),4)</f>
+        <f>TissueComp!F11*INDEX(VolumeFlow!$A9:$B22,MATCH('Average Properties Calc'!$A11,VolumeFlow!$A9:$A22,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E11" s="2" t="e">
-        <f>TissueComp!G11*INDEX(VolumeFlow!$A9:$B21,MATCH('Average Properties Calc'!$A11,VolumeFlow!$A9:$A21,0),4)</f>
+        <f>TissueComp!G11*INDEX(VolumeFlow!$A9:$B22,MATCH('Average Properties Calc'!$A11,VolumeFlow!$A9:$A22,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F11" s="2" t="e">
-        <f>TissueComp!H11*INDEX(VolumeFlow!$A9:$B21,MATCH('Average Properties Calc'!$A11,VolumeFlow!$A9:$A21,0),4)</f>
+        <f>TissueComp!H11*INDEX(VolumeFlow!$A9:$B22,MATCH('Average Properties Calc'!$A11,VolumeFlow!$A9:$A22,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G11" s="2" t="e">
-        <f>TissueComp!I11*INDEX(VolumeFlow!$A9:$B21,MATCH('Average Properties Calc'!$A11,VolumeFlow!$A9:$A21,0),4)</f>
+        <f>TissueComp!I11*INDEX(VolumeFlow!$A9:$B22,MATCH('Average Properties Calc'!$A11,VolumeFlow!$A9:$A22,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H11" s="2" t="e">
-        <f>TissueComp!J11*INDEX(VolumeFlow!$A9:$B21,MATCH('Average Properties Calc'!$A11,VolumeFlow!$A9:$A21,0),4)</f>
+        <f>TissueComp!J11*INDEX(VolumeFlow!$A9:$B22,MATCH('Average Properties Calc'!$A11,VolumeFlow!$A9:$A22,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I11" s="2" t="e">
-        <f>TissueComp!K11*INDEX(VolumeFlow!$A9:$B21,MATCH('Average Properties Calc'!$A11,VolumeFlow!$A9:$A21,0),4)</f>
+        <f>TissueComp!K11*INDEX(VolumeFlow!$A9:$B22,MATCH('Average Properties Calc'!$A11,VolumeFlow!$A9:$A22,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J11" s="2" t="e">
-        <f>TissueComp!L11*INDEX(VolumeFlow!$A9:$B21,MATCH('Average Properties Calc'!$A11,VolumeFlow!$A9:$A21,0),4)</f>
+        <f>TissueComp!L11*INDEX(VolumeFlow!$A9:$B22,MATCH('Average Properties Calc'!$A11,VolumeFlow!$A9:$A22,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K11" t="s">
@@ -3726,39 +3726,39 @@
         <v>Skin</v>
       </c>
       <c r="B12" s="2" t="e">
-        <f>TissueComp!D12*INDEX(VolumeFlow!$A10:$B22,MATCH('Average Properties Calc'!$A12,VolumeFlow!$A10:$A22,0),4)</f>
+        <f>TissueComp!D12*INDEX(VolumeFlow!$A10:$B23,MATCH('Average Properties Calc'!$A12,VolumeFlow!$A10:$A23,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C12" s="2" t="e">
-        <f>TissueComp!E12*INDEX(VolumeFlow!$A10:$B22,MATCH('Average Properties Calc'!$A12,VolumeFlow!$A10:$A22,0),4)</f>
+        <f>TissueComp!E12*INDEX(VolumeFlow!$A10:$B23,MATCH('Average Properties Calc'!$A12,VolumeFlow!$A10:$A23,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D12" s="2" t="e">
-        <f>TissueComp!F12*INDEX(VolumeFlow!$A10:$B22,MATCH('Average Properties Calc'!$A12,VolumeFlow!$A10:$A22,0),4)</f>
+        <f>TissueComp!F12*INDEX(VolumeFlow!$A10:$B23,MATCH('Average Properties Calc'!$A12,VolumeFlow!$A10:$A23,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E12" s="2" t="e">
-        <f>TissueComp!G12*INDEX(VolumeFlow!$A10:$B22,MATCH('Average Properties Calc'!$A12,VolumeFlow!$A10:$A22,0),4)</f>
+        <f>TissueComp!G12*INDEX(VolumeFlow!$A10:$B23,MATCH('Average Properties Calc'!$A12,VolumeFlow!$A10:$A23,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F12" s="2" t="e">
-        <f>TissueComp!H12*INDEX(VolumeFlow!$A10:$B22,MATCH('Average Properties Calc'!$A12,VolumeFlow!$A10:$A22,0),4)</f>
+        <f>TissueComp!H12*INDEX(VolumeFlow!$A10:$B23,MATCH('Average Properties Calc'!$A12,VolumeFlow!$A10:$A23,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G12" s="2" t="e">
-        <f>TissueComp!I12*INDEX(VolumeFlow!$A10:$B22,MATCH('Average Properties Calc'!$A12,VolumeFlow!$A10:$A22,0),4)</f>
+        <f>TissueComp!I12*INDEX(VolumeFlow!$A10:$B23,MATCH('Average Properties Calc'!$A12,VolumeFlow!$A10:$A23,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H12" s="2" t="e">
-        <f>TissueComp!J12*INDEX(VolumeFlow!$A10:$B22,MATCH('Average Properties Calc'!$A12,VolumeFlow!$A10:$A22,0),4)</f>
+        <f>TissueComp!J12*INDEX(VolumeFlow!$A10:$B23,MATCH('Average Properties Calc'!$A12,VolumeFlow!$A10:$A23,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I12" s="2" t="e">
-        <f>TissueComp!K12*INDEX(VolumeFlow!$A10:$B22,MATCH('Average Properties Calc'!$A12,VolumeFlow!$A10:$A22,0),4)</f>
+        <f>TissueComp!K12*INDEX(VolumeFlow!$A10:$B23,MATCH('Average Properties Calc'!$A12,VolumeFlow!$A10:$A23,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J12" s="2" t="e">
-        <f>TissueComp!L12*INDEX(VolumeFlow!$A10:$B22,MATCH('Average Properties Calc'!$A12,VolumeFlow!$A10:$A22,0),4)</f>
+        <f>TissueComp!L12*INDEX(VolumeFlow!$A10:$B23,MATCH('Average Properties Calc'!$A12,VolumeFlow!$A10:$A23,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K12" t="s">
@@ -3771,39 +3771,39 @@
         <v>Spleen</v>
       </c>
       <c r="B13" s="2" t="e">
-        <f>TissueComp!D13*INDEX(VolumeFlow!$A11:$B23,MATCH('Average Properties Calc'!$A13,VolumeFlow!$A11:$A23,0),4)</f>
+        <f>TissueComp!D13*INDEX(VolumeFlow!$A11:$B24,MATCH('Average Properties Calc'!$A13,VolumeFlow!$A11:$A24,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C13" s="2" t="e">
-        <f>TissueComp!E13*INDEX(VolumeFlow!$A11:$B23,MATCH('Average Properties Calc'!$A13,VolumeFlow!$A11:$A23,0),4)</f>
+        <f>TissueComp!E13*INDEX(VolumeFlow!$A11:$B24,MATCH('Average Properties Calc'!$A13,VolumeFlow!$A11:$A24,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D13" s="2" t="e">
-        <f>TissueComp!F13*INDEX(VolumeFlow!$A11:$B23,MATCH('Average Properties Calc'!$A13,VolumeFlow!$A11:$A23,0),4)</f>
+        <f>TissueComp!F13*INDEX(VolumeFlow!$A11:$B24,MATCH('Average Properties Calc'!$A13,VolumeFlow!$A11:$A24,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E13" s="2" t="e">
-        <f>TissueComp!G13*INDEX(VolumeFlow!$A11:$B23,MATCH('Average Properties Calc'!$A13,VolumeFlow!$A11:$A23,0),4)</f>
+        <f>TissueComp!G13*INDEX(VolumeFlow!$A11:$B24,MATCH('Average Properties Calc'!$A13,VolumeFlow!$A11:$A24,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F13" s="2" t="e">
-        <f>TissueComp!H13*INDEX(VolumeFlow!$A11:$B23,MATCH('Average Properties Calc'!$A13,VolumeFlow!$A11:$A23,0),4)</f>
+        <f>TissueComp!H13*INDEX(VolumeFlow!$A11:$B24,MATCH('Average Properties Calc'!$A13,VolumeFlow!$A11:$A24,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G13" s="2" t="e">
-        <f>TissueComp!I13*INDEX(VolumeFlow!$A11:$B23,MATCH('Average Properties Calc'!$A13,VolumeFlow!$A11:$A23,0),4)</f>
+        <f>TissueComp!I13*INDEX(VolumeFlow!$A11:$B24,MATCH('Average Properties Calc'!$A13,VolumeFlow!$A11:$A24,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H13" s="2" t="e">
-        <f>TissueComp!J13*INDEX(VolumeFlow!$A11:$B23,MATCH('Average Properties Calc'!$A13,VolumeFlow!$A11:$A23,0),4)</f>
+        <f>TissueComp!J13*INDEX(VolumeFlow!$A11:$B24,MATCH('Average Properties Calc'!$A13,VolumeFlow!$A11:$A24,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I13" s="2" t="e">
-        <f>TissueComp!K13*INDEX(VolumeFlow!$A11:$B23,MATCH('Average Properties Calc'!$A13,VolumeFlow!$A11:$A23,0),4)</f>
+        <f>TissueComp!K13*INDEX(VolumeFlow!$A11:$B24,MATCH('Average Properties Calc'!$A13,VolumeFlow!$A11:$A24,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J13" s="2" t="e">
-        <f>TissueComp!L13*INDEX(VolumeFlow!$A11:$B23,MATCH('Average Properties Calc'!$A13,VolumeFlow!$A11:$A23,0),4)</f>
+        <f>TissueComp!L13*INDEX(VolumeFlow!$A11:$B24,MATCH('Average Properties Calc'!$A13,VolumeFlow!$A11:$A24,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K13" t="s">
@@ -3854,39 +3854,39 @@
         <v>Adipose</v>
       </c>
       <c r="B15" s="2" t="e">
-        <f>TissueComp!D17*INDEX(VolumeFlow!$A13:$B25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!D17*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A14:$A26,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C15" s="2" t="e">
-        <f>TissueComp!E17*INDEX(VolumeFlow!$A13:$B25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!E17*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A14:$A26,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D15" s="2" t="e">
-        <f>TissueComp!F17*INDEX(VolumeFlow!$A13:$B25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!F17*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A14:$A26,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E15" s="2" t="e">
-        <f>TissueComp!G17*INDEX(VolumeFlow!$A13:$B25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!G17*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A14:$A26,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F15" s="2" t="e">
-        <f>TissueComp!H17*INDEX(VolumeFlow!$A13:$B25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!H17*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A14:$A26,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G15" s="2" t="e">
-        <f>TissueComp!I17*INDEX(VolumeFlow!$A13:$B25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!I17*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A14:$A26,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H15" s="2" t="e">
-        <f>TissueComp!J17*INDEX(VolumeFlow!$A13:$B25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!J17*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A14:$A26,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I15" s="2" t="e">
-        <f>TissueComp!K17*INDEX(VolumeFlow!$A13:$B25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!K17*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A14:$A26,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J15" s="2" t="e">
-        <f>TissueComp!L17*INDEX(VolumeFlow!$A13:$B25,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A13:$A25,0),4)</f>
+        <f>TissueComp!L17*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A15,VolumeFlow!$A14:$A26,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K15" t="s">
@@ -3899,39 +3899,39 @@
         <v>Bone</v>
       </c>
       <c r="B16" s="2" t="e">
-        <f>TissueComp!D18*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!D18*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A15:$A27,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C16" s="2" t="e">
-        <f>TissueComp!E18*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!E18*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A15:$A27,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D16" s="2" t="e">
-        <f>TissueComp!F18*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!F18*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A15:$A27,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E16" s="2" t="e">
-        <f>TissueComp!G18*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!G18*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A15:$A27,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F16" s="2" t="e">
-        <f>TissueComp!H18*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!H18*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A15:$A27,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G16" s="2" t="e">
-        <f>TissueComp!I18*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!I18*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A15:$A27,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H16" s="2" t="e">
-        <f>TissueComp!J18*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!J18*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A15:$A27,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I16" s="2" t="e">
-        <f>TissueComp!K18*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!K18*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A15:$A27,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J16" s="2" t="e">
-        <f>TissueComp!L18*INDEX(VolumeFlow!$A14:$B26,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A14:$A26,0),4)</f>
+        <f>TissueComp!L18*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A16,VolumeFlow!$A15:$A27,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K16" t="s">
@@ -3944,39 +3944,39 @@
         <v>Brain</v>
       </c>
       <c r="B17" s="2" t="e">
-        <f>TissueComp!D19*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!D19*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A16:$A28,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C17" s="2" t="e">
-        <f>TissueComp!E19*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!E19*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A16:$A28,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D17" s="2" t="e">
-        <f>TissueComp!F19*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!F19*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A16:$A28,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E17" s="2" t="e">
-        <f>TissueComp!G19*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!G19*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A16:$A28,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F17" s="2" t="e">
-        <f>TissueComp!H19*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!H19*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A16:$A28,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G17" s="2" t="e">
-        <f>TissueComp!I19*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!I19*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A16:$A28,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H17" s="2" t="e">
-        <f>TissueComp!J19*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!J19*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A16:$A28,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I17" s="2" t="e">
-        <f>TissueComp!K19*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!K19*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A16:$A28,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J17" s="2" t="e">
-        <f>TissueComp!L19*INDEX(VolumeFlow!$A15:$B27,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A15:$A27,0),4)</f>
+        <f>TissueComp!L19*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A17,VolumeFlow!$A16:$A28,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K17" t="s">
@@ -3989,39 +3989,39 @@
         <v>Gut</v>
       </c>
       <c r="B18" s="2" t="e">
-        <f>TissueComp!D20*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!D20*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A17:$A29,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C18" s="2" t="e">
-        <f>TissueComp!E20*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!E20*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A17:$A29,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D18" s="2" t="e">
-        <f>TissueComp!F20*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!F20*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A17:$A29,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E18" s="2" t="e">
-        <f>TissueComp!G20*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!G20*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A17:$A29,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F18" s="2" t="e">
-        <f>TissueComp!H20*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!H20*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A17:$A29,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G18" s="2" t="e">
-        <f>TissueComp!I20*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!I20*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A17:$A29,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H18" s="2" t="e">
-        <f>TissueComp!J20*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!J20*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A17:$A29,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I18" s="2" t="e">
-        <f>TissueComp!K20*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!K20*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A17:$A29,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J18" s="2" t="e">
-        <f>TissueComp!L20*INDEX(VolumeFlow!$A16:$B28,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A16:$A28,0),4)</f>
+        <f>TissueComp!L20*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A18,VolumeFlow!$A17:$A29,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K18" t="s">
@@ -4034,39 +4034,39 @@
         <v>Heart</v>
       </c>
       <c r="B19" s="2" t="e">
-        <f>TissueComp!D21*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!D21*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A18:$A30,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C19" s="2" t="e">
-        <f>TissueComp!E21*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!E21*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A18:$A30,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D19" s="2" t="e">
-        <f>TissueComp!F21*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!F21*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A18:$A30,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E19" s="2" t="e">
-        <f>TissueComp!G21*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!G21*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A18:$A30,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F19" s="2" t="e">
-        <f>TissueComp!H21*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!H21*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A18:$A30,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G19" s="2" t="e">
-        <f>TissueComp!I21*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!I21*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A18:$A30,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H19" s="2" t="e">
-        <f>TissueComp!J21*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!J21*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A18:$A30,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I19" s="2" t="e">
-        <f>TissueComp!K21*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!K21*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A18:$A30,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J19" s="2" t="e">
-        <f>TissueComp!L21*INDEX(VolumeFlow!$A17:$B29,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A17:$A29,0),4)</f>
+        <f>TissueComp!L21*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A19,VolumeFlow!$A18:$A30,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K19" t="s">
@@ -4079,39 +4079,39 @@
         <v>Kidney</v>
       </c>
       <c r="B20" s="2" t="e">
-        <f>TissueComp!D22*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!D22*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A19:$A31,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C20" s="2" t="e">
-        <f>TissueComp!E22*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!E22*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A19:$A31,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D20" s="2" t="e">
-        <f>TissueComp!F22*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!F22*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A19:$A31,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E20" s="2" t="e">
-        <f>TissueComp!G22*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!G22*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A19:$A31,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F20" s="2" t="e">
-        <f>TissueComp!H22*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!H22*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A19:$A31,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G20" s="2" t="e">
-        <f>TissueComp!I22*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!I22*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A19:$A31,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H20" s="2" t="e">
-        <f>TissueComp!J22*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!J22*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A19:$A31,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I20" s="2" t="e">
-        <f>TissueComp!K22*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!K22*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A19:$A31,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J20" s="2" t="e">
-        <f>TissueComp!L22*INDEX(VolumeFlow!$A18:$B30,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A18:$A30,0),4)</f>
+        <f>TissueComp!L22*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A20,VolumeFlow!$A19:$A31,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K20" t="s">
@@ -4124,39 +4124,39 @@
         <v>Liver</v>
       </c>
       <c r="B21" s="2" t="e">
-        <f>TissueComp!D23*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!D23*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A20:$A32,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C21" s="2" t="e">
-        <f>TissueComp!E23*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!E23*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A20:$A32,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D21" s="2" t="e">
-        <f>TissueComp!F23*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!F23*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A20:$A32,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E21" s="2" t="e">
-        <f>TissueComp!G23*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!G23*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A20:$A32,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F21" s="2" t="e">
-        <f>TissueComp!H23*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!H23*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A20:$A32,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G21" s="2" t="e">
-        <f>TissueComp!I23*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!I23*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A20:$A32,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H21" s="2" t="e">
-        <f>TissueComp!J23*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!J23*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A20:$A32,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I21" s="2" t="e">
-        <f>TissueComp!K23*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!K23*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A20:$A32,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J21" s="2" t="e">
-        <f>TissueComp!L23*INDEX(VolumeFlow!$A19:$B31,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A19:$A31,0),4)</f>
+        <f>TissueComp!L23*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A21,VolumeFlow!$A20:$A32,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K21" t="s">
@@ -4169,39 +4169,39 @@
         <v>Lung</v>
       </c>
       <c r="B22" s="2" t="e">
-        <f>TissueComp!D24*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!D24*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A21:$A33,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C22" s="2" t="e">
-        <f>TissueComp!E24*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!E24*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A21:$A33,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D22" s="2" t="e">
-        <f>TissueComp!F24*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!F24*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A21:$A33,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E22" s="2" t="e">
-        <f>TissueComp!G24*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!G24*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A21:$A33,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F22" s="2" t="e">
-        <f>TissueComp!H24*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!H24*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A21:$A33,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G22" s="2" t="e">
-        <f>TissueComp!I24*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!I24*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A21:$A33,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H22" s="2" t="e">
-        <f>TissueComp!J24*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!J24*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A21:$A33,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I22" s="2" t="e">
-        <f>TissueComp!K24*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!K24*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A21:$A33,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J22" s="2" t="e">
-        <f>TissueComp!L24*INDEX(VolumeFlow!$A20:$B32,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A20:$A32,0),4)</f>
+        <f>TissueComp!L24*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A22,VolumeFlow!$A21:$A33,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K22" t="s">
@@ -4214,39 +4214,39 @@
         <v>Muscle</v>
       </c>
       <c r="B23" s="2" t="e">
-        <f>TissueComp!D25*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!D25*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A22:$A34,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C23" s="2" t="e">
-        <f>TissueComp!E25*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!E25*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A22:$A34,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D23" s="2" t="e">
-        <f>TissueComp!F25*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!F25*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A22:$A34,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E23" s="2" t="e">
-        <f>TissueComp!G25*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!G25*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A22:$A34,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F23" s="2" t="e">
-        <f>TissueComp!H25*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!H25*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A22:$A34,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G23" s="2" t="e">
-        <f>TissueComp!I25*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!I25*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A22:$A34,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H23" s="2" t="e">
-        <f>TissueComp!J25*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!J25*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A22:$A34,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I23" s="2" t="e">
-        <f>TissueComp!K25*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!K25*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A22:$A34,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J23" s="2" t="e">
-        <f>TissueComp!L25*INDEX(VolumeFlow!$A21:$B33,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A21:$A33,0),4)</f>
+        <f>TissueComp!L25*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A23,VolumeFlow!$A22:$A34,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K23" t="s">
@@ -4259,39 +4259,39 @@
         <v>Skin</v>
       </c>
       <c r="B24" s="2" t="e">
-        <f>TissueComp!D26*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!D26*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A23:$A35,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C24" s="2" t="e">
-        <f>TissueComp!E26*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!E26*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A23:$A35,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D24" s="2" t="e">
-        <f>TissueComp!F26*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!F26*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A23:$A35,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E24" s="2" t="e">
-        <f>TissueComp!G26*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!G26*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A23:$A35,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F24" s="2" t="e">
-        <f>TissueComp!H26*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!H26*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A23:$A35,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G24" s="2" t="e">
-        <f>TissueComp!I26*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!I26*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A23:$A35,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H24" s="2" t="e">
-        <f>TissueComp!J26*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!J26*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A23:$A35,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I24" s="2" t="e">
-        <f>TissueComp!K26*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!K26*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A23:$A35,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J24" s="2" t="e">
-        <f>TissueComp!L26*INDEX(VolumeFlow!$A22:$B34,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A22:$A34,0),4)</f>
+        <f>TissueComp!L26*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A24,VolumeFlow!$A23:$A35,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K24" t="s">
@@ -4304,39 +4304,39 @@
         <v>Spleen</v>
       </c>
       <c r="B25" s="2" t="e">
-        <f>TissueComp!D27*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!D27*INDEX(VolumeFlow!$A24:$B36,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A24:$A36,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C25" s="2" t="e">
-        <f>TissueComp!E27*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!E27*INDEX(VolumeFlow!$A24:$B36,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A24:$A36,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D25" s="2" t="e">
-        <f>TissueComp!F27*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!F27*INDEX(VolumeFlow!$A24:$B36,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A24:$A36,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E25" s="2" t="e">
-        <f>TissueComp!G27*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!G27*INDEX(VolumeFlow!$A24:$B36,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A24:$A36,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F25" s="2" t="e">
-        <f>TissueComp!H27*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!H27*INDEX(VolumeFlow!$A24:$B36,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A24:$A36,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G25" s="2" t="e">
-        <f>TissueComp!I27*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!I27*INDEX(VolumeFlow!$A24:$B36,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A24:$A36,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H25" s="2" t="e">
-        <f>TissueComp!J27*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!J27*INDEX(VolumeFlow!$A24:$B36,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A24:$A36,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I25" s="2" t="e">
-        <f>TissueComp!K27*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!K27*INDEX(VolumeFlow!$A24:$B36,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A24:$A36,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J25" s="2" t="e">
-        <f>TissueComp!L27*INDEX(VolumeFlow!$A23:$B35,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A23:$A35,0),4)</f>
+        <f>TissueComp!L27*INDEX(VolumeFlow!$A24:$B36,MATCH('Average Properties Calc'!$A25,VolumeFlow!$A24:$A36,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K25" t="s">
@@ -4387,39 +4387,39 @@
         <v>Adipose</v>
       </c>
       <c r="B27" s="2" t="e">
-        <f>TissueComp!D$3*INDEX(VolumeFlow!$A25:$B37,MATCH('Average Properties Calc'!$A27,VolumeFlow!$A25:$A37,0),4)</f>
+        <f>TissueComp!D$3*INDEX(VolumeFlow!$A26:$B38,MATCH('Average Properties Calc'!$A27,VolumeFlow!$A26:$A38,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C27" s="2" t="e">
-        <f>TissueComp!E$3*INDEX(VolumeFlow!$A25:$B37,MATCH('Average Properties Calc'!$A27,VolumeFlow!$A25:$A37,0),4)</f>
+        <f>TissueComp!E$3*INDEX(VolumeFlow!$A26:$B38,MATCH('Average Properties Calc'!$A27,VolumeFlow!$A26:$A38,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D27" s="2" t="e">
-        <f>TissueComp!F$3*INDEX(VolumeFlow!$A25:$B37,MATCH('Average Properties Calc'!$A27,VolumeFlow!$A25:$A37,0),4)</f>
+        <f>TissueComp!F$3*INDEX(VolumeFlow!$A26:$B38,MATCH('Average Properties Calc'!$A27,VolumeFlow!$A26:$A38,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E27" s="2" t="e">
-        <f>TissueComp!G$3*INDEX(VolumeFlow!$A25:$B37,MATCH('Average Properties Calc'!$A27,VolumeFlow!$A25:$A37,0),4)</f>
+        <f>TissueComp!G$3*INDEX(VolumeFlow!$A26:$B38,MATCH('Average Properties Calc'!$A27,VolumeFlow!$A26:$A38,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F27" s="2" t="e">
-        <f>TissueComp!H$3*INDEX(VolumeFlow!$A25:$B37,MATCH('Average Properties Calc'!$A27,VolumeFlow!$A25:$A37,0),4)</f>
+        <f>TissueComp!H$3*INDEX(VolumeFlow!$A26:$B38,MATCH('Average Properties Calc'!$A27,VolumeFlow!$A26:$A38,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G27" s="2" t="e">
-        <f>TissueComp!I$3*INDEX(VolumeFlow!$A25:$B37,MATCH('Average Properties Calc'!$A27,VolumeFlow!$A25:$A37,0),4)</f>
+        <f>TissueComp!I$3*INDEX(VolumeFlow!$A26:$B38,MATCH('Average Properties Calc'!$A27,VolumeFlow!$A26:$A38,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H27" s="2" t="e">
-        <f>TissueComp!J$3*INDEX(VolumeFlow!$A25:$B37,MATCH('Average Properties Calc'!$A27,VolumeFlow!$A25:$A37,0),4)</f>
+        <f>TissueComp!J$3*INDEX(VolumeFlow!$A26:$B38,MATCH('Average Properties Calc'!$A27,VolumeFlow!$A26:$A38,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I27" s="2" t="e">
-        <f>TissueComp!K$3*INDEX(VolumeFlow!$A25:$B37,MATCH('Average Properties Calc'!$A27,VolumeFlow!$A25:$A37,0),4)</f>
+        <f>TissueComp!K$3*INDEX(VolumeFlow!$A26:$B38,MATCH('Average Properties Calc'!$A27,VolumeFlow!$A26:$A38,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J27" s="2" t="e">
-        <f>TissueComp!L$3*INDEX(VolumeFlow!$A25:$B37,MATCH('Average Properties Calc'!$A27,VolumeFlow!$A25:$A37,0),4)</f>
+        <f>TissueComp!L$3*INDEX(VolumeFlow!$A26:$B38,MATCH('Average Properties Calc'!$A27,VolumeFlow!$A26:$A38,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K27" t="s">
@@ -4432,39 +4432,39 @@
         <v>Bone</v>
       </c>
       <c r="B28" s="2" t="e">
-        <f>TissueComp!D$4*INDEX(VolumeFlow!$A26:$B38,MATCH('Average Properties Calc'!$A28,VolumeFlow!$A26:$A38,0),4)</f>
+        <f>TissueComp!D$4*INDEX(VolumeFlow!$A27:$B39,MATCH('Average Properties Calc'!$A28,VolumeFlow!$A27:$A39,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C28" s="2" t="e">
-        <f>TissueComp!E$4*INDEX(VolumeFlow!$A26:$B38,MATCH('Average Properties Calc'!$A28,VolumeFlow!$A26:$A38,0),4)</f>
+        <f>TissueComp!E$4*INDEX(VolumeFlow!$A27:$B39,MATCH('Average Properties Calc'!$A28,VolumeFlow!$A27:$A39,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D28" s="2" t="e">
-        <f>TissueComp!F$4*INDEX(VolumeFlow!$A26:$B38,MATCH('Average Properties Calc'!$A28,VolumeFlow!$A26:$A38,0),4)</f>
+        <f>TissueComp!F$4*INDEX(VolumeFlow!$A27:$B39,MATCH('Average Properties Calc'!$A28,VolumeFlow!$A27:$A39,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E28" s="2" t="e">
-        <f>TissueComp!G$4*INDEX(VolumeFlow!$A26:$B38,MATCH('Average Properties Calc'!$A28,VolumeFlow!$A26:$A38,0),4)</f>
+        <f>TissueComp!G$4*INDEX(VolumeFlow!$A27:$B39,MATCH('Average Properties Calc'!$A28,VolumeFlow!$A27:$A39,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F28" s="2" t="e">
-        <f>TissueComp!H$4*INDEX(VolumeFlow!$A26:$B38,MATCH('Average Properties Calc'!$A28,VolumeFlow!$A26:$A38,0),4)</f>
+        <f>TissueComp!H$4*INDEX(VolumeFlow!$A27:$B39,MATCH('Average Properties Calc'!$A28,VolumeFlow!$A27:$A39,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G28" s="2" t="e">
-        <f>TissueComp!I$4*INDEX(VolumeFlow!$A26:$B38,MATCH('Average Properties Calc'!$A28,VolumeFlow!$A26:$A38,0),4)</f>
+        <f>TissueComp!I$4*INDEX(VolumeFlow!$A27:$B39,MATCH('Average Properties Calc'!$A28,VolumeFlow!$A27:$A39,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H28" s="2" t="e">
-        <f>TissueComp!J$4*INDEX(VolumeFlow!$A26:$B38,MATCH('Average Properties Calc'!$A28,VolumeFlow!$A26:$A38,0),4)</f>
+        <f>TissueComp!J$4*INDEX(VolumeFlow!$A27:$B39,MATCH('Average Properties Calc'!$A28,VolumeFlow!$A27:$A39,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I28" s="2" t="e">
-        <f>TissueComp!K$4*INDEX(VolumeFlow!$A26:$B38,MATCH('Average Properties Calc'!$A28,VolumeFlow!$A26:$A38,0),4)</f>
+        <f>TissueComp!K$4*INDEX(VolumeFlow!$A27:$B39,MATCH('Average Properties Calc'!$A28,VolumeFlow!$A27:$A39,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J28" s="2" t="e">
-        <f>TissueComp!L$4*INDEX(VolumeFlow!$A26:$B38,MATCH('Average Properties Calc'!$A28,VolumeFlow!$A26:$A38,0),4)</f>
+        <f>TissueComp!L$4*INDEX(VolumeFlow!$A27:$B39,MATCH('Average Properties Calc'!$A28,VolumeFlow!$A27:$A39,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K28" t="s">
@@ -4477,39 +4477,39 @@
         <v>Brain</v>
       </c>
       <c r="B29" s="2" t="e">
-        <f>TissueComp!D$5*INDEX(VolumeFlow!$A27:$B39,MATCH('Average Properties Calc'!$A29,VolumeFlow!$A27:$A39,0),4)</f>
+        <f>TissueComp!D$5*INDEX(VolumeFlow!$A28:$B40,MATCH('Average Properties Calc'!$A29,VolumeFlow!$A28:$A40,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C29" s="2" t="e">
-        <f>TissueComp!E$5*INDEX(VolumeFlow!$A27:$B39,MATCH('Average Properties Calc'!$A29,VolumeFlow!$A27:$A39,0),4)</f>
+        <f>TissueComp!E$5*INDEX(VolumeFlow!$A28:$B40,MATCH('Average Properties Calc'!$A29,VolumeFlow!$A28:$A40,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D29" s="2" t="e">
-        <f>TissueComp!F$5*INDEX(VolumeFlow!$A27:$B39,MATCH('Average Properties Calc'!$A29,VolumeFlow!$A27:$A39,0),4)</f>
+        <f>TissueComp!F$5*INDEX(VolumeFlow!$A28:$B40,MATCH('Average Properties Calc'!$A29,VolumeFlow!$A28:$A40,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E29" s="2" t="e">
-        <f>TissueComp!G$5*INDEX(VolumeFlow!$A27:$B39,MATCH('Average Properties Calc'!$A29,VolumeFlow!$A27:$A39,0),4)</f>
+        <f>TissueComp!G$5*INDEX(VolumeFlow!$A28:$B40,MATCH('Average Properties Calc'!$A29,VolumeFlow!$A28:$A40,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F29" s="2" t="e">
-        <f>TissueComp!H$5*INDEX(VolumeFlow!$A27:$B39,MATCH('Average Properties Calc'!$A29,VolumeFlow!$A27:$A39,0),4)</f>
+        <f>TissueComp!H$5*INDEX(VolumeFlow!$A28:$B40,MATCH('Average Properties Calc'!$A29,VolumeFlow!$A28:$A40,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G29" s="2" t="e">
-        <f>TissueComp!I$5*INDEX(VolumeFlow!$A27:$B39,MATCH('Average Properties Calc'!$A29,VolumeFlow!$A27:$A39,0),4)</f>
+        <f>TissueComp!I$5*INDEX(VolumeFlow!$A28:$B40,MATCH('Average Properties Calc'!$A29,VolumeFlow!$A28:$A40,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H29" s="2" t="e">
-        <f>TissueComp!J$5*INDEX(VolumeFlow!$A27:$B39,MATCH('Average Properties Calc'!$A29,VolumeFlow!$A27:$A39,0),4)</f>
+        <f>TissueComp!J$5*INDEX(VolumeFlow!$A28:$B40,MATCH('Average Properties Calc'!$A29,VolumeFlow!$A28:$A40,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I29" s="2" t="e">
-        <f>TissueComp!K$5*INDEX(VolumeFlow!$A27:$B39,MATCH('Average Properties Calc'!$A29,VolumeFlow!$A27:$A39,0),4)</f>
+        <f>TissueComp!K$5*INDEX(VolumeFlow!$A28:$B40,MATCH('Average Properties Calc'!$A29,VolumeFlow!$A28:$A40,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J29" s="2" t="e">
-        <f>TissueComp!L$5*INDEX(VolumeFlow!$A27:$B39,MATCH('Average Properties Calc'!$A29,VolumeFlow!$A27:$A39,0),4)</f>
+        <f>TissueComp!L$5*INDEX(VolumeFlow!$A28:$B40,MATCH('Average Properties Calc'!$A29,VolumeFlow!$A28:$A40,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K29" t="s">
@@ -4522,39 +4522,39 @@
         <v>Gut</v>
       </c>
       <c r="B30" s="2" t="e">
-        <f>TissueComp!D$6*INDEX(VolumeFlow!$A28:$B40,MATCH('Average Properties Calc'!$A30,VolumeFlow!$A28:$A40,0),4)</f>
+        <f>TissueComp!D$6*INDEX(VolumeFlow!$A29:$B41,MATCH('Average Properties Calc'!$A30,VolumeFlow!$A29:$A41,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C30" s="2" t="e">
-        <f>TissueComp!E$6*INDEX(VolumeFlow!$A28:$B40,MATCH('Average Properties Calc'!$A30,VolumeFlow!$A28:$A40,0),4)</f>
+        <f>TissueComp!E$6*INDEX(VolumeFlow!$A29:$B41,MATCH('Average Properties Calc'!$A30,VolumeFlow!$A29:$A41,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D30" s="2" t="e">
-        <f>TissueComp!F$6*INDEX(VolumeFlow!$A28:$B40,MATCH('Average Properties Calc'!$A30,VolumeFlow!$A28:$A40,0),4)</f>
+        <f>TissueComp!F$6*INDEX(VolumeFlow!$A29:$B41,MATCH('Average Properties Calc'!$A30,VolumeFlow!$A29:$A41,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E30" s="2" t="e">
-        <f>TissueComp!G$6*INDEX(VolumeFlow!$A28:$B40,MATCH('Average Properties Calc'!$A30,VolumeFlow!$A28:$A40,0),4)</f>
+        <f>TissueComp!G$6*INDEX(VolumeFlow!$A29:$B41,MATCH('Average Properties Calc'!$A30,VolumeFlow!$A29:$A41,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F30" s="2" t="e">
-        <f>TissueComp!H$6*INDEX(VolumeFlow!$A28:$B40,MATCH('Average Properties Calc'!$A30,VolumeFlow!$A28:$A40,0),4)</f>
+        <f>TissueComp!H$6*INDEX(VolumeFlow!$A29:$B41,MATCH('Average Properties Calc'!$A30,VolumeFlow!$A29:$A41,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G30" s="2" t="e">
-        <f>TissueComp!I$6*INDEX(VolumeFlow!$A28:$B40,MATCH('Average Properties Calc'!$A30,VolumeFlow!$A28:$A40,0),4)</f>
+        <f>TissueComp!I$6*INDEX(VolumeFlow!$A29:$B41,MATCH('Average Properties Calc'!$A30,VolumeFlow!$A29:$A41,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H30" s="2" t="e">
-        <f>TissueComp!J$6*INDEX(VolumeFlow!$A28:$B40,MATCH('Average Properties Calc'!$A30,VolumeFlow!$A28:$A40,0),4)</f>
+        <f>TissueComp!J$6*INDEX(VolumeFlow!$A29:$B41,MATCH('Average Properties Calc'!$A30,VolumeFlow!$A29:$A41,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I30" s="2" t="e">
-        <f>TissueComp!K$6*INDEX(VolumeFlow!$A28:$B40,MATCH('Average Properties Calc'!$A30,VolumeFlow!$A28:$A40,0),4)</f>
+        <f>TissueComp!K$6*INDEX(VolumeFlow!$A29:$B41,MATCH('Average Properties Calc'!$A30,VolumeFlow!$A29:$A41,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J30" s="2" t="e">
-        <f>TissueComp!L$6*INDEX(VolumeFlow!$A28:$B40,MATCH('Average Properties Calc'!$A30,VolumeFlow!$A28:$A40,0),4)</f>
+        <f>TissueComp!L$6*INDEX(VolumeFlow!$A29:$B41,MATCH('Average Properties Calc'!$A30,VolumeFlow!$A29:$A41,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K30" t="s">
@@ -4567,39 +4567,39 @@
         <v>Heart</v>
       </c>
       <c r="B31" s="2" t="e">
-        <f>TissueComp!D$7*INDEX(VolumeFlow!$A29:$B41,MATCH('Average Properties Calc'!$A31,VolumeFlow!$A29:$A41,0),4)</f>
+        <f>TissueComp!D$7*INDEX(VolumeFlow!$A30:$B42,MATCH('Average Properties Calc'!$A31,VolumeFlow!$A30:$A42,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C31" s="2" t="e">
-        <f>TissueComp!E$7*INDEX(VolumeFlow!$A29:$B41,MATCH('Average Properties Calc'!$A31,VolumeFlow!$A29:$A41,0),4)</f>
+        <f>TissueComp!E$7*INDEX(VolumeFlow!$A30:$B42,MATCH('Average Properties Calc'!$A31,VolumeFlow!$A30:$A42,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D31" s="2" t="e">
-        <f>TissueComp!F$7*INDEX(VolumeFlow!$A29:$B41,MATCH('Average Properties Calc'!$A31,VolumeFlow!$A29:$A41,0),4)</f>
+        <f>TissueComp!F$7*INDEX(VolumeFlow!$A30:$B42,MATCH('Average Properties Calc'!$A31,VolumeFlow!$A30:$A42,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E31" s="2" t="e">
-        <f>TissueComp!G$7*INDEX(VolumeFlow!$A29:$B41,MATCH('Average Properties Calc'!$A31,VolumeFlow!$A29:$A41,0),4)</f>
+        <f>TissueComp!G$7*INDEX(VolumeFlow!$A30:$B42,MATCH('Average Properties Calc'!$A31,VolumeFlow!$A30:$A42,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F31" s="2" t="e">
-        <f>TissueComp!H$7*INDEX(VolumeFlow!$A29:$B41,MATCH('Average Properties Calc'!$A31,VolumeFlow!$A29:$A41,0),4)</f>
+        <f>TissueComp!H$7*INDEX(VolumeFlow!$A30:$B42,MATCH('Average Properties Calc'!$A31,VolumeFlow!$A30:$A42,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G31" s="2" t="e">
-        <f>TissueComp!I$7*INDEX(VolumeFlow!$A29:$B41,MATCH('Average Properties Calc'!$A31,VolumeFlow!$A29:$A41,0),4)</f>
+        <f>TissueComp!I$7*INDEX(VolumeFlow!$A30:$B42,MATCH('Average Properties Calc'!$A31,VolumeFlow!$A30:$A42,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H31" s="2" t="e">
-        <f>TissueComp!J$7*INDEX(VolumeFlow!$A29:$B41,MATCH('Average Properties Calc'!$A31,VolumeFlow!$A29:$A41,0),4)</f>
+        <f>TissueComp!J$7*INDEX(VolumeFlow!$A30:$B42,MATCH('Average Properties Calc'!$A31,VolumeFlow!$A30:$A42,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I31" s="2" t="e">
-        <f>TissueComp!K$7*INDEX(VolumeFlow!$A29:$B41,MATCH('Average Properties Calc'!$A31,VolumeFlow!$A29:$A41,0),4)</f>
+        <f>TissueComp!K$7*INDEX(VolumeFlow!$A30:$B42,MATCH('Average Properties Calc'!$A31,VolumeFlow!$A30:$A42,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J31" s="2" t="e">
-        <f>TissueComp!L$7*INDEX(VolumeFlow!$A29:$B41,MATCH('Average Properties Calc'!$A31,VolumeFlow!$A29:$A41,0),4)</f>
+        <f>TissueComp!L$7*INDEX(VolumeFlow!$A30:$B42,MATCH('Average Properties Calc'!$A31,VolumeFlow!$A30:$A42,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K31" t="s">
@@ -4612,39 +4612,39 @@
         <v>Kidney</v>
       </c>
       <c r="B32" s="2" t="e">
-        <f>TissueComp!D$8*INDEX(VolumeFlow!$A30:$B42,MATCH('Average Properties Calc'!$A32,VolumeFlow!$A30:$A42,0),4)</f>
+        <f>TissueComp!D$8*INDEX(VolumeFlow!$A31:$B43,MATCH('Average Properties Calc'!$A32,VolumeFlow!$A31:$A43,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C32" s="2" t="e">
-        <f>TissueComp!E$8*INDEX(VolumeFlow!$A30:$B42,MATCH('Average Properties Calc'!$A32,VolumeFlow!$A30:$A42,0),4)</f>
+        <f>TissueComp!E$8*INDEX(VolumeFlow!$A31:$B43,MATCH('Average Properties Calc'!$A32,VolumeFlow!$A31:$A43,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D32" s="2" t="e">
-        <f>TissueComp!F$8*INDEX(VolumeFlow!$A30:$B42,MATCH('Average Properties Calc'!$A32,VolumeFlow!$A30:$A42,0),4)</f>
+        <f>TissueComp!F$8*INDEX(VolumeFlow!$A31:$B43,MATCH('Average Properties Calc'!$A32,VolumeFlow!$A31:$A43,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E32" s="2" t="e">
-        <f>TissueComp!G$8*INDEX(VolumeFlow!$A30:$B42,MATCH('Average Properties Calc'!$A32,VolumeFlow!$A30:$A42,0),4)</f>
+        <f>TissueComp!G$8*INDEX(VolumeFlow!$A31:$B43,MATCH('Average Properties Calc'!$A32,VolumeFlow!$A31:$A43,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F32" s="2" t="e">
-        <f>TissueComp!H$8*INDEX(VolumeFlow!$A30:$B42,MATCH('Average Properties Calc'!$A32,VolumeFlow!$A30:$A42,0),4)</f>
+        <f>TissueComp!H$8*INDEX(VolumeFlow!$A31:$B43,MATCH('Average Properties Calc'!$A32,VolumeFlow!$A31:$A43,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G32" s="2" t="e">
-        <f>TissueComp!I$8*INDEX(VolumeFlow!$A30:$B42,MATCH('Average Properties Calc'!$A32,VolumeFlow!$A30:$A42,0),4)</f>
+        <f>TissueComp!I$8*INDEX(VolumeFlow!$A31:$B43,MATCH('Average Properties Calc'!$A32,VolumeFlow!$A31:$A43,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H32" s="2" t="e">
-        <f>TissueComp!J$8*INDEX(VolumeFlow!$A30:$B42,MATCH('Average Properties Calc'!$A32,VolumeFlow!$A30:$A42,0),4)</f>
+        <f>TissueComp!J$8*INDEX(VolumeFlow!$A31:$B43,MATCH('Average Properties Calc'!$A32,VolumeFlow!$A31:$A43,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I32" s="2" t="e">
-        <f>TissueComp!K$8*INDEX(VolumeFlow!$A30:$B42,MATCH('Average Properties Calc'!$A32,VolumeFlow!$A30:$A42,0),4)</f>
+        <f>TissueComp!K$8*INDEX(VolumeFlow!$A31:$B43,MATCH('Average Properties Calc'!$A32,VolumeFlow!$A31:$A43,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J32" s="2" t="e">
-        <f>TissueComp!L$8*INDEX(VolumeFlow!$A30:$B42,MATCH('Average Properties Calc'!$A32,VolumeFlow!$A30:$A42,0),4)</f>
+        <f>TissueComp!L$8*INDEX(VolumeFlow!$A31:$B43,MATCH('Average Properties Calc'!$A32,VolumeFlow!$A31:$A43,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K32" t="s">
@@ -4657,39 +4657,39 @@
         <v>Liver</v>
       </c>
       <c r="B33" s="2" t="e">
-        <f>TissueComp!D$9*INDEX(VolumeFlow!$A31:$B43,MATCH('Average Properties Calc'!$A33,VolumeFlow!$A31:$A43,0),4)</f>
+        <f>TissueComp!D$9*INDEX(VolumeFlow!$A32:$B44,MATCH('Average Properties Calc'!$A33,VolumeFlow!$A32:$A44,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C33" s="2" t="e">
-        <f>TissueComp!E$9*INDEX(VolumeFlow!$A31:$B43,MATCH('Average Properties Calc'!$A33,VolumeFlow!$A31:$A43,0),4)</f>
+        <f>TissueComp!E$9*INDEX(VolumeFlow!$A32:$B44,MATCH('Average Properties Calc'!$A33,VolumeFlow!$A32:$A44,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D33" s="2" t="e">
-        <f>TissueComp!F$9*INDEX(VolumeFlow!$A31:$B43,MATCH('Average Properties Calc'!$A33,VolumeFlow!$A31:$A43,0),4)</f>
+        <f>TissueComp!F$9*INDEX(VolumeFlow!$A32:$B44,MATCH('Average Properties Calc'!$A33,VolumeFlow!$A32:$A44,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E33" s="2" t="e">
-        <f>TissueComp!G$9*INDEX(VolumeFlow!$A31:$B43,MATCH('Average Properties Calc'!$A33,VolumeFlow!$A31:$A43,0),4)</f>
+        <f>TissueComp!G$9*INDEX(VolumeFlow!$A32:$B44,MATCH('Average Properties Calc'!$A33,VolumeFlow!$A32:$A44,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F33" s="2" t="e">
-        <f>TissueComp!H$9*INDEX(VolumeFlow!$A31:$B43,MATCH('Average Properties Calc'!$A33,VolumeFlow!$A31:$A43,0),4)</f>
+        <f>TissueComp!H$9*INDEX(VolumeFlow!$A32:$B44,MATCH('Average Properties Calc'!$A33,VolumeFlow!$A32:$A44,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G33" s="2" t="e">
-        <f>TissueComp!I$9*INDEX(VolumeFlow!$A31:$B43,MATCH('Average Properties Calc'!$A33,VolumeFlow!$A31:$A43,0),4)</f>
+        <f>TissueComp!I$9*INDEX(VolumeFlow!$A32:$B44,MATCH('Average Properties Calc'!$A33,VolumeFlow!$A32:$A44,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H33" s="2" t="e">
-        <f>TissueComp!J$9*INDEX(VolumeFlow!$A31:$B43,MATCH('Average Properties Calc'!$A33,VolumeFlow!$A31:$A43,0),4)</f>
+        <f>TissueComp!J$9*INDEX(VolumeFlow!$A32:$B44,MATCH('Average Properties Calc'!$A33,VolumeFlow!$A32:$A44,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I33" s="2" t="e">
-        <f>TissueComp!K$9*INDEX(VolumeFlow!$A31:$B43,MATCH('Average Properties Calc'!$A33,VolumeFlow!$A31:$A43,0),4)</f>
+        <f>TissueComp!K$9*INDEX(VolumeFlow!$A32:$B44,MATCH('Average Properties Calc'!$A33,VolumeFlow!$A32:$A44,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J33" s="2" t="e">
-        <f>TissueComp!L$9*INDEX(VolumeFlow!$A31:$B43,MATCH('Average Properties Calc'!$A33,VolumeFlow!$A31:$A43,0),4)</f>
+        <f>TissueComp!L$9*INDEX(VolumeFlow!$A32:$B44,MATCH('Average Properties Calc'!$A33,VolumeFlow!$A32:$A44,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K33" t="s">
@@ -4702,39 +4702,39 @@
         <v>Lung</v>
       </c>
       <c r="B34" s="2" t="e">
-        <f>TissueComp!D$10*INDEX(VolumeFlow!$A32:$B44,MATCH('Average Properties Calc'!$A34,VolumeFlow!$A32:$A44,0),4)</f>
+        <f>TissueComp!D$10*INDEX(VolumeFlow!$A33:$B45,MATCH('Average Properties Calc'!$A34,VolumeFlow!$A33:$A45,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C34" s="2" t="e">
-        <f>TissueComp!E$10*INDEX(VolumeFlow!$A32:$B44,MATCH('Average Properties Calc'!$A34,VolumeFlow!$A32:$A44,0),4)</f>
+        <f>TissueComp!E$10*INDEX(VolumeFlow!$A33:$B45,MATCH('Average Properties Calc'!$A34,VolumeFlow!$A33:$A45,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D34" s="2" t="e">
-        <f>TissueComp!F$10*INDEX(VolumeFlow!$A32:$B44,MATCH('Average Properties Calc'!$A34,VolumeFlow!$A32:$A44,0),4)</f>
+        <f>TissueComp!F$10*INDEX(VolumeFlow!$A33:$B45,MATCH('Average Properties Calc'!$A34,VolumeFlow!$A33:$A45,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E34" s="2" t="e">
-        <f>TissueComp!G$10*INDEX(VolumeFlow!$A32:$B44,MATCH('Average Properties Calc'!$A34,VolumeFlow!$A32:$A44,0),4)</f>
+        <f>TissueComp!G$10*INDEX(VolumeFlow!$A33:$B45,MATCH('Average Properties Calc'!$A34,VolumeFlow!$A33:$A45,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F34" s="2" t="e">
-        <f>TissueComp!H$10*INDEX(VolumeFlow!$A32:$B44,MATCH('Average Properties Calc'!$A34,VolumeFlow!$A32:$A44,0),4)</f>
+        <f>TissueComp!H$10*INDEX(VolumeFlow!$A33:$B45,MATCH('Average Properties Calc'!$A34,VolumeFlow!$A33:$A45,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G34" s="2" t="e">
-        <f>TissueComp!I$10*INDEX(VolumeFlow!$A32:$B44,MATCH('Average Properties Calc'!$A34,VolumeFlow!$A32:$A44,0),4)</f>
+        <f>TissueComp!I$10*INDEX(VolumeFlow!$A33:$B45,MATCH('Average Properties Calc'!$A34,VolumeFlow!$A33:$A45,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H34" s="2" t="e">
-        <f>TissueComp!J$10*INDEX(VolumeFlow!$A32:$B44,MATCH('Average Properties Calc'!$A34,VolumeFlow!$A32:$A44,0),4)</f>
+        <f>TissueComp!J$10*INDEX(VolumeFlow!$A33:$B45,MATCH('Average Properties Calc'!$A34,VolumeFlow!$A33:$A45,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I34" s="2" t="e">
-        <f>TissueComp!K$10*INDEX(VolumeFlow!$A32:$B44,MATCH('Average Properties Calc'!$A34,VolumeFlow!$A32:$A44,0),4)</f>
+        <f>TissueComp!K$10*INDEX(VolumeFlow!$A33:$B45,MATCH('Average Properties Calc'!$A34,VolumeFlow!$A33:$A45,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J34" s="2" t="e">
-        <f>TissueComp!L$10*INDEX(VolumeFlow!$A32:$B44,MATCH('Average Properties Calc'!$A34,VolumeFlow!$A32:$A44,0),4)</f>
+        <f>TissueComp!L$10*INDEX(VolumeFlow!$A33:$B45,MATCH('Average Properties Calc'!$A34,VolumeFlow!$A33:$A45,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K34" t="s">
@@ -4747,39 +4747,39 @@
         <v>Muscle</v>
       </c>
       <c r="B35" s="2" t="e">
-        <f>TissueComp!D$11*INDEX(VolumeFlow!$A33:$B45,MATCH('Average Properties Calc'!$A35,VolumeFlow!$A33:$A45,0),4)</f>
+        <f>TissueComp!D$11*INDEX(VolumeFlow!$A34:$B46,MATCH('Average Properties Calc'!$A35,VolumeFlow!$A34:$A46,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C35" s="2" t="e">
-        <f>TissueComp!E$11*INDEX(VolumeFlow!$A33:$B45,MATCH('Average Properties Calc'!$A35,VolumeFlow!$A33:$A45,0),4)</f>
+        <f>TissueComp!E$11*INDEX(VolumeFlow!$A34:$B46,MATCH('Average Properties Calc'!$A35,VolumeFlow!$A34:$A46,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D35" s="2" t="e">
-        <f>TissueComp!F$11*INDEX(VolumeFlow!$A33:$B45,MATCH('Average Properties Calc'!$A35,VolumeFlow!$A33:$A45,0),4)</f>
+        <f>TissueComp!F$11*INDEX(VolumeFlow!$A34:$B46,MATCH('Average Properties Calc'!$A35,VolumeFlow!$A34:$A46,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E35" s="2" t="e">
-        <f>TissueComp!G$11*INDEX(VolumeFlow!$A33:$B45,MATCH('Average Properties Calc'!$A35,VolumeFlow!$A33:$A45,0),4)</f>
+        <f>TissueComp!G$11*INDEX(VolumeFlow!$A34:$B46,MATCH('Average Properties Calc'!$A35,VolumeFlow!$A34:$A46,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F35" s="2" t="e">
-        <f>TissueComp!H$11*INDEX(VolumeFlow!$A33:$B45,MATCH('Average Properties Calc'!$A35,VolumeFlow!$A33:$A45,0),4)</f>
+        <f>TissueComp!H$11*INDEX(VolumeFlow!$A34:$B46,MATCH('Average Properties Calc'!$A35,VolumeFlow!$A34:$A46,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G35" s="2" t="e">
-        <f>TissueComp!I$11*INDEX(VolumeFlow!$A33:$B45,MATCH('Average Properties Calc'!$A35,VolumeFlow!$A33:$A45,0),4)</f>
+        <f>TissueComp!I$11*INDEX(VolumeFlow!$A34:$B46,MATCH('Average Properties Calc'!$A35,VolumeFlow!$A34:$A46,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H35" s="2" t="e">
-        <f>TissueComp!J$11*INDEX(VolumeFlow!$A33:$B45,MATCH('Average Properties Calc'!$A35,VolumeFlow!$A33:$A45,0),4)</f>
+        <f>TissueComp!J$11*INDEX(VolumeFlow!$A34:$B46,MATCH('Average Properties Calc'!$A35,VolumeFlow!$A34:$A46,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I35" s="2" t="e">
-        <f>TissueComp!K$11*INDEX(VolumeFlow!$A33:$B45,MATCH('Average Properties Calc'!$A35,VolumeFlow!$A33:$A45,0),4)</f>
+        <f>TissueComp!K$11*INDEX(VolumeFlow!$A34:$B46,MATCH('Average Properties Calc'!$A35,VolumeFlow!$A34:$A46,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J35" s="2" t="e">
-        <f>TissueComp!L$11*INDEX(VolumeFlow!$A33:$B45,MATCH('Average Properties Calc'!$A35,VolumeFlow!$A33:$A45,0),4)</f>
+        <f>TissueComp!L$11*INDEX(VolumeFlow!$A34:$B46,MATCH('Average Properties Calc'!$A35,VolumeFlow!$A34:$A46,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K35" t="s">
@@ -4792,39 +4792,39 @@
         <v>Skin</v>
       </c>
       <c r="B36" s="2" t="e">
-        <f>TissueComp!D$12*INDEX(VolumeFlow!$A34:$B46,MATCH('Average Properties Calc'!$A36,VolumeFlow!$A34:$A46,0),4)</f>
+        <f>TissueComp!D$12*INDEX(VolumeFlow!$A35:$B47,MATCH('Average Properties Calc'!$A36,VolumeFlow!$A35:$A47,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C36" s="2" t="e">
-        <f>TissueComp!E$12*INDEX(VolumeFlow!$A34:$B46,MATCH('Average Properties Calc'!$A36,VolumeFlow!$A34:$A46,0),4)</f>
+        <f>TissueComp!E$12*INDEX(VolumeFlow!$A35:$B47,MATCH('Average Properties Calc'!$A36,VolumeFlow!$A35:$A47,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D36" s="2" t="e">
-        <f>TissueComp!F$12*INDEX(VolumeFlow!$A34:$B46,MATCH('Average Properties Calc'!$A36,VolumeFlow!$A34:$A46,0),4)</f>
+        <f>TissueComp!F$12*INDEX(VolumeFlow!$A35:$B47,MATCH('Average Properties Calc'!$A36,VolumeFlow!$A35:$A47,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E36" s="2" t="e">
-        <f>TissueComp!G$12*INDEX(VolumeFlow!$A34:$B46,MATCH('Average Properties Calc'!$A36,VolumeFlow!$A34:$A46,0),4)</f>
+        <f>TissueComp!G$12*INDEX(VolumeFlow!$A35:$B47,MATCH('Average Properties Calc'!$A36,VolumeFlow!$A35:$A47,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F36" s="2" t="e">
-        <f>TissueComp!H$12*INDEX(VolumeFlow!$A34:$B46,MATCH('Average Properties Calc'!$A36,VolumeFlow!$A34:$A46,0),4)</f>
+        <f>TissueComp!H$12*INDEX(VolumeFlow!$A35:$B47,MATCH('Average Properties Calc'!$A36,VolumeFlow!$A35:$A47,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G36" s="2" t="e">
-        <f>TissueComp!I$12*INDEX(VolumeFlow!$A34:$B46,MATCH('Average Properties Calc'!$A36,VolumeFlow!$A34:$A46,0),4)</f>
+        <f>TissueComp!I$12*INDEX(VolumeFlow!$A35:$B47,MATCH('Average Properties Calc'!$A36,VolumeFlow!$A35:$A47,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H36" s="2" t="e">
-        <f>TissueComp!J$12*INDEX(VolumeFlow!$A34:$B46,MATCH('Average Properties Calc'!$A36,VolumeFlow!$A34:$A46,0),4)</f>
+        <f>TissueComp!J$12*INDEX(VolumeFlow!$A35:$B47,MATCH('Average Properties Calc'!$A36,VolumeFlow!$A35:$A47,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I36" s="2" t="e">
-        <f>TissueComp!K$12*INDEX(VolumeFlow!$A34:$B46,MATCH('Average Properties Calc'!$A36,VolumeFlow!$A34:$A46,0),4)</f>
+        <f>TissueComp!K$12*INDEX(VolumeFlow!$A35:$B47,MATCH('Average Properties Calc'!$A36,VolumeFlow!$A35:$A47,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J36" s="2" t="e">
-        <f>TissueComp!L$12*INDEX(VolumeFlow!$A34:$B46,MATCH('Average Properties Calc'!$A36,VolumeFlow!$A34:$A46,0),4)</f>
+        <f>TissueComp!L$12*INDEX(VolumeFlow!$A35:$B47,MATCH('Average Properties Calc'!$A36,VolumeFlow!$A35:$A47,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K36" t="s">
@@ -4837,39 +4837,39 @@
         <v>Spleen</v>
       </c>
       <c r="B37" s="2" t="e">
-        <f>TissueComp!D$13*INDEX(VolumeFlow!$A35:$B47,MATCH('Average Properties Calc'!$A37,VolumeFlow!$A35:$A47,0),4)</f>
+        <f>TissueComp!D$13*INDEX(VolumeFlow!$A36:$B48,MATCH('Average Properties Calc'!$A37,VolumeFlow!$A36:$A48,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C37" s="2" t="e">
-        <f>TissueComp!E$13*INDEX(VolumeFlow!$A35:$B47,MATCH('Average Properties Calc'!$A37,VolumeFlow!$A35:$A47,0),4)</f>
+        <f>TissueComp!E$13*INDEX(VolumeFlow!$A36:$B48,MATCH('Average Properties Calc'!$A37,VolumeFlow!$A36:$A48,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D37" s="2" t="e">
-        <f>TissueComp!F$13*INDEX(VolumeFlow!$A35:$B47,MATCH('Average Properties Calc'!$A37,VolumeFlow!$A35:$A47,0),4)</f>
+        <f>TissueComp!F$13*INDEX(VolumeFlow!$A36:$B48,MATCH('Average Properties Calc'!$A37,VolumeFlow!$A36:$A48,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E37" s="2" t="e">
-        <f>TissueComp!G$13*INDEX(VolumeFlow!$A35:$B47,MATCH('Average Properties Calc'!$A37,VolumeFlow!$A35:$A47,0),4)</f>
+        <f>TissueComp!G$13*INDEX(VolumeFlow!$A36:$B48,MATCH('Average Properties Calc'!$A37,VolumeFlow!$A36:$A48,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F37" s="2" t="e">
-        <f>TissueComp!H$13*INDEX(VolumeFlow!$A35:$B47,MATCH('Average Properties Calc'!$A37,VolumeFlow!$A35:$A47,0),4)</f>
+        <f>TissueComp!H$13*INDEX(VolumeFlow!$A36:$B48,MATCH('Average Properties Calc'!$A37,VolumeFlow!$A36:$A48,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G37" s="2" t="e">
-        <f>TissueComp!I$13*INDEX(VolumeFlow!$A35:$B47,MATCH('Average Properties Calc'!$A37,VolumeFlow!$A35:$A47,0),4)</f>
+        <f>TissueComp!I$13*INDEX(VolumeFlow!$A36:$B48,MATCH('Average Properties Calc'!$A37,VolumeFlow!$A36:$A48,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H37" s="2" t="e">
-        <f>TissueComp!J$13*INDEX(VolumeFlow!$A35:$B47,MATCH('Average Properties Calc'!$A37,VolumeFlow!$A35:$A47,0),4)</f>
+        <f>TissueComp!J$13*INDEX(VolumeFlow!$A36:$B48,MATCH('Average Properties Calc'!$A37,VolumeFlow!$A36:$A48,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I37" s="2" t="e">
-        <f>TissueComp!K$13*INDEX(VolumeFlow!$A35:$B47,MATCH('Average Properties Calc'!$A37,VolumeFlow!$A35:$A47,0),4)</f>
+        <f>TissueComp!K$13*INDEX(VolumeFlow!$A36:$B48,MATCH('Average Properties Calc'!$A37,VolumeFlow!$A36:$A48,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J37" s="2" t="e">
-        <f>TissueComp!L$13*INDEX(VolumeFlow!$A35:$B47,MATCH('Average Properties Calc'!$A37,VolumeFlow!$A35:$A47,0),4)</f>
+        <f>TissueComp!L$13*INDEX(VolumeFlow!$A36:$B48,MATCH('Average Properties Calc'!$A37,VolumeFlow!$A36:$A48,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K37" t="s">
@@ -4920,39 +4920,39 @@
         <v>Adipose</v>
       </c>
       <c r="B39" s="2" t="e">
-        <f>TissueComp!D$3*INDEX(VolumeFlow!$A37:$B49,MATCH('Average Properties Calc'!$A39,VolumeFlow!$A37:$A49,0),4)</f>
+        <f>TissueComp!D$3*INDEX(VolumeFlow!$A38:$B50,MATCH('Average Properties Calc'!$A39,VolumeFlow!$A38:$A50,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C39" s="2" t="e">
-        <f>TissueComp!E$3*INDEX(VolumeFlow!$A37:$B49,MATCH('Average Properties Calc'!$A39,VolumeFlow!$A37:$A49,0),4)</f>
+        <f>TissueComp!E$3*INDEX(VolumeFlow!$A38:$B50,MATCH('Average Properties Calc'!$A39,VolumeFlow!$A38:$A50,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D39" s="2" t="e">
-        <f>TissueComp!F$3*INDEX(VolumeFlow!$A37:$B49,MATCH('Average Properties Calc'!$A39,VolumeFlow!$A37:$A49,0),4)</f>
+        <f>TissueComp!F$3*INDEX(VolumeFlow!$A38:$B50,MATCH('Average Properties Calc'!$A39,VolumeFlow!$A38:$A50,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E39" s="2" t="e">
-        <f>TissueComp!G$3*INDEX(VolumeFlow!$A37:$B49,MATCH('Average Properties Calc'!$A39,VolumeFlow!$A37:$A49,0),4)</f>
+        <f>TissueComp!G$3*INDEX(VolumeFlow!$A38:$B50,MATCH('Average Properties Calc'!$A39,VolumeFlow!$A38:$A50,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F39" s="2" t="e">
-        <f>TissueComp!H$3*INDEX(VolumeFlow!$A37:$B49,MATCH('Average Properties Calc'!$A39,VolumeFlow!$A37:$A49,0),4)</f>
+        <f>TissueComp!H$3*INDEX(VolumeFlow!$A38:$B50,MATCH('Average Properties Calc'!$A39,VolumeFlow!$A38:$A50,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G39" s="2" t="e">
-        <f>TissueComp!I$3*INDEX(VolumeFlow!$A37:$B49,MATCH('Average Properties Calc'!$A39,VolumeFlow!$A37:$A49,0),4)</f>
+        <f>TissueComp!I$3*INDEX(VolumeFlow!$A38:$B50,MATCH('Average Properties Calc'!$A39,VolumeFlow!$A38:$A50,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H39" s="2" t="e">
-        <f>TissueComp!J$3*INDEX(VolumeFlow!$A37:$B49,MATCH('Average Properties Calc'!$A39,VolumeFlow!$A37:$A49,0),4)</f>
+        <f>TissueComp!J$3*INDEX(VolumeFlow!$A38:$B50,MATCH('Average Properties Calc'!$A39,VolumeFlow!$A38:$A50,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I39" s="2" t="e">
-        <f>TissueComp!K$3*INDEX(VolumeFlow!$A37:$B49,MATCH('Average Properties Calc'!$A39,VolumeFlow!$A37:$A49,0),4)</f>
+        <f>TissueComp!K$3*INDEX(VolumeFlow!$A38:$B50,MATCH('Average Properties Calc'!$A39,VolumeFlow!$A38:$A50,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J39" s="2" t="e">
-        <f>TissueComp!L$3*INDEX(VolumeFlow!$A37:$B49,MATCH('Average Properties Calc'!$A39,VolumeFlow!$A37:$A49,0),4)</f>
+        <f>TissueComp!L$3*INDEX(VolumeFlow!$A38:$B50,MATCH('Average Properties Calc'!$A39,VolumeFlow!$A38:$A50,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K39" t="s">
@@ -4965,39 +4965,39 @@
         <v>Bone</v>
       </c>
       <c r="B40" s="2" t="e">
-        <f>TissueComp!D$4*INDEX(VolumeFlow!$A38:$B50,MATCH('Average Properties Calc'!$A40,VolumeFlow!$A38:$A50,0),4)</f>
+        <f>TissueComp!D$4*INDEX(VolumeFlow!$A39:$B51,MATCH('Average Properties Calc'!$A40,VolumeFlow!$A39:$A51,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C40" s="2" t="e">
-        <f>TissueComp!E$4*INDEX(VolumeFlow!$A38:$B50,MATCH('Average Properties Calc'!$A40,VolumeFlow!$A38:$A50,0),4)</f>
+        <f>TissueComp!E$4*INDEX(VolumeFlow!$A39:$B51,MATCH('Average Properties Calc'!$A40,VolumeFlow!$A39:$A51,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D40" s="2" t="e">
-        <f>TissueComp!F$4*INDEX(VolumeFlow!$A38:$B50,MATCH('Average Properties Calc'!$A40,VolumeFlow!$A38:$A50,0),4)</f>
+        <f>TissueComp!F$4*INDEX(VolumeFlow!$A39:$B51,MATCH('Average Properties Calc'!$A40,VolumeFlow!$A39:$A51,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E40" s="2" t="e">
-        <f>TissueComp!G$4*INDEX(VolumeFlow!$A38:$B50,MATCH('Average Properties Calc'!$A40,VolumeFlow!$A38:$A50,0),4)</f>
+        <f>TissueComp!G$4*INDEX(VolumeFlow!$A39:$B51,MATCH('Average Properties Calc'!$A40,VolumeFlow!$A39:$A51,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F40" s="2" t="e">
-        <f>TissueComp!H$4*INDEX(VolumeFlow!$A38:$B50,MATCH('Average Properties Calc'!$A40,VolumeFlow!$A38:$A50,0),4)</f>
+        <f>TissueComp!H$4*INDEX(VolumeFlow!$A39:$B51,MATCH('Average Properties Calc'!$A40,VolumeFlow!$A39:$A51,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G40" s="2" t="e">
-        <f>TissueComp!I$4*INDEX(VolumeFlow!$A38:$B50,MATCH('Average Properties Calc'!$A40,VolumeFlow!$A38:$A50,0),4)</f>
+        <f>TissueComp!I$4*INDEX(VolumeFlow!$A39:$B51,MATCH('Average Properties Calc'!$A40,VolumeFlow!$A39:$A51,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H40" s="2" t="e">
-        <f>TissueComp!J$4*INDEX(VolumeFlow!$A38:$B50,MATCH('Average Properties Calc'!$A40,VolumeFlow!$A38:$A50,0),4)</f>
+        <f>TissueComp!J$4*INDEX(VolumeFlow!$A39:$B51,MATCH('Average Properties Calc'!$A40,VolumeFlow!$A39:$A51,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I40" s="2" t="e">
-        <f>TissueComp!K$4*INDEX(VolumeFlow!$A38:$B50,MATCH('Average Properties Calc'!$A40,VolumeFlow!$A38:$A50,0),4)</f>
+        <f>TissueComp!K$4*INDEX(VolumeFlow!$A39:$B51,MATCH('Average Properties Calc'!$A40,VolumeFlow!$A39:$A51,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J40" s="2" t="e">
-        <f>TissueComp!L$4*INDEX(VolumeFlow!$A38:$B50,MATCH('Average Properties Calc'!$A40,VolumeFlow!$A38:$A50,0),4)</f>
+        <f>TissueComp!L$4*INDEX(VolumeFlow!$A39:$B51,MATCH('Average Properties Calc'!$A40,VolumeFlow!$A39:$A51,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K40" t="s">
@@ -5010,39 +5010,39 @@
         <v>Brain</v>
       </c>
       <c r="B41" s="2" t="e">
-        <f>TissueComp!D$5*INDEX(VolumeFlow!$A39:$B51,MATCH('Average Properties Calc'!$A41,VolumeFlow!$A39:$A51,0),4)</f>
+        <f>TissueComp!D$5*INDEX(VolumeFlow!$A40:$B52,MATCH('Average Properties Calc'!$A41,VolumeFlow!$A40:$A52,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C41" s="2" t="e">
-        <f>TissueComp!E$5*INDEX(VolumeFlow!$A39:$B51,MATCH('Average Properties Calc'!$A41,VolumeFlow!$A39:$A51,0),4)</f>
+        <f>TissueComp!E$5*INDEX(VolumeFlow!$A40:$B52,MATCH('Average Properties Calc'!$A41,VolumeFlow!$A40:$A52,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D41" s="2" t="e">
-        <f>TissueComp!F$5*INDEX(VolumeFlow!$A39:$B51,MATCH('Average Properties Calc'!$A41,VolumeFlow!$A39:$A51,0),4)</f>
+        <f>TissueComp!F$5*INDEX(VolumeFlow!$A40:$B52,MATCH('Average Properties Calc'!$A41,VolumeFlow!$A40:$A52,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E41" s="2" t="e">
-        <f>TissueComp!G$5*INDEX(VolumeFlow!$A39:$B51,MATCH('Average Properties Calc'!$A41,VolumeFlow!$A39:$A51,0),4)</f>
+        <f>TissueComp!G$5*INDEX(VolumeFlow!$A40:$B52,MATCH('Average Properties Calc'!$A41,VolumeFlow!$A40:$A52,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F41" s="2" t="e">
-        <f>TissueComp!H$5*INDEX(VolumeFlow!$A39:$B51,MATCH('Average Properties Calc'!$A41,VolumeFlow!$A39:$A51,0),4)</f>
+        <f>TissueComp!H$5*INDEX(VolumeFlow!$A40:$B52,MATCH('Average Properties Calc'!$A41,VolumeFlow!$A40:$A52,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G41" s="2" t="e">
-        <f>TissueComp!I$5*INDEX(VolumeFlow!$A39:$B51,MATCH('Average Properties Calc'!$A41,VolumeFlow!$A39:$A51,0),4)</f>
+        <f>TissueComp!I$5*INDEX(VolumeFlow!$A40:$B52,MATCH('Average Properties Calc'!$A41,VolumeFlow!$A40:$A52,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H41" s="2" t="e">
-        <f>TissueComp!J$5*INDEX(VolumeFlow!$A39:$B51,MATCH('Average Properties Calc'!$A41,VolumeFlow!$A39:$A51,0),4)</f>
+        <f>TissueComp!J$5*INDEX(VolumeFlow!$A40:$B52,MATCH('Average Properties Calc'!$A41,VolumeFlow!$A40:$A52,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I41" s="2" t="e">
-        <f>TissueComp!K$5*INDEX(VolumeFlow!$A39:$B51,MATCH('Average Properties Calc'!$A41,VolumeFlow!$A39:$A51,0),4)</f>
+        <f>TissueComp!K$5*INDEX(VolumeFlow!$A40:$B52,MATCH('Average Properties Calc'!$A41,VolumeFlow!$A40:$A52,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J41" s="2" t="e">
-        <f>TissueComp!L$5*INDEX(VolumeFlow!$A39:$B51,MATCH('Average Properties Calc'!$A41,VolumeFlow!$A39:$A51,0),4)</f>
+        <f>TissueComp!L$5*INDEX(VolumeFlow!$A40:$B52,MATCH('Average Properties Calc'!$A41,VolumeFlow!$A40:$A52,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K41" t="s">
@@ -5055,39 +5055,39 @@
         <v>Gut</v>
       </c>
       <c r="B42" s="2" t="e">
-        <f>TissueComp!D$6*INDEX(VolumeFlow!$A40:$B52,MATCH('Average Properties Calc'!$A42,VolumeFlow!$A40:$A52,0),4)</f>
+        <f>TissueComp!D$6*INDEX(VolumeFlow!$A41:$B53,MATCH('Average Properties Calc'!$A42,VolumeFlow!$A41:$A53,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C42" s="2" t="e">
-        <f>TissueComp!E$6*INDEX(VolumeFlow!$A40:$B52,MATCH('Average Properties Calc'!$A42,VolumeFlow!$A40:$A52,0),4)</f>
+        <f>TissueComp!E$6*INDEX(VolumeFlow!$A41:$B53,MATCH('Average Properties Calc'!$A42,VolumeFlow!$A41:$A53,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D42" s="2" t="e">
-        <f>TissueComp!F$6*INDEX(VolumeFlow!$A40:$B52,MATCH('Average Properties Calc'!$A42,VolumeFlow!$A40:$A52,0),4)</f>
+        <f>TissueComp!F$6*INDEX(VolumeFlow!$A41:$B53,MATCH('Average Properties Calc'!$A42,VolumeFlow!$A41:$A53,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E42" s="2" t="e">
-        <f>TissueComp!G$6*INDEX(VolumeFlow!$A40:$B52,MATCH('Average Properties Calc'!$A42,VolumeFlow!$A40:$A52,0),4)</f>
+        <f>TissueComp!G$6*INDEX(VolumeFlow!$A41:$B53,MATCH('Average Properties Calc'!$A42,VolumeFlow!$A41:$A53,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F42" s="2" t="e">
-        <f>TissueComp!H$6*INDEX(VolumeFlow!$A40:$B52,MATCH('Average Properties Calc'!$A42,VolumeFlow!$A40:$A52,0),4)</f>
+        <f>TissueComp!H$6*INDEX(VolumeFlow!$A41:$B53,MATCH('Average Properties Calc'!$A42,VolumeFlow!$A41:$A53,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G42" s="2" t="e">
-        <f>TissueComp!I$6*INDEX(VolumeFlow!$A40:$B52,MATCH('Average Properties Calc'!$A42,VolumeFlow!$A40:$A52,0),4)</f>
+        <f>TissueComp!I$6*INDEX(VolumeFlow!$A41:$B53,MATCH('Average Properties Calc'!$A42,VolumeFlow!$A41:$A53,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H42" s="2" t="e">
-        <f>TissueComp!J$6*INDEX(VolumeFlow!$A40:$B52,MATCH('Average Properties Calc'!$A42,VolumeFlow!$A40:$A52,0),4)</f>
+        <f>TissueComp!J$6*INDEX(VolumeFlow!$A41:$B53,MATCH('Average Properties Calc'!$A42,VolumeFlow!$A41:$A53,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I42" s="2" t="e">
-        <f>TissueComp!K$6*INDEX(VolumeFlow!$A40:$B52,MATCH('Average Properties Calc'!$A42,VolumeFlow!$A40:$A52,0),4)</f>
+        <f>TissueComp!K$6*INDEX(VolumeFlow!$A41:$B53,MATCH('Average Properties Calc'!$A42,VolumeFlow!$A41:$A53,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J42" s="2" t="e">
-        <f>TissueComp!L$6*INDEX(VolumeFlow!$A40:$B52,MATCH('Average Properties Calc'!$A42,VolumeFlow!$A40:$A52,0),4)</f>
+        <f>TissueComp!L$6*INDEX(VolumeFlow!$A41:$B53,MATCH('Average Properties Calc'!$A42,VolumeFlow!$A41:$A53,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K42" t="s">
@@ -5100,39 +5100,39 @@
         <v>Heart</v>
       </c>
       <c r="B43" s="2" t="e">
-        <f>TissueComp!D$7*INDEX(VolumeFlow!$A41:$B53,MATCH('Average Properties Calc'!$A43,VolumeFlow!$A41:$A53,0),4)</f>
+        <f>TissueComp!D$7*INDEX(VolumeFlow!$A42:$B54,MATCH('Average Properties Calc'!$A43,VolumeFlow!$A42:$A54,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C43" s="2" t="e">
-        <f>TissueComp!E$7*INDEX(VolumeFlow!$A41:$B53,MATCH('Average Properties Calc'!$A43,VolumeFlow!$A41:$A53,0),4)</f>
+        <f>TissueComp!E$7*INDEX(VolumeFlow!$A42:$B54,MATCH('Average Properties Calc'!$A43,VolumeFlow!$A42:$A54,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D43" s="2" t="e">
-        <f>TissueComp!F$7*INDEX(VolumeFlow!$A41:$B53,MATCH('Average Properties Calc'!$A43,VolumeFlow!$A41:$A53,0),4)</f>
+        <f>TissueComp!F$7*INDEX(VolumeFlow!$A42:$B54,MATCH('Average Properties Calc'!$A43,VolumeFlow!$A42:$A54,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E43" s="2" t="e">
-        <f>TissueComp!G$7*INDEX(VolumeFlow!$A41:$B53,MATCH('Average Properties Calc'!$A43,VolumeFlow!$A41:$A53,0),4)</f>
+        <f>TissueComp!G$7*INDEX(VolumeFlow!$A42:$B54,MATCH('Average Properties Calc'!$A43,VolumeFlow!$A42:$A54,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F43" s="2" t="e">
-        <f>TissueComp!H$7*INDEX(VolumeFlow!$A41:$B53,MATCH('Average Properties Calc'!$A43,VolumeFlow!$A41:$A53,0),4)</f>
+        <f>TissueComp!H$7*INDEX(VolumeFlow!$A42:$B54,MATCH('Average Properties Calc'!$A43,VolumeFlow!$A42:$A54,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G43" s="2" t="e">
-        <f>TissueComp!I$7*INDEX(VolumeFlow!$A41:$B53,MATCH('Average Properties Calc'!$A43,VolumeFlow!$A41:$A53,0),4)</f>
+        <f>TissueComp!I$7*INDEX(VolumeFlow!$A42:$B54,MATCH('Average Properties Calc'!$A43,VolumeFlow!$A42:$A54,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H43" s="2" t="e">
-        <f>TissueComp!J$7*INDEX(VolumeFlow!$A41:$B53,MATCH('Average Properties Calc'!$A43,VolumeFlow!$A41:$A53,0),4)</f>
+        <f>TissueComp!J$7*INDEX(VolumeFlow!$A42:$B54,MATCH('Average Properties Calc'!$A43,VolumeFlow!$A42:$A54,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I43" s="2" t="e">
-        <f>TissueComp!K$7*INDEX(VolumeFlow!$A41:$B53,MATCH('Average Properties Calc'!$A43,VolumeFlow!$A41:$A53,0),4)</f>
+        <f>TissueComp!K$7*INDEX(VolumeFlow!$A42:$B54,MATCH('Average Properties Calc'!$A43,VolumeFlow!$A42:$A54,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J43" s="2" t="e">
-        <f>TissueComp!L$7*INDEX(VolumeFlow!$A41:$B53,MATCH('Average Properties Calc'!$A43,VolumeFlow!$A41:$A53,0),4)</f>
+        <f>TissueComp!L$7*INDEX(VolumeFlow!$A42:$B54,MATCH('Average Properties Calc'!$A43,VolumeFlow!$A42:$A54,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K43" t="s">
@@ -5145,39 +5145,39 @@
         <v>Kidney</v>
       </c>
       <c r="B44" s="2" t="e">
-        <f>TissueComp!D$8*INDEX(VolumeFlow!$A42:$B54,MATCH('Average Properties Calc'!$A44,VolumeFlow!$A42:$A54,0),4)</f>
+        <f>TissueComp!D$8*INDEX(VolumeFlow!$A43:$B55,MATCH('Average Properties Calc'!$A44,VolumeFlow!$A43:$A55,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C44" s="2" t="e">
-        <f>TissueComp!E$8*INDEX(VolumeFlow!$A42:$B54,MATCH('Average Properties Calc'!$A44,VolumeFlow!$A42:$A54,0),4)</f>
+        <f>TissueComp!E$8*INDEX(VolumeFlow!$A43:$B55,MATCH('Average Properties Calc'!$A44,VolumeFlow!$A43:$A55,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D44" s="2" t="e">
-        <f>TissueComp!F$8*INDEX(VolumeFlow!$A42:$B54,MATCH('Average Properties Calc'!$A44,VolumeFlow!$A42:$A54,0),4)</f>
+        <f>TissueComp!F$8*INDEX(VolumeFlow!$A43:$B55,MATCH('Average Properties Calc'!$A44,VolumeFlow!$A43:$A55,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E44" s="2" t="e">
-        <f>TissueComp!G$8*INDEX(VolumeFlow!$A42:$B54,MATCH('Average Properties Calc'!$A44,VolumeFlow!$A42:$A54,0),4)</f>
+        <f>TissueComp!G$8*INDEX(VolumeFlow!$A43:$B55,MATCH('Average Properties Calc'!$A44,VolumeFlow!$A43:$A55,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F44" s="2" t="e">
-        <f>TissueComp!H$8*INDEX(VolumeFlow!$A42:$B54,MATCH('Average Properties Calc'!$A44,VolumeFlow!$A42:$A54,0),4)</f>
+        <f>TissueComp!H$8*INDEX(VolumeFlow!$A43:$B55,MATCH('Average Properties Calc'!$A44,VolumeFlow!$A43:$A55,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G44" s="2" t="e">
-        <f>TissueComp!I$8*INDEX(VolumeFlow!$A42:$B54,MATCH('Average Properties Calc'!$A44,VolumeFlow!$A42:$A54,0),4)</f>
+        <f>TissueComp!I$8*INDEX(VolumeFlow!$A43:$B55,MATCH('Average Properties Calc'!$A44,VolumeFlow!$A43:$A55,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H44" s="2" t="e">
-        <f>TissueComp!J$8*INDEX(VolumeFlow!$A42:$B54,MATCH('Average Properties Calc'!$A44,VolumeFlow!$A42:$A54,0),4)</f>
+        <f>TissueComp!J$8*INDEX(VolumeFlow!$A43:$B55,MATCH('Average Properties Calc'!$A44,VolumeFlow!$A43:$A55,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I44" s="2" t="e">
-        <f>TissueComp!K$8*INDEX(VolumeFlow!$A42:$B54,MATCH('Average Properties Calc'!$A44,VolumeFlow!$A42:$A54,0),4)</f>
+        <f>TissueComp!K$8*INDEX(VolumeFlow!$A43:$B55,MATCH('Average Properties Calc'!$A44,VolumeFlow!$A43:$A55,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J44" s="2" t="e">
-        <f>TissueComp!L$8*INDEX(VolumeFlow!$A42:$B54,MATCH('Average Properties Calc'!$A44,VolumeFlow!$A42:$A54,0),4)</f>
+        <f>TissueComp!L$8*INDEX(VolumeFlow!$A43:$B55,MATCH('Average Properties Calc'!$A44,VolumeFlow!$A43:$A55,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K44" t="s">
@@ -5190,39 +5190,39 @@
         <v>Liver</v>
       </c>
       <c r="B45" s="2" t="e">
-        <f>TissueComp!D$9*INDEX(VolumeFlow!$A43:$B55,MATCH('Average Properties Calc'!$A45,VolumeFlow!$A43:$A55,0),4)</f>
+        <f>TissueComp!D$9*INDEX(VolumeFlow!$A44:$B56,MATCH('Average Properties Calc'!$A45,VolumeFlow!$A44:$A56,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C45" s="2" t="e">
-        <f>TissueComp!E$9*INDEX(VolumeFlow!$A43:$B55,MATCH('Average Properties Calc'!$A45,VolumeFlow!$A43:$A55,0),4)</f>
+        <f>TissueComp!E$9*INDEX(VolumeFlow!$A44:$B56,MATCH('Average Properties Calc'!$A45,VolumeFlow!$A44:$A56,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D45" s="2" t="e">
-        <f>TissueComp!F$9*INDEX(VolumeFlow!$A43:$B55,MATCH('Average Properties Calc'!$A45,VolumeFlow!$A43:$A55,0),4)</f>
+        <f>TissueComp!F$9*INDEX(VolumeFlow!$A44:$B56,MATCH('Average Properties Calc'!$A45,VolumeFlow!$A44:$A56,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E45" s="2" t="e">
-        <f>TissueComp!G$9*INDEX(VolumeFlow!$A43:$B55,MATCH('Average Properties Calc'!$A45,VolumeFlow!$A43:$A55,0),4)</f>
+        <f>TissueComp!G$9*INDEX(VolumeFlow!$A44:$B56,MATCH('Average Properties Calc'!$A45,VolumeFlow!$A44:$A56,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F45" s="2" t="e">
-        <f>TissueComp!H$9*INDEX(VolumeFlow!$A43:$B55,MATCH('Average Properties Calc'!$A45,VolumeFlow!$A43:$A55,0),4)</f>
+        <f>TissueComp!H$9*INDEX(VolumeFlow!$A44:$B56,MATCH('Average Properties Calc'!$A45,VolumeFlow!$A44:$A56,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G45" s="2" t="e">
-        <f>TissueComp!I$9*INDEX(VolumeFlow!$A43:$B55,MATCH('Average Properties Calc'!$A45,VolumeFlow!$A43:$A55,0),4)</f>
+        <f>TissueComp!I$9*INDEX(VolumeFlow!$A44:$B56,MATCH('Average Properties Calc'!$A45,VolumeFlow!$A44:$A56,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H45" s="2" t="e">
-        <f>TissueComp!J$9*INDEX(VolumeFlow!$A43:$B55,MATCH('Average Properties Calc'!$A45,VolumeFlow!$A43:$A55,0),4)</f>
+        <f>TissueComp!J$9*INDEX(VolumeFlow!$A44:$B56,MATCH('Average Properties Calc'!$A45,VolumeFlow!$A44:$A56,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I45" s="2" t="e">
-        <f>TissueComp!K$9*INDEX(VolumeFlow!$A43:$B55,MATCH('Average Properties Calc'!$A45,VolumeFlow!$A43:$A55,0),4)</f>
+        <f>TissueComp!K$9*INDEX(VolumeFlow!$A44:$B56,MATCH('Average Properties Calc'!$A45,VolumeFlow!$A44:$A56,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J45" s="2" t="e">
-        <f>TissueComp!L$9*INDEX(VolumeFlow!$A43:$B55,MATCH('Average Properties Calc'!$A45,VolumeFlow!$A43:$A55,0),4)</f>
+        <f>TissueComp!L$9*INDEX(VolumeFlow!$A44:$B56,MATCH('Average Properties Calc'!$A45,VolumeFlow!$A44:$A56,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K45" t="s">
@@ -5235,39 +5235,39 @@
         <v>Lung</v>
       </c>
       <c r="B46" s="2" t="e">
-        <f>TissueComp!D$10*INDEX(VolumeFlow!$A44:$B56,MATCH('Average Properties Calc'!$A46,VolumeFlow!$A44:$A56,0),4)</f>
+        <f>TissueComp!D$10*INDEX(VolumeFlow!$A45:$B57,MATCH('Average Properties Calc'!$A46,VolumeFlow!$A45:$A57,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C46" s="2" t="e">
-        <f>TissueComp!E$10*INDEX(VolumeFlow!$A44:$B56,MATCH('Average Properties Calc'!$A46,VolumeFlow!$A44:$A56,0),4)</f>
+        <f>TissueComp!E$10*INDEX(VolumeFlow!$A45:$B57,MATCH('Average Properties Calc'!$A46,VolumeFlow!$A45:$A57,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D46" s="2" t="e">
-        <f>TissueComp!F$10*INDEX(VolumeFlow!$A44:$B56,MATCH('Average Properties Calc'!$A46,VolumeFlow!$A44:$A56,0),4)</f>
+        <f>TissueComp!F$10*INDEX(VolumeFlow!$A45:$B57,MATCH('Average Properties Calc'!$A46,VolumeFlow!$A45:$A57,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E46" s="2" t="e">
-        <f>TissueComp!G$10*INDEX(VolumeFlow!$A44:$B56,MATCH('Average Properties Calc'!$A46,VolumeFlow!$A44:$A56,0),4)</f>
+        <f>TissueComp!G$10*INDEX(VolumeFlow!$A45:$B57,MATCH('Average Properties Calc'!$A46,VolumeFlow!$A45:$A57,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F46" s="2" t="e">
-        <f>TissueComp!H$10*INDEX(VolumeFlow!$A44:$B56,MATCH('Average Properties Calc'!$A46,VolumeFlow!$A44:$A56,0),4)</f>
+        <f>TissueComp!H$10*INDEX(VolumeFlow!$A45:$B57,MATCH('Average Properties Calc'!$A46,VolumeFlow!$A45:$A57,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G46" s="2" t="e">
-        <f>TissueComp!I$10*INDEX(VolumeFlow!$A44:$B56,MATCH('Average Properties Calc'!$A46,VolumeFlow!$A44:$A56,0),4)</f>
+        <f>TissueComp!I$10*INDEX(VolumeFlow!$A45:$B57,MATCH('Average Properties Calc'!$A46,VolumeFlow!$A45:$A57,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H46" s="2" t="e">
-        <f>TissueComp!J$10*INDEX(VolumeFlow!$A44:$B56,MATCH('Average Properties Calc'!$A46,VolumeFlow!$A44:$A56,0),4)</f>
+        <f>TissueComp!J$10*INDEX(VolumeFlow!$A45:$B57,MATCH('Average Properties Calc'!$A46,VolumeFlow!$A45:$A57,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I46" s="2" t="e">
-        <f>TissueComp!K$10*INDEX(VolumeFlow!$A44:$B56,MATCH('Average Properties Calc'!$A46,VolumeFlow!$A44:$A56,0),4)</f>
+        <f>TissueComp!K$10*INDEX(VolumeFlow!$A45:$B57,MATCH('Average Properties Calc'!$A46,VolumeFlow!$A45:$A57,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J46" s="2" t="e">
-        <f>TissueComp!L$10*INDEX(VolumeFlow!$A44:$B56,MATCH('Average Properties Calc'!$A46,VolumeFlow!$A44:$A56,0),4)</f>
+        <f>TissueComp!L$10*INDEX(VolumeFlow!$A45:$B57,MATCH('Average Properties Calc'!$A46,VolumeFlow!$A45:$A57,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K46" t="s">
@@ -5280,39 +5280,39 @@
         <v>Muscle</v>
       </c>
       <c r="B47" s="2" t="e">
-        <f>TissueComp!D$11*INDEX(VolumeFlow!$A45:$B57,MATCH('Average Properties Calc'!$A47,VolumeFlow!$A45:$A57,0),4)</f>
+        <f>TissueComp!D$11*INDEX(VolumeFlow!$A46:$B58,MATCH('Average Properties Calc'!$A47,VolumeFlow!$A46:$A58,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C47" s="2" t="e">
-        <f>TissueComp!E$11*INDEX(VolumeFlow!$A45:$B57,MATCH('Average Properties Calc'!$A47,VolumeFlow!$A45:$A57,0),4)</f>
+        <f>TissueComp!E$11*INDEX(VolumeFlow!$A46:$B58,MATCH('Average Properties Calc'!$A47,VolumeFlow!$A46:$A58,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D47" s="2" t="e">
-        <f>TissueComp!F$11*INDEX(VolumeFlow!$A45:$B57,MATCH('Average Properties Calc'!$A47,VolumeFlow!$A45:$A57,0),4)</f>
+        <f>TissueComp!F$11*INDEX(VolumeFlow!$A46:$B58,MATCH('Average Properties Calc'!$A47,VolumeFlow!$A46:$A58,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E47" s="2" t="e">
-        <f>TissueComp!G$11*INDEX(VolumeFlow!$A45:$B57,MATCH('Average Properties Calc'!$A47,VolumeFlow!$A45:$A57,0),4)</f>
+        <f>TissueComp!G$11*INDEX(VolumeFlow!$A46:$B58,MATCH('Average Properties Calc'!$A47,VolumeFlow!$A46:$A58,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F47" s="2" t="e">
-        <f>TissueComp!H$11*INDEX(VolumeFlow!$A45:$B57,MATCH('Average Properties Calc'!$A47,VolumeFlow!$A45:$A57,0),4)</f>
+        <f>TissueComp!H$11*INDEX(VolumeFlow!$A46:$B58,MATCH('Average Properties Calc'!$A47,VolumeFlow!$A46:$A58,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G47" s="2" t="e">
-        <f>TissueComp!I$11*INDEX(VolumeFlow!$A45:$B57,MATCH('Average Properties Calc'!$A47,VolumeFlow!$A45:$A57,0),4)</f>
+        <f>TissueComp!I$11*INDEX(VolumeFlow!$A46:$B58,MATCH('Average Properties Calc'!$A47,VolumeFlow!$A46:$A58,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H47" s="2" t="e">
-        <f>TissueComp!J$11*INDEX(VolumeFlow!$A45:$B57,MATCH('Average Properties Calc'!$A47,VolumeFlow!$A45:$A57,0),4)</f>
+        <f>TissueComp!J$11*INDEX(VolumeFlow!$A46:$B58,MATCH('Average Properties Calc'!$A47,VolumeFlow!$A46:$A58,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I47" s="2" t="e">
-        <f>TissueComp!K$11*INDEX(VolumeFlow!$A45:$B57,MATCH('Average Properties Calc'!$A47,VolumeFlow!$A45:$A57,0),4)</f>
+        <f>TissueComp!K$11*INDEX(VolumeFlow!$A46:$B58,MATCH('Average Properties Calc'!$A47,VolumeFlow!$A46:$A58,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J47" s="2" t="e">
-        <f>TissueComp!L$11*INDEX(VolumeFlow!$A45:$B57,MATCH('Average Properties Calc'!$A47,VolumeFlow!$A45:$A57,0),4)</f>
+        <f>TissueComp!L$11*INDEX(VolumeFlow!$A46:$B58,MATCH('Average Properties Calc'!$A47,VolumeFlow!$A46:$A58,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K47" t="s">
@@ -5325,39 +5325,39 @@
         <v>Skin</v>
       </c>
       <c r="B48" s="2" t="e">
-        <f>TissueComp!D$12*INDEX(VolumeFlow!$A46:$B58,MATCH('Average Properties Calc'!$A48,VolumeFlow!$A46:$A58,0),4)</f>
+        <f>TissueComp!D$12*INDEX(VolumeFlow!$A47:$B59,MATCH('Average Properties Calc'!$A48,VolumeFlow!$A47:$A59,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C48" s="2" t="e">
-        <f>TissueComp!E$12*INDEX(VolumeFlow!$A46:$B58,MATCH('Average Properties Calc'!$A48,VolumeFlow!$A46:$A58,0),4)</f>
+        <f>TissueComp!E$12*INDEX(VolumeFlow!$A47:$B59,MATCH('Average Properties Calc'!$A48,VolumeFlow!$A47:$A59,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D48" s="2" t="e">
-        <f>TissueComp!F$12*INDEX(VolumeFlow!$A46:$B58,MATCH('Average Properties Calc'!$A48,VolumeFlow!$A46:$A58,0),4)</f>
+        <f>TissueComp!F$12*INDEX(VolumeFlow!$A47:$B59,MATCH('Average Properties Calc'!$A48,VolumeFlow!$A47:$A59,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E48" s="2" t="e">
-        <f>TissueComp!G$12*INDEX(VolumeFlow!$A46:$B58,MATCH('Average Properties Calc'!$A48,VolumeFlow!$A46:$A58,0),4)</f>
+        <f>TissueComp!G$12*INDEX(VolumeFlow!$A47:$B59,MATCH('Average Properties Calc'!$A48,VolumeFlow!$A47:$A59,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F48" s="2" t="e">
-        <f>TissueComp!H$12*INDEX(VolumeFlow!$A46:$B58,MATCH('Average Properties Calc'!$A48,VolumeFlow!$A46:$A58,0),4)</f>
+        <f>TissueComp!H$12*INDEX(VolumeFlow!$A47:$B59,MATCH('Average Properties Calc'!$A48,VolumeFlow!$A47:$A59,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G48" s="2" t="e">
-        <f>TissueComp!I$12*INDEX(VolumeFlow!$A46:$B58,MATCH('Average Properties Calc'!$A48,VolumeFlow!$A46:$A58,0),4)</f>
+        <f>TissueComp!I$12*INDEX(VolumeFlow!$A47:$B59,MATCH('Average Properties Calc'!$A48,VolumeFlow!$A47:$A59,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H48" s="2" t="e">
-        <f>TissueComp!J$12*INDEX(VolumeFlow!$A46:$B58,MATCH('Average Properties Calc'!$A48,VolumeFlow!$A46:$A58,0),4)</f>
+        <f>TissueComp!J$12*INDEX(VolumeFlow!$A47:$B59,MATCH('Average Properties Calc'!$A48,VolumeFlow!$A47:$A59,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I48" s="2" t="e">
-        <f>TissueComp!K$12*INDEX(VolumeFlow!$A46:$B58,MATCH('Average Properties Calc'!$A48,VolumeFlow!$A46:$A58,0),4)</f>
+        <f>TissueComp!K$12*INDEX(VolumeFlow!$A47:$B59,MATCH('Average Properties Calc'!$A48,VolumeFlow!$A47:$A59,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J48" s="2" t="e">
-        <f>TissueComp!L$12*INDEX(VolumeFlow!$A46:$B58,MATCH('Average Properties Calc'!$A48,VolumeFlow!$A46:$A58,0),4)</f>
+        <f>TissueComp!L$12*INDEX(VolumeFlow!$A47:$B59,MATCH('Average Properties Calc'!$A48,VolumeFlow!$A47:$A59,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K48" t="s">
@@ -5370,39 +5370,39 @@
         <v>Spleen</v>
       </c>
       <c r="B49" s="2" t="e">
-        <f>TissueComp!D$13*INDEX(VolumeFlow!$A47:$B59,MATCH('Average Properties Calc'!$A49,VolumeFlow!$A47:$A59,0),4)</f>
+        <f>TissueComp!D$13*INDEX(VolumeFlow!$A48:$B60,MATCH('Average Properties Calc'!$A49,VolumeFlow!$A48:$A60,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C49" s="2" t="e">
-        <f>TissueComp!E$13*INDEX(VolumeFlow!$A47:$B59,MATCH('Average Properties Calc'!$A49,VolumeFlow!$A47:$A59,0),4)</f>
+        <f>TissueComp!E$13*INDEX(VolumeFlow!$A48:$B60,MATCH('Average Properties Calc'!$A49,VolumeFlow!$A48:$A60,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D49" s="2" t="e">
-        <f>TissueComp!F$13*INDEX(VolumeFlow!$A47:$B59,MATCH('Average Properties Calc'!$A49,VolumeFlow!$A47:$A59,0),4)</f>
+        <f>TissueComp!F$13*INDEX(VolumeFlow!$A48:$B60,MATCH('Average Properties Calc'!$A49,VolumeFlow!$A48:$A60,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E49" s="2" t="e">
-        <f>TissueComp!G$13*INDEX(VolumeFlow!$A47:$B59,MATCH('Average Properties Calc'!$A49,VolumeFlow!$A47:$A59,0),4)</f>
+        <f>TissueComp!G$13*INDEX(VolumeFlow!$A48:$B60,MATCH('Average Properties Calc'!$A49,VolumeFlow!$A48:$A60,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F49" s="2" t="e">
-        <f>TissueComp!H$13*INDEX(VolumeFlow!$A47:$B59,MATCH('Average Properties Calc'!$A49,VolumeFlow!$A47:$A59,0),4)</f>
+        <f>TissueComp!H$13*INDEX(VolumeFlow!$A48:$B60,MATCH('Average Properties Calc'!$A49,VolumeFlow!$A48:$A60,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G49" s="2" t="e">
-        <f>TissueComp!I$13*INDEX(VolumeFlow!$A47:$B59,MATCH('Average Properties Calc'!$A49,VolumeFlow!$A47:$A59,0),4)</f>
+        <f>TissueComp!I$13*INDEX(VolumeFlow!$A48:$B60,MATCH('Average Properties Calc'!$A49,VolumeFlow!$A48:$A60,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H49" s="2" t="e">
-        <f>TissueComp!J$13*INDEX(VolumeFlow!$A47:$B59,MATCH('Average Properties Calc'!$A49,VolumeFlow!$A47:$A59,0),4)</f>
+        <f>TissueComp!J$13*INDEX(VolumeFlow!$A48:$B60,MATCH('Average Properties Calc'!$A49,VolumeFlow!$A48:$A60,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I49" s="2" t="e">
-        <f>TissueComp!K$13*INDEX(VolumeFlow!$A47:$B59,MATCH('Average Properties Calc'!$A49,VolumeFlow!$A47:$A59,0),4)</f>
+        <f>TissueComp!K$13*INDEX(VolumeFlow!$A48:$B60,MATCH('Average Properties Calc'!$A49,VolumeFlow!$A48:$A60,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J49" s="2" t="e">
-        <f>TissueComp!L$13*INDEX(VolumeFlow!$A47:$B59,MATCH('Average Properties Calc'!$A49,VolumeFlow!$A47:$A59,0),4)</f>
+        <f>TissueComp!L$13*INDEX(VolumeFlow!$A48:$B60,MATCH('Average Properties Calc'!$A49,VolumeFlow!$A48:$A60,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K49" t="s">
@@ -5453,39 +5453,39 @@
         <v>Adipose</v>
       </c>
       <c r="B51" s="2" t="e">
-        <f>TissueComp!D$3*INDEX(VolumeFlow!$A49:$B61,MATCH('Average Properties Calc'!$A51,VolumeFlow!$A49:$A61,0),4)</f>
+        <f>TissueComp!D$3*INDEX(VolumeFlow!$A50:$B62,MATCH('Average Properties Calc'!$A51,VolumeFlow!$A50:$A62,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C51" s="2" t="e">
-        <f>TissueComp!E$3*INDEX(VolumeFlow!$A49:$B61,MATCH('Average Properties Calc'!$A51,VolumeFlow!$A49:$A61,0),4)</f>
+        <f>TissueComp!E$3*INDEX(VolumeFlow!$A50:$B62,MATCH('Average Properties Calc'!$A51,VolumeFlow!$A50:$A62,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D51" s="2" t="e">
-        <f>TissueComp!F$3*INDEX(VolumeFlow!$A49:$B61,MATCH('Average Properties Calc'!$A51,VolumeFlow!$A49:$A61,0),4)</f>
+        <f>TissueComp!F$3*INDEX(VolumeFlow!$A50:$B62,MATCH('Average Properties Calc'!$A51,VolumeFlow!$A50:$A62,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E51" s="2" t="e">
-        <f>TissueComp!G$3*INDEX(VolumeFlow!$A49:$B61,MATCH('Average Properties Calc'!$A51,VolumeFlow!$A49:$A61,0),4)</f>
+        <f>TissueComp!G$3*INDEX(VolumeFlow!$A50:$B62,MATCH('Average Properties Calc'!$A51,VolumeFlow!$A50:$A62,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F51" s="2" t="e">
-        <f>TissueComp!H$3*INDEX(VolumeFlow!$A49:$B61,MATCH('Average Properties Calc'!$A51,VolumeFlow!$A49:$A61,0),4)</f>
+        <f>TissueComp!H$3*INDEX(VolumeFlow!$A50:$B62,MATCH('Average Properties Calc'!$A51,VolumeFlow!$A50:$A62,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G51" s="2" t="e">
-        <f>TissueComp!I$3*INDEX(VolumeFlow!$A49:$B61,MATCH('Average Properties Calc'!$A51,VolumeFlow!$A49:$A61,0),4)</f>
+        <f>TissueComp!I$3*INDEX(VolumeFlow!$A50:$B62,MATCH('Average Properties Calc'!$A51,VolumeFlow!$A50:$A62,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H51" s="2" t="e">
-        <f>TissueComp!J$3*INDEX(VolumeFlow!$A49:$B61,MATCH('Average Properties Calc'!$A51,VolumeFlow!$A49:$A61,0),4)</f>
+        <f>TissueComp!J$3*INDEX(VolumeFlow!$A50:$B62,MATCH('Average Properties Calc'!$A51,VolumeFlow!$A50:$A62,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I51" s="2" t="e">
-        <f>TissueComp!K$3*INDEX(VolumeFlow!$A49:$B61,MATCH('Average Properties Calc'!$A51,VolumeFlow!$A49:$A61,0),4)</f>
+        <f>TissueComp!K$3*INDEX(VolumeFlow!$A50:$B62,MATCH('Average Properties Calc'!$A51,VolumeFlow!$A50:$A62,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J51" s="2" t="e">
-        <f>TissueComp!L$3*INDEX(VolumeFlow!$A49:$B61,MATCH('Average Properties Calc'!$A51,VolumeFlow!$A49:$A61,0),4)</f>
+        <f>TissueComp!L$3*INDEX(VolumeFlow!$A50:$B62,MATCH('Average Properties Calc'!$A51,VolumeFlow!$A50:$A62,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K51" t="s">
@@ -5498,39 +5498,39 @@
         <v>Bone</v>
       </c>
       <c r="B52" s="2" t="e">
-        <f>TissueComp!D$4*INDEX(VolumeFlow!$A50:$B75,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A50:$A75,0),4)</f>
+        <f>TissueComp!D$4*INDEX(VolumeFlow!$A51:$B76,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A51:$A76,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C52" s="2" t="e">
-        <f>TissueComp!E$4*INDEX(VolumeFlow!$A50:$B75,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A50:$A75,0),4)</f>
+        <f>TissueComp!E$4*INDEX(VolumeFlow!$A51:$B76,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A51:$A76,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D52" s="2" t="e">
-        <f>TissueComp!F$4*INDEX(VolumeFlow!$A50:$B75,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A50:$A75,0),4)</f>
+        <f>TissueComp!F$4*INDEX(VolumeFlow!$A51:$B76,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A51:$A76,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E52" s="2" t="e">
-        <f>TissueComp!G$4*INDEX(VolumeFlow!$A50:$B75,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A50:$A75,0),4)</f>
+        <f>TissueComp!G$4*INDEX(VolumeFlow!$A51:$B76,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A51:$A76,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F52" s="2" t="e">
-        <f>TissueComp!H$4*INDEX(VolumeFlow!$A50:$B75,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A50:$A75,0),4)</f>
+        <f>TissueComp!H$4*INDEX(VolumeFlow!$A51:$B76,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A51:$A76,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G52" s="2" t="e">
-        <f>TissueComp!I$4*INDEX(VolumeFlow!$A50:$B75,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A50:$A75,0),4)</f>
+        <f>TissueComp!I$4*INDEX(VolumeFlow!$A51:$B76,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A51:$A76,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H52" s="2" t="e">
-        <f>TissueComp!J$4*INDEX(VolumeFlow!$A50:$B75,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A50:$A75,0),4)</f>
+        <f>TissueComp!J$4*INDEX(VolumeFlow!$A51:$B76,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A51:$A76,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I52" s="2" t="e">
-        <f>TissueComp!K$4*INDEX(VolumeFlow!$A50:$B75,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A50:$A75,0),4)</f>
+        <f>TissueComp!K$4*INDEX(VolumeFlow!$A51:$B76,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A51:$A76,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J52" s="2" t="e">
-        <f>TissueComp!L$4*INDEX(VolumeFlow!$A50:$B75,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A50:$A75,0),4)</f>
+        <f>TissueComp!L$4*INDEX(VolumeFlow!$A51:$B76,MATCH('Average Properties Calc'!$A52,VolumeFlow!$A51:$A76,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K52" t="s">
@@ -5543,39 +5543,39 @@
         <v>Brain</v>
       </c>
       <c r="B53" s="2" t="e">
-        <f>TissueComp!D$5*INDEX(VolumeFlow!$A51:$B76,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A51:$A76,0),4)</f>
+        <f>TissueComp!D$5*INDEX(VolumeFlow!$A52:$B77,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A52:$A77,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C53" s="2" t="e">
-        <f>TissueComp!E$5*INDEX(VolumeFlow!$A51:$B76,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A51:$A76,0),4)</f>
+        <f>TissueComp!E$5*INDEX(VolumeFlow!$A52:$B77,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A52:$A77,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D53" s="2" t="e">
-        <f>TissueComp!F$5*INDEX(VolumeFlow!$A51:$B76,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A51:$A76,0),4)</f>
+        <f>TissueComp!F$5*INDEX(VolumeFlow!$A52:$B77,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A52:$A77,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E53" s="2" t="e">
-        <f>TissueComp!G$5*INDEX(VolumeFlow!$A51:$B76,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A51:$A76,0),4)</f>
+        <f>TissueComp!G$5*INDEX(VolumeFlow!$A52:$B77,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A52:$A77,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F53" s="2" t="e">
-        <f>TissueComp!H$5*INDEX(VolumeFlow!$A51:$B76,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A51:$A76,0),4)</f>
+        <f>TissueComp!H$5*INDEX(VolumeFlow!$A52:$B77,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A52:$A77,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G53" s="2" t="e">
-        <f>TissueComp!I$5*INDEX(VolumeFlow!$A51:$B76,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A51:$A76,0),4)</f>
+        <f>TissueComp!I$5*INDEX(VolumeFlow!$A52:$B77,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A52:$A77,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H53" s="2" t="e">
-        <f>TissueComp!J$5*INDEX(VolumeFlow!$A51:$B76,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A51:$A76,0),4)</f>
+        <f>TissueComp!J$5*INDEX(VolumeFlow!$A52:$B77,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A52:$A77,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I53" s="2" t="e">
-        <f>TissueComp!K$5*INDEX(VolumeFlow!$A51:$B76,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A51:$A76,0),4)</f>
+        <f>TissueComp!K$5*INDEX(VolumeFlow!$A52:$B77,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A52:$A77,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J53" s="2" t="e">
-        <f>TissueComp!L$5*INDEX(VolumeFlow!$A51:$B76,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A51:$A76,0),4)</f>
+        <f>TissueComp!L$5*INDEX(VolumeFlow!$A52:$B77,MATCH('Average Properties Calc'!$A53,VolumeFlow!$A52:$A77,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K53" t="s">
@@ -5588,39 +5588,39 @@
         <v>Gut</v>
       </c>
       <c r="B54" s="2" t="e">
-        <f>TissueComp!D$6*INDEX(VolumeFlow!$A52:$B77,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A52:$A77,0),4)</f>
+        <f>TissueComp!D$6*INDEX(VolumeFlow!$A53:$B78,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A53:$A78,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C54" s="2" t="e">
-        <f>TissueComp!E$6*INDEX(VolumeFlow!$A52:$B77,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A52:$A77,0),4)</f>
+        <f>TissueComp!E$6*INDEX(VolumeFlow!$A53:$B78,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A53:$A78,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D54" s="2" t="e">
-        <f>TissueComp!F$6*INDEX(VolumeFlow!$A52:$B77,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A52:$A77,0),4)</f>
+        <f>TissueComp!F$6*INDEX(VolumeFlow!$A53:$B78,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A53:$A78,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E54" s="2" t="e">
-        <f>TissueComp!G$6*INDEX(VolumeFlow!$A52:$B77,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A52:$A77,0),4)</f>
+        <f>TissueComp!G$6*INDEX(VolumeFlow!$A53:$B78,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A53:$A78,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F54" s="2" t="e">
-        <f>TissueComp!H$6*INDEX(VolumeFlow!$A52:$B77,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A52:$A77,0),4)</f>
+        <f>TissueComp!H$6*INDEX(VolumeFlow!$A53:$B78,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A53:$A78,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G54" s="2" t="e">
-        <f>TissueComp!I$6*INDEX(VolumeFlow!$A52:$B77,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A52:$A77,0),4)</f>
+        <f>TissueComp!I$6*INDEX(VolumeFlow!$A53:$B78,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A53:$A78,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H54" s="2" t="e">
-        <f>TissueComp!J$6*INDEX(VolumeFlow!$A52:$B77,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A52:$A77,0),4)</f>
+        <f>TissueComp!J$6*INDEX(VolumeFlow!$A53:$B78,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A53:$A78,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I54" s="2" t="e">
-        <f>TissueComp!K$6*INDEX(VolumeFlow!$A52:$B77,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A52:$A77,0),4)</f>
+        <f>TissueComp!K$6*INDEX(VolumeFlow!$A53:$B78,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A53:$A78,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J54" s="2" t="e">
-        <f>TissueComp!L$6*INDEX(VolumeFlow!$A52:$B77,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A52:$A77,0),4)</f>
+        <f>TissueComp!L$6*INDEX(VolumeFlow!$A53:$B78,MATCH('Average Properties Calc'!$A54,VolumeFlow!$A53:$A78,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K54" t="s">
@@ -5633,39 +5633,39 @@
         <v>Heart</v>
       </c>
       <c r="B55" s="2" t="e">
-        <f>TissueComp!D$7*INDEX(VolumeFlow!$A53:$B78,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A53:$A78,0),4)</f>
+        <f>TissueComp!D$7*INDEX(VolumeFlow!$A54:$B79,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A54:$A79,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C55" s="2" t="e">
-        <f>TissueComp!E$7*INDEX(VolumeFlow!$A53:$B78,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A53:$A78,0),4)</f>
+        <f>TissueComp!E$7*INDEX(VolumeFlow!$A54:$B79,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A54:$A79,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D55" s="2" t="e">
-        <f>TissueComp!F$7*INDEX(VolumeFlow!$A53:$B78,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A53:$A78,0),4)</f>
+        <f>TissueComp!F$7*INDEX(VolumeFlow!$A54:$B79,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A54:$A79,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E55" s="2" t="e">
-        <f>TissueComp!G$7*INDEX(VolumeFlow!$A53:$B78,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A53:$A78,0),4)</f>
+        <f>TissueComp!G$7*INDEX(VolumeFlow!$A54:$B79,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A54:$A79,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F55" s="2" t="e">
-        <f>TissueComp!H$7*INDEX(VolumeFlow!$A53:$B78,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A53:$A78,0),4)</f>
+        <f>TissueComp!H$7*INDEX(VolumeFlow!$A54:$B79,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A54:$A79,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G55" s="2" t="e">
-        <f>TissueComp!I$7*INDEX(VolumeFlow!$A53:$B78,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A53:$A78,0),4)</f>
+        <f>TissueComp!I$7*INDEX(VolumeFlow!$A54:$B79,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A54:$A79,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H55" s="2" t="e">
-        <f>TissueComp!J$7*INDEX(VolumeFlow!$A53:$B78,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A53:$A78,0),4)</f>
+        <f>TissueComp!J$7*INDEX(VolumeFlow!$A54:$B79,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A54:$A79,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I55" s="2" t="e">
-        <f>TissueComp!K$7*INDEX(VolumeFlow!$A53:$B78,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A53:$A78,0),4)</f>
+        <f>TissueComp!K$7*INDEX(VolumeFlow!$A54:$B79,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A54:$A79,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J55" s="2" t="e">
-        <f>TissueComp!L$7*INDEX(VolumeFlow!$A53:$B78,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A53:$A78,0),4)</f>
+        <f>TissueComp!L$7*INDEX(VolumeFlow!$A54:$B79,MATCH('Average Properties Calc'!$A55,VolumeFlow!$A54:$A79,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K55" t="s">
@@ -5678,39 +5678,39 @@
         <v>Kidney</v>
       </c>
       <c r="B56" s="2" t="e">
-        <f>TissueComp!D$8*INDEX(VolumeFlow!$A54:$B78,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A54:$A78,0),4)</f>
+        <f>TissueComp!D$8*INDEX(VolumeFlow!$A55:$B79,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A55:$A79,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C56" s="2" t="e">
-        <f>TissueComp!E$8*INDEX(VolumeFlow!$A54:$B78,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A54:$A78,0),4)</f>
+        <f>TissueComp!E$8*INDEX(VolumeFlow!$A55:$B79,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A55:$A79,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D56" s="2" t="e">
-        <f>TissueComp!F$8*INDEX(VolumeFlow!$A54:$B78,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A54:$A78,0),4)</f>
+        <f>TissueComp!F$8*INDEX(VolumeFlow!$A55:$B79,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A55:$A79,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E56" s="2" t="e">
-        <f>TissueComp!G$8*INDEX(VolumeFlow!$A54:$B78,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A54:$A78,0),4)</f>
+        <f>TissueComp!G$8*INDEX(VolumeFlow!$A55:$B79,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A55:$A79,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F56" s="2" t="e">
-        <f>TissueComp!H$8*INDEX(VolumeFlow!$A54:$B78,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A54:$A78,0),4)</f>
+        <f>TissueComp!H$8*INDEX(VolumeFlow!$A55:$B79,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A55:$A79,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G56" s="2" t="e">
-        <f>TissueComp!I$8*INDEX(VolumeFlow!$A54:$B78,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A54:$A78,0),4)</f>
+        <f>TissueComp!I$8*INDEX(VolumeFlow!$A55:$B79,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A55:$A79,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H56" s="2" t="e">
-        <f>TissueComp!J$8*INDEX(VolumeFlow!$A54:$B78,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A54:$A78,0),4)</f>
+        <f>TissueComp!J$8*INDEX(VolumeFlow!$A55:$B79,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A55:$A79,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I56" s="2" t="e">
-        <f>TissueComp!K$8*INDEX(VolumeFlow!$A54:$B78,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A54:$A78,0),4)</f>
+        <f>TissueComp!K$8*INDEX(VolumeFlow!$A55:$B79,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A55:$A79,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J56" s="2" t="e">
-        <f>TissueComp!L$8*INDEX(VolumeFlow!$A54:$B78,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A54:$A78,0),4)</f>
+        <f>TissueComp!L$8*INDEX(VolumeFlow!$A55:$B79,MATCH('Average Properties Calc'!$A56,VolumeFlow!$A55:$A79,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K56" t="s">
@@ -5723,39 +5723,39 @@
         <v>Liver</v>
       </c>
       <c r="B57" s="2" t="e">
-        <f>TissueComp!D$9*INDEX(VolumeFlow!$A55:$B79,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A55:$A79,0),4)</f>
+        <f>TissueComp!D$9*INDEX(VolumeFlow!$A56:$B80,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A56:$A80,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C57" s="2" t="e">
-        <f>TissueComp!E$9*INDEX(VolumeFlow!$A55:$B79,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A55:$A79,0),4)</f>
+        <f>TissueComp!E$9*INDEX(VolumeFlow!$A56:$B80,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A56:$A80,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D57" s="2" t="e">
-        <f>TissueComp!F$9*INDEX(VolumeFlow!$A55:$B79,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A55:$A79,0),4)</f>
+        <f>TissueComp!F$9*INDEX(VolumeFlow!$A56:$B80,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A56:$A80,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E57" s="2" t="e">
-        <f>TissueComp!G$9*INDEX(VolumeFlow!$A55:$B79,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A55:$A79,0),4)</f>
+        <f>TissueComp!G$9*INDEX(VolumeFlow!$A56:$B80,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A56:$A80,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F57" s="2" t="e">
-        <f>TissueComp!H$9*INDEX(VolumeFlow!$A55:$B79,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A55:$A79,0),4)</f>
+        <f>TissueComp!H$9*INDEX(VolumeFlow!$A56:$B80,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A56:$A80,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G57" s="2" t="e">
-        <f>TissueComp!I$9*INDEX(VolumeFlow!$A55:$B79,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A55:$A79,0),4)</f>
+        <f>TissueComp!I$9*INDEX(VolumeFlow!$A56:$B80,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A56:$A80,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H57" s="2" t="e">
-        <f>TissueComp!J$9*INDEX(VolumeFlow!$A55:$B79,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A55:$A79,0),4)</f>
+        <f>TissueComp!J$9*INDEX(VolumeFlow!$A56:$B80,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A56:$A80,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I57" s="2" t="e">
-        <f>TissueComp!K$9*INDEX(VolumeFlow!$A55:$B79,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A55:$A79,0),4)</f>
+        <f>TissueComp!K$9*INDEX(VolumeFlow!$A56:$B80,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A56:$A80,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J57" s="2" t="e">
-        <f>TissueComp!L$9*INDEX(VolumeFlow!$A55:$B79,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A55:$A79,0),4)</f>
+        <f>TissueComp!L$9*INDEX(VolumeFlow!$A56:$B80,MATCH('Average Properties Calc'!$A57,VolumeFlow!$A56:$A80,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K57" t="s">
@@ -5768,39 +5768,39 @@
         <v>Lung</v>
       </c>
       <c r="B58" s="2" t="e">
-        <f>TissueComp!D$10*INDEX(VolumeFlow!$A56:$B80,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A56:$A80,0),4)</f>
+        <f>TissueComp!D$10*INDEX(VolumeFlow!$A57:$B81,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A57:$A81,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C58" s="2" t="e">
-        <f>TissueComp!E$10*INDEX(VolumeFlow!$A56:$B80,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A56:$A80,0),4)</f>
+        <f>TissueComp!E$10*INDEX(VolumeFlow!$A57:$B81,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A57:$A81,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D58" s="2" t="e">
-        <f>TissueComp!F$10*INDEX(VolumeFlow!$A56:$B80,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A56:$A80,0),4)</f>
+        <f>TissueComp!F$10*INDEX(VolumeFlow!$A57:$B81,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A57:$A81,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E58" s="2" t="e">
-        <f>TissueComp!G$10*INDEX(VolumeFlow!$A56:$B80,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A56:$A80,0),4)</f>
+        <f>TissueComp!G$10*INDEX(VolumeFlow!$A57:$B81,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A57:$A81,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F58" s="2" t="e">
-        <f>TissueComp!H$10*INDEX(VolumeFlow!$A56:$B80,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A56:$A80,0),4)</f>
+        <f>TissueComp!H$10*INDEX(VolumeFlow!$A57:$B81,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A57:$A81,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G58" s="2" t="e">
-        <f>TissueComp!I$10*INDEX(VolumeFlow!$A56:$B80,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A56:$A80,0),4)</f>
+        <f>TissueComp!I$10*INDEX(VolumeFlow!$A57:$B81,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A57:$A81,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H58" s="2" t="e">
-        <f>TissueComp!J$10*INDEX(VolumeFlow!$A56:$B80,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A56:$A80,0),4)</f>
+        <f>TissueComp!J$10*INDEX(VolumeFlow!$A57:$B81,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A57:$A81,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I58" s="2" t="e">
-        <f>TissueComp!K$10*INDEX(VolumeFlow!$A56:$B80,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A56:$A80,0),4)</f>
+        <f>TissueComp!K$10*INDEX(VolumeFlow!$A57:$B81,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A57:$A81,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J58" s="2" t="e">
-        <f>TissueComp!L$10*INDEX(VolumeFlow!$A56:$B80,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A56:$A80,0),4)</f>
+        <f>TissueComp!L$10*INDEX(VolumeFlow!$A57:$B81,MATCH('Average Properties Calc'!$A58,VolumeFlow!$A57:$A81,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K58" t="s">
@@ -5813,39 +5813,39 @@
         <v>Muscle</v>
       </c>
       <c r="B59" s="2" t="e">
-        <f>TissueComp!D$11*INDEX(VolumeFlow!$A57:$B81,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A57:$A81,0),4)</f>
+        <f>TissueComp!D$11*INDEX(VolumeFlow!$A58:$B82,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A58:$A82,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C59" s="2" t="e">
-        <f>TissueComp!E$11*INDEX(VolumeFlow!$A57:$B81,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A57:$A81,0),4)</f>
+        <f>TissueComp!E$11*INDEX(VolumeFlow!$A58:$B82,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A58:$A82,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D59" s="2" t="e">
-        <f>TissueComp!F$11*INDEX(VolumeFlow!$A57:$B81,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A57:$A81,0),4)</f>
+        <f>TissueComp!F$11*INDEX(VolumeFlow!$A58:$B82,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A58:$A82,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E59" s="2" t="e">
-        <f>TissueComp!G$11*INDEX(VolumeFlow!$A57:$B81,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A57:$A81,0),4)</f>
+        <f>TissueComp!G$11*INDEX(VolumeFlow!$A58:$B82,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A58:$A82,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F59" s="2" t="e">
-        <f>TissueComp!H$11*INDEX(VolumeFlow!$A57:$B81,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A57:$A81,0),4)</f>
+        <f>TissueComp!H$11*INDEX(VolumeFlow!$A58:$B82,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A58:$A82,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G59" s="2" t="e">
-        <f>TissueComp!I$11*INDEX(VolumeFlow!$A57:$B81,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A57:$A81,0),4)</f>
+        <f>TissueComp!I$11*INDEX(VolumeFlow!$A58:$B82,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A58:$A82,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H59" s="2" t="e">
-        <f>TissueComp!J$11*INDEX(VolumeFlow!$A57:$B81,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A57:$A81,0),4)</f>
+        <f>TissueComp!J$11*INDEX(VolumeFlow!$A58:$B82,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A58:$A82,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I59" s="2" t="e">
-        <f>TissueComp!K$11*INDEX(VolumeFlow!$A57:$B81,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A57:$A81,0),4)</f>
+        <f>TissueComp!K$11*INDEX(VolumeFlow!$A58:$B82,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A58:$A82,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J59" s="2" t="e">
-        <f>TissueComp!L$11*INDEX(VolumeFlow!$A57:$B81,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A57:$A81,0),4)</f>
+        <f>TissueComp!L$11*INDEX(VolumeFlow!$A58:$B82,MATCH('Average Properties Calc'!$A59,VolumeFlow!$A58:$A82,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K59" t="s">
@@ -5858,39 +5858,39 @@
         <v>Skin</v>
       </c>
       <c r="B60" s="2" t="e">
-        <f>TissueComp!D$12*INDEX(VolumeFlow!$A58:$B82,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A58:$A82,0),4)</f>
+        <f>TissueComp!D$12*INDEX(VolumeFlow!$A59:$B83,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A59:$A83,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C60" s="2" t="e">
-        <f>TissueComp!E$12*INDEX(VolumeFlow!$A58:$B82,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A58:$A82,0),4)</f>
+        <f>TissueComp!E$12*INDEX(VolumeFlow!$A59:$B83,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A59:$A83,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D60" s="2" t="e">
-        <f>TissueComp!F$12*INDEX(VolumeFlow!$A58:$B82,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A58:$A82,0),4)</f>
+        <f>TissueComp!F$12*INDEX(VolumeFlow!$A59:$B83,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A59:$A83,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E60" s="2" t="e">
-        <f>TissueComp!G$12*INDEX(VolumeFlow!$A58:$B82,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A58:$A82,0),4)</f>
+        <f>TissueComp!G$12*INDEX(VolumeFlow!$A59:$B83,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A59:$A83,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F60" s="2" t="e">
-        <f>TissueComp!H$12*INDEX(VolumeFlow!$A58:$B82,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A58:$A82,0),4)</f>
+        <f>TissueComp!H$12*INDEX(VolumeFlow!$A59:$B83,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A59:$A83,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G60" s="2" t="e">
-        <f>TissueComp!I$12*INDEX(VolumeFlow!$A58:$B82,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A58:$A82,0),4)</f>
+        <f>TissueComp!I$12*INDEX(VolumeFlow!$A59:$B83,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A59:$A83,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H60" s="2" t="e">
-        <f>TissueComp!J$12*INDEX(VolumeFlow!$A58:$B82,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A58:$A82,0),4)</f>
+        <f>TissueComp!J$12*INDEX(VolumeFlow!$A59:$B83,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A59:$A83,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I60" s="2" t="e">
-        <f>TissueComp!K$12*INDEX(VolumeFlow!$A58:$B82,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A58:$A82,0),4)</f>
+        <f>TissueComp!K$12*INDEX(VolumeFlow!$A59:$B83,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A59:$A83,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J60" s="2" t="e">
-        <f>TissueComp!L$12*INDEX(VolumeFlow!$A58:$B82,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A58:$A82,0),4)</f>
+        <f>TissueComp!L$12*INDEX(VolumeFlow!$A59:$B83,MATCH('Average Properties Calc'!$A60,VolumeFlow!$A59:$A83,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K60" t="s">
@@ -5903,39 +5903,39 @@
         <v>Spleen</v>
       </c>
       <c r="B61" s="2" t="e">
-        <f>TissueComp!D$13*INDEX(VolumeFlow!$A59:$B83,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A59:$A83,0),4)</f>
+        <f>TissueComp!D$13*INDEX(VolumeFlow!$A60:$B84,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A60:$A84,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="C61" s="2" t="e">
-        <f>TissueComp!E$13*INDEX(VolumeFlow!$A59:$B83,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A59:$A83,0),4)</f>
+        <f>TissueComp!E$13*INDEX(VolumeFlow!$A60:$B84,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A60:$A84,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="D61" s="2" t="e">
-        <f>TissueComp!F$13*INDEX(VolumeFlow!$A59:$B83,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A59:$A83,0),4)</f>
+        <f>TissueComp!F$13*INDEX(VolumeFlow!$A60:$B84,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A60:$A84,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="E61" s="2" t="e">
-        <f>TissueComp!G$13*INDEX(VolumeFlow!$A59:$B83,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A59:$A83,0),4)</f>
+        <f>TissueComp!G$13*INDEX(VolumeFlow!$A60:$B84,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A60:$A84,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="F61" s="2" t="e">
-        <f>TissueComp!H$13*INDEX(VolumeFlow!$A59:$B83,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A59:$A83,0),4)</f>
+        <f>TissueComp!H$13*INDEX(VolumeFlow!$A60:$B84,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A60:$A84,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="G61" s="2" t="e">
-        <f>TissueComp!I$13*INDEX(VolumeFlow!$A59:$B83,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A59:$A83,0),4)</f>
+        <f>TissueComp!I$13*INDEX(VolumeFlow!$A60:$B84,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A60:$A84,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="H61" s="2" t="e">
-        <f>TissueComp!J$13*INDEX(VolumeFlow!$A59:$B83,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A59:$A83,0),4)</f>
+        <f>TissueComp!J$13*INDEX(VolumeFlow!$A60:$B84,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A60:$A84,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="I61" s="2" t="e">
-        <f>TissueComp!K$13*INDEX(VolumeFlow!$A59:$B83,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A59:$A83,0),4)</f>
+        <f>TissueComp!K$13*INDEX(VolumeFlow!$A60:$B84,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A60:$A84,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="J61" s="2" t="e">
-        <f>TissueComp!L$13*INDEX(VolumeFlow!$A59:$B83,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A59:$A83,0),4)</f>
+        <f>TissueComp!L$13*INDEX(VolumeFlow!$A60:$B84,MATCH('Average Properties Calc'!$A61,VolumeFlow!$A60:$A84,0),4)</f>
         <v>#REF!</v>
       </c>
       <c r="K61" t="s">
@@ -5995,8 +5995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6337,25 +6337,19 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B13" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="31">
-        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Total",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B13,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("GI Contents",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B13,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("Blood",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B13,'Percent BW'!$N$2:$X$2,0))-SUM(C2:C12)</f>
-        <v>5.1820372533547543E-2</v>
+      <c r="C13" s="21">
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="D13" s="21" t="s">
         <v>344</v>
       </c>
-      <c r="E13" s="22">
-        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A13,Flows!$A$3:$A$21,0),MATCH($B13,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A13,Flows!$A$3:$A$21,0),MATCH($B13,Flows!$B$2:$E$2,0)))</f>
-        <v>4.1900038786262614</v>
-      </c>
-      <c r="F13" s="20" t="s">
-        <v>342</v>
-      </c>
+      <c r="E13" s="22"/>
+      <c r="F13" s="20"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="2"/>
@@ -6365,21 +6359,21 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="21">
-        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A14,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B14,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>7.2598253275109076E-2</v>
+        <v>35</v>
+      </c>
+      <c r="C14" s="31">
+        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Total",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B14,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("GI Contents",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B14,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("Blood",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B14,'Percent BW'!$N$2:$X$2,0))-SUM(C2:C12)</f>
+        <v>5.1820372533547543E-2</v>
       </c>
       <c r="D14" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E14" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A14,Flows!$A$3:$A$21,0),MATCH($B14,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A14,Flows!$A$3:$A$21,0),MATCH($B14,Flows!$B$2:$E$2,0)))</f>
-        <v>1.131370849898476</v>
+        <v>4.1900038786262614</v>
       </c>
       <c r="F14" s="20" t="s">
         <v>342</v>
@@ -6393,21 +6387,21 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B15" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A15,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B15,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>3.6939633668305896E-2</v>
+        <v>7.2598253275109076E-2</v>
       </c>
       <c r="D15" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E15" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A15,Flows!$A$3:$A$21,0),MATCH($B15,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A15,Flows!$A$3:$A$21,0),MATCH($B15,Flows!$B$2:$E$2,0)))</f>
-        <v>25.535040082208603</v>
+        <v>1.131370849898476</v>
       </c>
       <c r="F15" s="20" t="s">
         <v>342</v>
@@ -6421,21 +6415,21 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A16,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B16,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>5.5045871559633031E-3</v>
+        <v>3.6939633668305896E-2</v>
       </c>
       <c r="D16" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E16" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A16,Flows!$A$3:$A$21,0),MATCH($B16,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A16,Flows!$A$3:$A$21,0),MATCH($B16,Flows!$B$2:$E$2,0)))</f>
-        <v>3.676955262170047</v>
+        <v>25.535040082208603</v>
       </c>
       <c r="F16" s="20" t="s">
         <v>342</v>
@@ -6449,21 +6443,21 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="B17" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="31">
-        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Stomach",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B17,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Large Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B17,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Small Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B17,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>2.5852334412265577E-2</v>
+      <c r="C17" s="21">
+        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A17,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B17,'Percent BW'!$N$2:$X$2,0))</f>
+        <v>5.5045871559633031E-3</v>
       </c>
       <c r="D17" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E17" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A17,Flows!$A$3:$A$21,0),MATCH($B17,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A17,Flows!$A$3:$A$21,0),MATCH($B17,Flows!$B$2:$E$2,0)))</f>
-        <v>27.718585822512662</v>
+        <v>3.676955262170047</v>
       </c>
       <c r="F17" s="20" t="s">
         <v>342</v>
@@ -6477,21 +6471,21 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="B18" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="21">
-        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A18,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B18,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>3.2038834951456309E-3</v>
+      <c r="C18" s="31">
+        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Stomach",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B18,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Large Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B18,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Small Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B18,'Percent BW'!$N$2:$X$2,0))</f>
+        <v>2.5852334412265577E-2</v>
       </c>
       <c r="D18" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E18" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A18,Flows!$A$3:$A$21,0),MATCH($B18,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A18,Flows!$A$3:$A$21,0),MATCH($B18,Flows!$B$2:$E$2,0)))</f>
-        <v>11.030865786510139</v>
+        <v>27.718585822512662</v>
       </c>
       <c r="F18" s="20" t="s">
         <v>342</v>
@@ -6505,21 +6499,21 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="B19" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A19,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B19,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>6.9523809523809521E-3</v>
+        <v>3.2038834951456309E-3</v>
       </c>
       <c r="D19" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E19" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A19,Flows!$A$3:$A$21,0),MATCH($B19,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A19,Flows!$A$3:$A$21,0),MATCH($B19,Flows!$B$2:$E$2,0)))</f>
-        <v>26.021529547664947</v>
+        <v>11.030865786510139</v>
       </c>
       <c r="F19" s="20" t="s">
         <v>342</v>
@@ -6533,21 +6527,21 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="B20" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A20,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B20,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>3.4857142857142857E-2</v>
+        <v>6.9523809523809521E-3</v>
       </c>
       <c r="D20" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E20" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A20,Flows!$A$3:$A$21,0),MATCH($B20,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A20,Flows!$A$3:$A$21,0),MATCH($B20,Flows!$B$2:$E$2,0)))</f>
-        <v>33.375440072005041</v>
+        <v>26.021529547664947</v>
       </c>
       <c r="F20" s="20" t="s">
         <v>342</v>
@@ -6561,21 +6555,21 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="B21" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A21,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B21,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>4.7596382674916704E-3</v>
+        <v>3.4857142857142857E-2</v>
       </c>
       <c r="D21" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E21" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A21,Flows!$A$3:$A$21,0),MATCH($B21,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A21,Flows!$A$3:$A$21,0),MATCH($B21,Flows!$B$2:$E$2,0)))</f>
-        <v>4.3953757518555792</v>
+        <v>33.375440072005041</v>
       </c>
       <c r="F21" s="20" t="s">
         <v>342</v>
@@ -6589,21 +6583,21 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B22" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A22,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B22,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>0.38837656099903939</v>
+        <v>4.7596382674916704E-3</v>
       </c>
       <c r="D22" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E22" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A22,Flows!$A$3:$A$21,0),MATCH($B22,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A22,Flows!$A$3:$A$21,0),MATCH($B22,Flows!$B$2:$E$2,0)))</f>
-        <v>21.213203435596427</v>
+        <v>4.3953757518555792</v>
       </c>
       <c r="F22" s="20" t="s">
         <v>342</v>
@@ -6617,21 +6611,21 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B23" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A23,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B23,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>0.17032054810459099</v>
+        <v>0.38837656099903939</v>
       </c>
       <c r="D23" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E23" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A23,Flows!$A$3:$A$21,0),MATCH($B23,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A23,Flows!$A$3:$A$21,0),MATCH($B23,Flows!$B$2:$E$2,0)))</f>
-        <v>16.404877323527902</v>
+        <v>21.213203435596427</v>
       </c>
       <c r="F23" s="20" t="s">
         <v>342</v>
@@ -6645,21 +6639,21 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B24" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A24,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B24,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>1.8975332068311196E-3</v>
+        <v>0.17032054810459099</v>
       </c>
       <c r="D24" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E24" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A24,Flows!$A$3:$A$21,0),MATCH($B24,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A24,Flows!$A$3:$A$21,0),MATCH($B24,Flows!$B$2:$E$2,0)))</f>
-        <v>2.8779245994292482</v>
+        <v>16.404877323527902</v>
       </c>
       <c r="F24" s="20" t="s">
         <v>342</v>
@@ -6673,21 +6667,21 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B25" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="31">
-        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Total",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B25,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("GI Contents",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B25,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("Blood",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B25,'Percent BW'!$N$2:$X$2,0))-SUM(C14:C24)</f>
-        <v>5.2399992921151606E-2</v>
+      <c r="C25" s="21">
+        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A25,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B25,'Percent BW'!$N$2:$X$2,0))</f>
+        <v>1.8975332068311196E-3</v>
       </c>
       <c r="D25" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E25" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A25,Flows!$A$3:$A$21,0),MATCH($B25,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A25,Flows!$A$3:$A$21,0),MATCH($B25,Flows!$B$2:$E$2,0)))</f>
-        <v>59.664255982958501</v>
+        <v>2.8779245994292482</v>
       </c>
       <c r="F25" s="20" t="s">
         <v>342</v>
@@ -6701,21 +6695,21 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="21">
-        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A26,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B26,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>7.3169652284369002E-2</v>
+        <v>17</v>
+      </c>
+      <c r="C26" s="31">
+        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Total",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B26,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("GI Contents",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B26,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("Blood",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B26,'Percent BW'!$N$2:$X$2,0))-SUM(C15:C25)</f>
+        <v>5.2399992921151606E-2</v>
       </c>
       <c r="D26" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E26" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A26,Flows!$A$3:$A$21,0),MATCH($B26,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A26,Flows!$A$3:$A$21,0),MATCH($B26,Flows!$B$2:$E$2,0)))</f>
-        <v>4.0614836065401096</v>
+        <v>59.664255982958501</v>
       </c>
       <c r="F26" s="20" t="s">
         <v>342</v>
@@ -6723,21 +6717,21 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B27" s="20" t="s">
         <v>34</v>
       </c>
       <c r="C27" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A27,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B27,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>5.429620126861949E-2</v>
+        <v>7.3169652284369002E-2</v>
       </c>
       <c r="D27" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E27" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A27,Flows!$A$3:$A$21,0),MATCH($B27,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A27,Flows!$A$3:$A$21,0),MATCH($B27,Flows!$B$2:$E$2,0)))</f>
-        <v>8.766383654772504</v>
+        <v>4.0614836065401096</v>
       </c>
       <c r="F27" s="20" t="s">
         <v>342</v>
@@ -6745,21 +6739,21 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28" s="20" t="s">
         <v>34</v>
       </c>
       <c r="C28" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A28,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B28,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>1.5934331240946405E-2</v>
+        <v>5.429620126861949E-2</v>
       </c>
       <c r="D28" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E28" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A28,Flows!$A$3:$A$21,0),MATCH($B28,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A28,Flows!$A$3:$A$21,0),MATCH($B28,Flows!$B$2:$E$2,0)))</f>
-        <v>4.963996082874039</v>
+        <v>8.766383654772504</v>
       </c>
       <c r="F28" s="20" t="s">
         <v>342</v>
@@ -6767,21 +6761,21 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="B29" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="31">
-        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Stomach",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B29,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Large Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B29,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Small Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B29,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>4.0408654780552319E-2</v>
+      <c r="C29" s="21">
+        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A29,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B29,'Percent BW'!$N$2:$X$2,0))</f>
+        <v>1.5934331240946405E-2</v>
       </c>
       <c r="D29" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E29" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A29,Flows!$A$3:$A$21,0),MATCH($B29,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A29,Flows!$A$3:$A$21,0),MATCH($B29,Flows!$B$2:$E$2,0)))</f>
-        <v>27.264372424876349</v>
+        <v>4.963996082874039</v>
       </c>
       <c r="F29" s="20" t="s">
         <v>342</v>
@@ -6789,21 +6783,21 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="B30" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="21">
-        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A30,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B30,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>4.8543689320388345E-3</v>
+      <c r="C30" s="31">
+        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Stomach",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B30,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Large Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B30,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Small Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B30,'Percent BW'!$N$2:$X$2,0))</f>
+        <v>4.0408654780552319E-2</v>
       </c>
       <c r="D30" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E30" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A30,Flows!$A$3:$A$21,0),MATCH($B30,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A30,Flows!$A$3:$A$21,0),MATCH($B30,Flows!$B$2:$E$2,0)))</f>
-        <v>5.2648443303209511</v>
+        <v>27.264372424876349</v>
       </c>
       <c r="F30" s="20" t="s">
         <v>342</v>
@@ -6811,21 +6805,21 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="B31" s="20" t="s">
         <v>34</v>
       </c>
       <c r="C31" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A31,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B31,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>1.5904761904761904E-2</v>
+        <v>4.8543689320388345E-3</v>
       </c>
       <c r="D31" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E31" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A31,Flows!$A$3:$A$21,0),MATCH($B31,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A31,Flows!$A$3:$A$21,0),MATCH($B31,Flows!$B$2:$E$2,0)))</f>
-        <v>24.443920105061554</v>
+        <v>5.2648443303209511</v>
       </c>
       <c r="F31" s="20" t="s">
         <v>342</v>
@@ -6833,21 +6827,21 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="B32" s="20" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A32,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B32,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>5.228571428571429E-2</v>
+        <v>1.5904761904761904E-2</v>
       </c>
       <c r="D32" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E32" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A32,Flows!$A$3:$A$21,0),MATCH($B32,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A32,Flows!$A$3:$A$21,0),MATCH($B32,Flows!$B$2:$E$2,0)))</f>
-        <v>33.845427837777535</v>
+        <v>24.443920105061554</v>
       </c>
       <c r="F32" s="20" t="s">
         <v>342</v>
@@ -6855,21 +6849,21 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="B33" s="20" t="s">
         <v>34</v>
       </c>
       <c r="C33" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A33,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B33,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>6.9490718705378391E-3</v>
+        <v>5.228571428571429E-2</v>
       </c>
       <c r="D33" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E33" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A33,Flows!$A$3:$A$21,0),MATCH($B33,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A33,Flows!$A$3:$A$21,0),MATCH($B33,Flows!$B$2:$E$2,0)))</f>
-        <v>0.75212061861727864</v>
+        <v>33.845427837777535</v>
       </c>
       <c r="F33" s="20" t="s">
         <v>342</v>
@@ -6877,21 +6871,21 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B34" s="20" t="s">
         <v>34</v>
       </c>
       <c r="C34" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A34,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B34,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>0.36887608069164268</v>
+        <v>6.9490718705378391E-3</v>
       </c>
       <c r="D34" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E34" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A34,Flows!$A$3:$A$21,0),MATCH($B34,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A34,Flows!$A$3:$A$21,0),MATCH($B34,Flows!$B$2:$E$2,0)))</f>
-        <v>17.110744073543088</v>
+        <v>0.75212061861727864</v>
       </c>
       <c r="F34" s="20" t="s">
         <v>342</v>
@@ -6899,21 +6893,21 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B35" s="20" t="s">
         <v>34</v>
       </c>
       <c r="C35" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A35,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B35,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>0.14794527904198049</v>
+        <v>0.36887608069164268</v>
       </c>
       <c r="D35" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E35" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A35,Flows!$A$3:$A$21,0),MATCH($B35,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A35,Flows!$A$3:$A$21,0),MATCH($B35,Flows!$B$2:$E$2,0)))</f>
-        <v>7.709236340827105</v>
+        <v>17.110744073543088</v>
       </c>
       <c r="F35" s="20" t="s">
         <v>342</v>
@@ -6921,21 +6915,21 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B36" s="20" t="s">
         <v>34</v>
       </c>
       <c r="C36" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A36,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B36,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>1.0473620615192194E-3</v>
+        <v>0.14794527904198049</v>
       </c>
       <c r="D36" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E36" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A36,Flows!$A$3:$A$21,0),MATCH($B36,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A36,Flows!$A$3:$A$21,0),MATCH($B36,Flows!$B$2:$E$2,0)))</f>
-        <v>2.0683317011975162</v>
+        <v>7.709236340827105</v>
       </c>
       <c r="F36" s="20" t="s">
         <v>342</v>
@@ -6943,21 +6937,21 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B37" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="31">
-        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Total",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B37,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("GI Contents",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B37,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("Blood",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B37,'Percent BW'!$N$2:$X$2,0))-SUM(C26:C36)</f>
-        <v>2.5418908119054118E-2</v>
+      <c r="C37" s="21">
+        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A37,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B37,'Percent BW'!$N$2:$X$2,0))</f>
+        <v>1.0473620615192194E-3</v>
       </c>
       <c r="D37" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E37" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A37,Flows!$A$3:$A$21,0),MATCH($B37,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A37,Flows!$A$3:$A$21,0),MATCH($B37,Flows!$B$2:$E$2,0)))</f>
-        <v>38.629718395752846</v>
+        <v>2.0683317011975162</v>
       </c>
       <c r="F37" s="20" t="s">
         <v>342</v>
@@ -6965,21 +6959,21 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" s="21">
-        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A38,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B38,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>4.7303493449781797E-2</v>
+        <v>34</v>
+      </c>
+      <c r="C38" s="31">
+        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Total",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B38,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("GI Contents",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B38,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("Blood",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B38,'Percent BW'!$N$2:$X$2,0))-SUM(C27:C37)</f>
+        <v>2.5418908119054118E-2</v>
       </c>
       <c r="D38" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E38" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A38,Flows!$A$3:$A$21,0),MATCH($B38,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A38,Flows!$A$3:$A$21,0),MATCH($B38,Flows!$B$2:$E$2,0)))</f>
-        <v>6.2239779351362285</v>
+        <v>38.629718395752846</v>
       </c>
       <c r="F38" s="20" t="s">
         <v>342</v>
@@ -6993,21 +6987,21 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B39" s="20" t="s">
         <v>18</v>
       </c>
       <c r="C39" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A39,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B39,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>4.098781270044901E-2</v>
+        <v>4.7303493449781797E-2</v>
       </c>
       <c r="D39" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E39" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A39,Flows!$A$3:$A$21,0),MATCH($B39,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A39,Flows!$A$3:$A$21,0),MATCH($B39,Flows!$B$2:$E$2,0)))</f>
-        <v>2.3117632330505993</v>
+        <v>6.2239779351362285</v>
       </c>
       <c r="F39" s="20" t="s">
         <v>342</v>
@@ -7021,21 +7015,21 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B40" s="20" t="s">
         <v>18</v>
       </c>
       <c r="C40" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A40,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B40,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>7.532592950265574E-3</v>
+        <v>4.098781270044901E-2</v>
       </c>
       <c r="D40" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E40" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A40,Flows!$A$3:$A$21,0),MATCH($B40,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A40,Flows!$A$3:$A$21,0),MATCH($B40,Flows!$B$2:$E$2,0)))</f>
-        <v>8.0022573451751509</v>
+        <v>2.3117632330505993</v>
       </c>
       <c r="F40" s="20" t="s">
         <v>342</v>
@@ -7049,21 +7043,21 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="B41" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="31">
-        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Stomach",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B41,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Large Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B41,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Small Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B41,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>3.521811975832758E-2</v>
+      <c r="C41" s="21">
+        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A41,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B41,'Percent BW'!$N$2:$X$2,0))</f>
+        <v>7.532592950265574E-3</v>
       </c>
       <c r="D41" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E41" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A41,Flows!$A$3:$A$21,0),MATCH($B41,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A41,Flows!$A$3:$A$21,0),MATCH($B41,Flows!$B$2:$E$2,0)))</f>
-        <v>40.900426430895223</v>
+        <v>8.0022573451751509</v>
       </c>
       <c r="F41" s="20" t="s">
         <v>342</v>
@@ -7077,21 +7071,21 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="B42" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C42" s="21">
-        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A42,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B42,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>7.5728155339805829E-3</v>
+      <c r="C42" s="31">
+        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Stomach",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B42,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Large Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B42,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Small Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B42,'Percent BW'!$N$2:$X$2,0))</f>
+        <v>3.521811975832758E-2</v>
       </c>
       <c r="D42" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E42" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A42,Flows!$A$3:$A$21,0),MATCH($B42,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A42,Flows!$A$3:$A$21,0),MATCH($B42,Flows!$B$2:$E$2,0)))</f>
-        <v>9.6027088142101817</v>
+        <v>40.900426430895223</v>
       </c>
       <c r="F42" s="20" t="s">
         <v>342</v>
@@ -7105,21 +7099,21 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="B43" s="20" t="s">
         <v>18</v>
       </c>
       <c r="C43" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A43,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B43,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>5.2380952380952387E-3</v>
+        <v>7.5728155339805829E-3</v>
       </c>
       <c r="D43" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E43" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A43,Flows!$A$3:$A$21,0),MATCH($B43,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A43,Flows!$A$3:$A$21,0),MATCH($B43,Flows!$B$2:$E$2,0)))</f>
-        <v>38.410835256840727</v>
+        <v>9.6027088142101817</v>
       </c>
       <c r="F43" s="20" t="s">
         <v>342</v>
@@ -7133,21 +7127,21 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="B44" s="20" t="s">
         <v>18</v>
       </c>
       <c r="C44" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A44,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B44,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>3.1333333333333331E-2</v>
+        <v>5.2380952380952387E-3</v>
       </c>
       <c r="D44" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E44" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A44,Flows!$A$3:$A$21,0),MATCH($B44,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A44,Flows!$A$3:$A$21,0),MATCH($B44,Flows!$B$2:$E$2,0)))</f>
-        <v>54.948833770202704</v>
+        <v>38.410835256840727</v>
       </c>
       <c r="F44" s="20" t="s">
         <v>342</v>
@@ -7161,21 +7155,21 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="B45" s="20" t="s">
         <v>18</v>
       </c>
       <c r="C45" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A45,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B45,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>7.8058067586863388E-3</v>
+        <v>3.1333333333333331E-2</v>
       </c>
       <c r="D45" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E45" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A45,Flows!$A$3:$A$21,0),MATCH($B45,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A45,Flows!$A$3:$A$21,0),MATCH($B45,Flows!$B$2:$E$2,0)))</f>
-        <v>18.778630570011025</v>
+        <v>54.948833770202704</v>
       </c>
       <c r="F45" s="20" t="s">
         <v>342</v>
@@ -7189,21 +7183,21 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B46" s="20" t="s">
         <v>18</v>
       </c>
       <c r="C46" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A46,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B46,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>0.43852065321805955</v>
+        <v>7.8058067586863388E-3</v>
       </c>
       <c r="D46" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E46" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A46,Flows!$A$3:$A$21,0),MATCH($B46,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A46,Flows!$A$3:$A$21,0),MATCH($B46,Flows!$B$2:$E$2,0)))</f>
-        <v>44.456985250973062</v>
+        <v>18.778630570011025</v>
       </c>
       <c r="F46" s="20" t="s">
         <v>342</v>
@@ -7217,21 +7211,21 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B47" s="20" t="s">
         <v>18</v>
       </c>
       <c r="C47" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A47,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B47,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>0.17005204487583964</v>
+        <v>0.43852065321805955</v>
       </c>
       <c r="D47" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E47" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A47,Flows!$A$3:$A$21,0),MATCH($B47,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A47,Flows!$A$3:$A$21,0),MATCH($B47,Flows!$B$2:$E$2,0)))</f>
-        <v>17.782794100389225</v>
+        <v>44.456985250973062</v>
       </c>
       <c r="F47" s="20" t="s">
         <v>342</v>
@@ -7245,21 +7239,21 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B48" s="20" t="s">
         <v>18</v>
       </c>
       <c r="C48" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A48,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B48,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>2.5616698292220113E-3</v>
+        <v>0.17005204487583964</v>
       </c>
       <c r="D48" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E48" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A48,Flows!$A$3:$A$21,0),MATCH($B48,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A48,Flows!$A$3:$A$21,0),MATCH($B48,Flows!$B$2:$E$2,0)))</f>
-        <v>2.934161026564222</v>
+        <v>17.782794100389225</v>
       </c>
       <c r="F48" s="20" t="s">
         <v>342</v>
@@ -7273,21 +7267,21 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B49" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C49" s="31">
-        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Total",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B49,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("GI Contents",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B49,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("Blood",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B49,'Percent BW'!$N$2:$X$2,0))-SUM(C38:C48)</f>
-        <v>2.3649226512727495E-3</v>
+      <c r="C49" s="21">
+        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A49,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B49,'Percent BW'!$N$2:$X$2,0))</f>
+        <v>2.5616698292220113E-3</v>
       </c>
       <c r="D49" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E49" s="22">
         <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A49,Flows!$A$3:$A$21,0),MATCH($B49,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A49,Flows!$A$3:$A$21,0),MATCH($B49,Flows!$B$2:$E$2,0)))</f>
-        <v>6.0994983764335551</v>
+        <v>2.934161026564222</v>
       </c>
       <c r="F49" s="20" t="s">
         <v>342</v>
@@ -7301,21 +7295,21 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="B50" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="C50" s="21">
-        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A50,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B50,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>4.8000000000000001E-2</v>
+        <v>18</v>
+      </c>
+      <c r="C50" s="31">
+        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Total",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B50,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("GI Contents",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B50,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("Blood",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B50,'Percent BW'!$N$2:$X$2,0))-SUM(C39:C49)</f>
+        <v>2.3649226512727495E-3</v>
       </c>
       <c r="D50" s="21" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="E50" s="22">
-        <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A50,Flows!$A$3:$A$21,0),MATCH($B50,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A50,Flows!$A$3:$A$21,0),MATCH($B50,Flows!$B$2:$G$2,0)))</f>
-        <v>16.095147899941573</v>
+        <f>IF(INDEX(Flows!$H$3:$K$21,MATCH($A50,Flows!$A$3:$A$21,0),MATCH($B50,Flows!$B$2:$E$2,0))=0,"",INDEX(Flows!$H$3:$K$21,MATCH($A50,Flows!$A$3:$A$21,0),MATCH($B50,Flows!$B$2:$E$2,0)))</f>
+        <v>6.0994983764335551</v>
       </c>
       <c r="F50" s="20" t="s">
         <v>342</v>
@@ -7329,21 +7323,21 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B51" s="20" t="s">
         <v>104</v>
       </c>
       <c r="C51" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A51,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B51,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>3.6900000000000002E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E51" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A51,Flows!$A$3:$A$21,0),MATCH($B51,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A51,Flows!$A$3:$A$21,0),MATCH($B51,Flows!$B$2:$G$2,0)))</f>
-        <v>15.535450308907148</v>
+        <v>16.095147899941573</v>
       </c>
       <c r="F51" s="20" t="s">
         <v>342</v>
@@ -7357,21 +7351,21 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B52" s="20" t="s">
         <v>104</v>
       </c>
       <c r="C52" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A52,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B52,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>5.4999999999999997E-3</v>
+        <v>3.6900000000000002E-2</v>
       </c>
       <c r="D52" s="21" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="E52" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A52,Flows!$A$3:$A$21,0),MATCH($B52,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A52,Flows!$A$3:$A$21,0),MATCH($B52,Flows!$B$2:$G$2,0)))</f>
-        <v>14.199668958756412</v>
+        <v>15.535450308907148</v>
       </c>
       <c r="F52" s="20" t="s">
         <v>342</v>
@@ -7385,21 +7379,21 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="B53" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="C53" s="31">
-        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Stomach",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B53,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Large Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B53,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Small Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B53,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>4.8000000000000001E-2</v>
+      <c r="C53" s="21">
+        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A53,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B53,'Percent BW'!$N$2:$X$2,0))</f>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="D53" s="21" t="s">
         <v>350</v>
       </c>
       <c r="E53" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A53,Flows!$A$3:$A$21,0),MATCH($B53,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A53,Flows!$A$3:$A$21,0),MATCH($B53,Flows!$B$2:$G$2,0)))</f>
-        <v>55.830044277922326</v>
+        <v>14.199668958756412</v>
       </c>
       <c r="F53" s="20" t="s">
         <v>342</v>
@@ -7413,21 +7407,21 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="B54" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="C54" s="21">
-        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A54,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B54,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>2.3999999999999998E-3</v>
+      <c r="C54" s="31">
+        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Stomach",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B54,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Large Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B54,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Small Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B54,'Percent BW'!$N$2:$X$2,0))</f>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="D54" s="21" t="s">
         <v>350</v>
       </c>
       <c r="E54" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A54,Flows!$A$3:$A$21,0),MATCH($B54,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A54,Flows!$A$3:$A$21,0),MATCH($B54,Flows!$B$2:$G$2,0)))</f>
-        <v>8.0475739499707863</v>
+        <v>55.830044277922326</v>
       </c>
       <c r="F54" s="20" t="s">
         <v>342</v>
@@ -7441,21 +7435,21 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="B55" s="20" t="s">
         <v>104</v>
       </c>
       <c r="C55" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A55,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B55,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>6.0000000000000001E-3</v>
+        <v>2.3999999999999998E-3</v>
       </c>
       <c r="D55" s="21" t="s">
         <v>350</v>
       </c>
       <c r="E55" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A55,Flows!$A$3:$A$21,0),MATCH($B55,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A55,Flows!$A$3:$A$21,0),MATCH($B55,Flows!$B$2:$G$2,0)))</f>
-        <v>40.237869749853928</v>
+        <v>8.0475739499707863</v>
       </c>
       <c r="F55" s="20" t="s">
         <v>342</v>
@@ -7469,21 +7463,21 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="B56" s="20" t="s">
         <v>104</v>
       </c>
       <c r="C56" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A56,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B56,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>0.04</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="D56" s="21" t="s">
         <v>350</v>
       </c>
       <c r="E56" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A56,Flows!$A$3:$A$21,0),MATCH($B56,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A56,Flows!$A$3:$A$21,0),MATCH($B56,Flows!$B$2:$G$2,0)))</f>
-        <v>89.026286821551821</v>
+        <v>40.237869749853928</v>
       </c>
       <c r="F56" s="20" t="s">
         <v>342</v>
@@ -7497,21 +7491,21 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="20" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="B57" s="20" t="s">
         <v>104</v>
       </c>
       <c r="C57" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A57,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B57,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>6.7999999999999996E-3</v>
+        <v>0.04</v>
       </c>
       <c r="D57" s="21" t="s">
         <v>350</v>
       </c>
       <c r="E57" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A57,Flows!$A$3:$A$21,0),MATCH($B57,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A57,Flows!$A$3:$A$21,0),MATCH($B57,Flows!$B$2:$G$2,0)))</f>
-        <v>9.2635120764741856</v>
+        <v>89.026286821551821</v>
       </c>
       <c r="F57" s="20" t="s">
         <v>342</v>
@@ -7525,21 +7519,21 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="20" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B58" s="20" t="s">
         <v>104</v>
       </c>
       <c r="C58" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A58,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B58,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>0.54</v>
+        <v>6.7999999999999996E-3</v>
       </c>
       <c r="D58" s="21" t="s">
         <v>350</v>
       </c>
       <c r="E58" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A58,Flows!$A$3:$A$21,0),MATCH($B58,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A58,Flows!$A$3:$A$21,0),MATCH($B58,Flows!$B$2:$G$2,0)))</f>
-        <v>77.960872640341989</v>
+        <v>9.2635120764741856</v>
       </c>
       <c r="F58" s="20" t="s">
         <v>342</v>
@@ -7553,21 +7547,21 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B59" s="20" t="s">
         <v>104</v>
       </c>
       <c r="C59" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A59,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B59,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>4.3999999999999997E-2</v>
+        <v>0.54</v>
       </c>
       <c r="D59" s="21" t="s">
         <v>350</v>
       </c>
       <c r="E59" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A59,Flows!$A$3:$A$21,0),MATCH($B59,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A59,Flows!$A$3:$A$21,0),MATCH($B59,Flows!$B$2:$G$2,0)))</f>
-        <v>17.762827077650776</v>
+        <v>77.960872640341989</v>
       </c>
       <c r="F59" s="20" t="s">
         <v>342</v>
@@ -7581,21 +7575,21 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B60" s="20" t="s">
         <v>104</v>
       </c>
       <c r="C60" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A60,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B60,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>4.0000000000000002E-4</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="D60" s="21" t="s">
         <v>350</v>
       </c>
       <c r="E60" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A60,Flows!$A$3:$A$21,0),MATCH($B60,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A60,Flows!$A$3:$A$21,0),MATCH($B60,Flows!$B$2:$G$2,0)))</f>
-        <v>4.5267603468585671</v>
+        <v>17.762827077650776</v>
       </c>
       <c r="F60" s="20" t="s">
         <v>342</v>
@@ -7609,20 +7603,21 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="20" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B61" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="C61" s="31">
-        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Total",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B61,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("GI Contents",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B61,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("Blood",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B61,'Percent BW'!$N$2:$X$2,0))-SUM(C50:C60)</f>
-        <v>2.5662489315418147E-2</v>
+      <c r="C61" s="21">
+        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A61,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B61,'Percent BW'!$N$2:$X$2,0))</f>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="D61" s="21" t="s">
         <v>350</v>
       </c>
       <c r="E61" s="22">
-        <v>0</v>
+        <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A61,Flows!$A$3:$A$21,0),MATCH($B61,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A61,Flows!$A$3:$A$21,0),MATCH($B61,Flows!$B$2:$G$2,0)))</f>
+        <v>4.5267603468585671</v>
       </c>
       <c r="F61" s="20" t="s">
         <v>342</v>
@@ -7636,21 +7631,20 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="20" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="B62" s="20" t="s">
-        <v>339</v>
-      </c>
-      <c r="C62" s="21">
-        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A62,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B62,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>2.7000000000000003E-2</v>
+        <v>104</v>
+      </c>
+      <c r="C62" s="31">
+        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Total",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B62,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("GI Contents",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B62,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("Blood",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B62,'Percent BW'!$N$2:$X$2,0))-SUM(C51:C61)</f>
+        <v>2.5662489315418147E-2</v>
       </c>
       <c r="D62" s="21" t="s">
         <v>350</v>
       </c>
       <c r="E62" s="22">
-        <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A62,Flows!$A$3:$A$21,0),MATCH($B62,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A62,Flows!$A$3:$A$21,0),MATCH($B62,Flows!$B$2:$G$2,0)))</f>
-        <v>5.9813951248848829</v>
+        <v>0</v>
       </c>
       <c r="F62" s="20" t="s">
         <v>342</v>
@@ -7664,19 +7658,21 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="20" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B63" s="20" t="s">
         <v>339</v>
       </c>
       <c r="C63" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A63,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B63,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>7.2310597961656342E-2</v>
-      </c>
-      <c r="D63" s="21"/>
+        <v>2.7000000000000003E-2</v>
+      </c>
+      <c r="D63" s="21" t="s">
+        <v>350</v>
+      </c>
       <c r="E63" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A63,Flows!$A$3:$A$21,0),MATCH($B63,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A63,Flows!$A$3:$A$21,0),MATCH($B63,Flows!$B$2:$G$2,0)))</f>
-        <v>0.34858241588912464</v>
+        <v>5.9813951248848829</v>
       </c>
       <c r="F63" s="20" t="s">
         <v>342</v>
@@ -7690,19 +7686,19 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B64" s="20" t="s">
         <v>339</v>
       </c>
       <c r="C64" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A64,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B64,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>1.9314340898116854E-2</v>
+        <v>7.2310597961656342E-2</v>
       </c>
       <c r="D64" s="21"/>
       <c r="E64" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A64,Flows!$A$3:$A$21,0),MATCH($B64,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A64,Flows!$A$3:$A$21,0),MATCH($B64,Flows!$B$2:$G$2,0)))</f>
-        <v>21.53302244958558</v>
+        <v>0.34858241588912464</v>
       </c>
       <c r="F64" s="20" t="s">
         <v>342</v>
@@ -7716,21 +7712,19 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="B65" s="20" t="s">
         <v>339</v>
       </c>
-      <c r="C65" s="31">
-        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Stomach",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B65,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Large Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B65,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Small Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B65,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>4.5999999999999999E-2</v>
-      </c>
-      <c r="D65" s="21" t="s">
-        <v>350</v>
-      </c>
+      <c r="C65" s="21">
+        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A65,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B65,'Percent BW'!$N$2:$X$2,0))</f>
+        <v>1.9314340898116854E-2</v>
+      </c>
+      <c r="D65" s="21"/>
       <c r="E65" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A65,Flows!$A$3:$A$21,0),MATCH($B65,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A65,Flows!$A$3:$A$21,0),MATCH($B65,Flows!$B$2:$G$2,0)))</f>
-        <v>37.38371953053052</v>
+        <v>21.53302244958558</v>
       </c>
       <c r="F65" s="20" t="s">
         <v>342</v>
@@ -7744,21 +7738,21 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="B66" s="20" t="s">
         <v>339</v>
       </c>
-      <c r="C66" s="21">
-        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A66,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B66,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>3.4000000000000002E-3</v>
+      <c r="C66" s="31">
+        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Stomach",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B66,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Large Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B66,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Small Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B66,'Percent BW'!$N$2:$X$2,0))</f>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="D66" s="21" t="s">
         <v>350</v>
       </c>
       <c r="E66" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A66,Flows!$A$3:$A$21,0),MATCH($B66,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A66,Flows!$A$3:$A$21,0),MATCH($B66,Flows!$B$2:$G$2,0)))</f>
-        <v>17.944185374654648</v>
+        <v>37.38371953053052</v>
       </c>
       <c r="F66" s="20" t="s">
         <v>342</v>
@@ -7772,21 +7766,21 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="20" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="B67" s="20" t="s">
         <v>339</v>
       </c>
       <c r="C67" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A67,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B67,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>6.0000000000000001E-3</v>
+        <v>3.4000000000000002E-3</v>
       </c>
       <c r="D67" s="21" t="s">
         <v>350</v>
       </c>
       <c r="E67" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A67,Flows!$A$3:$A$21,0),MATCH($B67,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A67,Flows!$A$3:$A$21,0),MATCH($B67,Flows!$B$2:$G$2,0)))</f>
-        <v>41.271626361705692</v>
+        <v>17.944185374654648</v>
       </c>
       <c r="F67" s="20" t="s">
         <v>342</v>
@@ -7800,21 +7794,21 @@
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="B68" s="20" t="s">
         <v>339</v>
       </c>
       <c r="C68" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A68,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B68,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>2.7000000000000003E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="D68" s="21" t="s">
         <v>350</v>
       </c>
       <c r="E68" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A68,Flows!$A$3:$A$21,0),MATCH($B68,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A68,Flows!$A$3:$A$21,0),MATCH($B68,Flows!$B$2:$G$2,0)))</f>
-        <v>65.19720686124522</v>
+        <v>41.271626361705692</v>
       </c>
       <c r="F68" s="20" t="s">
         <v>342</v>
@@ -7828,21 +7822,21 @@
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="20" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="B69" s="20" t="s">
         <v>339</v>
       </c>
       <c r="C69" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A69,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B69,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>7.234650166587339E-3</v>
+        <v>2.7000000000000003E-2</v>
       </c>
       <c r="D69" s="21" t="s">
         <v>350</v>
       </c>
       <c r="E69" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A69,Flows!$A$3:$A$21,0),MATCH($B69,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A69,Flows!$A$3:$A$21,0),MATCH($B69,Flows!$B$2:$G$2,0)))</f>
-        <v>11.286443996023408</v>
+        <v>65.19720686124522</v>
       </c>
       <c r="F69" s="20" t="s">
         <v>342</v>
@@ -7856,21 +7850,21 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="20" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B70" s="20" t="s">
         <v>339</v>
       </c>
       <c r="C70" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A70,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B70,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>0.5</v>
+        <v>7.234650166587339E-3</v>
       </c>
       <c r="D70" s="21" t="s">
         <v>350</v>
       </c>
       <c r="E70" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A70,Flows!$A$3:$A$21,0),MATCH($B70,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A70,Flows!$A$3:$A$21,0),MATCH($B70,Flows!$B$2:$G$2,0)))</f>
-        <v>26.916278061981973</v>
+        <v>11.286443996023408</v>
       </c>
       <c r="F70" s="20" t="s">
         <v>342</v>
@@ -7884,21 +7878,21 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B71" s="20" t="s">
         <v>339</v>
       </c>
       <c r="C71" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A71,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B71,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D71" s="21" t="s">
         <v>350</v>
       </c>
       <c r="E71" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A71,Flows!$A$3:$A$21,0),MATCH($B71,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A71,Flows!$A$3:$A$21,0),MATCH($B71,Flows!$B$2:$G$2,0)))</f>
-        <v>16.149766837189183</v>
+        <v>26.916278061981973</v>
       </c>
       <c r="F71" s="20" t="s">
         <v>342</v>
@@ -7912,21 +7906,21 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B72" s="20" t="s">
         <v>339</v>
       </c>
       <c r="C72" s="21">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A72,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B72,'Percent BW'!$N$2:$X$2,0))</f>
-        <v>2.4667931688804553E-3</v>
+        <v>0.1</v>
       </c>
       <c r="D72" s="21" t="s">
         <v>350</v>
       </c>
       <c r="E72" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A72,Flows!$A$3:$A$21,0),MATCH($B72,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A72,Flows!$A$3:$A$21,0),MATCH($B72,Flows!$B$2:$G$2,0)))</f>
-        <v>6.2804648811291273</v>
+        <v>16.149766837189183</v>
       </c>
       <c r="F72" s="20" t="s">
         <v>342</v>
@@ -7940,19 +7934,21 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="20" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B73" s="20" t="s">
         <v>339</v>
       </c>
-      <c r="C73" s="31">
-        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Total",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B73,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("GI Contents",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B73,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("Blood",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B73,'Percent BW'!$N$2:$X$2,0))-SUM(C62:C72)</f>
-        <v>1.7528264277473893E-2</v>
-      </c>
-      <c r="D73" s="21"/>
+      <c r="C73" s="21">
+        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH(VolumeFlow!A73,'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B73,'Percent BW'!$N$2:$X$2,0))</f>
+        <v>2.4667931688804553E-3</v>
+      </c>
+      <c r="D73" s="21" t="s">
+        <v>350</v>
+      </c>
       <c r="E73" s="22">
         <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A73,Flows!$A$3:$A$21,0),MATCH($B73,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A73,Flows!$A$3:$A$21,0),MATCH($B73,Flows!$B$2:$G$2,0)))</f>
-        <v>99.799527813744888</v>
+        <v>6.2804648811291273</v>
       </c>
       <c r="F73" s="20" t="s">
         <v>342</v>
@@ -7965,12 +7961,24 @@
       <c r="L73" s="2"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A74" s="20"/>
-      <c r="B74" s="20"/>
-      <c r="C74" s="21"/>
+      <c r="A74" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B74" s="20" t="s">
+        <v>339</v>
+      </c>
+      <c r="C74" s="31">
+        <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Total",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B74,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("GI Contents",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B74,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("Blood",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B74,'Percent BW'!$N$2:$X$2,0))-SUM(C63:C73)</f>
+        <v>1.7528264277473893E-2</v>
+      </c>
       <c r="D74" s="21"/>
-      <c r="E74" s="20"/>
-      <c r="F74" s="20"/>
+      <c r="E74" s="22">
+        <f>IF(INDEX(Flows!$H$3:$M$21,MATCH($A74,Flows!$A$3:$A$21,0),MATCH($B74,Flows!$B$2:$G$2,0))=0,"",INDEX(Flows!$H$3:$M$21,MATCH($A74,Flows!$A$3:$A$21,0),MATCH($B74,Flows!$B$2:$G$2,0)))</f>
+        <v>99.799527813744888</v>
+      </c>
+      <c r="F74" s="20" t="s">
+        <v>342</v>
+      </c>
       <c r="G74" s="7"/>
       <c r="H74" s="7"/>
       <c r="I74" s="2"/>
@@ -7979,25 +7987,33 @@
       <c r="L74" s="2"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A75" s="27"/>
+      <c r="A75" s="20"/>
+      <c r="B75" s="20"/>
+      <c r="C75" s="21"/>
+      <c r="D75" s="21"/>
+      <c r="E75" s="20"/>
+      <c r="F75" s="20"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A76" s="28" t="s">
+      <c r="A76" s="27"/>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" s="28" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A77" s="26" t="s">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78" s="26" t="s">
         <v>319</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>348</v>
       </c>
     </row>
@@ -8014,7 +8030,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -9243,7 +9259,7 @@
   <dimension ref="A1:T40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add thyroid blood flow scaled to mL/min/kg BW ^(3/4), citing ILSI-RSI 1994 report. There should be available thyroid data for an httk human      estimate now.
</commit_message>
<xml_diff>
--- a/pkdata.xlsx
+++ b/pkdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msfeir\httkdatatablesGitHub\httkdatatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32751531-4CE9-4B0E-9830-88215DE748DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078AD95C-8FA2-4542-985E-6430834AA393}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="630" yWindow="405" windowWidth="19560" windowHeight="10440" tabRatio="884" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="375">
   <si>
     <t>Tissue</t>
   </si>
@@ -6348,8 +6348,12 @@
       <c r="D13" s="21" t="s">
         <v>344</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="20"/>
+      <c r="E13" s="22">
+        <v>3.7</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>344</v>
+      </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="2"/>
@@ -8030,8 +8034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update the placenta pH value in the pkdata tissue comp section by averaging Lee 1972's presented values for average pH's of mothers and infants (measured within 30 min of delivery). Update documentation accordingly.
</commit_message>
<xml_diff>
--- a/pkdata.xlsx
+++ b/pkdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msfeir\httkdatatablesGitHub\httkdatatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078AD95C-8FA2-4542-985E-6430834AA393}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3052496-A338-4FDD-BB47-61042DF2E844}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="405" windowWidth="19560" windowHeight="10440" tabRatio="884" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="630" yWindow="405" windowWidth="19560" windowHeight="10440" tabRatio="884" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic PK" sheetId="7" r:id="rId1"/>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="376">
   <si>
     <t>Tissue</t>
   </si>
@@ -1798,9 +1798,6 @@
     <t xml:space="preserve">j Human thyroid tissue pH is estimated at 7.3, based on the measurements of turtle thyroid follicular cell pH made by Chow et al. 1982. Also, according to a study of mice by Wangemann et al. in 2009, thyroid follicular pH was measured at 7.6. </t>
   </si>
   <si>
-    <t>Httk estimate</t>
-  </si>
-  <si>
     <r>
       <t>Reference</t>
     </r>
@@ -1819,6 +1816,12 @@
   </si>
   <si>
     <t xml:space="preserve">k Httk collaborators have generally used estimates for placental parameters based on rapidly perfused tissue generally, and that is how the placental parameters were set here. More information on this estimate process is needed. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> K.H. Lee. "Correlation between fetal acid-base status and the Apgar score." Postgraduate Medical Journal: (1972) 48, 405-408.</t>
+  </si>
+  <si>
+    <t>Httk estimate, various references needed; Lee 1972</t>
   </si>
 </sst>
 </file>
@@ -5995,7 +5998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -8032,10 +8035,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L59"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8075,7 +8078,7 @@
         <v>118</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>54</v>
@@ -8607,7 +8610,7 @@
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="D16">
         <v>0.72399999999999998</v>
@@ -8637,7 +8640,7 @@
         <v>7.3804597691985455E-2</v>
       </c>
       <c r="L16">
-        <v>7.24</v>
+        <v>7.32</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -9158,7 +9161,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="27" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -9245,6 +9248,11 @@
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="26" t="s">
         <v>370</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="26" t="s">
+        <v>374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Peter Egeghy caught error with Monkey Cardiac Output
</commit_message>
<xml_diff>
--- a/pkdata.xlsx
+++ b/pkdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msfeir\httkdatatablesGitHub\httkdatatables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\httk-datatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3052496-A338-4FDD-BB47-61042DF2E844}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CB3359-D3F1-40C5-84BB-D773D6DCF24B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="405" windowWidth="19560" windowHeight="10440" tabRatio="884" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="884" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic PK" sheetId="7" r:id="rId1"/>
@@ -1828,10 +1828,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -2008,7 +2007,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2057,7 +2056,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2082,7 +2080,26 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2093,6 +2110,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB35B52E-DAB3-4133-BB0A-E817A59A59D5}" name="Table1" displayName="Table1" ref="A1:H17" totalsRowShown="0">
+  <autoFilter ref="A1:H17" xr:uid="{48C012F2-270A-4595-A0D1-2F8944A01E8D}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{36311C77-E515-44E1-B849-6BDC951DE56C}" name="Parameter"/>
+    <tableColumn id="2" xr3:uid="{7776CC9B-A6DC-4860-ACD5-A0A0A5E9CE64}" name="Units"/>
+    <tableColumn id="3" xr3:uid="{15048B8E-74C6-4F01-B347-1F3D1D0BCE1D}" name="Mouse" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{E035F9F8-6099-41AD-990A-4304E517B6C9}" name="Rat" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{2E4828F3-DFE8-4579-AE84-23E4C814C8A5}" name="Dog" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{777167EB-4D9E-4E37-9FB5-C616859928D2}" name="Human" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{C5ED6305-3946-434D-A087-079BFCE338DD}" name="Rabbit" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{1377A546-F4C2-437C-9EA2-83B9CAE992D5}" name="Monkey" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2418,14 +2452,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="3" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.3">
@@ -2461,27 +2496,27 @@
       <c r="B2" t="s">
         <v>113</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="4">
         <f>14.5/C5</f>
         <v>725</v>
       </c>
-      <c r="D2" s="24">
+      <c r="D2" s="4">
         <f>167/D5</f>
         <v>668</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="4">
         <f>6036/E5</f>
         <v>603.6</v>
       </c>
-      <c r="F2" s="24">
+      <c r="F2" s="4">
         <f>42000/F5</f>
         <v>600</v>
       </c>
-      <c r="G2" s="24">
+      <c r="G2" s="4">
         <f>716*G6</f>
         <v>40.812000000000005</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="4">
         <f>3465/5</f>
         <v>693</v>
       </c>
@@ -2493,27 +2528,27 @@
       <c r="B3" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="4">
         <f>1/C5</f>
         <v>50</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="4">
         <f>7.8/D5</f>
         <v>31.2</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="4">
         <f>515/E5</f>
         <v>51.5</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="4">
         <f>3000/F5</f>
         <v>42.857142857142854</v>
       </c>
-      <c r="G3" s="24">
+      <c r="G3" s="4">
         <f>44*G5</f>
         <v>110</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="4">
         <f>224/5</f>
         <v>44.8</v>
       </c>
@@ -2525,29 +2560,29 @@
       <c r="B4" t="s">
         <v>108</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="4">
         <f>Flows!H3</f>
         <v>150.42412372345572</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="4">
         <f>Flows!I3</f>
         <v>209.30360723121805</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="4">
         <f>Flows!J3</f>
         <v>213.3935292046707</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="4">
         <f>Flows!K3</f>
         <v>231.40060868152614</v>
       </c>
-      <c r="G4" s="24">
+      <c r="G4" s="4">
         <f>212*G5^(1/4)</f>
         <v>266.5758870927823</v>
       </c>
-      <c r="H4">
-        <f>375/24/60/5</f>
-        <v>5.2083333333333336E-2</v>
+      <c r="H4" s="4">
+        <f>Flows!L3</f>
+        <v>324.78975528124914</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2557,22 +2592,22 @@
       <c r="B5" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="4">
         <v>0.02</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="4">
         <v>0.25</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="4">
         <v>10</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="4">
         <v>70</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G5" s="4">
         <v>2.5</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="4">
         <v>5</v>
       </c>
     </row>
@@ -2583,26 +2618,26 @@
       <c r="B6" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="4">
         <f>6.2/100</f>
         <v>6.2E-2</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="4">
         <f>6.7/100</f>
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="4">
         <f>9/100</f>
         <v>0.09</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F6" s="4">
         <f>7.4/100</f>
         <v>7.400000000000001E-2</v>
       </c>
-      <c r="G6" s="24">
+      <c r="G6" s="4">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="4">
         <f>8.8/100</f>
         <v>8.8000000000000009E-2</v>
       </c>
@@ -2614,26 +2649,26 @@
       <c r="B7" t="s">
         <v>83</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="4">
         <f>3.27/100</f>
         <v>3.27E-2</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="4">
         <f>3.16/100</f>
         <v>3.1600000000000003E-2</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="4">
         <f>2.63/100</f>
         <v>2.63E-2</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="4">
         <f>4.18/100</f>
         <v>4.1799999999999997E-2</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="4">
         <v>3.8699999999999998E-2</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="4">
         <f>4.93/100</f>
         <v>4.9299999999999997E-2</v>
       </c>
@@ -2645,26 +2680,26 @@
       <c r="B8" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="4">
         <f>1.25/100</f>
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="4">
         <f>1.81/100</f>
         <v>1.8100000000000002E-2</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="4">
         <f>0.37/100</f>
         <v>3.7000000000000002E-3</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="4">
         <f>0.18/100</f>
         <v>1.8E-3</v>
       </c>
-      <c r="G8" s="24">
+      <c r="G8" s="4">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="4">
         <f>0.24/100</f>
         <v>2.3999999999999998E-3</v>
       </c>
@@ -2676,22 +2711,22 @@
       <c r="B9" t="s">
         <v>87</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="4">
         <v>0.45</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="4">
         <v>0.46</v>
       </c>
-      <c r="E9" s="24">
+      <c r="E9" s="4">
         <v>0.42</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="4">
         <v>0.44</v>
       </c>
-      <c r="G9" s="24">
+      <c r="G9" s="4">
         <v>0.36</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="4">
         <v>0.41</v>
       </c>
     </row>
@@ -2702,26 +2737,26 @@
       <c r="B10" t="s">
         <v>108</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="4">
         <f>Flows!H19</f>
         <v>1.3057649628772197E-2</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="4">
         <f>Flows!I19</f>
         <v>9.8209275164798271E-2</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="4">
         <f>Flows!J19</f>
         <v>3.704748770914422E-2</v>
       </c>
-      <c r="F10" s="24">
+      <c r="F10" s="4">
         <f>Flows!K19</f>
         <v>4.0173716784987171E-2</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="4">
         <v>4.1700000000000001E-2</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="4">
         <f>1086/24/60/5</f>
         <v>0.15083333333333332</v>
       </c>
@@ -2733,26 +2768,26 @@
       <c r="B11" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="4">
         <f>Flows!H20</f>
         <v>2.6115299257544394E-2</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="4">
         <f>Flows!I20</f>
         <v>4.4194173824159216E-2</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="4">
         <f>Flows!J20</f>
         <v>1.4818995083657686E-2</v>
       </c>
-      <c r="F11" s="24">
+      <c r="F11" s="4">
         <f>Flows!K20</f>
         <v>1.0043429196246793E-2</v>
       </c>
-      <c r="G11" s="24">
+      <c r="G11" s="4">
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="4">
         <f>125/24/260/5</f>
         <v>4.0064102564102561E-3</v>
       </c>
@@ -2764,26 +2799,26 @@
       <c r="B12" t="s">
         <v>108</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="4">
         <f>Flows!H21</f>
         <v>5.2648443303209502</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="4">
         <f>Flows!I21</f>
         <v>3.705239533417509</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="4">
         <f>Flows!J21</f>
         <v>10.900852783538594</v>
       </c>
-      <c r="F12" s="24">
+      <c r="F12" s="4">
         <f>Flows!K21</f>
         <v>5.1651921580697797</v>
       </c>
-      <c r="G12" s="24">
+      <c r="G12" s="4">
         <v>3.12</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="4">
         <f>10.4/5</f>
         <v>2.08</v>
       </c>
@@ -2795,23 +2830,23 @@
       <c r="B13" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="24">
+      <c r="C13" s="4">
         <v>37</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="4">
         <v>38.700000000000003</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13" s="4">
         <v>38.9</v>
       </c>
-      <c r="F13" s="24">
+      <c r="F13" s="4">
         <v>37</v>
       </c>
-      <c r="G13" s="24">
+      <c r="G13" s="4">
         <f>(40.1+38.6)/2</f>
         <v>39.35</v>
       </c>
-      <c r="H13" s="24">
+      <c r="H13" s="4">
         <v>38</v>
       </c>
     </row>
@@ -2822,26 +2857,26 @@
       <c r="B14" t="s">
         <v>311</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="4">
         <f xml:space="preserve"> (0.003+0.3*0.0021)/(0.003 + 0.0021+0.00088) * 0.006/(0.006+0.06+0.96)</f>
         <v>3.5498445109429094E-3</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="4">
         <f>0.0015 + 0.0008 *0.3</f>
         <v>1.74E-3</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14" s="4">
         <f xml:space="preserve"> (0.0006+0.3*0.0015)/(0.0006 + 0.0015+0.000036) * 0.002136/(0.002136+0.09+0.92)</f>
         <v>1.0374099923330462E-3</v>
       </c>
-      <c r="F14" s="24">
+      <c r="F14" s="4">
         <v>7.3000000000000001E-3</v>
       </c>
-      <c r="G14" s="24">
+      <c r="G14" s="4">
         <f xml:space="preserve"> (0.001+0.3*0.0008)/(0.001 + 0.0008+0.00009) * 0.003/(0.003+0.06+0.94)</f>
         <v>1.9623668676510149E-3</v>
       </c>
-      <c r="H14" s="24">
+      <c r="H14" s="4">
         <v>7.3000000000000001E-3</v>
       </c>
     </row>
@@ -2852,27 +2887,27 @@
       <c r="B15" t="s">
         <v>311</v>
       </c>
-      <c r="C15" s="24">
+      <c r="C15" s="4">
         <f xml:space="preserve"> 0.06/ (0.928+0.06+0.006)</f>
         <v>6.0362173038229376E-2</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="4">
         <f xml:space="preserve"> 0.06 / (0.96+0.06+0.002)</f>
         <v>5.8708414872798431E-2</v>
       </c>
-      <c r="E15" s="24">
+      <c r="E15" s="4">
         <f>E6</f>
         <v>0.09</v>
       </c>
-      <c r="F15" s="24">
+      <c r="F15" s="4">
         <f xml:space="preserve"> 0.07 / (0.928+0.07+0.009)</f>
         <v>6.95134061569017E-2</v>
       </c>
-      <c r="G15" s="24">
+      <c r="G15" s="4">
         <f>G6</f>
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="H15" s="24">
+      <c r="H15" s="4">
         <f xml:space="preserve"> 0.07 / (0.928+0.07+0.009)</f>
         <v>6.95134061569017E-2</v>
       </c>
@@ -2884,22 +2919,22 @@
       <c r="B16" t="s">
         <v>353</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="4">
         <v>24.75</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="4">
         <v>24.75</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="4">
         <v>24.75</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="4">
         <v>27.75</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="4">
         <v>24.75</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="4">
         <v>27.75</v>
       </c>
     </row>
@@ -2910,22 +2945,22 @@
       <c r="B17" t="s">
         <v>311</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="4">
         <v>0.33</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="4">
         <v>0.33</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="4">
         <v>0.33</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="4">
         <v>0.33</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="4">
         <v>0.33</v>
       </c>
-      <c r="H17" s="24">
+      <c r="H17" s="4">
         <v>0.33</v>
       </c>
     </row>
@@ -2945,17 +2980,17 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="25" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="25" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="s">
+      <c r="A25" s="25" t="s">
         <v>321</v>
       </c>
     </row>
@@ -2965,17 +3000,17 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="25" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="26" t="s">
+      <c r="A28" s="25" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="25" t="s">
         <v>340</v>
       </c>
     </row>
@@ -2983,6 +3018,9 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -3001,20 +3039,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33" t="s">
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
     </row>
     <row r="2" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -3274,20 +3312,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33" t="s">
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
     </row>
     <row r="2" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -5999,7 +6037,7 @@
   <dimension ref="A1:L95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6121,7 +6159,7 @@
       <c r="B5" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="30">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Stomach",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B5,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Large Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B5,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Small Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B5,'Percent BW'!$N$2:$X$2,0))</f>
         <v>1.5802847456629968E-2</v>
       </c>
@@ -6371,7 +6409,7 @@
       <c r="B14" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="31">
+      <c r="C14" s="30">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Total",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B14,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("GI Contents",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B14,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("Blood",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B14,'Percent BW'!$N$2:$X$2,0))-SUM(C2:C12)</f>
         <v>5.1820372533547543E-2</v>
       </c>
@@ -6483,7 +6521,7 @@
       <c r="B18" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="31">
+      <c r="C18" s="30">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Stomach",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B18,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Large Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B18,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Small Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B18,'Percent BW'!$N$2:$X$2,0))</f>
         <v>2.5852334412265577E-2</v>
       </c>
@@ -6707,7 +6745,7 @@
       <c r="B26" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="31">
+      <c r="C26" s="30">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Total",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B26,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("GI Contents",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B26,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("Blood",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B26,'Percent BW'!$N$2:$X$2,0))-SUM(C15:C25)</f>
         <v>5.2399992921151606E-2</v>
       </c>
@@ -6795,7 +6833,7 @@
       <c r="B30" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="31">
+      <c r="C30" s="30">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Stomach",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B30,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Large Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B30,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Small Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B30,'Percent BW'!$N$2:$X$2,0))</f>
         <v>4.0408654780552319E-2</v>
       </c>
@@ -6971,7 +7009,7 @@
       <c r="B38" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="31">
+      <c r="C38" s="30">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Total",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B38,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("GI Contents",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B38,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("Blood",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B38,'Percent BW'!$N$2:$X$2,0))-SUM(C27:C37)</f>
         <v>2.5418908119054118E-2</v>
       </c>
@@ -7083,7 +7121,7 @@
       <c r="B42" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C42" s="31">
+      <c r="C42" s="30">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Stomach",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B42,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Large Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B42,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Small Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B42,'Percent BW'!$N$2:$X$2,0))</f>
         <v>3.521811975832758E-2</v>
       </c>
@@ -7307,7 +7345,7 @@
       <c r="B50" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C50" s="31">
+      <c r="C50" s="30">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Total",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B50,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("GI Contents",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B50,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("Blood",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B50,'Percent BW'!$N$2:$X$2,0))-SUM(C39:C49)</f>
         <v>2.3649226512727495E-3</v>
       </c>
@@ -7419,7 +7457,7 @@
       <c r="B54" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="C54" s="31">
+      <c r="C54" s="30">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Stomach",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B54,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Large Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B54,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Small Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B54,'Percent BW'!$N$2:$X$2,0))</f>
         <v>4.8000000000000001E-2</v>
       </c>
@@ -7643,7 +7681,7 @@
       <c r="B62" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="C62" s="31">
+      <c r="C62" s="30">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Total",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B62,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("GI Contents",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B62,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("Blood",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B62,'Percent BW'!$N$2:$X$2,0))-SUM(C51:C61)</f>
         <v>2.5662489315418147E-2</v>
       </c>
@@ -7750,7 +7788,7 @@
       <c r="B66" s="20" t="s">
         <v>339</v>
       </c>
-      <c r="C66" s="31">
+      <c r="C66" s="30">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Stomach",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B66,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Large Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B66,'Percent BW'!$N$2:$X$2,0))+INDEX('Percent BW'!$N$4:$X$23,MATCH("Small Intestine",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B66,'Percent BW'!$N$2:$X$2,0))</f>
         <v>4.5999999999999999E-2</v>
       </c>
@@ -7974,7 +8012,7 @@
       <c r="B74" s="20" t="s">
         <v>339</v>
       </c>
-      <c r="C74" s="31">
+      <c r="C74" s="30">
         <f>INDEX('Percent BW'!$N$4:$X$23,MATCH("Total",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B74,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("GI Contents",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B74,'Percent BW'!$N$2:$X$2,0))-INDEX('Percent BW'!$N$4:$X$23,MATCH("Blood",'Percent BW'!$A$4:$A$23,0),MATCH(VolumeFlow!B74,'Percent BW'!$N$2:$X$2,0))-SUM(C63:C73)</f>
         <v>1.7528264277473893E-2</v>
       </c>
@@ -8002,15 +8040,15 @@
       <c r="F75" s="20"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A76" s="27"/>
+      <c r="A76" s="26"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A77" s="28" t="s">
+      <c r="A77" s="27" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A78" s="26" t="s">
+      <c r="A78" s="25" t="s">
         <v>319</v>
       </c>
     </row>
@@ -8037,8 +8075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A41" sqref="A31:A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8054,20 +8092,20 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="31" t="s">
         <v>360</v>
       </c>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32" t="s">
+      <c r="E1" s="31"/>
+      <c r="F1" s="31" t="s">
         <v>361</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32" t="s">
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31" t="s">
         <v>364</v>
       </c>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
@@ -9103,72 +9141,72 @@
       <c r="L30" s="2"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="26" t="s">
         <v>43</v>
       </c>
       <c r="L31" s="2"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="27" t="s">
+      <c r="A32" s="26" t="s">
         <v>42</v>
       </c>
       <c r="L32" s="2"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="27" t="s">
+      <c r="A33" s="26" t="s">
         <v>41</v>
       </c>
       <c r="L33" s="2"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="29" t="s">
+      <c r="A34" s="28" t="s">
         <v>359</v>
       </c>
       <c r="L34" s="2"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="26" t="s">
         <v>40</v>
       </c>
       <c r="L35" s="2"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="27" t="s">
+      <c r="A36" s="26" t="s">
         <v>358</v>
       </c>
       <c r="L36" s="2"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="27" t="s">
+      <c r="A37" s="26" t="s">
         <v>362</v>
       </c>
       <c r="L37" s="2"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="27" t="s">
+      <c r="A38" s="26" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="27" t="s">
+      <c r="A39" s="26" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="27" t="s">
+      <c r="A40" s="26" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="27" t="s">
+      <c r="A41" s="26" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="27"/>
+      <c r="A42" s="26"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="27"/>
+      <c r="A43" s="26"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
@@ -9176,82 +9214,82 @@
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="26" t="s">
+      <c r="A45" s="25" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="26" t="s">
+      <c r="A46" s="25" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="26" t="s">
+      <c r="A47" s="25" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="26" t="s">
+      <c r="A48" s="25" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="26" t="s">
+      <c r="A49" s="25" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="26" t="s">
+      <c r="A50" s="25" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="26" t="s">
+      <c r="A51" s="25" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="26" t="s">
+      <c r="A52" s="25" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="26" t="s">
+      <c r="A53" s="25" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="26" t="s">
+      <c r="A54" s="25" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="26" t="s">
+      <c r="A55" s="25" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="26" t="s">
+      <c r="A56" s="25" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="26" t="s">
+      <c r="A57" s="25" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="26" t="s">
+      <c r="A58" s="25" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="26" t="s">
+      <c r="A59" s="25" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="26" t="s">
+      <c r="A60" s="25" t="s">
         <v>374</v>
       </c>
     </row>
@@ -9277,28 +9315,28 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="33" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="33" t="s">
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -10766,17 +10804,17 @@
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="25" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="s">
+      <c r="A25" s="25" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
+      <c r="A26" s="25" t="s">
         <v>321</v>
       </c>
     </row>
@@ -11079,30 +11117,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="33" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -12743,16 +12781,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>

</xml_diff>

<commit_message>
Johanna noticed rabbit was off
</commit_message>
<xml_diff>
--- a/pkdata.xlsx
+++ b/pkdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\httk-datatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CB3359-D3F1-40C5-84BB-D773D6DCF24B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7041BCFB-8A65-471C-944F-D995B1FAC060}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="884" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="675" yWindow="7860" windowWidth="23040" windowHeight="7845" tabRatio="884" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic PK" sheetId="7" r:id="rId1"/>
@@ -2452,8 +2452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2513,8 +2513,7 @@
         <v>600</v>
       </c>
       <c r="G2" s="4">
-        <f>716*G6</f>
-        <v>40.812000000000005</v>
+        <v>716</v>
       </c>
       <c r="H2" s="4">
         <f>3465/5</f>
@@ -2545,8 +2544,7 @@
         <v>42.857142857142854</v>
       </c>
       <c r="G3" s="4">
-        <f>44*G5</f>
-        <v>110</v>
+        <v>44</v>
       </c>
       <c r="H3" s="4">
         <f>224/5</f>
@@ -2577,8 +2575,7 @@
         <v>231.40060868152614</v>
       </c>
       <c r="G4" s="4">
-        <f>212*G5^(1/4)</f>
-        <v>266.5758870927823</v>
+        <v>212</v>
       </c>
       <c r="H4" s="4">
         <f>Flows!L3</f>

</xml_diff>

<commit_message>
Fixed some incorrect txt outputs and added density info
</commit_message>
<xml_diff>
--- a/pkdata.xlsx
+++ b/pkdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\httk-datatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7041BCFB-8A65-471C-944F-D995B1FAC060}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDE74C9-4EC4-4609-9BA7-A8D9BFAABFB8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="7860" windowWidth="23040" windowHeight="7845" tabRatio="884" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2505" yWindow="735" windowWidth="21600" windowHeight="11835" tabRatio="884" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic PK" sheetId="7" r:id="rId1"/>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="378">
   <si>
     <t>Tissue</t>
   </si>
@@ -1822,6 +1822,12 @@
   </si>
   <si>
     <t>Httk estimate, various references needed; Lee 1972</t>
+  </si>
+  <si>
+    <t>Del Nero (2002)</t>
+  </si>
+  <si>
+    <t>Sun and Sethu (2017)</t>
   </si>
 </sst>
 </file>
@@ -2452,7 +2458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -10833,8 +10839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10849,6 +10855,9 @@
       <c r="B1" t="s">
         <v>32</v>
       </c>
+      <c r="C1" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -10857,6 +10866,9 @@
       <c r="B2" s="2">
         <v>0.91600000000000004</v>
       </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
       <c r="J2" t="str">
         <f>IF(ISBLANK('Percent BW'!I4),"",'Percent BW'!I4/'Human Density'!$B2)</f>
         <v/>
@@ -10870,6 +10882,9 @@
         <f>(1.016+1.033)/2</f>
         <v>1.0245</v>
       </c>
+      <c r="C3" t="s">
+        <v>338</v>
+      </c>
       <c r="J3" t="str">
         <f>IF(ISBLANK('Percent BW'!I5),"",'Percent BW'!I5/'Human Density'!$B3)</f>
         <v/>
@@ -10883,6 +10898,9 @@
         <f>'Composition of Bone'!G4</f>
         <v>1.9761971830985914</v>
       </c>
+      <c r="C4" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -10891,6 +10909,9 @@
       <c r="B5" s="2">
         <v>1.99</v>
       </c>
+      <c r="C5" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -10899,6 +10920,9 @@
       <c r="B6" s="2">
         <v>1.92</v>
       </c>
+      <c r="C6" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -10907,6 +10931,9 @@
       <c r="B7" s="2">
         <v>1.028</v>
       </c>
+      <c r="C7" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -10915,6 +10942,9 @@
       <c r="B8" s="2">
         <v>0.78300000000000003</v>
       </c>
+      <c r="C8" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -10924,6 +10954,9 @@
         <f>(1.03+1.041)/2</f>
         <v>1.0354999999999999</v>
       </c>
+      <c r="C9" t="s">
+        <v>338</v>
+      </c>
       <c r="J9" t="str">
         <f>IF(ISBLANK('Percent BW'!I7),"",'Percent BW'!I10/'Human Density'!$B6)</f>
         <v/>
@@ -10937,6 +10970,9 @@
         <f>('Percent BW'!B8*'Human Density'!B11+'Percent BW'!B9*'Human Density'!B12+'Percent BW'!B10*'Human Density'!B13)/SUM('Percent BW'!B8:B10)</f>
         <v>1.0443364928909953</v>
       </c>
+      <c r="C10" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -10946,6 +10982,9 @@
         <f>(1.048+1.052)/2</f>
         <v>1.05</v>
       </c>
+      <c r="C11" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -10955,6 +10994,9 @@
         <f>(1.041+1.047)/2</f>
         <v>1.044</v>
       </c>
+      <c r="C12" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -10963,6 +11005,9 @@
       <c r="B13" s="2">
         <v>1.042</v>
       </c>
+      <c r="C13" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -10971,6 +11016,9 @@
       <c r="B14" s="2">
         <v>1.03</v>
       </c>
+      <c r="C14" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -10979,6 +11027,9 @@
       <c r="B15" s="2">
         <v>1.05</v>
       </c>
+      <c r="C15" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -10987,8 +11038,11 @@
       <c r="B16" s="2">
         <v>1.05</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -10996,16 +11050,22 @@
         <f>(1.045+1.056)/2</f>
         <v>1.0505</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
       <c r="B18" s="2">
         <v>1.0409999999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -11013,8 +11073,11 @@
         <f>(1.04+1.05)/2</f>
         <v>1.0449999999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -11022,16 +11085,22 @@
         <f>(0.955*B23+0.045*B22)</f>
         <v>1.117305</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="2">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -11039,32 +11108,44 @@
         <f>(1.1+1.19)/2</f>
         <v>1.145</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="2">
         <v>1.1160000000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="2">
         <v>0.97099999999999997</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>14</v>
       </c>
       <c r="B25" s="2">
         <v>1.054</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -11072,26 +11153,52 @@
         <f>(1.036+1.066)/2</f>
         <v>1.0510000000000002</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
       <c r="B27" s="2">
         <v>1.125</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>70</v>
       </c>
       <c r="B28" s="2">
         <v>1.0249999999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>357</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1.02</v>
+      </c>
+      <c r="C29" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>338</v>
+        <v>44</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1.08</v>
+      </c>
+      <c r="C30" t="s">
+        <v>377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>